<commit_message>
Add 'No Helmet Hack 1_6'
This module hides helmets from view by placing helmets in the cloak slot. Each character maintains their own visibility setting. The helmets are visible on the inventory paperdoll for comparison and easy swapping. Item sets function normally.

closes #296
</commit_message>
<xml_diff>
--- a/source/tlk/strings.xlsx
+++ b/source/tlk/strings.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\DAO\archid\source\tlk\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D2432983-A989-46E1-ABE5-FB48D6BF19D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01709E5A-E30C-4E33-8676-95F069CAF8EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32265" yWindow="1830" windowWidth="24090" windowHeight="14835" xr2:uid="{A42EE72D-E1C4-43B6-AEA5-0014ED5180B1}"/>
+    <workbookView xWindow="1980" yWindow="2205" windowWidth="23625" windowHeight="14700" xr2:uid="{A42EE72D-E1C4-43B6-AEA5-0014ED5180B1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>C:/Users/Jim/Documents/BioWare/Dragon Age/addins/af_archid/module/override/</t>
   </si>
@@ -53,6 +53,28 @@
   </si>
   <si>
     <t>The Archid mod is a compilation of other mods plus some custom content. Some of teh external mods have been imported in to allow them to be merged together.</t>
+  </si>
+  <si>
+    <t>6610001</t>
+  </si>
+  <si>
+    <t>No Helmet Rulebook</t>
+  </si>
+  <si>
+    <t>6610002</t>
+  </si>
+  <si>
+    <t>The character using this book will toggle on/off helmet graphics.</t>
+  </si>
+  <si>
+    <t>6610003</t>
+  </si>
+  <si>
+    <t>WARNING!  The No_Helmet_Hack module failed to hide the helmets.  This is likely due to an incompatibility with a loaded module.  Possible solutions:
+1)  Check the My Documents/Bioware/Packages/Core/Overrides file for any BITM_* file.  Delete it if there is, as this would be the likely conflicting mod.
+2)  Remove this mod and reinstall it as the last mod
+3)  Remove other mods until this mod succeeds.  Suspect mods that change item properties.
+4)  Download and install the master override file.</t>
   </si>
 </sst>
 </file>
@@ -86,7 +108,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -105,6 +127,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -118,7 +146,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -128,6 +156,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -446,11 +475,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{723D158D-1FBF-4946-A52B-028752432AE5}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B12" sqref="B12"/>
+      <selection pane="bottomLeft" activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -469,11 +498,35 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="5" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="56.25" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -482,5 +535,8 @@
   </sortState>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="A3:A5" numberStoredAsText="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add 'Grey Wardens of Ferelden' mod
This mod will give you DA2 style Grey Warden armors and weapons for DA:O. This mod also changes the appearances of all Grey Warden NPCs into wearing a uniform Grey Warden armors.

closes #302
</commit_message>
<xml_diff>
--- a/source/tlk/strings.xlsx
+++ b/source/tlk/strings.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\DAO\archid\source\tlk\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01709E5A-E30C-4E33-8676-95F069CAF8EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{158A1E7D-DA4A-4A74-B01A-ADDAC156A55E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1980" yWindow="2205" windowWidth="23625" windowHeight="14700" xr2:uid="{A42EE72D-E1C4-43B6-AEA5-0014ED5180B1}"/>
+    <workbookView xWindow="2175" yWindow="3015" windowWidth="23625" windowHeight="14535" xr2:uid="{A42EE72D-E1C4-43B6-AEA5-0014ED5180B1}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="strings" localSheetId="0">Sheet1!$A$1:$B$2</definedName>
+    <definedName name="strings_1" localSheetId="0">Sheet2!$A$1:$B$57</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -29,10 +29,11 @@
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
-  <connection id="1" xr16:uid="{967CDDC0-4DDB-40A2-9474-C4C5CBF505D3}" name="strings" type="6" refreshedVersion="8" background="1" saveData="1">
-    <textPr codePage="65001" sourceFile="C:\Projects\DAO\archid_mod\source\strings.txt">
-      <textFields count="2">
-        <textField type="text"/>
+  <connection id="1" xr16:uid="{1EB83944-AEF7-421D-B818-FA2C25A3345F}" name="strings1" type="6" refreshedVersion="8" background="1" saveData="1">
+    <textPr sourceFile="C:\Projects\DAO\archid\source\tlk\strings.txt">
+      <textFields count="3">
+        <textField/>
+        <textField/>
         <textField/>
       </textFields>
     </textPr>
@@ -41,33 +42,156 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
-  <si>
-    <t>C:/Users/Jim/Documents/BioWare/Dragon Age/addins/af_archid/module/override/</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
   <si>
     <t>af_archid_en-us.tlk</t>
   </si>
   <si>
-    <t>6610000</t>
-  </si>
-  <si>
-    <t>The Archid mod is a compilation of other mods plus some custom content. Some of teh external mods have been imported in to allow them to be merged together.</t>
-  </si>
-  <si>
-    <t>6610001</t>
-  </si>
-  <si>
     <t>No Helmet Rulebook</t>
   </si>
   <si>
-    <t>6610002</t>
-  </si>
-  <si>
     <t>The character using this book will toggle on/off helmet graphics.</t>
   </si>
   <si>
-    <t>6610003</t>
+    <t>Grey Warden Heavy Boots</t>
+  </si>
+  <si>
+    <t>Heavy boots made by Grey Warden Smiths specially designed to be worn by Grey Warden Warriors.</t>
+  </si>
+  <si>
+    <t>Grey Warden Arcane Boots</t>
+  </si>
+  <si>
+    <t>Arcane boots made by Grey Warden Enchanters specially designed to be worn by Grey Warden Mages.</t>
+  </si>
+  <si>
+    <t>Grey Warden Commander Boots</t>
+  </si>
+  <si>
+    <t>Massive boots made by Grey Warden Mastersmiths specially designed to be worn by Grey Warden Commanders.</t>
+  </si>
+  <si>
+    <t>Blighted Grey Warden Commander Boots</t>
+  </si>
+  <si>
+    <t>Grey Warden Scout Boots</t>
+  </si>
+  <si>
+    <t>Medium boots made by Grey Warden Tailors specially designed to be worn by Grey Warden Scouts.</t>
+  </si>
+  <si>
+    <t>Grey Warden Heavy Armour</t>
+  </si>
+  <si>
+    <t>Heavy armour made by Grey Warden Smiths specially designed to be worn by Grey Warden Warriors.</t>
+  </si>
+  <si>
+    <t>Grey Warden Arcane Robes</t>
+  </si>
+  <si>
+    <t>Arcane robes made by Grey Warden Enchanters specially designed to be worn by Grey Warden Mages.</t>
+  </si>
+  <si>
+    <t>Grey Warden Commander Armour</t>
+  </si>
+  <si>
+    <t>Massive armour made by Grey Warden Mastersmiths specially designed to be worn by Grey Warden Commanders.</t>
+  </si>
+  <si>
+    <t>Grey Warden Scout Armour</t>
+  </si>
+  <si>
+    <t>Medium suits made by Grey Warden Tailors specially designed to be worn by Grey Warden Scouts.</t>
+  </si>
+  <si>
+    <t>Grey Warden Heavy Gloves</t>
+  </si>
+  <si>
+    <t>Heavy gloves made by Grey Warden Smiths specially designed to be worn by Grey Warden Warriors.</t>
+  </si>
+  <si>
+    <t>Grey Warden Arcane Gloves</t>
+  </si>
+  <si>
+    <t>Arcane gloves made by Grey Warden Enchanters specially designed to be worn by Grey Warden Mages.</t>
+  </si>
+  <si>
+    <t>Grey Warden Commander Gloves</t>
+  </si>
+  <si>
+    <t>Massive gloves made by Grey Warden Mastersmiths specially designed to be worn by Grey Warden Commanders.</t>
+  </si>
+  <si>
+    <t>Blighted Grey Warden Commander Gloves</t>
+  </si>
+  <si>
+    <t>Grey Warden Scout Gloves</t>
+  </si>
+  <si>
+    <t>Medium gloves made by Grey Warden Tailors specially designed to be worn by Grey Warden Scouts.</t>
+  </si>
+  <si>
+    <t>Grey Warden Heavy Helmet</t>
+  </si>
+  <si>
+    <t>Heavy helmets made by Grey Warden Smiths specially designed to be worn by Grey Warden Warriors.</t>
+  </si>
+  <si>
+    <t>Grey Warden Arcane Hood</t>
+  </si>
+  <si>
+    <t>Arcane hoods made by Grey Warden Enchanters specially designed to be worn by Grey Warden Mages.</t>
+  </si>
+  <si>
+    <t>Grey Warden Commander Helmet</t>
+  </si>
+  <si>
+    <t>Massive helmets made by Grey Warden Mastersmiths specially designed to be worn by Grey Warden Commanders.</t>
+  </si>
+  <si>
+    <t>Blighted Grey Warden Commander Helmet</t>
+  </si>
+  <si>
+    <t>Grey Warden Scout Hood</t>
+  </si>
+  <si>
+    <t>Medium hoods made by Grey Warden Tailors specially designed to be worn by Grey Warden Scouts.</t>
+  </si>
+  <si>
+    <t>Grey Warden Shield</t>
+  </si>
+  <si>
+    <t>The Shield of the Grey Wardens, marked with the stamp of the griffon upon its surface.</t>
+  </si>
+  <si>
+    <t>Grey Warden Staff</t>
+  </si>
+  <si>
+    <t>The Magic Staff of the Grey Wardens, marked with the shape of the griffon upon its head.</t>
+  </si>
+  <si>
+    <t>Grey Warden Dagger</t>
+  </si>
+  <si>
+    <t>The Dagger of the Grey Wardens, marked with the stamp of the griffon upon its blade.</t>
+  </si>
+  <si>
+    <t>Grey Warden Greatsword</t>
+  </si>
+  <si>
+    <t>The Greatsword of the Grey Wardens, marked with the stamp of the griffon upon its blade.</t>
+  </si>
+  <si>
+    <t>Grey Warden Longsword</t>
+  </si>
+  <si>
+    <t>The Longsword of the Grey Wardens, marked with the stamp of the griffon upon its blade.</t>
+  </si>
+  <si>
+    <t>Grey Warden Longbow</t>
+  </si>
+  <si>
+    <t>The Longbow of the Grey Wardens, marked with the stamp of the griffon upon its wooden surface.</t>
   </si>
   <si>
     <t>WARNING!  The No_Helmet_Hack module failed to hide the helmets.  This is likely due to an incompatibility with a loaded module.  Possible solutions:
@@ -76,21 +200,40 @@
 3)  Remove other mods until this mod succeeds.  Suspect mods that change item properties.
 4)  Download and install the master override file.</t>
   </si>
+  <si>
+    <t>When the darkspawn taint gets into contact with any material, it will corrode them and turning them into a blighted variant of itself if not regularly cleaned.
+This has happened to this pair of boots. Being worn by grey wardens for long periods of time with constant exposure to the darkspawn taint whether it is from the blood or from the wearer itself, corrode the metal parts and the cloth materials into a twisted reflection of what they once were.</t>
+  </si>
+  <si>
+    <t>When the darkspawn taint gets into contact with any material, it will corrode them and turning them into a blighted variant of itself if not regularly cleaned.
+This has happened to this armour. Being worn by grey wardens for long periods of time with constant exposure to the darkspawn taint whether it is from the blood or from the wearer itself, corrode the metal parts and the cloth materials into a twisted reflection of what they once were.</t>
+  </si>
+  <si>
+    <t>When the darkspawn taint gets into contact with any material, it will corrode them and turning them into a blighted variant of itself if not regularly cleaned.
+This has happened to this pair of gloves. Being worn by grey wardens for long periods of time with constant exposure to the darkspawn taint whether it is from the blood or from the wearer itself, corrode the metal parts and the cloth materials into a twisted reflection of what they once were.</t>
+  </si>
+  <si>
+    <t>When the darkspawn taint gets into contact with any material, it will corrode them and turning them into a blighted variant of itself if not regularly cleaned.
+This has happened to this helmet. Being worn by grey wardens for long periods of time with constant exposure to the darkspawn taint whether it is from the blood or from the wearer itself, corrode the metal parts and the cloth materials into a twisted reflection of what they once were.</t>
+  </si>
+  <si>
+    <t>Blighted Grey Warden Commander Armour</t>
+  </si>
+  <si>
+    <t>The Archid mod is a compilation of other mods plus some custom content. Some of the external mods have been imported in to allow them to be merged together.</t>
+  </si>
+  <si>
+    <t>C:\Projects\DAO\archid\addin\module\override\</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -148,15 +291,15 @@
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -175,7 +318,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="strings" connectionId="1" xr16:uid="{A368800C-0AC9-4A1C-8C15-22BE213D0D8C}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="strings_1" connectionId="1" xr16:uid="{6F9C22DF-D535-4A8C-ADBD-FD8727B0A604}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -474,69 +617,475 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{723D158D-1FBF-4946-A52B-028752432AE5}">
-  <dimension ref="A1:B5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C8288F5-46B5-435A-B9FC-40522281A8A6}">
+  <dimension ref="A1:B57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B10" sqref="B10"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12" style="2" customWidth="1"/>
-    <col min="2" max="2" width="164" style="3" customWidth="1"/>
+    <col min="1" max="1" width="11.85546875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="129.85546875" style="2" customWidth="1"/>
     <col min="3" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="3">
+        <v>6610000</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="4">
+        <v>6610001</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="5" t="s">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="4">
+        <v>6610002</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="3" t="s">
+    </row>
+    <row r="5" spans="1:2" ht="56.25" x14ac:dyDescent="0.2">
+      <c r="A5" s="4">
+        <v>6610003</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="3">
+        <v>6610004</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="3">
+        <v>6610005</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="3" t="s">
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="3">
+        <v>6610006</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="4" t="s">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="3">
+        <v>6610007</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="3" t="s">
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="3">
+        <v>6610008</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="56.25" x14ac:dyDescent="0.2">
-      <c r="A5" s="4" t="s">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="3">
+        <v>6610009</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="3" t="s">
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="3">
+        <v>6610010</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>9</v>
       </c>
     </row>
+    <row r="13" spans="1:2" ht="45" x14ac:dyDescent="0.2">
+      <c r="A13" s="3">
+        <v>6610011</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" s="3">
+        <v>6610012</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" s="3">
+        <v>6610013</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" s="3">
+        <v>6610014</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="3">
+        <v>6610015</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" s="3">
+        <v>6610016</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" s="3">
+        <v>6610017</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" s="3">
+        <v>6610018</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" s="3">
+        <v>6610019</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" s="3">
+        <v>6610020</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="45" x14ac:dyDescent="0.2">
+      <c r="A23" s="3">
+        <v>6610021</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" s="3">
+        <v>6610022</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" s="3">
+        <v>6610023</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" s="3">
+        <v>6610024</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" s="3">
+        <v>6610025</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" s="3">
+        <v>6610026</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29" s="3">
+        <v>6610027</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30" s="3">
+        <v>6610028</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31" s="3">
+        <v>6610029</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32" s="3">
+        <v>6610030</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="45" x14ac:dyDescent="0.2">
+      <c r="A33" s="3">
+        <v>6610031</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34" s="3">
+        <v>6610032</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35" s="3">
+        <v>6610033</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36" s="3">
+        <v>6610034</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37" s="3">
+        <v>6610035</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A38" s="3">
+        <v>6610036</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A39" s="3">
+        <v>6610037</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A40" s="3">
+        <v>6610038</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A41" s="3">
+        <v>6610039</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A42" s="3">
+        <v>6610040</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" ht="45" x14ac:dyDescent="0.2">
+      <c r="A43" s="3">
+        <v>6610041</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A44" s="3">
+        <v>6610042</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A45" s="3">
+        <v>6610043</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A46" s="3">
+        <v>6610044</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A47" s="3">
+        <v>6610045</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A48" s="3">
+        <v>6610046</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A49" s="3">
+        <v>6610047</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A50" s="3">
+        <v>6610048</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A51" s="3">
+        <v>6610049</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A52" s="3">
+        <v>6610050</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A53" s="3">
+        <v>6610051</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A54" s="3">
+        <v>6610052</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A55" s="3">
+        <v>6610053</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A56" s="3">
+        <v>6610054</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A57" s="3">
+        <v>6610055</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B2">
-    <sortCondition ref="A2"/>
-  </sortState>
-  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <ignoredErrors>
-    <ignoredError sqref="A3:A5" numberStoredAsText="1"/>
-  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add 'Improved Companion Items'
Most, if not all, companion items suck. They are effective and comparable to other similar items only at low levels at best. This mod boosts the item bonuses so you can keep them during at least most of the playthrough for a better roleplay and less headache.

closes #311
</commit_message>
<xml_diff>
--- a/source/tlk/strings.xlsx
+++ b/source/tlk/strings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\DAO\archid\source\tlk\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{158A1E7D-DA4A-4A74-B01A-ADDAC156A55E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAC5F8E8-842A-423E-B9F6-343E279CE4B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2175" yWindow="3015" windowWidth="23625" windowHeight="14535" xr2:uid="{A42EE72D-E1C4-43B6-AEA5-0014ED5180B1}"/>
   </bookViews>
@@ -27,6 +27,44 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Jim</author>
+  </authors>
+  <commentList>
+    <comment ref="A3" authorId="0" shapeId="0" xr:uid="{561C90B3-07F8-4450-A3DC-F2D3D8D0130B}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>No Helmet Hack</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A6" authorId="0" shapeId="0" xr:uid="{4B925596-9842-4317-936E-A5656940C5B0}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Grey Wardens of Ferelden</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
   <connection id="1" xr16:uid="{1EB83944-AEF7-421D-B818-FA2C25A3345F}" name="strings1" type="6" refreshedVersion="8" background="1" saveData="1">
@@ -230,7 +268,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -249,6 +287,13 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="5">
@@ -617,10 +662,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C8288F5-46B5-435A-B9FC-40522281A8A6}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C8288F5-46B5-435A-B9FC-40522281A8A6}">
   <dimension ref="A1:B57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1087,5 +1134,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Merge 'TSM Alistair's Rose'
A wearable amulet called ‘Alistair’s Rose’ will appear in inventory on first load after Alistair offers the plot version to the Warden. Requires an active romance with Alistair.

The script files have been reworked to use a bit flag rather than a plot and the game resources renamed to fit the mod convention.

closes #314
</commit_message>
<xml_diff>
--- a/source/tlk/strings.xlsx
+++ b/source/tlk/strings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\DAO\archid\source\tlk\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAC5F8E8-842A-423E-B9F6-343E279CE4B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40492A53-5D83-4640-8B79-ED0B1417E5BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2175" yWindow="3015" windowWidth="23625" windowHeight="14535" xr2:uid="{A42EE72D-E1C4-43B6-AEA5-0014ED5180B1}"/>
+    <workbookView xWindow="30075" yWindow="2010" windowWidth="23625" windowHeight="14535" xr2:uid="{A42EE72D-E1C4-43B6-AEA5-0014ED5180B1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -61,6 +61,20 @@
         </r>
       </text>
     </comment>
+    <comment ref="A58" authorId="0" shapeId="0" xr:uid="{30610ECD-9DBC-4D54-BDD2-CDE5D899BFDB}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>TSM Alistairs Rose</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
@@ -80,7 +94,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
   <si>
     <t>af_archid_en-us.tlk</t>
   </si>
@@ -262,6 +276,13 @@
   </si>
   <si>
     <t>C:\Projects\DAO\archid\addin\module\override\</t>
+  </si>
+  <si>
+    <t>Alistair's Rose</t>
+  </si>
+  <si>
+    <t>A beautiful rose with velvety petals of deep red. This was a gift from Alistair.
+Whether infused with lyrium, magically preserved, or just the perfect cultivar for cut flower arrangements, the enduring loveliness of this single perfect bloom serves as a reminder that rare and wonderful things can indeed be found amidst all the darkness.</t>
   </si>
 </sst>
 </file>
@@ -663,10 +684,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C8288F5-46B5-435A-B9FC-40522281A8A6}">
-  <dimension ref="A1:B57"/>
+  <dimension ref="A1:B59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="B73" sqref="B73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -1132,6 +1153,22 @@
         <v>49</v>
       </c>
     </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A58" s="4">
+        <v>6610056</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" ht="45" x14ac:dyDescent="0.2">
+      <c r="A59" s="4">
+        <v>6610057</v>
+      </c>
+      <c r="B59" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>

</xml_diff>

<commit_message>
Merge 'TSM Cord of the Beresaad'
With this mod, Sten will be equipped at recruitment with 'Cord of the Beresaad', an amulet-slot accessory with modest stats and restricted to Sten
Resources have been renamed to match the mod standard

closes #317
</commit_message>
<xml_diff>
--- a/source/tlk/strings.xlsx
+++ b/source/tlk/strings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\DAO\archid\source\tlk\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40492A53-5D83-4640-8B79-ED0B1417E5BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E480610-2B4B-4B12-8C3F-B55A878D8508}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="30075" yWindow="2010" windowWidth="23625" windowHeight="14535" xr2:uid="{A42EE72D-E1C4-43B6-AEA5-0014ED5180B1}"/>
   </bookViews>
@@ -75,6 +75,20 @@
         </r>
       </text>
     </comment>
+    <comment ref="A60" authorId="0" shapeId="0" xr:uid="{6EB613F7-15B2-484E-8A68-211C8FB011B7}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>TSM Cord of the Beresaad</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
@@ -94,7 +108,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="62">
   <si>
     <t>af_archid_en-us.tlk</t>
   </si>
@@ -284,12 +298,18 @@
     <t>A beautiful rose with velvety petals of deep red. This was a gift from Alistair.
 Whether infused with lyrium, magically preserved, or just the perfect cultivar for cut flower arrangements, the enduring loveliness of this single perfect bloom serves as a reminder that rare and wonderful things can indeed be found amidst all the darkness.</t>
   </si>
+  <si>
+    <t>Cord of the Beresaad</t>
+  </si>
+  <si>
+    <t>Intricately braided of many thin leather strands, this sturdy torc is otherwise unornamented.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -315,6 +335,13 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -684,10 +711,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C8288F5-46B5-435A-B9FC-40522281A8A6}">
-  <dimension ref="A1:B59"/>
+  <dimension ref="A1:B61"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="B73" sqref="B73"/>
+      <selection activeCell="B74" sqref="B74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -1169,6 +1196,22 @@
         <v>59</v>
       </c>
     </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A60" s="3">
+        <v>6610058</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A61" s="3">
+        <v>6610059</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>

</xml_diff>

<commit_message>
Add 'Armor of the Sten' plus updates
The base Armor of the Sten mod adds a really cool armor set for Sten to the game. However, because the item is a piece of clothing, it does not offer any armor bonus or fatigue penalties. This mod author did add an armor bonus, however without the fatigue penalty, it causes the armor to be overpowered.

I have added a fatigue penalty to the armor, and a set bonus with Heavy Chainmail boot and gloves. The armor has been moved to the mercenary outside of Lothering, who previously carried the Heavy Chainmail armor (meant for Sten).

Allows Epilogue!Sten to wear the snazzy Armor of the Sten, rather than some random massive armour I never put on him.

closes #321
</commit_message>
<xml_diff>
--- a/source/tlk/strings.xlsx
+++ b/source/tlk/strings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\DAO\archid\source\tlk\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E480610-2B4B-4B12-8C3F-B55A878D8508}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BED56DAE-8AF7-4348-8AC5-01203C8A6609}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30075" yWindow="2010" windowWidth="23625" windowHeight="14535" xr2:uid="{A42EE72D-E1C4-43B6-AEA5-0014ED5180B1}"/>
+    <workbookView xWindow="2250" yWindow="1845" windowWidth="23625" windowHeight="14535" xr2:uid="{A42EE72D-E1C4-43B6-AEA5-0014ED5180B1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -89,6 +89,20 @@
         </r>
       </text>
     </comment>
+    <comment ref="A62" authorId="0" shapeId="0" xr:uid="{D6F7610A-53A1-43C0-87AD-A9E18D4BFEC3}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Armour of the Sten</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
@@ -108,7 +122,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
   <si>
     <t>af_archid_en-us.tlk</t>
   </si>
@@ -303,6 +317,14 @@
   </si>
   <si>
     <t>Intricately braided of many thin leather strands, this sturdy torc is otherwise unornamented.</t>
+  </si>
+  <si>
+    <t>Armour of the Sten</t>
+  </si>
+  <si>
+    <t>Traditionally worn by a Sten of the Berasaad, this armour is light and functional for the protection it offers.
+Finely linked chainmail, exotic hardened leather plates, and carefully ornamented metals show the craftsmanship that went into this piece.
+As Qunari do not go by names, it is impossible to trace the origin of this armour, though it looks to have seen use in combat.</t>
   </si>
 </sst>
 </file>
@@ -711,10 +733,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C8288F5-46B5-435A-B9FC-40522281A8A6}">
-  <dimension ref="A1:B61"/>
+  <dimension ref="A1:B63"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="B74" sqref="B74"/>
+      <selection activeCell="B70" sqref="B70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -1212,6 +1234,22 @@
         <v>61</v>
       </c>
     </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A62" s="4">
+        <v>6610060</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
+      <c r="A63" s="4">
+        <v>6610061</v>
+      </c>
+      <c r="B63" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>

</xml_diff>

<commit_message>
Add 'Branch of the Cursed Tree Barnstokkr'
New mage staff with a cool vfx and projectiles, based on the Staff of the Magister Lord.
It replaces the 'piece of wood' found by your Mabari for immersion

closes #324
</commit_message>
<xml_diff>
--- a/source/tlk/strings.xlsx
+++ b/source/tlk/strings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\DAO\archid\source\tlk\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BED56DAE-8AF7-4348-8AC5-01203C8A6609}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8409EDED-89DF-47F1-9693-0D625C4DC837}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2250" yWindow="1845" windowWidth="23625" windowHeight="14535" xr2:uid="{A42EE72D-E1C4-43B6-AEA5-0014ED5180B1}"/>
+    <workbookView xWindow="30750" yWindow="1950" windowWidth="23625" windowHeight="14535" xr2:uid="{A42EE72D-E1C4-43B6-AEA5-0014ED5180B1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -122,7 +122,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="66">
   <si>
     <t>af_archid_en-us.tlk</t>
   </si>
@@ -325,6 +325,12 @@
     <t>Traditionally worn by a Sten of the Berasaad, this armour is light and functional for the protection it offers.
 Finely linked chainmail, exotic hardened leather plates, and carefully ornamented metals show the craftsmanship that went into this piece.
 As Qunari do not go by names, it is impossible to trace the origin of this armour, though it looks to have seen use in combat.</t>
+  </si>
+  <si>
+    <t>Branch of the Cursed Tree Barnstokkr</t>
+  </si>
+  <si>
+    <t>This twisted length of wood, carved with strange symbols, is one of the branches of the legendary Barnstokkr, a cursed tree located south of Kokari Wilds, in lands unknown. The legend says that the tree is doomed to burn forever because of a curse invoked by a witch who, before dying, killed all the Templars that was hunting, causing a huge explosion of flames malignant, near the oldest tree the forest where she lived. Since then, the tree burns eternally in these flames that are full of hatred, bitterness and rage. Probably, the symbols that were carved on the branch, used to contain and control the terrible evil energy emanating from these flames. Do not want to know where your Mabari found this branch, much less whom he belonged.</t>
   </si>
 </sst>
 </file>
@@ -733,10 +739,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C8288F5-46B5-435A-B9FC-40522281A8A6}">
-  <dimension ref="A1:B63"/>
+  <dimension ref="A1:B65"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="B70" sqref="B70"/>
+      <selection activeCell="A64" sqref="A64:A65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -1250,6 +1256,22 @@
         <v>63</v>
       </c>
     </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A64" s="3">
+        <v>6610062</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A65" s="3">
+        <v>6610063</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>

</xml_diff>

<commit_message>
Add 'Spell Shaping Skill'
Spell Shaping is a new skill for Dragon Age Origins that allows spell casters to shape and direct wide-area spells in a manner that does not hurt allies.

    Level 1: Spell Shaping Toggle is added. When active, the caster will shape and direct wide-area spells to avoid friendly-fire damage. Only party members are protected
    Level 2: Spell Shaping Toggle now provides Party members protection from the secondary effects of friendly spells such as knockdown, freezing and slow movement.
    Level 3: Spell Shaping Toggle now provides friendly-fire damage protection to all allies on the battlefield. Only Party members recieve protection from secondary effects.
    Level 4: Spell Shaping Toggle protects allies and party members from all friendly-fire damage and secondary effects.

The skill causes mana drain, which increases with game difficulty

closes #332
</commit_message>
<xml_diff>
--- a/source/tlk/strings.xlsx
+++ b/source/tlk/strings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\DAO\archid\source\tlk\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{974B52DC-2135-4E0B-B587-C16DDD66DEB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E25048A0-F6B5-43D1-8D86-0D331998D3FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2100" yWindow="1215" windowWidth="23625" windowHeight="14535" xr2:uid="{A42EE72D-E1C4-43B6-AEA5-0014ED5180B1}"/>
+    <workbookView xWindow="945" yWindow="2505" windowWidth="23625" windowHeight="14535" xr2:uid="{A42EE72D-E1C4-43B6-AEA5-0014ED5180B1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -41,7 +41,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>No Helmet Hack</t>
         </r>
@@ -55,7 +55,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Grey Wardens of Ferelden</t>
         </r>
@@ -69,7 +69,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>TSM Alistairs Rose</t>
         </r>
@@ -97,7 +97,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Armour of the Sten</t>
         </r>
@@ -111,7 +111,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Barnstokkr Staff</t>
         </r>
@@ -125,9 +125,47 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Character Respec</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A94" authorId="0" shapeId="0" xr:uid="{CA8EB93A-B44A-4333-83DF-FA4483E54830}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Spell Shaping</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A103" authorId="0" shapeId="0" xr:uid="{1C086E3D-48E6-447D-905B-7D8A28A7BDBD}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
             <charset val="1"/>
           </rPr>
-          <t>Character Respec</t>
+          <t>Generic spell tooltip text</t>
         </r>
       </text>
     </comment>
@@ -150,7 +188,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="106">
   <si>
     <t>af_archid_en-us.tlk</t>
   </si>
@@ -448,12 +486,61 @@
   <si>
     <t>Drink me!</t>
   </si>
+  <si>
+    <t>Spell Shaping</t>
+  </si>
+  <si>
+    <t>When active, the caster will shape and direct wide-area spells to avoid friendly fire at a cost of additional mana. Party members gain protection from the damage, with the additional mana spent based on the number of allies in the target area.</t>
+  </si>
+  <si>
+    <t>Improved Spell Shaping</t>
+  </si>
+  <si>
+    <t>Party members gain protection from the secondary effects of friendly spells such as knockdown, freezing and slow movement rate.</t>
+  </si>
+  <si>
+    <t>Expert Spell Shaping</t>
+  </si>
+  <si>
+    <t>Friendly fire damage protection is extended to all allies on the battlefield.</t>
+  </si>
+  <si>
+    <t>Master Spell Shaping</t>
+  </si>
+  <si>
+    <t>Allies and party members no longer experience any damage or secondary effects from friendly wide-area spells.</t>
+  </si>
+  <si>
+    <t>Warning: Spell Shaping Mod has detected a compatibility issue with one of the mods you have installed. Spell Shaping may not work properly.</t>
+  </si>
+  <si>
+    <t>&lt;name/&gt; (&lt;guitypename/&gt;)
+&lt;usetype/&gt;
+&lt;description/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;name/&gt; (&lt;guitypename/&gt;)
+&lt;usetype/&gt;
+Range: &lt;range/&gt;
+Activation: &lt;cost/&gt;
+Cooldown: &lt;cooldown/&gt;s
+&lt;requirements/&gt;
+&lt;description/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;name/&gt; (&lt;guitypename/&gt;)
+&lt;usetype/&gt;
+Range: &lt;range/&gt;
+Activation: &lt;cost/&gt;
+Cooldown: &lt;cooldown/&gt;s
+&lt;description/&gt;</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -478,14 +565,20 @@
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <charset val="1"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="5">
@@ -858,10 +951,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C8288F5-46B5-435A-B9FC-40522281A8A6}">
-  <dimension ref="A1:B93"/>
+  <dimension ref="A1:B105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="B79" sqref="B79"/>
+    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
+      <selection activeCell="A103" sqref="A103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -1615,6 +1708,102 @@
         <v>93</v>
       </c>
     </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A94" s="3">
+        <v>6610092</v>
+      </c>
+      <c r="B94" s="6" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A95" s="3">
+        <v>6610093</v>
+      </c>
+      <c r="B95" s="6" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A96" s="3">
+        <v>6610094</v>
+      </c>
+      <c r="B96" s="6" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A97" s="3">
+        <v>6610095</v>
+      </c>
+      <c r="B97" s="6" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A98" s="3">
+        <v>6610096</v>
+      </c>
+      <c r="B98" s="6" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A99" s="3">
+        <v>6610097</v>
+      </c>
+      <c r="B99" s="6" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A100" s="3">
+        <v>6610098</v>
+      </c>
+      <c r="B100" s="6" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A101" s="3">
+        <v>6610099</v>
+      </c>
+      <c r="B101" s="6" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A102" s="3">
+        <v>6610100</v>
+      </c>
+      <c r="B102" s="6" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" ht="45" x14ac:dyDescent="0.2">
+      <c r="A103" s="4">
+        <v>6610101</v>
+      </c>
+      <c r="B103" s="6" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" ht="101.25" x14ac:dyDescent="0.2">
+      <c r="A104" s="4">
+        <v>6610102</v>
+      </c>
+      <c r="B104" s="6" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" ht="78.75" x14ac:dyDescent="0.2">
+      <c r="A105" s="4">
+        <v>6610103</v>
+      </c>
+      <c r="B105" s="6" t="s">
+        <v>105</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>

</xml_diff>

<commit_message>
Add 'Shale Talents Reworked'
Shale Talents Reworked (STR) is a compilation of fixes and tweaks for Shale's talents that aims to iron out all bugs that were never officially fixed, as well as tweak all talents so that every tree fulfills effectively the tasks they are meant to fulfill.

Include the Stronger Regenerating Burst optional component

closes #337
</commit_message>
<xml_diff>
--- a/source/tlk/strings.xlsx
+++ b/source/tlk/strings.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\DAO\archid\source\tlk\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E25048A0-F6B5-43D1-8D86-0D331998D3FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BCF9F63-E28F-44DE-A15B-B673E6205AF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="945" yWindow="2505" windowWidth="23625" windowHeight="14535" xr2:uid="{A42EE72D-E1C4-43B6-AEA5-0014ED5180B1}"/>
+    <workbookView xWindow="3045" yWindow="1410" windowWidth="23625" windowHeight="16110" xr2:uid="{A42EE72D-E1C4-43B6-AEA5-0014ED5180B1}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="strings_1" localSheetId="0">Sheet2!$A$1:$B$57</definedName>
+    <definedName name="strings_1" localSheetId="0">Sheet1!$A$1:$B$57</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -169,6 +169,20 @@
         </r>
       </text>
     </comment>
+    <comment ref="A106" authorId="0" shapeId="0" xr:uid="{36F2032A-7E2E-4D1D-80E4-FBAD677E3696}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Shale Talents Reworked</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
@@ -188,7 +202,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="139">
   <si>
     <t>af_archid_en-us.tlk</t>
   </si>
@@ -534,6 +548,105 @@
 Activation: &lt;cost/&gt;
 Cooldown: &lt;cooldown/&gt;s
 &lt;description/&gt;</t>
+  </si>
+  <si>
+    <t>Shale activates a mode that focuses on offense, taking penalties to defense and armor in exchange for bonuses to damage and attack. Slam, Quake, and Killing Blow add bonuses to this mode.</t>
+  </si>
+  <si>
+    <t>Shale slams a stony fist into the enemy target. If the blow connects, it generates an automatic critical hit and knocks the target back. The target is also stunned briefly unless it passes a physical resistance check. After learning this talent, Shale gains bonuses to damage, attack, and armor penetration whenever Pulverizing Blows is active.</t>
+  </si>
+  <si>
+    <t>Shale strikes the ground repeatedly, sending out multiple shockwaves. Nearby creatures take damage and are knocked to the ground unless they pass a physical resistance check. They are also slowed briefly unless they pass another physical resistance check. After learning this talent, Shale gains a bonus to movement speed, while suffering a greater penalty to defense, whenever Pulverizing Blows is active.</t>
+  </si>
+  <si>
+    <t>Shale focuses strength into one devastating blow against an enemy. This attack gains bonus armor penetration and is an automatic critical hit if it connects. If the target has less than 50% health, this attack inflicts increasing damage as the target’s health diminishes. Shale suffers penalties to attack and stamina regeneration for a short time after using this attack. After learning this talent, Shale gains bonuses to damage, attack, armor penetration, and critical chance whenever Pulverizing Blows is active.</t>
+  </si>
+  <si>
+    <t>Shale activates a mode that focuses on defense, gaining bonuses to armor, physical, and elemental resistances, while suffering penalties to damage and critical chance. Whenever this mode is active, Shale’s threat toward all nearby enemies increases over time, making them more likely to target Shale. Bellow, Stone Will, and Regenerating Burst add bonuses to this mode.</t>
+  </si>
+  <si>
+    <t>Shale erupts with the sound of the Rock itself, stunning nearby enemies unless they pass a mental resistance check against Shale’s constitution. They are also dazed, and suffer penalties to attack and defense, unless they pass another mental resistance check against Shale’s constitution. Enemies stunned by this attack cannot resist being dazed. The power of this talent depends on Shale's constitution. This talent increases the bonuses of Stoneheart.</t>
+  </si>
+  <si>
+    <t>Shale attracts the attention of a single enemy, who now views Shale as the most urgent threat on the battlefield and is likely to target Shale. After this talent is learned, Stoneheart will also give Shale bonuses to health regeneration and stamina regeneration, and enemies are even more likely to target Shale when that mode is active.</t>
+  </si>
+  <si>
+    <t>Shale explodes with energy, damaging all nearby enemies. Enemies hit by the explosion are knocked down or knocked back unless they pass a physical resistance check against Shale’s constitution. They are also stunned unless they pass a mental resistance check against Shale’s constitution. The energy gives Shale a burst of health regeneration and stamina regeneration. The lower Shale's health or stamina, the stronger the regeneration. The power of this talent also depends on Shale's constitution. This talent further increases the bonuses of Stoneheart.</t>
+  </si>
+  <si>
+    <t>Shale activates a mode that enables long-range attacks, gaining a large defense bonus against missile attacks while suffering penalties to attack and movement speed. While in this mode, Shale emanates an aura that grants nearby party members bonuses to ranged critical chance and ranged attack speed. Hurl Rock, Earthen Grasp, and Rock Barrage add bonuses to this mode.</t>
+  </si>
+  <si>
+    <t>Shale pulls a rock from the ground and hurls it to a location, dealing physical damage to all creatures in the impact area. Creatures closer to the center of the impact take more damage, and those within 3 meters of the center are also knocked down unless they pass a physical resistance check against Shale's strength. Friendly fire possible. This talent increases the bonuses for party members and Shale’s missile deflection.</t>
+  </si>
+  <si>
+    <t>Shale pounds the earth, immobilizing enemies unless they pass a physical resistance check, in which case they suffer penalties to attack speed and movement speed instead. Shale’s willpower increases the duration of the effects. This talent further increases Shale’s missile deflection.</t>
+  </si>
+  <si>
+    <t>Shale tosses up multiple rocks that crash down in the targeted area. Creatures within the area take damage and are knocked down or knocked back unless they pass a physical resistance check. Friendly fire possible. This talent increases the bonuses for party members and Shale’s missile deflection. Nearby party members now also gain bonuses to attack and damage when using ranged weapons. Additionally, Shale’s aura can now shield others, granting party members within 3 meters a bonus to missile deflection.</t>
+  </si>
+  <si>
+    <t>Shale activates a support mode that imbues nearby party members with bonuses to defense, armor, and all resistances. Shale is immobilized when in this mode, suffering a penalty to defense while gaining bonuses to armor, physical, spell, and elemental resistances. Inner Reserves, Renewed Assault, and Supernatural Resilience add bonuses to this mode.</t>
+  </si>
+  <si>
+    <t>Whenever Stone Aura is active, party members within the aura now receive bonuses to health regeneration, stamina regeneration, and spellpower. This talent also increases the radius of Stone Aura.</t>
+  </si>
+  <si>
+    <t>Whenever Stone Aura is active, Shale gains additional bonuses to armor, spell, and elemental resistances. Party members within the aura gain additional bonuses to health regeneration, stamina regeneration, and spellpower, as well as a bonus to movement speed. This talent also increases the radius of Stone Aura.</t>
+  </si>
+  <si>
+    <t>Whenever Stone Aura is active, Shale gains additional bonuses to armor, physical, spell, and elemental resistances. Party members within the aura gain additional bonuses to defense, armor, and all resistances. The aura now also grants additional bonuses to party members when they stay close to Shale. This talent also increases the radius of Stone Aura.</t>
+  </si>
+  <si>
+    <t>Bonuses to damage and attack; penalties to defense and armor (Slam: bonus to armor penetration; Quake: bonus to movement speed).</t>
+  </si>
+  <si>
+    <t>Knocked down; possible penalty to movement speed.</t>
+  </si>
+  <si>
+    <t>Shale suffers reduced attack and stamina regeneration. Target is knocked down or knocked back.</t>
+  </si>
+  <si>
+    <t>Bonuses to armor, physical, and elemental resistances; penalties to damage and critical chance (Stone Will: bonus to health regeneration and stamina regeneration).</t>
+  </si>
+  <si>
+    <t>Stunned; possible penalties to attack and defense.</t>
+  </si>
+  <si>
+    <t>Shale gains increased health regeneration and stamina regeneration. Enemies are knocked down, knocked back, or stunned.</t>
+  </si>
+  <si>
+    <t>Shale gains increased missile deflection, but suffers reduced movement speed and attack. Party members gain bonuses to ranged critical chance and aim speed.</t>
+  </si>
+  <si>
+    <t>Paralyzed; penalties to attack speed and movement speed.</t>
+  </si>
+  <si>
+    <t>Knocked down or knocked back.</t>
+  </si>
+  <si>
+    <t>Shale is paralyzed but gains bonuses to armor and resistances. Party members gain bonuses to defense, armor, and resistances.</t>
+  </si>
+  <si>
+    <t>Bonuses to ranged attack and damage; possible bonus to missile deflection.</t>
+  </si>
+  <si>
+    <t>Bonuses to defense, armor, resistances, and spellpower.</t>
+  </si>
+  <si>
+    <t>Stone Will</t>
+  </si>
+  <si>
+    <t>With a will of stone, Shale becomes a living fortress. All active movement speed modifiers are immediately removed. For a time, Shale gains increased physical and mental resistances, and becomes immune to knockdown, knockback, and slip effects. All incoming damage is partially absorbed, until a maximum amount is reached. Shale is slowed during this time, but will also shrug off any incoming effect that would alter movement speed. The power of this talent depends on Shale's constitution. After this talent is learned, Shale gains bonuses to health regeneration and stamina regeneration whenever Stoneheart is active, and enemies are even more likely to target Shale.</t>
+  </si>
+  <si>
+    <t>Bonuses to physical and mental resistances; incoming damage is partially absorbed; immune to knockdown, knockback, slip, and movement speed modifications.</t>
+  </si>
+  <si>
+    <t>With a will of stone, Shale becomes a living fortress. All active movement speed modifiers are immediately removed. For a time, Shale gains increased physical and mental resistances, and becomes immune to knockdown, stun, and slip effects. All incoming damage is partially absorbed, until a maximum amount is reached. Shale is slowed during this time, but will also shrug off any incoming effect that would alter movement speed. The power of this talent depends on Shale's constitution. After this talent is learned, Shale gains bonuses to health regeneration and stamina regeneration whenever Stoneheart is active, and enemies are even more likely to target Shale.</t>
+  </si>
+  <si>
+    <t>Bonuses to physical and mental resistances; incoming damage is partially absorbed; immune to knockdown, stun, slip, and movement speed modifications.</t>
   </si>
 </sst>
 </file>
@@ -951,16 +1064,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C8288F5-46B5-435A-B9FC-40522281A8A6}">
-  <dimension ref="A1:B105"/>
+  <dimension ref="A1:B138"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
-      <selection activeCell="A103" sqref="A103"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B148" sqref="B148"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11.85546875" style="2" customWidth="1"/>
-    <col min="2" max="2" width="129.85546875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="152.85546875" style="2" customWidth="1"/>
     <col min="3" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
@@ -1804,6 +1917,270 @@
         <v>105</v>
       </c>
     </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A106" s="3">
+        <v>6610104</v>
+      </c>
+      <c r="B106" s="6" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A107" s="3">
+        <v>6610105</v>
+      </c>
+      <c r="B107" s="6" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A108" s="3">
+        <v>6610106</v>
+      </c>
+      <c r="B108" s="6" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
+      <c r="A109" s="3">
+        <v>6610107</v>
+      </c>
+      <c r="B109" s="6" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A110" s="3">
+        <v>6610108</v>
+      </c>
+      <c r="B110" s="6" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
+      <c r="A111" s="3">
+        <v>6610109</v>
+      </c>
+      <c r="B111" s="6" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A112" s="3">
+        <v>6610110</v>
+      </c>
+      <c r="B112" s="6" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
+      <c r="A113" s="3">
+        <v>6610111</v>
+      </c>
+      <c r="B113" s="6" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A114" s="3">
+        <v>6610112</v>
+      </c>
+      <c r="B114" s="6" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A115" s="3">
+        <v>6610113</v>
+      </c>
+      <c r="B115" s="6" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A116" s="3">
+        <v>6610114</v>
+      </c>
+      <c r="B116" s="6" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
+      <c r="A117" s="3">
+        <v>6610115</v>
+      </c>
+      <c r="B117" s="6" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A118" s="3">
+        <v>6610116</v>
+      </c>
+      <c r="B118" s="6" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A119" s="3">
+        <v>6610117</v>
+      </c>
+      <c r="B119" s="6" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A120" s="3">
+        <v>6610118</v>
+      </c>
+      <c r="B120" s="6" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A121" s="3">
+        <v>6610119</v>
+      </c>
+      <c r="B121" s="6" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A122" s="3">
+        <v>6610120</v>
+      </c>
+      <c r="B122" s="6" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A123" s="3">
+        <v>6610121</v>
+      </c>
+      <c r="B123" s="6" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A124" s="3">
+        <v>6610122</v>
+      </c>
+      <c r="B124" s="6" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A125" s="3">
+        <v>6610123</v>
+      </c>
+      <c r="B125" s="6" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A126" s="3">
+        <v>6610124</v>
+      </c>
+      <c r="B126" s="6" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A127" s="3">
+        <v>6610125</v>
+      </c>
+      <c r="B127" s="6" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A128" s="3">
+        <v>6610126</v>
+      </c>
+      <c r="B128" s="6" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A129" s="3">
+        <v>6610127</v>
+      </c>
+      <c r="B129" s="6" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A130" s="3">
+        <v>6610128</v>
+      </c>
+      <c r="B130" s="6" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A131" s="3">
+        <v>6610129</v>
+      </c>
+      <c r="B131" s="6" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A132" s="3">
+        <v>6610130</v>
+      </c>
+      <c r="B132" s="6" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A133" s="3">
+        <v>6610131</v>
+      </c>
+      <c r="B133" s="6" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A134" s="3">
+        <v>6610132</v>
+      </c>
+      <c r="B134" s="6" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" ht="45" x14ac:dyDescent="0.2">
+      <c r="A135" s="3">
+        <v>6610133</v>
+      </c>
+      <c r="B135" s="6" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A136" s="3">
+        <v>6610134</v>
+      </c>
+      <c r="B136" s="6" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" ht="45" x14ac:dyDescent="0.2">
+      <c r="A137" s="3">
+        <v>6610135</v>
+      </c>
+      <c r="B137" s="6" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A138" s="3">
+        <v>6610136</v>
+      </c>
+      <c r="B138" s="6" t="s">
+        <v>138</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>

</xml_diff>

<commit_message>
Add spells to open locks
Three spells have been created with increasing power, enabling the unlocking of more difficult locks. The power of the spell is modified by the casters spellpower, with each level of spell allowing for 2 levels of lock given sufficient spellpower:

Tier 1 spell: Simple & Very Easy
Tier 2 spell: Easy & Medium
Tier 3 spell: Hard & Very Hard

closes #344
</commit_message>
<xml_diff>
--- a/source/tlk/strings.xlsx
+++ b/source/tlk/strings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\DAO\archid\source\tlk\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BCF9F63-E28F-44DE-A15B-B673E6205AF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC2D4A93-1F75-4F7B-A5CF-E16233C659FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3045" yWindow="1410" windowWidth="23625" windowHeight="16110" xr2:uid="{A42EE72D-E1C4-43B6-AEA5-0014ED5180B1}"/>
+    <workbookView xWindow="4515" yWindow="1110" windowWidth="23625" windowHeight="16110" xr2:uid="{A42EE72D-E1C4-43B6-AEA5-0014ED5180B1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -183,6 +183,20 @@
         </r>
       </text>
     </comment>
+    <comment ref="A139" authorId="0" shapeId="0" xr:uid="{4B7B5849-A92F-4EEE-AF72-C63C79C3E804}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Unlock Spells</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
@@ -202,7 +216,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="149">
   <si>
     <t>af_archid_en-us.tlk</t>
   </si>
@@ -647,6 +661,36 @@
   </si>
   <si>
     <t>Bonuses to physical and mental resistances; incoming damage is partially absorbed; immune to knockdown, stun, slip, and movement speed modifications.</t>
+  </si>
+  <si>
+    <t>Arcane Unlock</t>
+  </si>
+  <si>
+    <t>A short burst of arcane magic will deal with most simple locks.</t>
+  </si>
+  <si>
+    <t>Finesse Unlock</t>
+  </si>
+  <si>
+    <t>More stubborn locks require some finesse. This spell is able to manipulate some of the inner components allowing opening of more complex locks.</t>
+  </si>
+  <si>
+    <t>Power Unlock</t>
+  </si>
+  <si>
+    <t>This spell allows you to channel more of your power into the lock, opening more complex varieties.</t>
+  </si>
+  <si>
+    <t>Spell too weak to unlock</t>
+  </si>
+  <si>
+    <t>Lock cannot be unlocked with magic</t>
+  </si>
+  <si>
+    <t>Wrong type of target to unlock</t>
+  </si>
+  <si>
+    <t>Target already unlocked</t>
   </si>
 </sst>
 </file>
@@ -1064,9 +1108,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C8288F5-46B5-435A-B9FC-40522281A8A6}">
-  <dimension ref="A1:B138"/>
+  <dimension ref="A1:B148"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A127" workbookViewId="0">
       <selection activeCell="B148" sqref="B148"/>
     </sheetView>
   </sheetViews>
@@ -2181,6 +2225,86 @@
         <v>138</v>
       </c>
     </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A139" s="4">
+        <v>6610137</v>
+      </c>
+      <c r="B139" s="6" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A140" s="4">
+        <v>6610138</v>
+      </c>
+      <c r="B140" s="6" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A141" s="4">
+        <v>6610139</v>
+      </c>
+      <c r="B141" s="6" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A142" s="4">
+        <v>6610140</v>
+      </c>
+      <c r="B142" s="6" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A143" s="4">
+        <v>6610141</v>
+      </c>
+      <c r="B143" s="6" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A144" s="4">
+        <v>6610142</v>
+      </c>
+      <c r="B144" s="6" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A145" s="4">
+        <v>6610143</v>
+      </c>
+      <c r="B145" s="6" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A146" s="4">
+        <v>6610144</v>
+      </c>
+      <c r="B146" s="6" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A147" s="4">
+        <v>6610145</v>
+      </c>
+      <c r="B147" s="6" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A148" s="4">
+        <v>6610146</v>
+      </c>
+      <c r="B148" s="6" t="s">
+        <v>148</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>

</xml_diff>

<commit_message>
Add 'Camp Merchant Chest'
Creates a storage chest by Bodahn Feddic's wagon in the Party Camp. Uses the Merchant UI, thereby providing categories, comparison with equipped gear, and far more space than a standard chest (such as the one at Warden's Keep). Simply 'Sell' to stash items (no, you won't make any money), and 'Buy' to retrieve (at no cost, of course).

This commit has not been tested so the issue cannot be closed at this time

see #358
</commit_message>
<xml_diff>
--- a/source/tlk/strings.xlsx
+++ b/source/tlk/strings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\DAO\archid\source\tlk\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC2D4A93-1F75-4F7B-A5CF-E16233C659FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CE088EB-7700-41CC-934D-54E58E6432EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4515" yWindow="1110" windowWidth="23625" windowHeight="16110" xr2:uid="{A42EE72D-E1C4-43B6-AEA5-0014ED5180B1}"/>
+    <workbookView xWindow="31815" yWindow="1410" windowWidth="23625" windowHeight="16110" xr2:uid="{A42EE72D-E1C4-43B6-AEA5-0014ED5180B1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -197,6 +197,20 @@
         </r>
       </text>
     </comment>
+    <comment ref="A149" authorId="0" shapeId="0" xr:uid="{6213D320-0ED5-4EB5-BA3A-56B633C2EE46}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Party Storage Chest</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
@@ -216,7 +230,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="150">
   <si>
     <t>af_archid_en-us.tlk</t>
   </si>
@@ -691,6 +705,9 @@
   </si>
   <si>
     <t>Target already unlocked</t>
+  </si>
+  <si>
+    <t>Party Storage Chest</t>
   </si>
 </sst>
 </file>
@@ -1108,10 +1125,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C8288F5-46B5-435A-B9FC-40522281A8A6}">
-  <dimension ref="A1:B148"/>
+  <dimension ref="A1:B149"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A127" workbookViewId="0">
-      <selection activeCell="B148" sqref="B148"/>
+    <sheetView tabSelected="1" topLeftCell="A124" workbookViewId="0">
+      <selection activeCell="B154" sqref="B154"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -2305,6 +2322,14 @@
         <v>148</v>
       </c>
     </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A149" s="3">
+        <v>6610147</v>
+      </c>
+      <c r="B149" s="2" t="s">
+        <v>149</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>

</xml_diff>

<commit_message>
Add 'Extra Dog Slot'
This mod allows the dog to tag along with the PC for most of the game as a
fifth companion residing in the top-most available summon slot. (summon slots
are mini-portraits that reside to the right of each NPC portrait.)

When presented with a party selection screen, if you do not choose the dog as
one of your 4 primary companions, he will automatically appear next to the PC
as a fifth companion after the selection screen goes away.

When present as a 5th party member, you can tell the dog to leave or call him
back by using a new Dog Whistle item which will appear in your inventory after
you aquire the dog as a companion.

While the mini-slot is normally used for summoned creatures, this mod manages
the slot so that the dog is a full blown party member and not a simple summon.
All dialog options, banter and special events and abilities involving the dog
will still work.

see #364
</commit_message>
<xml_diff>
--- a/source/tlk/strings.xlsx
+++ b/source/tlk/strings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\DAO\archid\source\tlk\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{479C38BD-011C-4287-839F-A2B4325ECF1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59C756A2-C020-4924-AB55-B81037FA8962}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2040" yWindow="1140" windowWidth="23625" windowHeight="16110" xr2:uid="{A42EE72D-E1C4-43B6-AEA5-0014ED5180B1}"/>
+    <workbookView xWindow="2790" yWindow="1335" windowWidth="23625" windowHeight="16110" xr2:uid="{A42EE72D-E1C4-43B6-AEA5-0014ED5180B1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -163,7 +163,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Generic spell tooltip text</t>
         </r>
@@ -177,7 +177,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Shale Talents Reworked</t>
         </r>
@@ -191,7 +191,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Unlock Spells</t>
         </r>
@@ -205,13 +205,13 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Party Storage Chest</t>
         </r>
       </text>
     </comment>
-    <comment ref="A150" authorId="0" shapeId="0" xr:uid="{15B7CDC5-6F21-45A0-9997-3CC9AFCCF646}">
+    <comment ref="A150" authorId="0" shapeId="0" xr:uid="{FB1284FC-F0BF-4154-AD86-621FF89FB794}">
       <text>
         <r>
           <rPr>
@@ -219,13 +219,13 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
-          <t>Spiders and Knives (1)</t>
+          <t>Extra Dog Slot</t>
         </r>
       </text>
     </comment>
-    <comment ref="A277" authorId="0" shapeId="0" xr:uid="{08441945-669A-47E4-A77A-BA32248BBBE4}">
+    <comment ref="A158" authorId="0" shapeId="0" xr:uid="{15B7CDC5-6F21-45A0-9997-3CC9AFCCF646}">
       <text>
         <r>
           <rPr>
@@ -233,7 +233,21 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
+          </rPr>
+          <t>Spiders and Knives (1)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A285" authorId="0" shapeId="0" xr:uid="{08441945-669A-47E4-A77A-BA32248BBBE4}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>Spiders and Knives (2)</t>
         </r>
@@ -258,7 +272,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="822" uniqueCount="789">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="830" uniqueCount="797">
   <si>
     <t>af_archid_en-us.tlk</t>
   </si>
@@ -2669,12 +2683,54 @@
   <si>
     <t>When Lothering fell to the darkspawn, Ser Bryant and his men were able to withdraw to Knife Edge. However they were unable to fight off subsequent darkspawn incursions, and the manor's defenders were all slaughtered.</t>
   </si>
+  <si>
+    <t>The Extra Dog Slot (EDS) Mod has detected a minor conflict with another mod.
+EVENT_TYPE_SUMMON_DIED is not getting routed to EDS. As a result, when summoned creatures die, the dog will not shift up to the uppermost summon slot. You will have to blow the whistle to re-summon the dog and shift the dog up manually.</t>
+  </si>
+  <si>
+    <t>The Extra Dog Slot (EDS) Mod has detected a conflict with another mod that you have installed.
+EVENT_TYPE_DYING is not getting routed to EDS. As a result, when the owner of the dog dies, the dog will die as well and the portrait will disappear. If this happens, you will have to blow the whistle following combat to dismiss and then summon the dog.</t>
+  </si>
+  <si>
+    <t>The Extra Dog Slot (EDS) Mod has detected a conflict with another mod that you have installed.
+EVENT_TYPE_PARTY_MEMBER_FIRED is not getting routed to EDS. As a result, you should make sure you blow the whistle and remove the dog BEFORE the game removes the party, or you may break the game.  Here is a known list of offending locations (you should probably write these down):
+Red Cliff:  When entering the fade to save the boy
+Circle OF Magi: When entering the fade because of the sloth demon on the 4th floor
+Orzamar : The provings.  Each round removes the party members
+Denerim : At the pearl. If you sleep with anyone, the party is removed.
+Denerim: If you win the lands meet and chose a 1 on 1 match with Logain.</t>
+  </si>
+  <si>
+    <t>The Extra Dog Slot (EDS) Mod has detected a conflict with another mod that you have installed.
+EVENT_TYPE_DYING is not getting routed to EDS. As a result, when the owner of the dog dies, the dog will die as well and the portrait will disappear. If this happens, you will have to blow the whistle following combat to dismiss and then summon the dog.
+EVENT_TYPE_PARTY_MEMBER_FIRED is not getting routed to EDS. As a result, you should make sure you blow the whistle and remove the dog BEFORE the game removes the party, or you may break the game.  Here is a known list of offending locations (you should probably write these down):
+Red Cliff:  When entering the fade to save the boy
+Circle OF Magi: When entering the fade because of the sloth demon on the 4th floor
+Orzamar : The provings.  Each round removes the party members
+Denerim : At the pearl. If you sleep with anyone, the party is removed.
+Denerim: If you win the lands meet and chose a 1 on 1 match with Logain.</t>
+  </si>
+  <si>
+    <t>The Extra Dog Slot (EDS) Mod has detected a minor conflict with another mod.
+EVENT_TYPE_COMMAND_PENDING or EVENT_TYPE_COMMAND_COMPLETE  is not getting routed to EDS. As a result, you should blow the whistle and remove the dog from the party before allowing Mages or Rogue-Rangers from summoning any creatures.</t>
+  </si>
+  <si>
+    <t>The Extra Dog Slot (EDS) Mod has detected a minor conflict with another mod.
+EVENT_TYPE_SUMMON_DIED is not getting routed to EDS. As a result, when summoned creatures die, the dog will not shift up to the uppermost summon slot. You will have to blow the whistle to re-summon the dog and shift the dog up manually.
+EVENT_TYPE_COMMAND_PENDING or EVENT_TYPE_COMMAND_COMPLETE  is not getting routed to EDS. As a result, you should blow the whistle and remove the dog from the party before allowing Mages or Rogue-Rangers from summoning any creatures.</t>
+  </si>
+  <si>
+    <t>Dog Wistle</t>
+  </si>
+  <si>
+    <t>You found this whistle around the neck of your Mabari.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2706,13 +2762,6 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="7">
@@ -3102,10 +3151,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C8288F5-46B5-435A-B9FC-40522281A8A6}">
-  <dimension ref="A1:B485"/>
+  <dimension ref="A1:B493"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A445" workbookViewId="0">
-      <selection activeCell="B282" sqref="B282"/>
+    <sheetView tabSelected="1" topLeftCell="A134" workbookViewId="0">
+      <selection activeCell="B151" sqref="B151"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -4307,2691 +4356,2755 @@
         <v>149</v>
       </c>
     </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A150" s="8" t="s">
-        <v>150</v>
+    <row r="150" spans="1:2" ht="45" x14ac:dyDescent="0.2">
+      <c r="A150" s="4">
+        <v>6610148</v>
       </c>
       <c r="B150" s="6" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A151" s="8" t="s">
-        <v>152</v>
+        <v>789</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" ht="45" x14ac:dyDescent="0.2">
+      <c r="A151" s="4">
+        <v>6610149</v>
       </c>
       <c r="B151" s="6" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A152" s="8" t="s">
-        <v>154</v>
+        <v>790</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" ht="101.25" x14ac:dyDescent="0.2">
+      <c r="A152" s="4">
+        <v>6610150</v>
       </c>
       <c r="B152" s="6" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="153" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A153" s="8" t="s">
-        <v>156</v>
+        <v>791</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" ht="135" x14ac:dyDescent="0.2">
+      <c r="A153" s="4">
+        <v>6610151</v>
       </c>
       <c r="B153" s="6" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A154" s="8" t="s">
-        <v>158</v>
+        <v>792</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" ht="45" x14ac:dyDescent="0.2">
+      <c r="A154" s="4">
+        <v>6610152</v>
       </c>
       <c r="B154" s="6" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="155" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
-      <c r="A155" s="8" t="s">
-        <v>160</v>
+        <v>793</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" ht="78.75" x14ac:dyDescent="0.2">
+      <c r="A155" s="4">
+        <v>6610153</v>
       </c>
       <c r="B155" s="6" t="s">
-        <v>161</v>
+        <v>794</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A156" s="8" t="s">
-        <v>162</v>
+      <c r="A156" s="4">
+        <v>6610154</v>
       </c>
       <c r="B156" s="6" t="s">
-        <v>163</v>
+        <v>795</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A157" s="8" t="s">
-        <v>164</v>
+      <c r="A157" s="4">
+        <v>6610155</v>
       </c>
       <c r="B157" s="6" t="s">
-        <v>165</v>
+        <v>796</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A158" s="8" t="s">
-        <v>166</v>
+        <v>150</v>
       </c>
       <c r="B158" s="6" t="s">
-        <v>167</v>
+        <v>151</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A159" s="8" t="s">
-        <v>168</v>
+        <v>152</v>
       </c>
       <c r="B159" s="6" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="160" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A160" s="8" t="s">
-        <v>170</v>
+        <v>154</v>
       </c>
       <c r="B160" s="6" t="s">
-        <v>171</v>
+        <v>155</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A161" s="8" t="s">
-        <v>172</v>
+        <v>156</v>
       </c>
       <c r="B161" s="6" t="s">
-        <v>173</v>
+        <v>157</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A162" s="8" t="s">
-        <v>174</v>
+        <v>158</v>
       </c>
       <c r="B162" s="6" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="163" spans="1:2" x14ac:dyDescent="0.2">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A163" s="8" t="s">
-        <v>176</v>
+        <v>160</v>
       </c>
       <c r="B163" s="6" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="164" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A164" s="8" t="s">
-        <v>177</v>
+        <v>162</v>
       </c>
       <c r="B164" s="6" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="165" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A165" s="8" t="s">
-        <v>179</v>
+        <v>164</v>
       </c>
       <c r="B165" s="6" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="166" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A166" s="8" t="s">
-        <v>181</v>
+        <v>166</v>
       </c>
       <c r="B166" s="6" t="s">
-        <v>182</v>
+        <v>167</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A167" s="8" t="s">
-        <v>183</v>
+        <v>168</v>
       </c>
       <c r="B167" s="6" t="s">
-        <v>184</v>
+        <v>169</v>
       </c>
     </row>
     <row r="168" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A168" s="8" t="s">
-        <v>185</v>
+        <v>170</v>
       </c>
       <c r="B168" s="6" t="s">
-        <v>186</v>
+        <v>171</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A169" s="8" t="s">
-        <v>187</v>
+        <v>172</v>
       </c>
       <c r="B169" s="6" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="170" spans="1:2" ht="90" x14ac:dyDescent="0.2">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A170" s="8" t="s">
-        <v>189</v>
+        <v>174</v>
       </c>
       <c r="B170" s="6" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="171" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="171" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A171" s="8" t="s">
-        <v>191</v>
+        <v>176</v>
       </c>
       <c r="B171" s="6" t="s">
-        <v>192</v>
+        <v>151</v>
       </c>
     </row>
     <row r="172" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A172" s="8" t="s">
-        <v>193</v>
+        <v>177</v>
       </c>
       <c r="B172" s="6" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="173" spans="1:2" x14ac:dyDescent="0.2">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A173" s="8" t="s">
-        <v>195</v>
+        <v>179</v>
       </c>
       <c r="B173" s="6" t="s">
-        <v>196</v>
+        <v>180</v>
       </c>
     </row>
     <row r="174" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A174" s="8" t="s">
-        <v>197</v>
+        <v>181</v>
       </c>
       <c r="B174" s="6" t="s">
-        <v>198</v>
+        <v>182</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A175" s="8" t="s">
-        <v>199</v>
+        <v>183</v>
       </c>
       <c r="B175" s="6" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="176" spans="1:2" x14ac:dyDescent="0.2">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="176" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A176" s="8" t="s">
-        <v>201</v>
+        <v>185</v>
       </c>
       <c r="B176" s="6" t="s">
-        <v>202</v>
+        <v>186</v>
       </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A177" s="8" t="s">
-        <v>203</v>
+        <v>187</v>
       </c>
       <c r="B177" s="6" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="178" spans="1:2" x14ac:dyDescent="0.2">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2" ht="90" x14ac:dyDescent="0.2">
       <c r="A178" s="8" t="s">
-        <v>204</v>
+        <v>189</v>
       </c>
       <c r="B178" s="6" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="179" spans="1:2" x14ac:dyDescent="0.2">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A179" s="8" t="s">
-        <v>206</v>
+        <v>191</v>
       </c>
       <c r="B179" s="6" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="180" spans="1:2" x14ac:dyDescent="0.2">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="180" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A180" s="8" t="s">
-        <v>208</v>
+        <v>193</v>
       </c>
       <c r="B180" s="6" t="s">
-        <v>209</v>
+        <v>194</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A181" s="8" t="s">
-        <v>210</v>
+        <v>195</v>
       </c>
       <c r="B181" s="6" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="182" spans="1:2" x14ac:dyDescent="0.2">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="182" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A182" s="8" t="s">
-        <v>212</v>
+        <v>197</v>
       </c>
       <c r="B182" s="6" t="s">
-        <v>213</v>
+        <v>198</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A183" s="8" t="s">
-        <v>214</v>
+        <v>199</v>
       </c>
       <c r="B183" s="6" t="s">
-        <v>215</v>
+        <v>200</v>
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A184" s="8" t="s">
-        <v>216</v>
+        <v>201</v>
       </c>
       <c r="B184" s="6" t="s">
-        <v>217</v>
+        <v>202</v>
       </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A185" s="8" t="s">
-        <v>218</v>
+        <v>203</v>
       </c>
       <c r="B185" s="6" t="s">
-        <v>219</v>
+        <v>153</v>
       </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A186" s="8" t="s">
-        <v>220</v>
+        <v>204</v>
       </c>
       <c r="B186" s="6" t="s">
-        <v>221</v>
+        <v>205</v>
       </c>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A187" s="8" t="s">
-        <v>222</v>
+        <v>206</v>
       </c>
       <c r="B187" s="6" t="s">
-        <v>223</v>
+        <v>207</v>
       </c>
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A188" s="8" t="s">
-        <v>224</v>
+        <v>208</v>
       </c>
       <c r="B188" s="6" t="s">
-        <v>225</v>
+        <v>209</v>
       </c>
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A189" s="8" t="s">
-        <v>226</v>
+        <v>210</v>
       </c>
       <c r="B189" s="6" t="s">
-        <v>227</v>
+        <v>211</v>
       </c>
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A190" s="8" t="s">
-        <v>228</v>
+        <v>212</v>
       </c>
       <c r="B190" s="6" t="s">
-        <v>229</v>
+        <v>213</v>
       </c>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A191" s="8" t="s">
-        <v>230</v>
+        <v>214</v>
       </c>
       <c r="B191" s="6" t="s">
-        <v>231</v>
+        <v>215</v>
       </c>
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A192" s="8" t="s">
-        <v>232</v>
+        <v>216</v>
       </c>
       <c r="B192" s="6" t="s">
-        <v>233</v>
+        <v>217</v>
       </c>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A193" s="8" t="s">
-        <v>234</v>
+        <v>218</v>
       </c>
       <c r="B193" s="6" t="s">
-        <v>235</v>
+        <v>219</v>
       </c>
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A194" s="8" t="s">
-        <v>236</v>
+        <v>220</v>
       </c>
       <c r="B194" s="6" t="s">
-        <v>237</v>
+        <v>221</v>
       </c>
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A195" s="8" t="s">
-        <v>238</v>
+        <v>222</v>
       </c>
       <c r="B195" s="6" t="s">
-        <v>239</v>
+        <v>223</v>
       </c>
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A196" s="8" t="s">
-        <v>240</v>
+        <v>224</v>
       </c>
       <c r="B196" s="6" t="s">
-        <v>241</v>
+        <v>225</v>
       </c>
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A197" s="8" t="s">
-        <v>242</v>
+        <v>226</v>
       </c>
       <c r="B197" s="6" t="s">
-        <v>243</v>
+        <v>227</v>
       </c>
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A198" s="8" t="s">
-        <v>244</v>
+        <v>228</v>
       </c>
       <c r="B198" s="6" t="s">
-        <v>245</v>
+        <v>229</v>
       </c>
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A199" s="8" t="s">
-        <v>246</v>
+        <v>230</v>
       </c>
       <c r="B199" s="6" t="s">
-        <v>247</v>
+        <v>231</v>
       </c>
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A200" s="8" t="s">
-        <v>248</v>
+        <v>232</v>
       </c>
       <c r="B200" s="6" t="s">
-        <v>249</v>
+        <v>233</v>
       </c>
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A201" s="8" t="s">
-        <v>250</v>
+        <v>234</v>
       </c>
       <c r="B201" s="6" t="s">
-        <v>251</v>
+        <v>235</v>
       </c>
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A202" s="8" t="s">
-        <v>252</v>
+        <v>236</v>
       </c>
       <c r="B202" s="6" t="s">
-        <v>253</v>
+        <v>237</v>
       </c>
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A203" s="8" t="s">
-        <v>254</v>
+        <v>238</v>
       </c>
       <c r="B203" s="6" t="s">
-        <v>255</v>
+        <v>239</v>
       </c>
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A204" s="8" t="s">
-        <v>256</v>
+        <v>240</v>
       </c>
       <c r="B204" s="6" t="s">
-        <v>257</v>
+        <v>241</v>
       </c>
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A205" s="8" t="s">
-        <v>258</v>
+        <v>242</v>
       </c>
       <c r="B205" s="6" t="s">
-        <v>259</v>
+        <v>243</v>
       </c>
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A206" s="8" t="s">
-        <v>260</v>
+        <v>244</v>
       </c>
       <c r="B206" s="6" t="s">
-        <v>261</v>
+        <v>245</v>
       </c>
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A207" s="8" t="s">
-        <v>262</v>
+        <v>246</v>
       </c>
       <c r="B207" s="6" t="s">
-        <v>263</v>
+        <v>247</v>
       </c>
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A208" s="8" t="s">
-        <v>264</v>
+        <v>248</v>
       </c>
       <c r="B208" s="6" t="s">
-        <v>265</v>
+        <v>249</v>
       </c>
     </row>
     <row r="209" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A209" s="8" t="s">
-        <v>266</v>
+        <v>250</v>
       </c>
       <c r="B209" s="6" t="s">
-        <v>267</v>
+        <v>251</v>
       </c>
     </row>
     <row r="210" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A210" s="8" t="s">
-        <v>268</v>
+        <v>252</v>
       </c>
       <c r="B210" s="6" t="s">
-        <v>269</v>
+        <v>253</v>
       </c>
     </row>
     <row r="211" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A211" s="8" t="s">
-        <v>270</v>
+        <v>254</v>
       </c>
       <c r="B211" s="6" t="s">
-        <v>271</v>
+        <v>255</v>
       </c>
     </row>
     <row r="212" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A212" s="8" t="s">
-        <v>272</v>
+        <v>256</v>
       </c>
       <c r="B212" s="6" t="s">
-        <v>273</v>
+        <v>257</v>
       </c>
     </row>
     <row r="213" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A213" s="8" t="s">
-        <v>274</v>
+        <v>258</v>
       </c>
       <c r="B213" s="6" t="s">
-        <v>275</v>
+        <v>259</v>
       </c>
     </row>
     <row r="214" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A214" s="8" t="s">
-        <v>276</v>
+        <v>260</v>
       </c>
       <c r="B214" s="6" t="s">
-        <v>277</v>
+        <v>261</v>
       </c>
     </row>
     <row r="215" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A215" s="8" t="s">
-        <v>278</v>
+        <v>262</v>
       </c>
       <c r="B215" s="6" t="s">
-        <v>279</v>
+        <v>263</v>
       </c>
     </row>
     <row r="216" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A216" s="8" t="s">
-        <v>280</v>
+        <v>264</v>
       </c>
       <c r="B216" s="6" t="s">
-        <v>281</v>
+        <v>265</v>
       </c>
     </row>
     <row r="217" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A217" s="8" t="s">
-        <v>282</v>
+        <v>266</v>
       </c>
       <c r="B217" s="6" t="s">
-        <v>283</v>
+        <v>267</v>
       </c>
     </row>
     <row r="218" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A218" s="8" t="s">
-        <v>284</v>
+        <v>268</v>
       </c>
       <c r="B218" s="6" t="s">
-        <v>285</v>
+        <v>269</v>
       </c>
     </row>
     <row r="219" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A219" s="8" t="s">
-        <v>286</v>
+        <v>270</v>
       </c>
       <c r="B219" s="6" t="s">
-        <v>287</v>
+        <v>271</v>
       </c>
     </row>
     <row r="220" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A220" s="8" t="s">
-        <v>288</v>
+        <v>272</v>
       </c>
       <c r="B220" s="6" t="s">
-        <v>289</v>
+        <v>273</v>
       </c>
     </row>
     <row r="221" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A221" s="8" t="s">
-        <v>290</v>
+        <v>274</v>
       </c>
       <c r="B221" s="6" t="s">
-        <v>291</v>
+        <v>275</v>
       </c>
     </row>
     <row r="222" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A222" s="8" t="s">
-        <v>292</v>
+        <v>276</v>
       </c>
       <c r="B222" s="6" t="s">
-        <v>293</v>
+        <v>277</v>
       </c>
     </row>
     <row r="223" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A223" s="8" t="s">
-        <v>294</v>
+        <v>278</v>
       </c>
       <c r="B223" s="6" t="s">
-        <v>295</v>
+        <v>279</v>
       </c>
     </row>
     <row r="224" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A224" s="8" t="s">
-        <v>296</v>
+        <v>280</v>
       </c>
       <c r="B224" s="6" t="s">
-        <v>295</v>
+        <v>281</v>
       </c>
     </row>
     <row r="225" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A225" s="8" t="s">
-        <v>297</v>
+        <v>282</v>
       </c>
       <c r="B225" s="6" t="s">
-        <v>298</v>
+        <v>283</v>
       </c>
     </row>
     <row r="226" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A226" s="8" t="s">
-        <v>299</v>
+        <v>284</v>
       </c>
       <c r="B226" s="6" t="s">
-        <v>237</v>
+        <v>285</v>
       </c>
     </row>
     <row r="227" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A227" s="8" t="s">
-        <v>300</v>
+        <v>286</v>
       </c>
       <c r="B227" s="6" t="s">
-        <v>239</v>
+        <v>287</v>
       </c>
     </row>
     <row r="228" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A228" s="8" t="s">
-        <v>301</v>
+        <v>288</v>
       </c>
       <c r="B228" s="6" t="s">
-        <v>302</v>
+        <v>289</v>
       </c>
     </row>
     <row r="229" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A229" s="8" t="s">
-        <v>303</v>
+        <v>290</v>
       </c>
       <c r="B229" s="6" t="s">
-        <v>304</v>
+        <v>291</v>
       </c>
     </row>
     <row r="230" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A230" s="8" t="s">
-        <v>305</v>
+        <v>292</v>
       </c>
       <c r="B230" s="6" t="s">
-        <v>306</v>
+        <v>293</v>
       </c>
     </row>
     <row r="231" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A231" s="8" t="s">
-        <v>307</v>
+        <v>294</v>
       </c>
       <c r="B231" s="6" t="s">
-        <v>308</v>
+        <v>295</v>
       </c>
     </row>
     <row r="232" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A232" s="8" t="s">
-        <v>309</v>
+        <v>296</v>
       </c>
       <c r="B232" s="6" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="233" spans="1:2" ht="22.5" x14ac:dyDescent="0.2">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="233" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A233" s="8" t="s">
-        <v>311</v>
-      </c>
-      <c r="B233" s="7" t="s">
-        <v>312</v>
+        <v>297</v>
+      </c>
+      <c r="B233" s="6" t="s">
+        <v>298</v>
       </c>
     </row>
     <row r="234" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A234" s="8" t="s">
-        <v>313</v>
+        <v>299</v>
       </c>
       <c r="B234" s="6" t="s">
-        <v>314</v>
+        <v>237</v>
       </c>
     </row>
     <row r="235" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A235" s="8" t="s">
-        <v>315</v>
+        <v>300</v>
       </c>
       <c r="B235" s="6" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="236" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="236" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A236" s="8" t="s">
-        <v>317</v>
+        <v>301</v>
       </c>
       <c r="B236" s="6" t="s">
-        <v>318</v>
+        <v>302</v>
       </c>
     </row>
     <row r="237" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A237" s="8" t="s">
-        <v>319</v>
+        <v>303</v>
       </c>
       <c r="B237" s="6" t="s">
-        <v>320</v>
+        <v>304</v>
       </c>
     </row>
     <row r="238" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A238" s="8" t="s">
-        <v>321</v>
+        <v>305</v>
       </c>
       <c r="B238" s="6" t="s">
-        <v>322</v>
+        <v>306</v>
       </c>
     </row>
     <row r="239" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A239" s="8" t="s">
-        <v>323</v>
+        <v>307</v>
       </c>
       <c r="B239" s="6" t="s">
-        <v>324</v>
+        <v>308</v>
       </c>
     </row>
     <row r="240" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A240" s="8" t="s">
-        <v>325</v>
+        <v>309</v>
       </c>
       <c r="B240" s="6" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="241" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="241" spans="1:2" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A241" s="8" t="s">
-        <v>327</v>
-      </c>
-      <c r="B241" s="6" t="s">
-        <v>328</v>
+        <v>311</v>
+      </c>
+      <c r="B241" s="7" t="s">
+        <v>312</v>
       </c>
     </row>
     <row r="242" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A242" s="8" t="s">
-        <v>329</v>
+        <v>313</v>
       </c>
       <c r="B242" s="6" t="s">
-        <v>295</v>
+        <v>314</v>
       </c>
     </row>
     <row r="243" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A243" s="8" t="s">
-        <v>330</v>
+        <v>315</v>
       </c>
       <c r="B243" s="6" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="244" spans="1:2" x14ac:dyDescent="0.2">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="244" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A244" s="8" t="s">
-        <v>332</v>
+        <v>317</v>
       </c>
       <c r="B244" s="6" t="s">
-        <v>333</v>
+        <v>318</v>
       </c>
     </row>
     <row r="245" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A245" s="8" t="s">
-        <v>334</v>
+        <v>319</v>
       </c>
       <c r="B245" s="6" t="s">
-        <v>335</v>
+        <v>320</v>
       </c>
     </row>
     <row r="246" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A246" s="8" t="s">
-        <v>336</v>
+        <v>321</v>
       </c>
       <c r="B246" s="6" t="s">
-        <v>337</v>
+        <v>322</v>
       </c>
     </row>
     <row r="247" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A247" s="8" t="s">
-        <v>338</v>
+        <v>323</v>
       </c>
       <c r="B247" s="6" t="s">
-        <v>339</v>
+        <v>324</v>
       </c>
     </row>
     <row r="248" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A248" s="8" t="s">
-        <v>340</v>
+        <v>325</v>
       </c>
       <c r="B248" s="6" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="249" spans="1:2" x14ac:dyDescent="0.2">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="249" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A249" s="8" t="s">
-        <v>342</v>
+        <v>327</v>
       </c>
       <c r="B249" s="6" t="s">
-        <v>343</v>
+        <v>328</v>
       </c>
     </row>
     <row r="250" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A250" s="8" t="s">
-        <v>344</v>
+        <v>329</v>
       </c>
       <c r="B250" s="6" t="s">
-        <v>345</v>
+        <v>295</v>
       </c>
     </row>
     <row r="251" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A251" s="8" t="s">
-        <v>346</v>
+        <v>330</v>
       </c>
       <c r="B251" s="6" t="s">
-        <v>347</v>
+        <v>331</v>
       </c>
     </row>
     <row r="252" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A252" s="8" t="s">
-        <v>348</v>
+        <v>332</v>
       </c>
       <c r="B252" s="6" t="s">
-        <v>349</v>
+        <v>333</v>
       </c>
     </row>
     <row r="253" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A253" s="8" t="s">
-        <v>350</v>
+        <v>334</v>
       </c>
       <c r="B253" s="6" t="s">
-        <v>351</v>
+        <v>335</v>
       </c>
     </row>
     <row r="254" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A254" s="8" t="s">
-        <v>352</v>
+        <v>336</v>
       </c>
       <c r="B254" s="6" t="s">
-        <v>353</v>
+        <v>337</v>
       </c>
     </row>
     <row r="255" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A255" s="8" t="s">
-        <v>354</v>
+        <v>338</v>
       </c>
       <c r="B255" s="6" t="s">
-        <v>355</v>
+        <v>339</v>
       </c>
     </row>
     <row r="256" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A256" s="8" t="s">
-        <v>356</v>
+        <v>340</v>
       </c>
       <c r="B256" s="6" t="s">
-        <v>357</v>
+        <v>341</v>
       </c>
     </row>
     <row r="257" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A257" s="8" t="s">
-        <v>358</v>
+        <v>342</v>
       </c>
       <c r="B257" s="6" t="s">
-        <v>359</v>
+        <v>343</v>
       </c>
     </row>
     <row r="258" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A258" s="8" t="s">
-        <v>360</v>
+        <v>344</v>
       </c>
       <c r="B258" s="6" t="s">
-        <v>77</v>
+        <v>345</v>
       </c>
     </row>
     <row r="259" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A259" s="8" t="s">
-        <v>361</v>
+        <v>346</v>
       </c>
       <c r="B259" s="6" t="s">
-        <v>362</v>
+        <v>347</v>
       </c>
     </row>
     <row r="260" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A260" s="8" t="s">
-        <v>363</v>
+        <v>348</v>
       </c>
       <c r="B260" s="6" t="s">
-        <v>364</v>
+        <v>349</v>
       </c>
     </row>
     <row r="261" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A261" s="8" t="s">
-        <v>365</v>
+        <v>350</v>
       </c>
       <c r="B261" s="6" t="s">
-        <v>366</v>
+        <v>351</v>
       </c>
     </row>
     <row r="262" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A262" s="8" t="s">
-        <v>367</v>
+        <v>352</v>
       </c>
       <c r="B262" s="6" t="s">
-        <v>368</v>
+        <v>353</v>
       </c>
     </row>
     <row r="263" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A263" s="8" t="s">
-        <v>369</v>
+        <v>354</v>
       </c>
       <c r="B263" s="6" t="s">
-        <v>370</v>
+        <v>355</v>
       </c>
     </row>
     <row r="264" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A264" s="8" t="s">
-        <v>371</v>
+        <v>356</v>
       </c>
       <c r="B264" s="6" t="s">
-        <v>372</v>
+        <v>357</v>
       </c>
     </row>
     <row r="265" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A265" s="8" t="s">
-        <v>373</v>
+        <v>358</v>
       </c>
       <c r="B265" s="6" t="s">
-        <v>77</v>
+        <v>359</v>
       </c>
     </row>
     <row r="266" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A266" s="8" t="s">
-        <v>374</v>
+        <v>360</v>
       </c>
       <c r="B266" s="6" t="s">
-        <v>281</v>
+        <v>77</v>
       </c>
     </row>
     <row r="267" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A267" s="8" t="s">
-        <v>375</v>
+        <v>361</v>
       </c>
       <c r="B267" s="6" t="s">
-        <v>376</v>
+        <v>362</v>
       </c>
     </row>
     <row r="268" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A268" s="8" t="s">
-        <v>377</v>
+        <v>363</v>
       </c>
       <c r="B268" s="6" t="s">
-        <v>378</v>
+        <v>364</v>
       </c>
     </row>
     <row r="269" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A269" s="8" t="s">
-        <v>379</v>
+        <v>365</v>
       </c>
       <c r="B269" s="6" t="s">
-        <v>380</v>
+        <v>366</v>
       </c>
     </row>
     <row r="270" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A270" s="8" t="s">
-        <v>381</v>
+        <v>367</v>
       </c>
       <c r="B270" s="6" t="s">
-        <v>382</v>
+        <v>368</v>
       </c>
     </row>
     <row r="271" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A271" s="8" t="s">
-        <v>383</v>
+        <v>369</v>
       </c>
       <c r="B271" s="6" t="s">
-        <v>384</v>
+        <v>370</v>
       </c>
     </row>
     <row r="272" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A272" s="8" t="s">
-        <v>385</v>
+        <v>371</v>
       </c>
       <c r="B272" s="6" t="s">
-        <v>386</v>
+        <v>372</v>
       </c>
     </row>
     <row r="273" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A273" s="8" t="s">
-        <v>387</v>
+        <v>373</v>
       </c>
       <c r="B273" s="6" t="s">
-        <v>388</v>
+        <v>77</v>
       </c>
     </row>
     <row r="274" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A274" s="8" t="s">
-        <v>389</v>
+        <v>374</v>
       </c>
       <c r="B274" s="6" t="s">
-        <v>175</v>
+        <v>281</v>
       </c>
     </row>
     <row r="275" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A275" s="8" t="s">
-        <v>390</v>
+        <v>375</v>
       </c>
       <c r="B275" s="6" t="s">
-        <v>391</v>
+        <v>376</v>
       </c>
     </row>
     <row r="276" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A276" s="8" t="s">
+        <v>377</v>
+      </c>
+      <c r="B276" s="6" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="277" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A277" s="8" t="s">
+        <v>379</v>
+      </c>
+      <c r="B277" s="6" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="278" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A278" s="8" t="s">
+        <v>381</v>
+      </c>
+      <c r="B278" s="6" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="279" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A279" s="8" t="s">
+        <v>383</v>
+      </c>
+      <c r="B279" s="6" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="280" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A280" s="8" t="s">
+        <v>385</v>
+      </c>
+      <c r="B280" s="6" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="281" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A281" s="8" t="s">
+        <v>387</v>
+      </c>
+      <c r="B281" s="6" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="282" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A282" s="8" t="s">
+        <v>389</v>
+      </c>
+      <c r="B282" s="6" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="283" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A283" s="8" t="s">
+        <v>390</v>
+      </c>
+      <c r="B283" s="6" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="284" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A284" s="8" t="s">
         <v>392</v>
       </c>
-      <c r="B276" s="6" t="s">
+      <c r="B284" s="6" t="s">
         <v>393</v>
-      </c>
-    </row>
-    <row r="277" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A277" s="9" t="s">
-        <v>394</v>
-      </c>
-      <c r="B277" s="6" t="s">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="278" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A278" s="9" t="s">
-        <v>396</v>
-      </c>
-      <c r="B278" s="6" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="279" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A279" s="9" t="s">
-        <v>398</v>
-      </c>
-      <c r="B279" s="6" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="280" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A280" s="9" t="s">
-        <v>400</v>
-      </c>
-      <c r="B280" s="6" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="281" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A281" s="9" t="s">
-        <v>402</v>
-      </c>
-      <c r="B281" s="6" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="282" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A282" s="9" t="s">
-        <v>404</v>
-      </c>
-      <c r="B282" s="6" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="283" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A283" s="9" t="s">
-        <v>406</v>
-      </c>
-      <c r="B283" s="6" t="s">
-        <v>407</v>
-      </c>
-    </row>
-    <row r="284" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A284" s="9" t="s">
-        <v>408</v>
-      </c>
-      <c r="B284" s="6" t="s">
-        <v>409</v>
       </c>
     </row>
     <row r="285" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A285" s="9" t="s">
-        <v>410</v>
+        <v>394</v>
       </c>
       <c r="B285" s="6" t="s">
-        <v>409</v>
+        <v>395</v>
       </c>
     </row>
     <row r="286" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A286" s="9" t="s">
-        <v>411</v>
+        <v>396</v>
       </c>
       <c r="B286" s="6" t="s">
-        <v>412</v>
+        <v>397</v>
       </c>
     </row>
     <row r="287" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A287" s="9" t="s">
-        <v>413</v>
+        <v>398</v>
       </c>
       <c r="B287" s="6" t="s">
-        <v>412</v>
+        <v>399</v>
       </c>
     </row>
     <row r="288" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A288" s="9" t="s">
-        <v>414</v>
+        <v>400</v>
       </c>
       <c r="B288" s="6" t="s">
-        <v>215</v>
+        <v>401</v>
       </c>
     </row>
     <row r="289" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A289" s="9" t="s">
-        <v>415</v>
+        <v>402</v>
       </c>
       <c r="B289" s="6" t="s">
-        <v>217</v>
+        <v>403</v>
       </c>
     </row>
     <row r="290" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A290" s="9" t="s">
-        <v>416</v>
+        <v>404</v>
       </c>
       <c r="B290" s="6" t="s">
-        <v>401</v>
+        <v>405</v>
       </c>
     </row>
     <row r="291" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A291" s="9" t="s">
-        <v>417</v>
+        <v>406</v>
       </c>
       <c r="B291" s="6" t="s">
-        <v>403</v>
+        <v>407</v>
       </c>
     </row>
     <row r="292" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A292" s="9" t="s">
-        <v>418</v>
+        <v>408</v>
       </c>
       <c r="B292" s="6" t="s">
-        <v>405</v>
+        <v>409</v>
       </c>
     </row>
     <row r="293" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A293" s="9" t="s">
-        <v>419</v>
+        <v>410</v>
       </c>
       <c r="B293" s="6" t="s">
-        <v>407</v>
+        <v>409</v>
       </c>
     </row>
     <row r="294" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A294" s="9" t="s">
-        <v>420</v>
+        <v>411</v>
       </c>
       <c r="B294" s="6" t="s">
-        <v>395</v>
+        <v>412</v>
       </c>
     </row>
     <row r="295" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A295" s="9" t="s">
-        <v>421</v>
+        <v>413</v>
       </c>
       <c r="B295" s="6" t="s">
-        <v>397</v>
+        <v>412</v>
       </c>
     </row>
     <row r="296" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A296" s="9" t="s">
-        <v>422</v>
+        <v>414</v>
       </c>
       <c r="B296" s="6" t="s">
-        <v>399</v>
+        <v>215</v>
       </c>
     </row>
     <row r="297" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A297" s="9" t="s">
-        <v>423</v>
+        <v>415</v>
       </c>
       <c r="B297" s="6" t="s">
-        <v>273</v>
+        <v>217</v>
       </c>
     </row>
     <row r="298" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A298" s="9" t="s">
-        <v>424</v>
+        <v>416</v>
       </c>
       <c r="B298" s="6" t="s">
-        <v>275</v>
+        <v>401</v>
       </c>
     </row>
     <row r="299" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A299" s="9" t="s">
-        <v>425</v>
+        <v>417</v>
       </c>
       <c r="B299" s="6" t="s">
-        <v>320</v>
+        <v>403</v>
       </c>
     </row>
     <row r="300" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A300" s="9" t="s">
-        <v>426</v>
+        <v>418</v>
       </c>
       <c r="B300" s="6" t="s">
-        <v>281</v>
+        <v>405</v>
       </c>
     </row>
     <row r="301" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A301" s="9" t="s">
-        <v>427</v>
+        <v>419</v>
       </c>
       <c r="B301" s="6" t="s">
-        <v>428</v>
+        <v>407</v>
       </c>
     </row>
     <row r="302" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A302" s="9" t="s">
-        <v>429</v>
+        <v>420</v>
       </c>
       <c r="B302" s="6" t="s">
-        <v>295</v>
+        <v>395</v>
       </c>
     </row>
     <row r="303" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A303" s="9" t="s">
-        <v>430</v>
+        <v>421</v>
       </c>
       <c r="B303" s="6" t="s">
-        <v>431</v>
+        <v>397</v>
       </c>
     </row>
     <row r="304" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A304" s="9" t="s">
-        <v>432</v>
+        <v>422</v>
       </c>
       <c r="B304" s="6" t="s">
-        <v>433</v>
+        <v>399</v>
       </c>
     </row>
     <row r="305" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A305" s="9" t="s">
-        <v>434</v>
+        <v>423</v>
       </c>
       <c r="B305" s="6" t="s">
-        <v>435</v>
+        <v>273</v>
       </c>
     </row>
     <row r="306" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A306" s="9" t="s">
-        <v>436</v>
+        <v>424</v>
       </c>
       <c r="B306" s="6" t="s">
-        <v>437</v>
+        <v>275</v>
       </c>
     </row>
     <row r="307" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A307" s="9" t="s">
-        <v>438</v>
+        <v>425</v>
       </c>
       <c r="B307" s="6" t="s">
-        <v>439</v>
+        <v>320</v>
       </c>
     </row>
     <row r="308" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A308" s="9" t="s">
-        <v>440</v>
+        <v>426</v>
       </c>
       <c r="B308" s="6" t="s">
-        <v>441</v>
+        <v>281</v>
       </c>
     </row>
     <row r="309" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A309" s="9" t="s">
-        <v>442</v>
+        <v>427</v>
       </c>
       <c r="B309" s="6" t="s">
-        <v>443</v>
+        <v>428</v>
       </c>
     </row>
     <row r="310" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A310" s="9" t="s">
-        <v>444</v>
+        <v>429</v>
       </c>
       <c r="B310" s="6" t="s">
-        <v>407</v>
+        <v>295</v>
       </c>
     </row>
     <row r="311" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A311" s="9" t="s">
-        <v>445</v>
+        <v>430</v>
       </c>
       <c r="B311" s="6" t="s">
-        <v>446</v>
+        <v>431</v>
       </c>
     </row>
     <row r="312" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A312" s="9" t="s">
-        <v>447</v>
+        <v>432</v>
       </c>
       <c r="B312" s="6" t="s">
-        <v>448</v>
+        <v>433</v>
       </c>
     </row>
     <row r="313" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A313" s="9" t="s">
-        <v>449</v>
+        <v>434</v>
       </c>
       <c r="B313" s="6" t="s">
-        <v>450</v>
+        <v>435</v>
       </c>
     </row>
     <row r="314" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A314" s="9" t="s">
-        <v>451</v>
+        <v>436</v>
       </c>
       <c r="B314" s="6" t="s">
-        <v>452</v>
+        <v>437</v>
       </c>
     </row>
     <row r="315" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A315" s="9" t="s">
-        <v>453</v>
+        <v>438</v>
       </c>
       <c r="B315" s="6" t="s">
-        <v>454</v>
+        <v>439</v>
       </c>
     </row>
     <row r="316" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A316" s="9" t="s">
-        <v>455</v>
+        <v>440</v>
       </c>
       <c r="B316" s="6" t="s">
-        <v>456</v>
+        <v>441</v>
       </c>
     </row>
     <row r="317" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A317" s="9" t="s">
-        <v>457</v>
+        <v>442</v>
       </c>
       <c r="B317" s="6" t="s">
-        <v>458</v>
+        <v>443</v>
       </c>
     </row>
     <row r="318" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A318" s="9" t="s">
-        <v>459</v>
+        <v>444</v>
       </c>
       <c r="B318" s="6" t="s">
-        <v>460</v>
+        <v>407</v>
       </c>
     </row>
     <row r="319" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A319" s="9" t="s">
-        <v>461</v>
+        <v>445</v>
       </c>
       <c r="B319" s="6" t="s">
-        <v>462</v>
+        <v>446</v>
       </c>
     </row>
     <row r="320" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A320" s="9" t="s">
-        <v>463</v>
+        <v>447</v>
       </c>
       <c r="B320" s="6" t="s">
-        <v>464</v>
+        <v>448</v>
       </c>
     </row>
     <row r="321" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A321" s="9" t="s">
-        <v>465</v>
+        <v>449</v>
       </c>
       <c r="B321" s="6" t="s">
-        <v>466</v>
+        <v>450</v>
       </c>
     </row>
     <row r="322" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A322" s="9" t="s">
-        <v>467</v>
+        <v>451</v>
       </c>
       <c r="B322" s="6" t="s">
-        <v>468</v>
+        <v>452</v>
       </c>
     </row>
     <row r="323" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A323" s="9" t="s">
-        <v>469</v>
+        <v>453</v>
       </c>
       <c r="B323" s="6" t="s">
-        <v>470</v>
+        <v>454</v>
       </c>
     </row>
     <row r="324" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A324" s="9" t="s">
-        <v>471</v>
+        <v>455</v>
       </c>
       <c r="B324" s="6" t="s">
-        <v>472</v>
+        <v>456</v>
       </c>
     </row>
     <row r="325" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A325" s="9" t="s">
-        <v>473</v>
+        <v>457</v>
       </c>
       <c r="B325" s="6" t="s">
-        <v>474</v>
+        <v>458</v>
       </c>
     </row>
     <row r="326" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A326" s="9" t="s">
-        <v>475</v>
+        <v>459</v>
       </c>
       <c r="B326" s="6" t="s">
-        <v>476</v>
+        <v>460</v>
       </c>
     </row>
     <row r="327" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A327" s="9" t="s">
-        <v>477</v>
+        <v>461</v>
       </c>
       <c r="B327" s="6" t="s">
-        <v>478</v>
+        <v>462</v>
       </c>
     </row>
     <row r="328" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A328" s="9" t="s">
-        <v>479</v>
+        <v>463</v>
       </c>
       <c r="B328" s="6" t="s">
-        <v>480</v>
+        <v>464</v>
       </c>
     </row>
     <row r="329" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A329" s="9" t="s">
-        <v>481</v>
+        <v>465</v>
       </c>
       <c r="B329" s="6" t="s">
-        <v>482</v>
+        <v>466</v>
       </c>
     </row>
     <row r="330" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A330" s="9" t="s">
-        <v>483</v>
+        <v>467</v>
       </c>
       <c r="B330" s="6" t="s">
-        <v>484</v>
+        <v>468</v>
       </c>
     </row>
     <row r="331" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A331" s="9" t="s">
-        <v>485</v>
+        <v>469</v>
       </c>
       <c r="B331" s="6" t="s">
-        <v>486</v>
+        <v>470</v>
       </c>
     </row>
     <row r="332" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A332" s="9" t="s">
-        <v>487</v>
+        <v>471</v>
       </c>
       <c r="B332" s="6" t="s">
-        <v>488</v>
+        <v>472</v>
       </c>
     </row>
     <row r="333" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A333" s="9" t="s">
-        <v>489</v>
+        <v>473</v>
       </c>
       <c r="B333" s="6" t="s">
-        <v>490</v>
+        <v>474</v>
       </c>
     </row>
     <row r="334" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A334" s="9" t="s">
-        <v>491</v>
+        <v>475</v>
       </c>
       <c r="B334" s="6" t="s">
-        <v>492</v>
+        <v>476</v>
       </c>
     </row>
     <row r="335" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A335" s="9" t="s">
-        <v>493</v>
+        <v>477</v>
       </c>
       <c r="B335" s="6" t="s">
-        <v>494</v>
+        <v>478</v>
       </c>
     </row>
     <row r="336" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A336" s="9" t="s">
-        <v>495</v>
+        <v>479</v>
       </c>
       <c r="B336" s="6" t="s">
-        <v>496</v>
+        <v>480</v>
       </c>
     </row>
     <row r="337" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A337" s="9" t="s">
-        <v>497</v>
+        <v>481</v>
       </c>
       <c r="B337" s="6" t="s">
-        <v>498</v>
+        <v>482</v>
       </c>
     </row>
     <row r="338" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A338" s="9" t="s">
-        <v>499</v>
+        <v>483</v>
       </c>
       <c r="B338" s="6" t="s">
-        <v>500</v>
+        <v>484</v>
       </c>
     </row>
     <row r="339" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A339" s="9" t="s">
-        <v>501</v>
+        <v>485</v>
       </c>
       <c r="B339" s="6" t="s">
-        <v>502</v>
+        <v>486</v>
       </c>
     </row>
     <row r="340" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A340" s="9" t="s">
-        <v>503</v>
+        <v>487</v>
       </c>
       <c r="B340" s="6" t="s">
-        <v>504</v>
+        <v>488</v>
       </c>
     </row>
     <row r="341" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A341" s="9" t="s">
-        <v>505</v>
+        <v>489</v>
       </c>
       <c r="B341" s="6" t="s">
-        <v>506</v>
+        <v>490</v>
       </c>
     </row>
     <row r="342" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A342" s="9" t="s">
-        <v>507</v>
+        <v>491</v>
       </c>
       <c r="B342" s="6" t="s">
-        <v>508</v>
+        <v>492</v>
       </c>
     </row>
     <row r="343" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A343" s="9" t="s">
-        <v>509</v>
+        <v>493</v>
       </c>
       <c r="B343" s="6" t="s">
-        <v>510</v>
+        <v>494</v>
       </c>
     </row>
     <row r="344" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A344" s="9" t="s">
-        <v>511</v>
+        <v>495</v>
       </c>
       <c r="B344" s="6" t="s">
-        <v>512</v>
+        <v>496</v>
       </c>
     </row>
     <row r="345" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A345" s="9" t="s">
-        <v>513</v>
+        <v>497</v>
       </c>
       <c r="B345" s="6" t="s">
-        <v>514</v>
+        <v>498</v>
       </c>
     </row>
     <row r="346" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A346" s="9" t="s">
-        <v>515</v>
+        <v>499</v>
       </c>
       <c r="B346" s="6" t="s">
-        <v>516</v>
+        <v>500</v>
       </c>
     </row>
     <row r="347" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A347" s="9" t="s">
-        <v>517</v>
+        <v>501</v>
       </c>
       <c r="B347" s="6" t="s">
-        <v>518</v>
+        <v>502</v>
       </c>
     </row>
     <row r="348" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A348" s="9" t="s">
-        <v>519</v>
+        <v>503</v>
       </c>
       <c r="B348" s="6" t="s">
-        <v>520</v>
+        <v>504</v>
       </c>
     </row>
     <row r="349" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A349" s="9" t="s">
-        <v>521</v>
+        <v>505</v>
       </c>
       <c r="B349" s="6" t="s">
-        <v>522</v>
+        <v>506</v>
       </c>
     </row>
     <row r="350" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A350" s="9" t="s">
-        <v>523</v>
+        <v>507</v>
       </c>
       <c r="B350" s="6" t="s">
-        <v>524</v>
+        <v>508</v>
       </c>
     </row>
     <row r="351" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A351" s="9" t="s">
-        <v>525</v>
+        <v>509</v>
       </c>
       <c r="B351" s="6" t="s">
-        <v>526</v>
+        <v>510</v>
       </c>
     </row>
     <row r="352" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A352" s="9" t="s">
-        <v>527</v>
+        <v>511</v>
       </c>
       <c r="B352" s="6" t="s">
-        <v>528</v>
+        <v>512</v>
       </c>
     </row>
     <row r="353" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A353" s="9" t="s">
-        <v>529</v>
+        <v>513</v>
       </c>
       <c r="B353" s="6" t="s">
-        <v>530</v>
+        <v>514</v>
       </c>
     </row>
     <row r="354" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A354" s="9" t="s">
-        <v>531</v>
+        <v>515</v>
       </c>
       <c r="B354" s="6" t="s">
-        <v>532</v>
+        <v>516</v>
       </c>
     </row>
     <row r="355" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A355" s="9" t="s">
-        <v>533</v>
+        <v>517</v>
       </c>
       <c r="B355" s="6" t="s">
-        <v>534</v>
+        <v>518</v>
       </c>
     </row>
     <row r="356" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A356" s="9" t="s">
-        <v>535</v>
+        <v>519</v>
       </c>
       <c r="B356" s="6" t="s">
-        <v>536</v>
+        <v>520</v>
       </c>
     </row>
     <row r="357" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A357" s="9" t="s">
-        <v>537</v>
+        <v>521</v>
       </c>
       <c r="B357" s="6" t="s">
-        <v>538</v>
+        <v>522</v>
       </c>
     </row>
     <row r="358" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A358" s="9" t="s">
-        <v>539</v>
+        <v>523</v>
       </c>
       <c r="B358" s="6" t="s">
-        <v>540</v>
+        <v>524</v>
       </c>
     </row>
     <row r="359" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A359" s="9" t="s">
-        <v>541</v>
+        <v>525</v>
       </c>
       <c r="B359" s="6" t="s">
-        <v>542</v>
+        <v>526</v>
       </c>
     </row>
     <row r="360" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A360" s="9" t="s">
-        <v>543</v>
+        <v>527</v>
       </c>
       <c r="B360" s="6" t="s">
-        <v>544</v>
+        <v>528</v>
       </c>
     </row>
     <row r="361" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A361" s="9" t="s">
-        <v>545</v>
+        <v>529</v>
       </c>
       <c r="B361" s="6" t="s">
-        <v>546</v>
+        <v>530</v>
       </c>
     </row>
     <row r="362" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A362" s="9" t="s">
-        <v>547</v>
+        <v>531</v>
       </c>
       <c r="B362" s="6" t="s">
-        <v>548</v>
+        <v>532</v>
       </c>
     </row>
     <row r="363" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A363" s="9" t="s">
-        <v>549</v>
+        <v>533</v>
       </c>
       <c r="B363" s="6" t="s">
-        <v>550</v>
+        <v>534</v>
       </c>
     </row>
     <row r="364" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A364" s="9" t="s">
-        <v>551</v>
+        <v>535</v>
       </c>
       <c r="B364" s="6" t="s">
-        <v>552</v>
+        <v>536</v>
       </c>
     </row>
     <row r="365" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A365" s="9" t="s">
-        <v>553</v>
+        <v>537</v>
       </c>
       <c r="B365" s="6" t="s">
-        <v>554</v>
+        <v>538</v>
       </c>
     </row>
     <row r="366" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A366" s="9" t="s">
-        <v>555</v>
+        <v>539</v>
       </c>
       <c r="B366" s="6" t="s">
-        <v>556</v>
+        <v>540</v>
       </c>
     </row>
     <row r="367" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A367" s="9" t="s">
-        <v>557</v>
+        <v>541</v>
       </c>
       <c r="B367" s="6" t="s">
-        <v>558</v>
+        <v>542</v>
       </c>
     </row>
     <row r="368" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A368" s="9" t="s">
-        <v>559</v>
+        <v>543</v>
       </c>
       <c r="B368" s="6" t="s">
-        <v>560</v>
+        <v>544</v>
       </c>
     </row>
     <row r="369" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A369" s="9" t="s">
-        <v>561</v>
+        <v>545</v>
       </c>
       <c r="B369" s="6" t="s">
-        <v>562</v>
+        <v>546</v>
       </c>
     </row>
     <row r="370" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A370" s="9" t="s">
-        <v>563</v>
+        <v>547</v>
       </c>
       <c r="B370" s="6" t="s">
-        <v>564</v>
+        <v>548</v>
       </c>
     </row>
     <row r="371" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A371" s="9" t="s">
-        <v>565</v>
+        <v>549</v>
       </c>
       <c r="B371" s="6" t="s">
-        <v>566</v>
+        <v>550</v>
       </c>
     </row>
     <row r="372" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A372" s="9" t="s">
-        <v>567</v>
+        <v>551</v>
       </c>
       <c r="B372" s="6" t="s">
-        <v>568</v>
+        <v>552</v>
       </c>
     </row>
     <row r="373" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A373" s="9" t="s">
-        <v>569</v>
+        <v>553</v>
       </c>
       <c r="B373" s="6" t="s">
-        <v>570</v>
+        <v>554</v>
       </c>
     </row>
     <row r="374" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A374" s="9" t="s">
-        <v>571</v>
+        <v>555</v>
       </c>
       <c r="B374" s="6" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
     </row>
     <row r="375" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A375" s="9" t="s">
-        <v>573</v>
+        <v>557</v>
       </c>
       <c r="B375" s="6" t="s">
-        <v>574</v>
+        <v>558</v>
       </c>
     </row>
     <row r="376" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A376" s="9" t="s">
-        <v>575</v>
+        <v>559</v>
       </c>
       <c r="B376" s="6" t="s">
-        <v>576</v>
+        <v>560</v>
       </c>
     </row>
     <row r="377" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A377" s="9" t="s">
-        <v>577</v>
+        <v>561</v>
       </c>
       <c r="B377" s="6" t="s">
-        <v>578</v>
+        <v>562</v>
       </c>
     </row>
     <row r="378" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A378" s="9" t="s">
-        <v>579</v>
+        <v>563</v>
       </c>
       <c r="B378" s="6" t="s">
-        <v>580</v>
+        <v>564</v>
       </c>
     </row>
     <row r="379" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A379" s="9" t="s">
-        <v>581</v>
+        <v>565</v>
       </c>
       <c r="B379" s="6" t="s">
-        <v>582</v>
+        <v>566</v>
       </c>
     </row>
     <row r="380" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A380" s="9" t="s">
-        <v>583</v>
+        <v>567</v>
       </c>
       <c r="B380" s="6" t="s">
-        <v>584</v>
+        <v>568</v>
       </c>
     </row>
     <row r="381" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A381" s="9" t="s">
-        <v>585</v>
+        <v>569</v>
       </c>
       <c r="B381" s="6" t="s">
-        <v>586</v>
+        <v>570</v>
       </c>
     </row>
     <row r="382" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A382" s="9" t="s">
-        <v>587</v>
+        <v>571</v>
       </c>
       <c r="B382" s="6" t="s">
-        <v>588</v>
+        <v>572</v>
       </c>
     </row>
     <row r="383" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A383" s="9" t="s">
-        <v>589</v>
+        <v>573</v>
       </c>
       <c r="B383" s="6" t="s">
-        <v>590</v>
+        <v>574</v>
       </c>
     </row>
     <row r="384" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A384" s="9" t="s">
-        <v>591</v>
+        <v>575</v>
       </c>
       <c r="B384" s="6" t="s">
-        <v>592</v>
+        <v>576</v>
       </c>
     </row>
     <row r="385" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A385" s="9" t="s">
-        <v>593</v>
+        <v>577</v>
       </c>
       <c r="B385" s="6" t="s">
-        <v>594</v>
+        <v>578</v>
       </c>
     </row>
     <row r="386" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A386" s="9" t="s">
-        <v>595</v>
+        <v>579</v>
       </c>
       <c r="B386" s="6" t="s">
-        <v>596</v>
+        <v>580</v>
       </c>
     </row>
     <row r="387" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A387" s="9" t="s">
-        <v>597</v>
+        <v>581</v>
       </c>
       <c r="B387" s="6" t="s">
-        <v>598</v>
+        <v>582</v>
       </c>
     </row>
     <row r="388" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A388" s="9" t="s">
-        <v>599</v>
+        <v>583</v>
       </c>
       <c r="B388" s="6" t="s">
-        <v>600</v>
+        <v>584</v>
       </c>
     </row>
     <row r="389" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A389" s="9" t="s">
-        <v>601</v>
+        <v>585</v>
       </c>
       <c r="B389" s="6" t="s">
-        <v>602</v>
+        <v>586</v>
       </c>
     </row>
     <row r="390" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A390" s="9" t="s">
-        <v>603</v>
+        <v>587</v>
       </c>
       <c r="B390" s="6" t="s">
-        <v>604</v>
+        <v>588</v>
       </c>
     </row>
     <row r="391" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A391" s="9" t="s">
-        <v>605</v>
+        <v>589</v>
       </c>
       <c r="B391" s="6" t="s">
-        <v>606</v>
+        <v>590</v>
       </c>
     </row>
     <row r="392" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A392" s="9" t="s">
-        <v>607</v>
+        <v>591</v>
       </c>
       <c r="B392" s="6" t="s">
-        <v>608</v>
+        <v>592</v>
       </c>
     </row>
     <row r="393" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A393" s="9" t="s">
-        <v>609</v>
+        <v>593</v>
       </c>
       <c r="B393" s="6" t="s">
-        <v>610</v>
+        <v>594</v>
       </c>
     </row>
     <row r="394" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A394" s="9" t="s">
-        <v>611</v>
+        <v>595</v>
       </c>
       <c r="B394" s="6" t="s">
-        <v>612</v>
+        <v>596</v>
       </c>
     </row>
     <row r="395" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A395" s="9" t="s">
-        <v>613</v>
+        <v>597</v>
       </c>
       <c r="B395" s="6" t="s">
-        <v>614</v>
+        <v>598</v>
       </c>
     </row>
     <row r="396" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A396" s="9" t="s">
-        <v>615</v>
+        <v>599</v>
       </c>
       <c r="B396" s="6" t="s">
-        <v>616</v>
+        <v>600</v>
       </c>
     </row>
     <row r="397" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A397" s="9" t="s">
-        <v>617</v>
+        <v>601</v>
       </c>
       <c r="B397" s="6" t="s">
-        <v>618</v>
+        <v>602</v>
       </c>
     </row>
     <row r="398" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A398" s="9" t="s">
-        <v>619</v>
+        <v>603</v>
       </c>
       <c r="B398" s="6" t="s">
-        <v>620</v>
+        <v>604</v>
       </c>
     </row>
     <row r="399" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A399" s="9" t="s">
-        <v>621</v>
+        <v>605</v>
       </c>
       <c r="B399" s="6" t="s">
-        <v>622</v>
+        <v>606</v>
       </c>
     </row>
     <row r="400" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A400" s="9" t="s">
-        <v>623</v>
+        <v>607</v>
       </c>
       <c r="B400" s="6" t="s">
-        <v>624</v>
+        <v>608</v>
       </c>
     </row>
     <row r="401" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A401" s="9" t="s">
-        <v>625</v>
+        <v>609</v>
       </c>
       <c r="B401" s="6" t="s">
-        <v>626</v>
+        <v>610</v>
       </c>
     </row>
     <row r="402" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A402" s="9" t="s">
-        <v>627</v>
+        <v>611</v>
       </c>
       <c r="B402" s="6" t="s">
-        <v>628</v>
+        <v>612</v>
       </c>
     </row>
     <row r="403" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A403" s="9" t="s">
-        <v>629</v>
+        <v>613</v>
       </c>
       <c r="B403" s="6" t="s">
-        <v>630</v>
+        <v>614</v>
       </c>
     </row>
     <row r="404" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A404" s="9" t="s">
-        <v>631</v>
+        <v>615</v>
       </c>
       <c r="B404" s="6" t="s">
-        <v>632</v>
+        <v>616</v>
       </c>
     </row>
     <row r="405" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A405" s="9" t="s">
-        <v>633</v>
+        <v>617</v>
       </c>
       <c r="B405" s="6" t="s">
-        <v>634</v>
+        <v>618</v>
       </c>
     </row>
     <row r="406" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A406" s="9" t="s">
-        <v>635</v>
+        <v>619</v>
       </c>
       <c r="B406" s="6" t="s">
-        <v>636</v>
+        <v>620</v>
       </c>
     </row>
     <row r="407" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A407" s="9" t="s">
-        <v>637</v>
+        <v>621</v>
       </c>
       <c r="B407" s="6" t="s">
-        <v>638</v>
+        <v>622</v>
       </c>
     </row>
     <row r="408" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A408" s="9" t="s">
-        <v>639</v>
+        <v>623</v>
       </c>
       <c r="B408" s="6" t="s">
-        <v>640</v>
+        <v>624</v>
       </c>
     </row>
     <row r="409" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A409" s="9" t="s">
-        <v>641</v>
+        <v>625</v>
       </c>
       <c r="B409" s="6" t="s">
-        <v>642</v>
+        <v>626</v>
       </c>
     </row>
     <row r="410" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A410" s="9" t="s">
-        <v>643</v>
+        <v>627</v>
       </c>
       <c r="B410" s="6" t="s">
-        <v>644</v>
+        <v>628</v>
       </c>
     </row>
     <row r="411" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A411" s="9" t="s">
-        <v>645</v>
+        <v>629</v>
       </c>
       <c r="B411" s="6" t="s">
-        <v>646</v>
+        <v>630</v>
       </c>
     </row>
     <row r="412" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A412" s="9" t="s">
-        <v>647</v>
+        <v>631</v>
       </c>
       <c r="B412" s="6" t="s">
-        <v>648</v>
+        <v>632</v>
       </c>
     </row>
     <row r="413" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A413" s="9" t="s">
-        <v>649</v>
+        <v>633</v>
       </c>
       <c r="B413" s="6" t="s">
-        <v>650</v>
+        <v>634</v>
       </c>
     </row>
     <row r="414" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A414" s="9" t="s">
-        <v>651</v>
+        <v>635</v>
       </c>
       <c r="B414" s="6" t="s">
-        <v>652</v>
+        <v>636</v>
       </c>
     </row>
     <row r="415" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A415" s="9" t="s">
-        <v>653</v>
+        <v>637</v>
       </c>
       <c r="B415" s="6" t="s">
-        <v>654</v>
+        <v>638</v>
       </c>
     </row>
     <row r="416" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A416" s="9" t="s">
-        <v>655</v>
+        <v>639</v>
       </c>
       <c r="B416" s="6" t="s">
-        <v>656</v>
+        <v>640</v>
       </c>
     </row>
     <row r="417" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A417" s="9" t="s">
-        <v>657</v>
+        <v>641</v>
       </c>
       <c r="B417" s="6" t="s">
-        <v>658</v>
+        <v>642</v>
       </c>
     </row>
     <row r="418" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A418" s="9" t="s">
-        <v>659</v>
+        <v>643</v>
       </c>
       <c r="B418" s="6" t="s">
-        <v>660</v>
+        <v>644</v>
       </c>
     </row>
     <row r="419" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A419" s="9" t="s">
-        <v>661</v>
+        <v>645</v>
       </c>
       <c r="B419" s="6" t="s">
-        <v>662</v>
+        <v>646</v>
       </c>
     </row>
     <row r="420" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A420" s="9" t="s">
-        <v>663</v>
+        <v>647</v>
       </c>
       <c r="B420" s="6" t="s">
-        <v>664</v>
+        <v>648</v>
       </c>
     </row>
     <row r="421" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A421" s="9" t="s">
-        <v>665</v>
+        <v>649</v>
       </c>
       <c r="B421" s="6" t="s">
-        <v>666</v>
+        <v>650</v>
       </c>
     </row>
     <row r="422" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A422" s="9" t="s">
-        <v>667</v>
+        <v>651</v>
       </c>
       <c r="B422" s="6" t="s">
-        <v>668</v>
+        <v>652</v>
       </c>
     </row>
     <row r="423" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A423" s="9" t="s">
-        <v>669</v>
+        <v>653</v>
       </c>
       <c r="B423" s="6" t="s">
-        <v>670</v>
+        <v>654</v>
       </c>
     </row>
     <row r="424" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A424" s="9" t="s">
-        <v>671</v>
+        <v>655</v>
       </c>
       <c r="B424" s="6" t="s">
-        <v>672</v>
+        <v>656</v>
       </c>
     </row>
     <row r="425" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A425" s="9" t="s">
-        <v>673</v>
+        <v>657</v>
       </c>
       <c r="B425" s="6" t="s">
-        <v>674</v>
+        <v>658</v>
       </c>
     </row>
     <row r="426" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A426" s="9" t="s">
-        <v>675</v>
+        <v>659</v>
       </c>
       <c r="B426" s="6" t="s">
-        <v>676</v>
+        <v>660</v>
       </c>
     </row>
     <row r="427" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A427" s="9" t="s">
-        <v>677</v>
+        <v>661</v>
       </c>
       <c r="B427" s="6" t="s">
-        <v>678</v>
+        <v>662</v>
       </c>
     </row>
     <row r="428" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A428" s="9" t="s">
-        <v>679</v>
+        <v>663</v>
       </c>
       <c r="B428" s="6" t="s">
-        <v>680</v>
+        <v>664</v>
       </c>
     </row>
     <row r="429" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A429" s="9" t="s">
-        <v>681</v>
+        <v>665</v>
       </c>
       <c r="B429" s="6" t="s">
-        <v>682</v>
+        <v>666</v>
       </c>
     </row>
     <row r="430" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A430" s="9" t="s">
-        <v>683</v>
+        <v>667</v>
       </c>
       <c r="B430" s="6" t="s">
-        <v>684</v>
+        <v>668</v>
       </c>
     </row>
     <row r="431" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A431" s="9" t="s">
-        <v>685</v>
+        <v>669</v>
       </c>
       <c r="B431" s="6" t="s">
-        <v>686</v>
+        <v>670</v>
       </c>
     </row>
     <row r="432" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A432" s="9" t="s">
-        <v>687</v>
+        <v>671</v>
       </c>
       <c r="B432" s="6" t="s">
-        <v>688</v>
+        <v>672</v>
       </c>
     </row>
     <row r="433" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A433" s="9" t="s">
-        <v>689</v>
+        <v>673</v>
       </c>
       <c r="B433" s="6" t="s">
-        <v>690</v>
+        <v>674</v>
       </c>
     </row>
     <row r="434" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A434" s="9" t="s">
-        <v>691</v>
+        <v>675</v>
       </c>
       <c r="B434" s="6" t="s">
-        <v>692</v>
+        <v>676</v>
       </c>
     </row>
     <row r="435" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A435" s="9" t="s">
-        <v>693</v>
+        <v>677</v>
       </c>
       <c r="B435" s="6" t="s">
-        <v>694</v>
+        <v>678</v>
       </c>
     </row>
     <row r="436" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A436" s="9" t="s">
-        <v>695</v>
+        <v>679</v>
       </c>
       <c r="B436" s="6" t="s">
-        <v>696</v>
+        <v>680</v>
       </c>
     </row>
     <row r="437" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A437" s="9" t="s">
-        <v>697</v>
+        <v>681</v>
       </c>
       <c r="B437" s="6" t="s">
-        <v>698</v>
+        <v>682</v>
       </c>
     </row>
     <row r="438" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A438" s="9" t="s">
-        <v>699</v>
+        <v>683</v>
       </c>
       <c r="B438" s="6" t="s">
-        <v>700</v>
+        <v>684</v>
       </c>
     </row>
     <row r="439" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A439" s="9" t="s">
-        <v>701</v>
+        <v>685</v>
       </c>
       <c r="B439" s="6" t="s">
-        <v>702</v>
+        <v>686</v>
       </c>
     </row>
     <row r="440" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A440" s="9" t="s">
-        <v>703</v>
+        <v>687</v>
       </c>
       <c r="B440" s="6" t="s">
-        <v>704</v>
+        <v>688</v>
       </c>
     </row>
     <row r="441" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A441" s="9" t="s">
-        <v>705</v>
+        <v>689</v>
       </c>
       <c r="B441" s="6" t="s">
-        <v>706</v>
+        <v>690</v>
       </c>
     </row>
     <row r="442" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A442" s="9" t="s">
-        <v>707</v>
+        <v>691</v>
       </c>
       <c r="B442" s="6" t="s">
-        <v>708</v>
+        <v>692</v>
       </c>
     </row>
     <row r="443" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A443" s="9" t="s">
-        <v>709</v>
+        <v>693</v>
       </c>
       <c r="B443" s="6" t="s">
-        <v>710</v>
+        <v>694</v>
       </c>
     </row>
     <row r="444" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A444" s="9" t="s">
-        <v>711</v>
+        <v>695</v>
       </c>
       <c r="B444" s="6" t="s">
-        <v>712</v>
+        <v>696</v>
       </c>
     </row>
     <row r="445" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A445" s="9" t="s">
-        <v>713</v>
+        <v>697</v>
       </c>
       <c r="B445" s="6" t="s">
-        <v>714</v>
+        <v>698</v>
       </c>
     </row>
     <row r="446" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A446" s="9" t="s">
-        <v>715</v>
+        <v>699</v>
       </c>
       <c r="B446" s="6" t="s">
-        <v>716</v>
+        <v>700</v>
       </c>
     </row>
     <row r="447" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A447" s="9" t="s">
-        <v>717</v>
+        <v>701</v>
       </c>
       <c r="B447" s="6" t="s">
-        <v>718</v>
+        <v>702</v>
       </c>
     </row>
     <row r="448" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A448" s="9" t="s">
-        <v>719</v>
+        <v>703</v>
       </c>
       <c r="B448" s="6" t="s">
-        <v>720</v>
+        <v>704</v>
       </c>
     </row>
     <row r="449" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A449" s="9" t="s">
-        <v>721</v>
+        <v>705</v>
       </c>
       <c r="B449" s="6" t="s">
-        <v>722</v>
+        <v>706</v>
       </c>
     </row>
     <row r="450" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A450" s="9" t="s">
-        <v>723</v>
+        <v>707</v>
       </c>
       <c r="B450" s="6" t="s">
-        <v>724</v>
+        <v>708</v>
       </c>
     </row>
     <row r="451" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A451" s="9" t="s">
-        <v>725</v>
+        <v>709</v>
       </c>
       <c r="B451" s="6" t="s">
-        <v>726</v>
+        <v>710</v>
       </c>
     </row>
     <row r="452" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A452" s="9" t="s">
-        <v>727</v>
+        <v>711</v>
       </c>
       <c r="B452" s="6" t="s">
-        <v>728</v>
+        <v>712</v>
       </c>
     </row>
     <row r="453" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A453" s="9" t="s">
-        <v>729</v>
+        <v>713</v>
       </c>
       <c r="B453" s="6" t="s">
-        <v>730</v>
+        <v>714</v>
       </c>
     </row>
     <row r="454" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A454" s="9" t="s">
-        <v>731</v>
+        <v>715</v>
       </c>
       <c r="B454" s="6" t="s">
-        <v>732</v>
+        <v>716</v>
       </c>
     </row>
     <row r="455" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A455" s="9" t="s">
-        <v>733</v>
+        <v>717</v>
       </c>
       <c r="B455" s="6" t="s">
-        <v>734</v>
+        <v>718</v>
       </c>
     </row>
     <row r="456" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A456" s="9" t="s">
-        <v>735</v>
+        <v>719</v>
       </c>
       <c r="B456" s="6" t="s">
-        <v>736</v>
+        <v>720</v>
       </c>
     </row>
     <row r="457" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A457" s="9" t="s">
-        <v>737</v>
+        <v>721</v>
       </c>
       <c r="B457" s="6" t="s">
-        <v>738</v>
+        <v>722</v>
       </c>
     </row>
     <row r="458" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A458" s="9" t="s">
-        <v>739</v>
+        <v>723</v>
       </c>
       <c r="B458" s="6" t="s">
-        <v>740</v>
+        <v>724</v>
       </c>
     </row>
     <row r="459" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A459" s="9" t="s">
-        <v>741</v>
+        <v>725</v>
       </c>
       <c r="B459" s="6" t="s">
-        <v>742</v>
+        <v>726</v>
       </c>
     </row>
     <row r="460" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A460" s="9" t="s">
-        <v>743</v>
+        <v>727</v>
       </c>
       <c r="B460" s="6" t="s">
-        <v>744</v>
+        <v>728</v>
       </c>
     </row>
     <row r="461" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A461" s="9" t="s">
-        <v>745</v>
+        <v>729</v>
       </c>
       <c r="B461" s="6" t="s">
-        <v>746</v>
+        <v>730</v>
       </c>
     </row>
     <row r="462" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A462" s="9" t="s">
-        <v>747</v>
+        <v>731</v>
       </c>
       <c r="B462" s="6" t="s">
-        <v>748</v>
+        <v>732</v>
       </c>
     </row>
     <row r="463" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A463" s="9" t="s">
-        <v>749</v>
+        <v>733</v>
       </c>
       <c r="B463" s="6" t="s">
-        <v>750</v>
+        <v>734</v>
       </c>
     </row>
     <row r="464" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A464" s="9" t="s">
-        <v>751</v>
+        <v>735</v>
       </c>
       <c r="B464" s="6" t="s">
-        <v>752</v>
+        <v>736</v>
       </c>
     </row>
     <row r="465" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A465" s="9" t="s">
-        <v>753</v>
+        <v>737</v>
       </c>
       <c r="B465" s="6" t="s">
-        <v>754</v>
+        <v>738</v>
       </c>
     </row>
     <row r="466" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A466" s="9" t="s">
-        <v>755</v>
+        <v>739</v>
       </c>
       <c r="B466" s="6" t="s">
-        <v>756</v>
+        <v>740</v>
       </c>
     </row>
     <row r="467" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A467" s="9" t="s">
-        <v>757</v>
+        <v>741</v>
       </c>
       <c r="B467" s="6" t="s">
-        <v>758</v>
+        <v>742</v>
       </c>
     </row>
     <row r="468" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A468" s="9" t="s">
-        <v>759</v>
+        <v>743</v>
       </c>
       <c r="B468" s="6" t="s">
-        <v>760</v>
+        <v>744</v>
       </c>
     </row>
     <row r="469" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A469" s="9" t="s">
-        <v>761</v>
+        <v>745</v>
       </c>
       <c r="B469" s="6" t="s">
-        <v>762</v>
+        <v>746</v>
       </c>
     </row>
     <row r="470" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A470" s="9" t="s">
-        <v>763</v>
+        <v>747</v>
       </c>
       <c r="B470" s="6" t="s">
-        <v>764</v>
+        <v>748</v>
       </c>
     </row>
     <row r="471" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A471" s="9" t="s">
-        <v>765</v>
+        <v>749</v>
       </c>
       <c r="B471" s="6" t="s">
-        <v>766</v>
+        <v>750</v>
       </c>
     </row>
     <row r="472" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A472" s="9" t="s">
-        <v>767</v>
+        <v>751</v>
       </c>
       <c r="B472" s="6" t="s">
-        <v>304</v>
+        <v>752</v>
       </c>
     </row>
     <row r="473" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A473" s="9" t="s">
-        <v>768</v>
+        <v>753</v>
       </c>
       <c r="B473" s="6" t="s">
-        <v>769</v>
+        <v>754</v>
       </c>
     </row>
     <row r="474" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A474" s="9" t="s">
-        <v>770</v>
+        <v>755</v>
       </c>
       <c r="B474" s="6" t="s">
-        <v>316</v>
+        <v>756</v>
       </c>
     </row>
     <row r="475" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A475" s="9" t="s">
-        <v>771</v>
+        <v>757</v>
       </c>
       <c r="B475" s="6" t="s">
-        <v>211</v>
+        <v>758</v>
       </c>
     </row>
     <row r="476" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A476" s="9" t="s">
-        <v>772</v>
+        <v>759</v>
       </c>
       <c r="B476" s="6" t="s">
-        <v>213</v>
+        <v>760</v>
       </c>
     </row>
     <row r="477" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A477" s="9" t="s">
-        <v>773</v>
+        <v>761</v>
       </c>
       <c r="B477" s="6" t="s">
-        <v>774</v>
-      </c>
-    </row>
-    <row r="478" spans="1:2" ht="22.5" x14ac:dyDescent="0.2">
+        <v>762</v>
+      </c>
+    </row>
+    <row r="478" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A478" s="9" t="s">
-        <v>775</v>
-      </c>
-      <c r="B478" s="7" t="s">
-        <v>312</v>
+        <v>763</v>
+      </c>
+      <c r="B478" s="6" t="s">
+        <v>764</v>
       </c>
     </row>
     <row r="479" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A479" s="9" t="s">
-        <v>776</v>
+        <v>765</v>
       </c>
       <c r="B479" s="6" t="s">
-        <v>777</v>
+        <v>766</v>
       </c>
     </row>
     <row r="480" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A480" s="9" t="s">
-        <v>778</v>
+        <v>767</v>
       </c>
       <c r="B480" s="6" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
     </row>
     <row r="481" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A481" s="9" t="s">
-        <v>779</v>
+        <v>768</v>
       </c>
       <c r="B481" s="6" t="s">
-        <v>780</v>
+        <v>769</v>
       </c>
     </row>
     <row r="482" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A482" s="9" t="s">
-        <v>781</v>
+        <v>770</v>
       </c>
       <c r="B482" s="6" t="s">
-        <v>782</v>
+        <v>316</v>
       </c>
     </row>
     <row r="483" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A483" s="9" t="s">
-        <v>783</v>
+        <v>771</v>
       </c>
       <c r="B483" s="6" t="s">
-        <v>784</v>
+        <v>211</v>
       </c>
     </row>
     <row r="484" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A484" s="9" t="s">
+        <v>772</v>
+      </c>
+      <c r="B484" s="6" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="485" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A485" s="9" t="s">
+        <v>773</v>
+      </c>
+      <c r="B485" s="6" t="s">
+        <v>774</v>
+      </c>
+    </row>
+    <row r="486" spans="1:2" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A486" s="9" t="s">
+        <v>775</v>
+      </c>
+      <c r="B486" s="7" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="487" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A487" s="9" t="s">
+        <v>776</v>
+      </c>
+      <c r="B487" s="6" t="s">
+        <v>777</v>
+      </c>
+    </row>
+    <row r="488" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A488" s="9" t="s">
+        <v>778</v>
+      </c>
+      <c r="B488" s="6" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="489" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A489" s="9" t="s">
+        <v>779</v>
+      </c>
+      <c r="B489" s="6" t="s">
+        <v>780</v>
+      </c>
+    </row>
+    <row r="490" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A490" s="9" t="s">
+        <v>781</v>
+      </c>
+      <c r="B490" s="6" t="s">
+        <v>782</v>
+      </c>
+    </row>
+    <row r="491" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A491" s="9" t="s">
+        <v>783</v>
+      </c>
+      <c r="B491" s="6" t="s">
+        <v>784</v>
+      </c>
+    </row>
+    <row r="492" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A492" s="9" t="s">
         <v>785</v>
       </c>
-      <c r="B484" s="6" t="s">
+      <c r="B492" s="6" t="s">
         <v>786</v>
       </c>
     </row>
-    <row r="485" spans="1:2" ht="22.5" x14ac:dyDescent="0.2">
-      <c r="A485" s="9" t="s">
+    <row r="493" spans="1:2" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A493" s="9" t="s">
         <v>787</v>
       </c>
-      <c r="B485" s="6" t="s">
+      <c r="B493" s="6" t="s">
         <v>788</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Merge AT tactics preset IDs
Update the ID of the custom user tactics presets in the advanced tactics mod
along with the associated m2da values so align with the mod

see #374
</commit_message>
<xml_diff>
--- a/source/tlk/strings.xlsx
+++ b/source/tlk/strings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\DAO\archid\source\tlk\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AE0A72D-86DA-4D8E-A27A-E4ABD1838EEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFE2FA24-88A0-478C-B203-5E7BAD55CC90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3405" yWindow="975" windowWidth="23625" windowHeight="16110" xr2:uid="{A42EE72D-E1C4-43B6-AEA5-0014ED5180B1}"/>
+    <workbookView xWindow="32535" yWindow="555" windowWidth="23625" windowHeight="16110" xr2:uid="{A42EE72D-E1C4-43B6-AEA5-0014ED5180B1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -5095,8 +5095,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C8288F5-46B5-435A-B9FC-40522281A8A6}">
   <dimension ref="A1:B1140"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A781" workbookViewId="0">
-      <selection activeCell="B810" sqref="B810"/>
+    <sheetView tabSelected="1" topLeftCell="A766" workbookViewId="0">
+      <selection activeCell="A773" sqref="A773"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Add scripts to restrict items based on gender
Created a pair of scripts that may be added as properties to items to restrict their usage based on gender.

closes #376
</commit_message>
<xml_diff>
--- a/source/tlk/strings.xlsx
+++ b/source/tlk/strings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\DAO\archid\source\tlk\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFE2FA24-88A0-478C-B203-5E7BAD55CC90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E62B1BB3-47DD-4652-AB77-B60509904D8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32535" yWindow="555" windowWidth="23625" windowHeight="16110" xr2:uid="{A42EE72D-E1C4-43B6-AEA5-0014ED5180B1}"/>
+    <workbookView xWindow="29190" yWindow="390" windowWidth="26610" windowHeight="16110" xr2:uid="{A42EE72D-E1C4-43B6-AEA5-0014ED5180B1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -247,7 +247,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Leliana Stories</t>
         </r>
@@ -261,7 +261,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Advanced quickbar</t>
         </r>
@@ -275,13 +275,27 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Advanced Tactics</t>
         </r>
       </text>
     </comment>
-    <comment ref="A805" authorId="0" shapeId="0" xr:uid="{15B7CDC5-6F21-45A0-9997-3CC9AFCCF646}">
+    <comment ref="A805" authorId="0" shapeId="0" xr:uid="{56003026-C53F-4338-A29E-3DAC6AE3A3C0}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Item restrictions</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A807" authorId="0" shapeId="0" xr:uid="{15B7CDC5-6F21-45A0-9997-3CC9AFCCF646}">
       <text>
         <r>
           <rPr>
@@ -295,7 +309,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A932" authorId="0" shapeId="0" xr:uid="{08441945-669A-47E4-A77A-BA32248BBBE4}">
+    <comment ref="A934" authorId="0" shapeId="0" xr:uid="{08441945-669A-47E4-A77A-BA32248BBBE4}">
       <text>
         <r>
           <rPr>
@@ -328,7 +342,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1477" uniqueCount="1420">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1479" uniqueCount="1422">
   <si>
     <t>af_archid_en-us.tlk</t>
   </si>
@@ -4651,6 +4665,12 @@
   </si>
   <si>
     <t>Templar Stationary</t>
+  </si>
+  <si>
+    <t>Required: Female</t>
+  </si>
+  <si>
+    <t>Required: Male</t>
   </si>
 </sst>
 </file>
@@ -4691,18 +4711,18 @@
       <family val="2"/>
     </font>
     <font>
+      <u/>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
       <b/>
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="8"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="7">
@@ -4774,7 +4794,7 @@
     </xf>
     <xf numFmtId="49" fontId="2" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="2" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5093,10 +5113,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C8288F5-46B5-435A-B9FC-40522281A8A6}">
-  <dimension ref="A1:B1140"/>
+  <dimension ref="A1:B1142"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A766" workbookViewId="0">
-      <selection activeCell="A773" sqref="A773"/>
+    <sheetView tabSelected="1" topLeftCell="A775" workbookViewId="0">
+      <selection activeCell="B807" sqref="B807"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -11539,2690 +11559,2706 @@
       </c>
     </row>
     <row r="805" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A805" s="8" t="s">
-        <v>150</v>
-      </c>
-      <c r="B805" s="6" t="s">
-        <v>151</v>
+      <c r="A805" s="3">
+        <v>6610803</v>
+      </c>
+      <c r="B805" s="2" t="s">
+        <v>1420</v>
       </c>
     </row>
     <row r="806" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A806" s="8" t="s">
-        <v>152</v>
-      </c>
-      <c r="B806" s="6" t="s">
-        <v>153</v>
+      <c r="A806" s="3">
+        <v>6610804</v>
+      </c>
+      <c r="B806" s="2" t="s">
+        <v>1421</v>
       </c>
     </row>
     <row r="807" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A807" s="8" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="B807" s="6" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
     <row r="808" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A808" s="8" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="B808" s="6" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
     </row>
     <row r="809" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A809" s="8" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="B809" s="6" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="810" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="810" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A810" s="8" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="B810" s="6" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
     </row>
     <row r="811" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A811" s="8" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="B811" s="6" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="812" spans="1:2" x14ac:dyDescent="0.2">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="812" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A812" s="8" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="B812" s="6" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
     </row>
     <row r="813" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A813" s="8" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="B813" s="6" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
     </row>
     <row r="814" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A814" s="8" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="B814" s="6" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="815" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="815" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A815" s="8" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="B815" s="6" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
     </row>
     <row r="816" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A816" s="8" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="B816" s="6" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="817" spans="1:2" x14ac:dyDescent="0.2">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="817" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A817" s="8" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="B817" s="6" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
     </row>
     <row r="818" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A818" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="B818" s="6" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="819" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A819" s="8" t="s">
+        <v>174</v>
+      </c>
+      <c r="B819" s="6" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="820" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A820" s="8" t="s">
         <v>176</v>
       </c>
-      <c r="B818" s="6" t="s">
+      <c r="B820" s="6" t="s">
         <v>151</v>
-      </c>
-    </row>
-    <row r="819" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
-      <c r="A819" s="8" t="s">
-        <v>177</v>
-      </c>
-      <c r="B819" s="6" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="820" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
-      <c r="A820" s="8" t="s">
-        <v>179</v>
-      </c>
-      <c r="B820" s="6" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="821" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A821" s="8" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="B821" s="6" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="822" spans="1:2" x14ac:dyDescent="0.2">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="822" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A822" s="8" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="B822" s="6" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
     </row>
     <row r="823" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A823" s="8" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="B823" s="6" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
     </row>
     <row r="824" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A824" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="B824" s="6" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="825" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
+      <c r="A825" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="B825" s="6" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="826" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A826" s="8" t="s">
         <v>187</v>
       </c>
-      <c r="B824" s="6" t="s">
+      <c r="B826" s="6" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="825" spans="1:2" ht="90" x14ac:dyDescent="0.2">
-      <c r="A825" s="8" t="s">
+    <row r="827" spans="1:2" ht="90" x14ac:dyDescent="0.2">
+      <c r="A827" s="8" t="s">
         <v>189</v>
       </c>
-      <c r="B825" s="6" t="s">
+      <c r="B827" s="6" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="826" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
-      <c r="A826" s="8" t="s">
+    <row r="828" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
+      <c r="A828" s="8" t="s">
         <v>191</v>
       </c>
-      <c r="B826" s="6" t="s">
+      <c r="B828" s="6" t="s">
         <v>192</v>
-      </c>
-    </row>
-    <row r="827" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
-      <c r="A827" s="8" t="s">
-        <v>193</v>
-      </c>
-      <c r="B827" s="6" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="828" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A828" s="8" t="s">
-        <v>195</v>
-      </c>
-      <c r="B828" s="6" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="829" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A829" s="8" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="B829" s="6" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
     </row>
     <row r="830" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A830" s="8" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="B830" s="6" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="831" spans="1:2" x14ac:dyDescent="0.2">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="831" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A831" s="8" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="B831" s="6" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
     </row>
     <row r="832" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A832" s="8" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="B832" s="6" t="s">
-        <v>153</v>
+        <v>200</v>
       </c>
     </row>
     <row r="833" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A833" s="8" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="B833" s="6" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
     </row>
     <row r="834" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A834" s="8" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="B834" s="6" t="s">
-        <v>207</v>
+        <v>153</v>
       </c>
     </row>
     <row r="835" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A835" s="8" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="B835" s="6" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
     </row>
     <row r="836" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A836" s="8" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="B836" s="6" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
     </row>
     <row r="837" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A837" s="8" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="B837" s="6" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
     </row>
     <row r="838" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A838" s="8" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="B838" s="6" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
     </row>
     <row r="839" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A839" s="8" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="B839" s="6" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
     </row>
     <row r="840" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A840" s="8" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="B840" s="6" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
     </row>
     <row r="841" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A841" s="8" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="B841" s="6" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
     </row>
     <row r="842" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A842" s="8" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="B842" s="6" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
     </row>
     <row r="843" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A843" s="8" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="B843" s="6" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
     </row>
     <row r="844" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A844" s="8" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="B844" s="6" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
     </row>
     <row r="845" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A845" s="8" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="B845" s="6" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
     </row>
     <row r="846" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A846" s="8" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="B846" s="6" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
     </row>
     <row r="847" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A847" s="8" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="B847" s="6" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
     </row>
     <row r="848" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A848" s="8" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="B848" s="6" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
     </row>
     <row r="849" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A849" s="8" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="B849" s="6" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
     </row>
     <row r="850" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A850" s="8" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="B850" s="6" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
     </row>
     <row r="851" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A851" s="8" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="B851" s="6" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
     </row>
     <row r="852" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A852" s="8" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="B852" s="6" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
     </row>
     <row r="853" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A853" s="8" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="B853" s="6" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
     </row>
     <row r="854" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A854" s="8" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="B854" s="6" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
     </row>
     <row r="855" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A855" s="8" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="B855" s="6" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
     </row>
     <row r="856" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A856" s="8" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="B856" s="6" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
     </row>
     <row r="857" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A857" s="8" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="B857" s="6" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
     </row>
     <row r="858" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A858" s="8" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="B858" s="6" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
     </row>
     <row r="859" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A859" s="8" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="B859" s="6" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
     </row>
     <row r="860" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A860" s="8" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="B860" s="6" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
     </row>
     <row r="861" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A861" s="8" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="B861" s="6" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
     </row>
     <row r="862" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A862" s="8" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="B862" s="6" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
     </row>
     <row r="863" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A863" s="8" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="B863" s="6" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
     </row>
     <row r="864" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A864" s="8" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="B864" s="6" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
     </row>
     <row r="865" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A865" s="8" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="B865" s="6" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
     </row>
     <row r="866" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A866" s="8" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="B866" s="6" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
     </row>
     <row r="867" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A867" s="8" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="B867" s="6" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
     </row>
     <row r="868" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A868" s="8" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="B868" s="6" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
     </row>
     <row r="869" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A869" s="8" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="B869" s="6" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
     </row>
     <row r="870" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A870" s="8" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="B870" s="6" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
     </row>
     <row r="871" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A871" s="8" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="B871" s="6" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
     </row>
     <row r="872" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A872" s="8" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="B872" s="6" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
     </row>
     <row r="873" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A873" s="8" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="B873" s="6" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
     </row>
     <row r="874" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A874" s="8" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="B874" s="6" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
     </row>
     <row r="875" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A875" s="8" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="B875" s="6" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="876" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A876" s="8" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="B876" s="6" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
     </row>
     <row r="877" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A877" s="8" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="B877" s="6" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
     </row>
     <row r="878" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A878" s="8" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="B878" s="6" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
     </row>
     <row r="879" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A879" s="8" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="B879" s="6" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="880" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A880" s="8" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="B880" s="6" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
     </row>
     <row r="881" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A881" s="8" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="B881" s="6" t="s">
-        <v>237</v>
+        <v>295</v>
       </c>
     </row>
     <row r="882" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A882" s="8" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="B882" s="6" t="s">
-        <v>239</v>
+        <v>298</v>
       </c>
     </row>
     <row r="883" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A883" s="8" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="B883" s="6" t="s">
-        <v>302</v>
+        <v>237</v>
       </c>
     </row>
     <row r="884" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A884" s="8" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="B884" s="6" t="s">
-        <v>304</v>
+        <v>239</v>
       </c>
     </row>
     <row r="885" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A885" s="8" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="B885" s="6" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
     </row>
     <row r="886" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A886" s="8" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="B886" s="6" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
     </row>
     <row r="887" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A887" s="8" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="B887" s="6" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="888" spans="1:2" ht="22.5" x14ac:dyDescent="0.2">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="888" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A888" s="8" t="s">
-        <v>311</v>
-      </c>
-      <c r="B888" s="7" t="s">
-        <v>312</v>
+        <v>307</v>
+      </c>
+      <c r="B888" s="6" t="s">
+        <v>308</v>
       </c>
     </row>
     <row r="889" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A889" s="8" t="s">
+        <v>309</v>
+      </c>
+      <c r="B889" s="6" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="890" spans="1:2" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A890" s="8" t="s">
+        <v>311</v>
+      </c>
+      <c r="B890" s="7" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="891" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A891" s="8" t="s">
         <v>313</v>
       </c>
-      <c r="B889" s="6" t="s">
+      <c r="B891" s="6" t="s">
         <v>314</v>
-      </c>
-    </row>
-    <row r="890" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A890" s="8" t="s">
-        <v>315</v>
-      </c>
-      <c r="B890" s="6" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="891" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
-      <c r="A891" s="8" t="s">
-        <v>317</v>
-      </c>
-      <c r="B891" s="6" t="s">
-        <v>318</v>
       </c>
     </row>
     <row r="892" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A892" s="8" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="B892" s="6" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="893" spans="1:2" x14ac:dyDescent="0.2">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="893" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A893" s="8" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="B893" s="6" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
     </row>
     <row r="894" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A894" s="8" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="B894" s="6" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
     </row>
     <row r="895" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A895" s="8" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="B895" s="6" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="896" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="896" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A896" s="8" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="B896" s="6" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
     </row>
     <row r="897" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A897" s="8" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="B897" s="6" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="898" spans="1:2" x14ac:dyDescent="0.2">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="898" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A898" s="8" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="B898" s="6" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
     </row>
     <row r="899" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A899" s="8" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="B899" s="6" t="s">
-        <v>333</v>
+        <v>295</v>
       </c>
     </row>
     <row r="900" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A900" s="8" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="B900" s="6" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="901" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A901" s="8" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B901" s="6" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
     </row>
     <row r="902" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A902" s="8" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="B902" s="6" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
     </row>
     <row r="903" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A903" s="8" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="B903" s="6" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
     </row>
     <row r="904" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A904" s="8" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="B904" s="6" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
     </row>
     <row r="905" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A905" s="8" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="B905" s="6" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
     </row>
     <row r="906" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A906" s="8" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="B906" s="6" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
     </row>
     <row r="907" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A907" s="8" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="B907" s="6" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
     </row>
     <row r="908" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A908" s="8" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="B908" s="6" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
     </row>
     <row r="909" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A909" s="8" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="B909" s="6" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
     </row>
     <row r="910" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A910" s="8" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="B910" s="6" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
     </row>
     <row r="911" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A911" s="8" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="B911" s="6" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
     </row>
     <row r="912" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A912" s="8" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="B912" s="6" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
     </row>
     <row r="913" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A913" s="8" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="B913" s="6" t="s">
-        <v>77</v>
+        <v>357</v>
       </c>
     </row>
     <row r="914" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A914" s="8" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="B914" s="6" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
     </row>
     <row r="915" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A915" s="8" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="B915" s="6" t="s">
-        <v>364</v>
+        <v>77</v>
       </c>
     </row>
     <row r="916" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A916" s="8" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="B916" s="6" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
     </row>
     <row r="917" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A917" s="8" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="B917" s="6" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
     </row>
     <row r="918" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A918" s="8" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
       <c r="B918" s="6" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
     </row>
     <row r="919" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A919" s="8" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="B919" s="6" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
     </row>
     <row r="920" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A920" s="8" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="B920" s="6" t="s">
-        <v>77</v>
+        <v>370</v>
       </c>
     </row>
     <row r="921" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A921" s="8" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="B921" s="6" t="s">
-        <v>281</v>
+        <v>372</v>
       </c>
     </row>
     <row r="922" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A922" s="8" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="B922" s="6" t="s">
-        <v>376</v>
+        <v>77</v>
       </c>
     </row>
     <row r="923" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A923" s="8" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="B923" s="6" t="s">
-        <v>378</v>
+        <v>281</v>
       </c>
     </row>
     <row r="924" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A924" s="8" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
       <c r="B924" s="6" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
     </row>
     <row r="925" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A925" s="8" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
       <c r="B925" s="6" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
     </row>
     <row r="926" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A926" s="8" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
       <c r="B926" s="6" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
     </row>
     <row r="927" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A927" s="8" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
       <c r="B927" s="6" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
     </row>
     <row r="928" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A928" s="8" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
       <c r="B928" s="6" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
     </row>
     <row r="929" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A929" s="8" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
       <c r="B929" s="6" t="s">
-        <v>175</v>
+        <v>386</v>
       </c>
     </row>
     <row r="930" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A930" s="8" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="B930" s="6" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
     </row>
     <row r="931" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A931" s="8" t="s">
+        <v>389</v>
+      </c>
+      <c r="B931" s="6" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="932" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A932" s="8" t="s">
+        <v>390</v>
+      </c>
+      <c r="B932" s="6" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="933" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A933" s="8" t="s">
         <v>392</v>
       </c>
-      <c r="B931" s="6" t="s">
+      <c r="B933" s="6" t="s">
         <v>393</v>
-      </c>
-    </row>
-    <row r="932" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A932" s="9" t="s">
-        <v>394</v>
-      </c>
-      <c r="B932" s="6" t="s">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="933" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A933" s="9" t="s">
-        <v>396</v>
-      </c>
-      <c r="B933" s="6" t="s">
-        <v>397</v>
       </c>
     </row>
     <row r="934" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A934" s="9" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
       <c r="B934" s="6" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
     </row>
     <row r="935" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A935" s="9" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
       <c r="B935" s="6" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
     </row>
     <row r="936" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A936" s="9" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="B936" s="6" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
     </row>
     <row r="937" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A937" s="9" t="s">
-        <v>404</v>
+        <v>400</v>
       </c>
       <c r="B937" s="6" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
     </row>
     <row r="938" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A938" s="9" t="s">
-        <v>406</v>
+        <v>402</v>
       </c>
       <c r="B938" s="6" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
     </row>
     <row r="939" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A939" s="9" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
       <c r="B939" s="6" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
     </row>
     <row r="940" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A940" s="9" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="B940" s="6" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
     </row>
     <row r="941" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A941" s="9" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="B941" s="6" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
     </row>
     <row r="942" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A942" s="9" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="B942" s="6" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
     </row>
     <row r="943" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A943" s="9" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="B943" s="6" t="s">
-        <v>215</v>
+        <v>412</v>
       </c>
     </row>
     <row r="944" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A944" s="9" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="B944" s="6" t="s">
-        <v>217</v>
+        <v>412</v>
       </c>
     </row>
     <row r="945" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A945" s="9" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="B945" s="6" t="s">
-        <v>401</v>
+        <v>215</v>
       </c>
     </row>
     <row r="946" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A946" s="9" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="B946" s="6" t="s">
-        <v>403</v>
+        <v>217</v>
       </c>
     </row>
     <row r="947" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A947" s="9" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="B947" s="6" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
     </row>
     <row r="948" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A948" s="9" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="B948" s="6" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
     </row>
     <row r="949" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A949" s="9" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="B949" s="6" t="s">
-        <v>395</v>
+        <v>405</v>
       </c>
     </row>
     <row r="950" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A950" s="9" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="B950" s="6" t="s">
-        <v>397</v>
+        <v>407</v>
       </c>
     </row>
     <row r="951" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A951" s="9" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="B951" s="6" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
     </row>
     <row r="952" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A952" s="9" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="B952" s="6" t="s">
-        <v>273</v>
+        <v>397</v>
       </c>
     </row>
     <row r="953" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A953" s="9" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="B953" s="6" t="s">
-        <v>275</v>
+        <v>399</v>
       </c>
     </row>
     <row r="954" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A954" s="9" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="B954" s="6" t="s">
-        <v>320</v>
+        <v>273</v>
       </c>
     </row>
     <row r="955" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A955" s="9" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="B955" s="6" t="s">
-        <v>281</v>
+        <v>275</v>
       </c>
     </row>
     <row r="956" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A956" s="9" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="B956" s="6" t="s">
-        <v>428</v>
+        <v>320</v>
       </c>
     </row>
     <row r="957" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A957" s="9" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
       <c r="B957" s="6" t="s">
-        <v>295</v>
+        <v>281</v>
       </c>
     </row>
     <row r="958" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A958" s="9" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
       <c r="B958" s="6" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
     </row>
     <row r="959" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A959" s="9" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="B959" s="6" t="s">
-        <v>433</v>
+        <v>295</v>
       </c>
     </row>
     <row r="960" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A960" s="9" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
       <c r="B960" s="6" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
     </row>
     <row r="961" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A961" s="9" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="B961" s="6" t="s">
-        <v>437</v>
+        <v>433</v>
       </c>
     </row>
     <row r="962" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A962" s="9" t="s">
-        <v>438</v>
+        <v>434</v>
       </c>
       <c r="B962" s="6" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
     </row>
     <row r="963" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A963" s="9" t="s">
-        <v>440</v>
+        <v>436</v>
       </c>
       <c r="B963" s="6" t="s">
-        <v>441</v>
+        <v>437</v>
       </c>
     </row>
     <row r="964" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A964" s="9" t="s">
-        <v>442</v>
+        <v>438</v>
       </c>
       <c r="B964" s="6" t="s">
-        <v>443</v>
+        <v>439</v>
       </c>
     </row>
     <row r="965" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A965" s="9" t="s">
-        <v>444</v>
+        <v>440</v>
       </c>
       <c r="B965" s="6" t="s">
-        <v>407</v>
+        <v>441</v>
       </c>
     </row>
     <row r="966" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A966" s="9" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
       <c r="B966" s="6" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
     </row>
     <row r="967" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A967" s="9" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
       <c r="B967" s="6" t="s">
-        <v>448</v>
+        <v>407</v>
       </c>
     </row>
     <row r="968" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A968" s="9" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
       <c r="B968" s="6" t="s">
-        <v>450</v>
+        <v>446</v>
       </c>
     </row>
     <row r="969" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A969" s="9" t="s">
-        <v>451</v>
+        <v>447</v>
       </c>
       <c r="B969" s="6" t="s">
-        <v>452</v>
+        <v>448</v>
       </c>
     </row>
     <row r="970" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A970" s="9" t="s">
-        <v>453</v>
+        <v>449</v>
       </c>
       <c r="B970" s="6" t="s">
-        <v>454</v>
+        <v>450</v>
       </c>
     </row>
     <row r="971" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A971" s="9" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
       <c r="B971" s="6" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
     </row>
     <row r="972" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A972" s="9" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
       <c r="B972" s="6" t="s">
-        <v>458</v>
+        <v>454</v>
       </c>
     </row>
     <row r="973" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A973" s="9" t="s">
-        <v>459</v>
+        <v>455</v>
       </c>
       <c r="B973" s="6" t="s">
-        <v>460</v>
+        <v>456</v>
       </c>
     </row>
     <row r="974" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A974" s="9" t="s">
-        <v>461</v>
+        <v>457</v>
       </c>
       <c r="B974" s="6" t="s">
-        <v>462</v>
+        <v>458</v>
       </c>
     </row>
     <row r="975" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A975" s="9" t="s">
-        <v>463</v>
+        <v>459</v>
       </c>
       <c r="B975" s="6" t="s">
-        <v>464</v>
+        <v>460</v>
       </c>
     </row>
     <row r="976" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A976" s="9" t="s">
-        <v>465</v>
+        <v>461</v>
       </c>
       <c r="B976" s="6" t="s">
-        <v>466</v>
+        <v>462</v>
       </c>
     </row>
     <row r="977" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A977" s="9" t="s">
-        <v>467</v>
+        <v>463</v>
       </c>
       <c r="B977" s="6" t="s">
-        <v>468</v>
+        <v>464</v>
       </c>
     </row>
     <row r="978" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A978" s="9" t="s">
-        <v>469</v>
+        <v>465</v>
       </c>
       <c r="B978" s="6" t="s">
-        <v>470</v>
+        <v>466</v>
       </c>
     </row>
     <row r="979" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A979" s="9" t="s">
-        <v>471</v>
+        <v>467</v>
       </c>
       <c r="B979" s="6" t="s">
-        <v>472</v>
+        <v>468</v>
       </c>
     </row>
     <row r="980" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A980" s="9" t="s">
-        <v>473</v>
+        <v>469</v>
       </c>
       <c r="B980" s="6" t="s">
-        <v>474</v>
+        <v>470</v>
       </c>
     </row>
     <row r="981" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A981" s="9" t="s">
-        <v>475</v>
+        <v>471</v>
       </c>
       <c r="B981" s="6" t="s">
-        <v>476</v>
+        <v>472</v>
       </c>
     </row>
     <row r="982" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A982" s="9" t="s">
-        <v>477</v>
+        <v>473</v>
       </c>
       <c r="B982" s="6" t="s">
-        <v>478</v>
+        <v>474</v>
       </c>
     </row>
     <row r="983" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A983" s="9" t="s">
-        <v>479</v>
+        <v>475</v>
       </c>
       <c r="B983" s="6" t="s">
-        <v>480</v>
+        <v>476</v>
       </c>
     </row>
     <row r="984" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A984" s="9" t="s">
-        <v>481</v>
+        <v>477</v>
       </c>
       <c r="B984" s="6" t="s">
-        <v>482</v>
+        <v>478</v>
       </c>
     </row>
     <row r="985" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A985" s="9" t="s">
-        <v>483</v>
+        <v>479</v>
       </c>
       <c r="B985" s="6" t="s">
-        <v>484</v>
+        <v>480</v>
       </c>
     </row>
     <row r="986" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A986" s="9" t="s">
-        <v>485</v>
+        <v>481</v>
       </c>
       <c r="B986" s="6" t="s">
-        <v>486</v>
+        <v>482</v>
       </c>
     </row>
     <row r="987" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A987" s="9" t="s">
-        <v>487</v>
+        <v>483</v>
       </c>
       <c r="B987" s="6" t="s">
-        <v>488</v>
+        <v>484</v>
       </c>
     </row>
     <row r="988" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A988" s="9" t="s">
-        <v>489</v>
+        <v>485</v>
       </c>
       <c r="B988" s="6" t="s">
-        <v>490</v>
+        <v>486</v>
       </c>
     </row>
     <row r="989" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A989" s="9" t="s">
-        <v>491</v>
+        <v>487</v>
       </c>
       <c r="B989" s="6" t="s">
-        <v>492</v>
+        <v>488</v>
       </c>
     </row>
     <row r="990" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A990" s="9" t="s">
-        <v>493</v>
+        <v>489</v>
       </c>
       <c r="B990" s="6" t="s">
-        <v>494</v>
+        <v>490</v>
       </c>
     </row>
     <row r="991" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A991" s="9" t="s">
-        <v>495</v>
+        <v>491</v>
       </c>
       <c r="B991" s="6" t="s">
-        <v>496</v>
+        <v>492</v>
       </c>
     </row>
     <row r="992" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A992" s="9" t="s">
-        <v>497</v>
+        <v>493</v>
       </c>
       <c r="B992" s="6" t="s">
-        <v>498</v>
+        <v>494</v>
       </c>
     </row>
     <row r="993" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A993" s="9" t="s">
-        <v>499</v>
+        <v>495</v>
       </c>
       <c r="B993" s="6" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
     </row>
     <row r="994" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A994" s="9" t="s">
-        <v>501</v>
+        <v>497</v>
       </c>
       <c r="B994" s="6" t="s">
-        <v>502</v>
+        <v>498</v>
       </c>
     </row>
     <row r="995" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A995" s="9" t="s">
-        <v>503</v>
+        <v>499</v>
       </c>
       <c r="B995" s="6" t="s">
-        <v>504</v>
+        <v>500</v>
       </c>
     </row>
     <row r="996" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A996" s="9" t="s">
-        <v>505</v>
+        <v>501</v>
       </c>
       <c r="B996" s="6" t="s">
-        <v>506</v>
+        <v>502</v>
       </c>
     </row>
     <row r="997" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A997" s="9" t="s">
-        <v>507</v>
+        <v>503</v>
       </c>
       <c r="B997" s="6" t="s">
-        <v>508</v>
+        <v>504</v>
       </c>
     </row>
     <row r="998" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A998" s="9" t="s">
-        <v>509</v>
+        <v>505</v>
       </c>
       <c r="B998" s="6" t="s">
-        <v>510</v>
+        <v>506</v>
       </c>
     </row>
     <row r="999" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A999" s="9" t="s">
-        <v>511</v>
+        <v>507</v>
       </c>
       <c r="B999" s="6" t="s">
-        <v>512</v>
+        <v>508</v>
       </c>
     </row>
     <row r="1000" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1000" s="9" t="s">
-        <v>513</v>
+        <v>509</v>
       </c>
       <c r="B1000" s="6" t="s">
-        <v>514</v>
+        <v>510</v>
       </c>
     </row>
     <row r="1001" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1001" s="9" t="s">
-        <v>515</v>
+        <v>511</v>
       </c>
       <c r="B1001" s="6" t="s">
-        <v>516</v>
+        <v>512</v>
       </c>
     </row>
     <row r="1002" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1002" s="9" t="s">
-        <v>517</v>
+        <v>513</v>
       </c>
       <c r="B1002" s="6" t="s">
-        <v>518</v>
+        <v>514</v>
       </c>
     </row>
     <row r="1003" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1003" s="9" t="s">
-        <v>519</v>
+        <v>515</v>
       </c>
       <c r="B1003" s="6" t="s">
-        <v>520</v>
+        <v>516</v>
       </c>
     </row>
     <row r="1004" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1004" s="9" t="s">
-        <v>521</v>
+        <v>517</v>
       </c>
       <c r="B1004" s="6" t="s">
-        <v>522</v>
+        <v>518</v>
       </c>
     </row>
     <row r="1005" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1005" s="9" t="s">
-        <v>523</v>
+        <v>519</v>
       </c>
       <c r="B1005" s="6" t="s">
-        <v>524</v>
+        <v>520</v>
       </c>
     </row>
     <row r="1006" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1006" s="9" t="s">
-        <v>525</v>
+        <v>521</v>
       </c>
       <c r="B1006" s="6" t="s">
-        <v>526</v>
+        <v>522</v>
       </c>
     </row>
     <row r="1007" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1007" s="9" t="s">
-        <v>527</v>
+        <v>523</v>
       </c>
       <c r="B1007" s="6" t="s">
-        <v>528</v>
+        <v>524</v>
       </c>
     </row>
     <row r="1008" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1008" s="9" t="s">
-        <v>529</v>
+        <v>525</v>
       </c>
       <c r="B1008" s="6" t="s">
-        <v>530</v>
+        <v>526</v>
       </c>
     </row>
     <row r="1009" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1009" s="9" t="s">
-        <v>531</v>
+        <v>527</v>
       </c>
       <c r="B1009" s="6" t="s">
-        <v>532</v>
+        <v>528</v>
       </c>
     </row>
     <row r="1010" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1010" s="9" t="s">
-        <v>533</v>
+        <v>529</v>
       </c>
       <c r="B1010" s="6" t="s">
-        <v>534</v>
+        <v>530</v>
       </c>
     </row>
     <row r="1011" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1011" s="9" t="s">
-        <v>535</v>
+        <v>531</v>
       </c>
       <c r="B1011" s="6" t="s">
-        <v>536</v>
+        <v>532</v>
       </c>
     </row>
     <row r="1012" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1012" s="9" t="s">
-        <v>537</v>
+        <v>533</v>
       </c>
       <c r="B1012" s="6" t="s">
-        <v>538</v>
+        <v>534</v>
       </c>
     </row>
     <row r="1013" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1013" s="9" t="s">
-        <v>539</v>
+        <v>535</v>
       </c>
       <c r="B1013" s="6" t="s">
-        <v>540</v>
+        <v>536</v>
       </c>
     </row>
     <row r="1014" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1014" s="9" t="s">
-        <v>541</v>
+        <v>537</v>
       </c>
       <c r="B1014" s="6" t="s">
-        <v>542</v>
+        <v>538</v>
       </c>
     </row>
     <row r="1015" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1015" s="9" t="s">
-        <v>543</v>
+        <v>539</v>
       </c>
       <c r="B1015" s="6" t="s">
-        <v>544</v>
+        <v>540</v>
       </c>
     </row>
     <row r="1016" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1016" s="9" t="s">
-        <v>545</v>
+        <v>541</v>
       </c>
       <c r="B1016" s="6" t="s">
-        <v>546</v>
+        <v>542</v>
       </c>
     </row>
     <row r="1017" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1017" s="9" t="s">
-        <v>547</v>
+        <v>543</v>
       </c>
       <c r="B1017" s="6" t="s">
-        <v>548</v>
+        <v>544</v>
       </c>
     </row>
     <row r="1018" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1018" s="9" t="s">
-        <v>549</v>
+        <v>545</v>
       </c>
       <c r="B1018" s="6" t="s">
-        <v>550</v>
+        <v>546</v>
       </c>
     </row>
     <row r="1019" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1019" s="9" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B1019" s="6" t="s">
-        <v>552</v>
+        <v>548</v>
       </c>
     </row>
     <row r="1020" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1020" s="9" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="B1020" s="6" t="s">
-        <v>554</v>
+        <v>550</v>
       </c>
     </row>
     <row r="1021" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1021" s="9" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
       <c r="B1021" s="6" t="s">
-        <v>556</v>
+        <v>552</v>
       </c>
     </row>
     <row r="1022" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1022" s="9" t="s">
-        <v>557</v>
+        <v>553</v>
       </c>
       <c r="B1022" s="6" t="s">
-        <v>558</v>
+        <v>554</v>
       </c>
     </row>
     <row r="1023" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1023" s="9" t="s">
-        <v>559</v>
+        <v>555</v>
       </c>
       <c r="B1023" s="6" t="s">
-        <v>560</v>
+        <v>556</v>
       </c>
     </row>
     <row r="1024" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1024" s="9" t="s">
-        <v>561</v>
+        <v>557</v>
       </c>
       <c r="B1024" s="6" t="s">
-        <v>562</v>
+        <v>558</v>
       </c>
     </row>
     <row r="1025" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1025" s="9" t="s">
-        <v>563</v>
+        <v>559</v>
       </c>
       <c r="B1025" s="6" t="s">
-        <v>564</v>
+        <v>560</v>
       </c>
     </row>
     <row r="1026" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1026" s="9" t="s">
-        <v>565</v>
+        <v>561</v>
       </c>
       <c r="B1026" s="6" t="s">
-        <v>566</v>
+        <v>562</v>
       </c>
     </row>
     <row r="1027" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1027" s="9" t="s">
-        <v>567</v>
+        <v>563</v>
       </c>
       <c r="B1027" s="6" t="s">
-        <v>568</v>
+        <v>564</v>
       </c>
     </row>
     <row r="1028" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1028" s="9" t="s">
-        <v>569</v>
+        <v>565</v>
       </c>
       <c r="B1028" s="6" t="s">
-        <v>570</v>
+        <v>566</v>
       </c>
     </row>
     <row r="1029" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1029" s="9" t="s">
-        <v>571</v>
+        <v>567</v>
       </c>
       <c r="B1029" s="6" t="s">
-        <v>572</v>
+        <v>568</v>
       </c>
     </row>
     <row r="1030" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1030" s="9" t="s">
-        <v>573</v>
+        <v>569</v>
       </c>
       <c r="B1030" s="6" t="s">
-        <v>574</v>
+        <v>570</v>
       </c>
     </row>
     <row r="1031" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1031" s="9" t="s">
-        <v>575</v>
+        <v>571</v>
       </c>
       <c r="B1031" s="6" t="s">
-        <v>576</v>
+        <v>572</v>
       </c>
     </row>
     <row r="1032" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1032" s="9" t="s">
-        <v>577</v>
+        <v>573</v>
       </c>
       <c r="B1032" s="6" t="s">
-        <v>578</v>
+        <v>574</v>
       </c>
     </row>
     <row r="1033" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1033" s="9" t="s">
-        <v>579</v>
+        <v>575</v>
       </c>
       <c r="B1033" s="6" t="s">
-        <v>580</v>
+        <v>576</v>
       </c>
     </row>
     <row r="1034" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1034" s="9" t="s">
-        <v>581</v>
+        <v>577</v>
       </c>
       <c r="B1034" s="6" t="s">
-        <v>582</v>
+        <v>578</v>
       </c>
     </row>
     <row r="1035" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1035" s="9" t="s">
-        <v>583</v>
+        <v>579</v>
       </c>
       <c r="B1035" s="6" t="s">
-        <v>584</v>
+        <v>580</v>
       </c>
     </row>
     <row r="1036" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1036" s="9" t="s">
-        <v>585</v>
+        <v>581</v>
       </c>
       <c r="B1036" s="6" t="s">
-        <v>586</v>
+        <v>582</v>
       </c>
     </row>
     <row r="1037" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1037" s="9" t="s">
-        <v>587</v>
+        <v>583</v>
       </c>
       <c r="B1037" s="6" t="s">
-        <v>588</v>
+        <v>584</v>
       </c>
     </row>
     <row r="1038" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1038" s="9" t="s">
-        <v>589</v>
+        <v>585</v>
       </c>
       <c r="B1038" s="6" t="s">
-        <v>590</v>
+        <v>586</v>
       </c>
     </row>
     <row r="1039" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1039" s="9" t="s">
-        <v>591</v>
+        <v>587</v>
       </c>
       <c r="B1039" s="6" t="s">
-        <v>592</v>
+        <v>588</v>
       </c>
     </row>
     <row r="1040" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1040" s="9" t="s">
-        <v>593</v>
+        <v>589</v>
       </c>
       <c r="B1040" s="6" t="s">
-        <v>594</v>
+        <v>590</v>
       </c>
     </row>
     <row r="1041" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1041" s="9" t="s">
-        <v>595</v>
+        <v>591</v>
       </c>
       <c r="B1041" s="6" t="s">
-        <v>596</v>
+        <v>592</v>
       </c>
     </row>
     <row r="1042" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1042" s="9" t="s">
-        <v>597</v>
+        <v>593</v>
       </c>
       <c r="B1042" s="6" t="s">
-        <v>598</v>
+        <v>594</v>
       </c>
     </row>
     <row r="1043" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1043" s="9" t="s">
-        <v>599</v>
+        <v>595</v>
       </c>
       <c r="B1043" s="6" t="s">
-        <v>600</v>
+        <v>596</v>
       </c>
     </row>
     <row r="1044" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1044" s="9" t="s">
-        <v>601</v>
+        <v>597</v>
       </c>
       <c r="B1044" s="6" t="s">
-        <v>602</v>
+        <v>598</v>
       </c>
     </row>
     <row r="1045" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1045" s="9" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
       <c r="B1045" s="6" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
     </row>
     <row r="1046" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1046" s="9" t="s">
-        <v>605</v>
+        <v>601</v>
       </c>
       <c r="B1046" s="6" t="s">
-        <v>606</v>
+        <v>602</v>
       </c>
     </row>
     <row r="1047" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1047" s="9" t="s">
-        <v>607</v>
+        <v>603</v>
       </c>
       <c r="B1047" s="6" t="s">
-        <v>608</v>
+        <v>604</v>
       </c>
     </row>
     <row r="1048" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1048" s="9" t="s">
-        <v>609</v>
+        <v>605</v>
       </c>
       <c r="B1048" s="6" t="s">
-        <v>610</v>
+        <v>606</v>
       </c>
     </row>
     <row r="1049" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1049" s="9" t="s">
-        <v>611</v>
+        <v>607</v>
       </c>
       <c r="B1049" s="6" t="s">
-        <v>612</v>
+        <v>608</v>
       </c>
     </row>
     <row r="1050" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1050" s="9" t="s">
-        <v>613</v>
+        <v>609</v>
       </c>
       <c r="B1050" s="6" t="s">
-        <v>614</v>
+        <v>610</v>
       </c>
     </row>
     <row r="1051" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1051" s="9" t="s">
-        <v>615</v>
+        <v>611</v>
       </c>
       <c r="B1051" s="6" t="s">
-        <v>616</v>
+        <v>612</v>
       </c>
     </row>
     <row r="1052" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1052" s="9" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="B1052" s="6" t="s">
-        <v>618</v>
+        <v>614</v>
       </c>
     </row>
     <row r="1053" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1053" s="9" t="s">
-        <v>619</v>
+        <v>615</v>
       </c>
       <c r="B1053" s="6" t="s">
-        <v>620</v>
+        <v>616</v>
       </c>
     </row>
     <row r="1054" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1054" s="9" t="s">
-        <v>621</v>
+        <v>617</v>
       </c>
       <c r="B1054" s="6" t="s">
-        <v>622</v>
+        <v>618</v>
       </c>
     </row>
     <row r="1055" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1055" s="9" t="s">
-        <v>623</v>
+        <v>619</v>
       </c>
       <c r="B1055" s="6" t="s">
-        <v>624</v>
+        <v>620</v>
       </c>
     </row>
     <row r="1056" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1056" s="9" t="s">
-        <v>625</v>
+        <v>621</v>
       </c>
       <c r="B1056" s="6" t="s">
-        <v>626</v>
+        <v>622</v>
       </c>
     </row>
     <row r="1057" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1057" s="9" t="s">
-        <v>627</v>
+        <v>623</v>
       </c>
       <c r="B1057" s="6" t="s">
-        <v>628</v>
+        <v>624</v>
       </c>
     </row>
     <row r="1058" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1058" s="9" t="s">
-        <v>629</v>
+        <v>625</v>
       </c>
       <c r="B1058" s="6" t="s">
-        <v>630</v>
+        <v>626</v>
       </c>
     </row>
     <row r="1059" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1059" s="9" t="s">
-        <v>631</v>
+        <v>627</v>
       </c>
       <c r="B1059" s="6" t="s">
-        <v>632</v>
+        <v>628</v>
       </c>
     </row>
     <row r="1060" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1060" s="9" t="s">
-        <v>633</v>
+        <v>629</v>
       </c>
       <c r="B1060" s="6" t="s">
-        <v>634</v>
+        <v>630</v>
       </c>
     </row>
     <row r="1061" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1061" s="9" t="s">
-        <v>635</v>
+        <v>631</v>
       </c>
       <c r="B1061" s="6" t="s">
-        <v>636</v>
+        <v>632</v>
       </c>
     </row>
     <row r="1062" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1062" s="9" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
       <c r="B1062" s="6" t="s">
-        <v>638</v>
+        <v>634</v>
       </c>
     </row>
     <row r="1063" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1063" s="9" t="s">
-        <v>639</v>
+        <v>635</v>
       </c>
       <c r="B1063" s="6" t="s">
-        <v>640</v>
+        <v>636</v>
       </c>
     </row>
     <row r="1064" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1064" s="9" t="s">
-        <v>641</v>
+        <v>637</v>
       </c>
       <c r="B1064" s="6" t="s">
-        <v>642</v>
+        <v>638</v>
       </c>
     </row>
     <row r="1065" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1065" s="9" t="s">
-        <v>643</v>
+        <v>639</v>
       </c>
       <c r="B1065" s="6" t="s">
-        <v>644</v>
+        <v>640</v>
       </c>
     </row>
     <row r="1066" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1066" s="9" t="s">
-        <v>645</v>
+        <v>641</v>
       </c>
       <c r="B1066" s="6" t="s">
-        <v>646</v>
+        <v>642</v>
       </c>
     </row>
     <row r="1067" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1067" s="9" t="s">
-        <v>647</v>
+        <v>643</v>
       </c>
       <c r="B1067" s="6" t="s">
-        <v>648</v>
+        <v>644</v>
       </c>
     </row>
     <row r="1068" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1068" s="9" t="s">
-        <v>649</v>
+        <v>645</v>
       </c>
       <c r="B1068" s="6" t="s">
-        <v>650</v>
+        <v>646</v>
       </c>
     </row>
     <row r="1069" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1069" s="9" t="s">
-        <v>651</v>
+        <v>647</v>
       </c>
       <c r="B1069" s="6" t="s">
-        <v>652</v>
+        <v>648</v>
       </c>
     </row>
     <row r="1070" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1070" s="9" t="s">
-        <v>653</v>
+        <v>649</v>
       </c>
       <c r="B1070" s="6" t="s">
-        <v>654</v>
+        <v>650</v>
       </c>
     </row>
     <row r="1071" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1071" s="9" t="s">
-        <v>655</v>
+        <v>651</v>
       </c>
       <c r="B1071" s="6" t="s">
-        <v>656</v>
+        <v>652</v>
       </c>
     </row>
     <row r="1072" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1072" s="9" t="s">
-        <v>657</v>
+        <v>653</v>
       </c>
       <c r="B1072" s="6" t="s">
-        <v>658</v>
+        <v>654</v>
       </c>
     </row>
     <row r="1073" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1073" s="9" t="s">
-        <v>659</v>
+        <v>655</v>
       </c>
       <c r="B1073" s="6" t="s">
-        <v>660</v>
+        <v>656</v>
       </c>
     </row>
     <row r="1074" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1074" s="9" t="s">
-        <v>661</v>
+        <v>657</v>
       </c>
       <c r="B1074" s="6" t="s">
-        <v>662</v>
+        <v>658</v>
       </c>
     </row>
     <row r="1075" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1075" s="9" t="s">
-        <v>663</v>
+        <v>659</v>
       </c>
       <c r="B1075" s="6" t="s">
-        <v>664</v>
+        <v>660</v>
       </c>
     </row>
     <row r="1076" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1076" s="9" t="s">
-        <v>665</v>
+        <v>661</v>
       </c>
       <c r="B1076" s="6" t="s">
-        <v>666</v>
+        <v>662</v>
       </c>
     </row>
     <row r="1077" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1077" s="9" t="s">
-        <v>667</v>
+        <v>663</v>
       </c>
       <c r="B1077" s="6" t="s">
-        <v>668</v>
+        <v>664</v>
       </c>
     </row>
     <row r="1078" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1078" s="9" t="s">
-        <v>669</v>
+        <v>665</v>
       </c>
       <c r="B1078" s="6" t="s">
-        <v>670</v>
+        <v>666</v>
       </c>
     </row>
     <row r="1079" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1079" s="9" t="s">
-        <v>671</v>
+        <v>667</v>
       </c>
       <c r="B1079" s="6" t="s">
-        <v>672</v>
+        <v>668</v>
       </c>
     </row>
     <row r="1080" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1080" s="9" t="s">
-        <v>673</v>
+        <v>669</v>
       </c>
       <c r="B1080" s="6" t="s">
-        <v>674</v>
+        <v>670</v>
       </c>
     </row>
     <row r="1081" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1081" s="9" t="s">
-        <v>675</v>
+        <v>671</v>
       </c>
       <c r="B1081" s="6" t="s">
-        <v>676</v>
+        <v>672</v>
       </c>
     </row>
     <row r="1082" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1082" s="9" t="s">
-        <v>677</v>
+        <v>673</v>
       </c>
       <c r="B1082" s="6" t="s">
-        <v>678</v>
+        <v>674</v>
       </c>
     </row>
     <row r="1083" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1083" s="9" t="s">
-        <v>679</v>
+        <v>675</v>
       </c>
       <c r="B1083" s="6" t="s">
-        <v>680</v>
+        <v>676</v>
       </c>
     </row>
     <row r="1084" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1084" s="9" t="s">
-        <v>681</v>
+        <v>677</v>
       </c>
       <c r="B1084" s="6" t="s">
-        <v>682</v>
+        <v>678</v>
       </c>
     </row>
     <row r="1085" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1085" s="9" t="s">
-        <v>683</v>
+        <v>679</v>
       </c>
       <c r="B1085" s="6" t="s">
-        <v>684</v>
+        <v>680</v>
       </c>
     </row>
     <row r="1086" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1086" s="9" t="s">
-        <v>685</v>
+        <v>681</v>
       </c>
       <c r="B1086" s="6" t="s">
-        <v>686</v>
+        <v>682</v>
       </c>
     </row>
     <row r="1087" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1087" s="9" t="s">
-        <v>687</v>
+        <v>683</v>
       </c>
       <c r="B1087" s="6" t="s">
-        <v>688</v>
+        <v>684</v>
       </c>
     </row>
     <row r="1088" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1088" s="9" t="s">
-        <v>689</v>
+        <v>685</v>
       </c>
       <c r="B1088" s="6" t="s">
-        <v>690</v>
+        <v>686</v>
       </c>
     </row>
     <row r="1089" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1089" s="9" t="s">
-        <v>691</v>
+        <v>687</v>
       </c>
       <c r="B1089" s="6" t="s">
-        <v>692</v>
+        <v>688</v>
       </c>
     </row>
     <row r="1090" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1090" s="9" t="s">
-        <v>693</v>
+        <v>689</v>
       </c>
       <c r="B1090" s="6" t="s">
-        <v>694</v>
+        <v>690</v>
       </c>
     </row>
     <row r="1091" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1091" s="9" t="s">
-        <v>695</v>
+        <v>691</v>
       </c>
       <c r="B1091" s="6" t="s">
-        <v>696</v>
+        <v>692</v>
       </c>
     </row>
     <row r="1092" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1092" s="9" t="s">
-        <v>697</v>
+        <v>693</v>
       </c>
       <c r="B1092" s="6" t="s">
-        <v>698</v>
+        <v>694</v>
       </c>
     </row>
     <row r="1093" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1093" s="9" t="s">
-        <v>699</v>
+        <v>695</v>
       </c>
       <c r="B1093" s="6" t="s">
-        <v>700</v>
+        <v>696</v>
       </c>
     </row>
     <row r="1094" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1094" s="9" t="s">
-        <v>701</v>
+        <v>697</v>
       </c>
       <c r="B1094" s="6" t="s">
-        <v>702</v>
+        <v>698</v>
       </c>
     </row>
     <row r="1095" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1095" s="9" t="s">
-        <v>703</v>
+        <v>699</v>
       </c>
       <c r="B1095" s="6" t="s">
-        <v>704</v>
+        <v>700</v>
       </c>
     </row>
     <row r="1096" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1096" s="9" t="s">
-        <v>705</v>
+        <v>701</v>
       </c>
       <c r="B1096" s="6" t="s">
-        <v>706</v>
+        <v>702</v>
       </c>
     </row>
     <row r="1097" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1097" s="9" t="s">
-        <v>707</v>
+        <v>703</v>
       </c>
       <c r="B1097" s="6" t="s">
-        <v>708</v>
+        <v>704</v>
       </c>
     </row>
     <row r="1098" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1098" s="9" t="s">
-        <v>709</v>
+        <v>705</v>
       </c>
       <c r="B1098" s="6" t="s">
-        <v>710</v>
+        <v>706</v>
       </c>
     </row>
     <row r="1099" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1099" s="9" t="s">
-        <v>711</v>
+        <v>707</v>
       </c>
       <c r="B1099" s="6" t="s">
-        <v>712</v>
+        <v>708</v>
       </c>
     </row>
     <row r="1100" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1100" s="9" t="s">
-        <v>713</v>
+        <v>709</v>
       </c>
       <c r="B1100" s="6" t="s">
-        <v>714</v>
+        <v>710</v>
       </c>
     </row>
     <row r="1101" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1101" s="9" t="s">
-        <v>715</v>
+        <v>711</v>
       </c>
       <c r="B1101" s="6" t="s">
-        <v>716</v>
+        <v>712</v>
       </c>
     </row>
     <row r="1102" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1102" s="9" t="s">
-        <v>717</v>
+        <v>713</v>
       </c>
       <c r="B1102" s="6" t="s">
-        <v>718</v>
+        <v>714</v>
       </c>
     </row>
     <row r="1103" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1103" s="9" t="s">
-        <v>719</v>
+        <v>715</v>
       </c>
       <c r="B1103" s="6" t="s">
-        <v>720</v>
+        <v>716</v>
       </c>
     </row>
     <row r="1104" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1104" s="9" t="s">
-        <v>721</v>
+        <v>717</v>
       </c>
       <c r="B1104" s="6" t="s">
-        <v>722</v>
+        <v>718</v>
       </c>
     </row>
     <row r="1105" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1105" s="9" t="s">
-        <v>723</v>
+        <v>719</v>
       </c>
       <c r="B1105" s="6" t="s">
-        <v>724</v>
+        <v>720</v>
       </c>
     </row>
     <row r="1106" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1106" s="9" t="s">
-        <v>725</v>
+        <v>721</v>
       </c>
       <c r="B1106" s="6" t="s">
-        <v>726</v>
+        <v>722</v>
       </c>
     </row>
     <row r="1107" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1107" s="9" t="s">
-        <v>727</v>
+        <v>723</v>
       </c>
       <c r="B1107" s="6" t="s">
-        <v>728</v>
+        <v>724</v>
       </c>
     </row>
     <row r="1108" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1108" s="9" t="s">
-        <v>729</v>
+        <v>725</v>
       </c>
       <c r="B1108" s="6" t="s">
-        <v>730</v>
+        <v>726</v>
       </c>
     </row>
     <row r="1109" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1109" s="9" t="s">
-        <v>731</v>
+        <v>727</v>
       </c>
       <c r="B1109" s="6" t="s">
-        <v>732</v>
+        <v>728</v>
       </c>
     </row>
     <row r="1110" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1110" s="9" t="s">
-        <v>733</v>
+        <v>729</v>
       </c>
       <c r="B1110" s="6" t="s">
-        <v>734</v>
+        <v>730</v>
       </c>
     </row>
     <row r="1111" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1111" s="9" t="s">
-        <v>735</v>
+        <v>731</v>
       </c>
       <c r="B1111" s="6" t="s">
-        <v>736</v>
+        <v>732</v>
       </c>
     </row>
     <row r="1112" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1112" s="9" t="s">
-        <v>737</v>
+        <v>733</v>
       </c>
       <c r="B1112" s="6" t="s">
-        <v>738</v>
+        <v>734</v>
       </c>
     </row>
     <row r="1113" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1113" s="9" t="s">
-        <v>739</v>
+        <v>735</v>
       </c>
       <c r="B1113" s="6" t="s">
-        <v>740</v>
+        <v>736</v>
       </c>
     </row>
     <row r="1114" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1114" s="9" t="s">
-        <v>741</v>
+        <v>737</v>
       </c>
       <c r="B1114" s="6" t="s">
-        <v>742</v>
+        <v>738</v>
       </c>
     </row>
     <row r="1115" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1115" s="9" t="s">
-        <v>743</v>
+        <v>739</v>
       </c>
       <c r="B1115" s="6" t="s">
-        <v>744</v>
+        <v>740</v>
       </c>
     </row>
     <row r="1116" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1116" s="9" t="s">
-        <v>745</v>
+        <v>741</v>
       </c>
       <c r="B1116" s="6" t="s">
-        <v>746</v>
+        <v>742</v>
       </c>
     </row>
     <row r="1117" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1117" s="9" t="s">
-        <v>747</v>
+        <v>743</v>
       </c>
       <c r="B1117" s="6" t="s">
-        <v>748</v>
+        <v>744</v>
       </c>
     </row>
     <row r="1118" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1118" s="9" t="s">
-        <v>749</v>
+        <v>745</v>
       </c>
       <c r="B1118" s="6" t="s">
-        <v>750</v>
+        <v>746</v>
       </c>
     </row>
     <row r="1119" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1119" s="9" t="s">
-        <v>751</v>
+        <v>747</v>
       </c>
       <c r="B1119" s="6" t="s">
-        <v>752</v>
+        <v>748</v>
       </c>
     </row>
     <row r="1120" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1120" s="9" t="s">
-        <v>753</v>
+        <v>749</v>
       </c>
       <c r="B1120" s="6" t="s">
-        <v>754</v>
+        <v>750</v>
       </c>
     </row>
     <row r="1121" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1121" s="9" t="s">
-        <v>755</v>
+        <v>751</v>
       </c>
       <c r="B1121" s="6" t="s">
-        <v>756</v>
+        <v>752</v>
       </c>
     </row>
     <row r="1122" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1122" s="9" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
       <c r="B1122" s="6" t="s">
-        <v>758</v>
+        <v>754</v>
       </c>
     </row>
     <row r="1123" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1123" s="9" t="s">
-        <v>759</v>
+        <v>755</v>
       </c>
       <c r="B1123" s="6" t="s">
-        <v>760</v>
+        <v>756</v>
       </c>
     </row>
     <row r="1124" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1124" s="9" t="s">
-        <v>761</v>
+        <v>757</v>
       </c>
       <c r="B1124" s="6" t="s">
-        <v>762</v>
+        <v>758</v>
       </c>
     </row>
     <row r="1125" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1125" s="9" t="s">
-        <v>763</v>
+        <v>759</v>
       </c>
       <c r="B1125" s="6" t="s">
-        <v>764</v>
+        <v>760</v>
       </c>
     </row>
     <row r="1126" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1126" s="9" t="s">
-        <v>765</v>
+        <v>761</v>
       </c>
       <c r="B1126" s="6" t="s">
-        <v>766</v>
+        <v>762</v>
       </c>
     </row>
     <row r="1127" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1127" s="9" t="s">
-        <v>767</v>
+        <v>763</v>
       </c>
       <c r="B1127" s="6" t="s">
-        <v>304</v>
+        <v>764</v>
       </c>
     </row>
     <row r="1128" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1128" s="9" t="s">
-        <v>768</v>
+        <v>765</v>
       </c>
       <c r="B1128" s="6" t="s">
-        <v>769</v>
+        <v>766</v>
       </c>
     </row>
     <row r="1129" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1129" s="9" t="s">
-        <v>770</v>
+        <v>767</v>
       </c>
       <c r="B1129" s="6" t="s">
-        <v>316</v>
+        <v>304</v>
       </c>
     </row>
     <row r="1130" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1130" s="9" t="s">
-        <v>771</v>
+        <v>768</v>
       </c>
       <c r="B1130" s="6" t="s">
-        <v>211</v>
+        <v>769</v>
       </c>
     </row>
     <row r="1131" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1131" s="9" t="s">
-        <v>772</v>
+        <v>770</v>
       </c>
       <c r="B1131" s="6" t="s">
-        <v>213</v>
+        <v>316</v>
       </c>
     </row>
     <row r="1132" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1132" s="9" t="s">
-        <v>773</v>
+        <v>771</v>
       </c>
       <c r="B1132" s="6" t="s">
-        <v>774</v>
-      </c>
-    </row>
-    <row r="1133" spans="1:2" ht="22.5" x14ac:dyDescent="0.2">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="1133" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1133" s="9" t="s">
-        <v>775</v>
-      </c>
-      <c r="B1133" s="7" t="s">
-        <v>312</v>
+        <v>772</v>
+      </c>
+      <c r="B1133" s="6" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="1134" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1134" s="9" t="s">
-        <v>776</v>
+        <v>773</v>
       </c>
       <c r="B1134" s="6" t="s">
-        <v>777</v>
-      </c>
-    </row>
-    <row r="1135" spans="1:2" x14ac:dyDescent="0.2">
+        <v>774</v>
+      </c>
+    </row>
+    <row r="1135" spans="1:2" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A1135" s="9" t="s">
-        <v>778</v>
-      </c>
-      <c r="B1135" s="6" t="s">
-        <v>308</v>
+        <v>775</v>
+      </c>
+      <c r="B1135" s="7" t="s">
+        <v>312</v>
       </c>
     </row>
     <row r="1136" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1136" s="9" t="s">
-        <v>779</v>
+        <v>776</v>
       </c>
       <c r="B1136" s="6" t="s">
-        <v>780</v>
+        <v>777</v>
       </c>
     </row>
     <row r="1137" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1137" s="9" t="s">
-        <v>781</v>
+        <v>778</v>
       </c>
       <c r="B1137" s="6" t="s">
-        <v>782</v>
+        <v>308</v>
       </c>
     </row>
     <row r="1138" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1138" s="9" t="s">
-        <v>783</v>
+        <v>779</v>
       </c>
       <c r="B1138" s="6" t="s">
-        <v>784</v>
+        <v>780</v>
       </c>
     </row>
     <row r="1139" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1139" s="9" t="s">
+        <v>781</v>
+      </c>
+      <c r="B1139" s="6" t="s">
+        <v>782</v>
+      </c>
+    </row>
+    <row r="1140" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1140" s="9" t="s">
+        <v>783</v>
+      </c>
+      <c r="B1140" s="6" t="s">
+        <v>784</v>
+      </c>
+    </row>
+    <row r="1141" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1141" s="9" t="s">
         <v>785</v>
       </c>
-      <c r="B1139" s="6" t="s">
+      <c r="B1141" s="6" t="s">
         <v>786</v>
       </c>
     </row>
-    <row r="1140" spans="1:2" ht="22.5" x14ac:dyDescent="0.2">
-      <c r="A1140" s="9" t="s">
+    <row r="1142" spans="1:2" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A1142" s="9" t="s">
         <v>787</v>
       </c>
-      <c r="B1140" s="6" t="s">
+      <c r="B1142" s="6" t="s">
         <v>788</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add Ring of Survival
A new ring item has been created with the following properties:

- Constitution: +3
- Combat health regen: 1.5/3
- Exploration health regen: +5
- Dodge chance: 5%

It has been placed in the Iron Chest guarded by wolves in the Korcari Wilds prelude area

closes #380
</commit_message>
<xml_diff>
--- a/source/tlk/strings.xlsx
+++ b/source/tlk/strings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\DAO\archid\source\tlk\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E62B1BB3-47DD-4652-AB77-B60509904D8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64F18D4E-305D-4294-830E-FAA4B4803AD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="29190" yWindow="390" windowWidth="26610" windowHeight="16110" xr2:uid="{A42EE72D-E1C4-43B6-AEA5-0014ED5180B1}"/>
   </bookViews>
@@ -295,7 +295,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A807" authorId="0" shapeId="0" xr:uid="{15B7CDC5-6F21-45A0-9997-3CC9AFCCF646}">
+    <comment ref="A809" authorId="0" shapeId="0" xr:uid="{15B7CDC5-6F21-45A0-9997-3CC9AFCCF646}">
       <text>
         <r>
           <rPr>
@@ -309,7 +309,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A934" authorId="0" shapeId="0" xr:uid="{08441945-669A-47E4-A77A-BA32248BBBE4}">
+    <comment ref="A936" authorId="0" shapeId="0" xr:uid="{08441945-669A-47E4-A77A-BA32248BBBE4}">
       <text>
         <r>
           <rPr>
@@ -342,7 +342,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1479" uniqueCount="1422">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1481" uniqueCount="1424">
   <si>
     <t>af_archid_en-us.tlk</t>
   </si>
@@ -4671,6 +4671,12 @@
   </si>
   <si>
     <t>Required: Male</t>
+  </si>
+  <si>
+    <t>Ring of Survival</t>
+  </si>
+  <si>
+    <t>This plain looking ring was once the posession of a Telvinter mage who fell during the First Blight and subsequently found and worn by a Chasind chief during their occupation of Ostagar. How it came to be lost again is a mystery, but it's power has remain undimished over the ages.</t>
   </si>
 </sst>
 </file>
@@ -5113,10 +5119,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C8288F5-46B5-435A-B9FC-40522281A8A6}">
-  <dimension ref="A1:B1142"/>
+  <dimension ref="A1:B1144"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A775" workbookViewId="0">
-      <selection activeCell="B807" sqref="B807"/>
+    <sheetView tabSelected="1" topLeftCell="A758" workbookViewId="0">
+      <selection activeCell="B810" sqref="B810"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -11575,2690 +11581,2706 @@
       </c>
     </row>
     <row r="807" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A807" s="8" t="s">
-        <v>150</v>
-      </c>
-      <c r="B807" s="6" t="s">
-        <v>151</v>
+      <c r="A807" s="4">
+        <v>6610805</v>
+      </c>
+      <c r="B807" s="2" t="s">
+        <v>1422</v>
       </c>
     </row>
     <row r="808" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A808" s="8" t="s">
-        <v>152</v>
-      </c>
-      <c r="B808" s="6" t="s">
-        <v>153</v>
+      <c r="A808" s="4">
+        <v>6610806</v>
+      </c>
+      <c r="B808" s="2" t="s">
+        <v>1423</v>
       </c>
     </row>
     <row r="809" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A809" s="8" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="B809" s="6" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
     <row r="810" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A810" s="8" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="B810" s="6" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
     </row>
     <row r="811" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A811" s="8" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="B811" s="6" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="812" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="812" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A812" s="8" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="B812" s="6" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
     </row>
     <row r="813" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A813" s="8" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="B813" s="6" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="814" spans="1:2" x14ac:dyDescent="0.2">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="814" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A814" s="8" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="B814" s="6" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
     </row>
     <row r="815" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A815" s="8" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="B815" s="6" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
     </row>
     <row r="816" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A816" s="8" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="B816" s="6" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="817" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="817" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A817" s="8" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="B817" s="6" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
     </row>
     <row r="818" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A818" s="8" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="B818" s="6" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="819" spans="1:2" x14ac:dyDescent="0.2">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="819" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A819" s="8" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="B819" s="6" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
     </row>
     <row r="820" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A820" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="B820" s="6" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="821" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A821" s="8" t="s">
+        <v>174</v>
+      </c>
+      <c r="B821" s="6" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="822" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A822" s="8" t="s">
         <v>176</v>
       </c>
-      <c r="B820" s="6" t="s">
+      <c r="B822" s="6" t="s">
         <v>151</v>
-      </c>
-    </row>
-    <row r="821" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
-      <c r="A821" s="8" t="s">
-        <v>177</v>
-      </c>
-      <c r="B821" s="6" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="822" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
-      <c r="A822" s="8" t="s">
-        <v>179</v>
-      </c>
-      <c r="B822" s="6" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="823" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A823" s="8" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="B823" s="6" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="824" spans="1:2" x14ac:dyDescent="0.2">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="824" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A824" s="8" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="B824" s="6" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
     </row>
     <row r="825" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A825" s="8" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="B825" s="6" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
     </row>
     <row r="826" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A826" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="B826" s="6" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="827" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
+      <c r="A827" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="B827" s="6" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="828" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A828" s="8" t="s">
         <v>187</v>
       </c>
-      <c r="B826" s="6" t="s">
+      <c r="B828" s="6" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="827" spans="1:2" ht="90" x14ac:dyDescent="0.2">
-      <c r="A827" s="8" t="s">
+    <row r="829" spans="1:2" ht="90" x14ac:dyDescent="0.2">
+      <c r="A829" s="8" t="s">
         <v>189</v>
       </c>
-      <c r="B827" s="6" t="s">
+      <c r="B829" s="6" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="828" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
-      <c r="A828" s="8" t="s">
+    <row r="830" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
+      <c r="A830" s="8" t="s">
         <v>191</v>
       </c>
-      <c r="B828" s="6" t="s">
+      <c r="B830" s="6" t="s">
         <v>192</v>
-      </c>
-    </row>
-    <row r="829" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
-      <c r="A829" s="8" t="s">
-        <v>193</v>
-      </c>
-      <c r="B829" s="6" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="830" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A830" s="8" t="s">
-        <v>195</v>
-      </c>
-      <c r="B830" s="6" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="831" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A831" s="8" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="B831" s="6" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
     </row>
     <row r="832" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A832" s="8" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="B832" s="6" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="833" spans="1:2" x14ac:dyDescent="0.2">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="833" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A833" s="8" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="B833" s="6" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
     </row>
     <row r="834" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A834" s="8" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="B834" s="6" t="s">
-        <v>153</v>
+        <v>200</v>
       </c>
     </row>
     <row r="835" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A835" s="8" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="B835" s="6" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
     </row>
     <row r="836" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A836" s="8" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="B836" s="6" t="s">
-        <v>207</v>
+        <v>153</v>
       </c>
     </row>
     <row r="837" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A837" s="8" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="B837" s="6" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
     </row>
     <row r="838" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A838" s="8" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="B838" s="6" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
     </row>
     <row r="839" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A839" s="8" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="B839" s="6" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
     </row>
     <row r="840" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A840" s="8" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="B840" s="6" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
     </row>
     <row r="841" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A841" s="8" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="B841" s="6" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
     </row>
     <row r="842" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A842" s="8" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="B842" s="6" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
     </row>
     <row r="843" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A843" s="8" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="B843" s="6" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
     </row>
     <row r="844" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A844" s="8" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="B844" s="6" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
     </row>
     <row r="845" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A845" s="8" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="B845" s="6" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
     </row>
     <row r="846" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A846" s="8" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="B846" s="6" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
     </row>
     <row r="847" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A847" s="8" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="B847" s="6" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
     </row>
     <row r="848" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A848" s="8" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="B848" s="6" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
     </row>
     <row r="849" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A849" s="8" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="B849" s="6" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
     </row>
     <row r="850" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A850" s="8" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="B850" s="6" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
     </row>
     <row r="851" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A851" s="8" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="B851" s="6" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
     </row>
     <row r="852" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A852" s="8" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="B852" s="6" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
     </row>
     <row r="853" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A853" s="8" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="B853" s="6" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
     </row>
     <row r="854" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A854" s="8" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="B854" s="6" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
     </row>
     <row r="855" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A855" s="8" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="B855" s="6" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
     </row>
     <row r="856" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A856" s="8" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="B856" s="6" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
     </row>
     <row r="857" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A857" s="8" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="B857" s="6" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
     </row>
     <row r="858" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A858" s="8" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="B858" s="6" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
     </row>
     <row r="859" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A859" s="8" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="B859" s="6" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
     </row>
     <row r="860" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A860" s="8" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="B860" s="6" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
     </row>
     <row r="861" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A861" s="8" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="B861" s="6" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
     </row>
     <row r="862" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A862" s="8" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="B862" s="6" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
     </row>
     <row r="863" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A863" s="8" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="B863" s="6" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
     </row>
     <row r="864" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A864" s="8" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="B864" s="6" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
     </row>
     <row r="865" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A865" s="8" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="B865" s="6" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
     </row>
     <row r="866" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A866" s="8" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="B866" s="6" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
     </row>
     <row r="867" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A867" s="8" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="B867" s="6" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
     </row>
     <row r="868" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A868" s="8" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="B868" s="6" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
     </row>
     <row r="869" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A869" s="8" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="B869" s="6" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
     </row>
     <row r="870" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A870" s="8" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="B870" s="6" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
     </row>
     <row r="871" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A871" s="8" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="B871" s="6" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
     </row>
     <row r="872" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A872" s="8" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="B872" s="6" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
     </row>
     <row r="873" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A873" s="8" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="B873" s="6" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
     </row>
     <row r="874" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A874" s="8" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="B874" s="6" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
     </row>
     <row r="875" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A875" s="8" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="B875" s="6" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
     </row>
     <row r="876" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A876" s="8" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="B876" s="6" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
     </row>
     <row r="877" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A877" s="8" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="B877" s="6" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="878" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A878" s="8" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="B878" s="6" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
     </row>
     <row r="879" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A879" s="8" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="B879" s="6" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
     </row>
     <row r="880" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A880" s="8" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="B880" s="6" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
     </row>
     <row r="881" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A881" s="8" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="B881" s="6" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="882" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A882" s="8" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="B882" s="6" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
     </row>
     <row r="883" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A883" s="8" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="B883" s="6" t="s">
-        <v>237</v>
+        <v>295</v>
       </c>
     </row>
     <row r="884" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A884" s="8" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="B884" s="6" t="s">
-        <v>239</v>
+        <v>298</v>
       </c>
     </row>
     <row r="885" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A885" s="8" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="B885" s="6" t="s">
-        <v>302</v>
+        <v>237</v>
       </c>
     </row>
     <row r="886" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A886" s="8" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="B886" s="6" t="s">
-        <v>304</v>
+        <v>239</v>
       </c>
     </row>
     <row r="887" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A887" s="8" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="B887" s="6" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
     </row>
     <row r="888" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A888" s="8" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="B888" s="6" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
     </row>
     <row r="889" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A889" s="8" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="B889" s="6" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="890" spans="1:2" ht="22.5" x14ac:dyDescent="0.2">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="890" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A890" s="8" t="s">
-        <v>311</v>
-      </c>
-      <c r="B890" s="7" t="s">
-        <v>312</v>
+        <v>307</v>
+      </c>
+      <c r="B890" s="6" t="s">
+        <v>308</v>
       </c>
     </row>
     <row r="891" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A891" s="8" t="s">
+        <v>309</v>
+      </c>
+      <c r="B891" s="6" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="892" spans="1:2" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A892" s="8" t="s">
+        <v>311</v>
+      </c>
+      <c r="B892" s="7" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="893" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A893" s="8" t="s">
         <v>313</v>
       </c>
-      <c r="B891" s="6" t="s">
+      <c r="B893" s="6" t="s">
         <v>314</v>
-      </c>
-    </row>
-    <row r="892" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A892" s="8" t="s">
-        <v>315</v>
-      </c>
-      <c r="B892" s="6" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="893" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
-      <c r="A893" s="8" t="s">
-        <v>317</v>
-      </c>
-      <c r="B893" s="6" t="s">
-        <v>318</v>
       </c>
     </row>
     <row r="894" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A894" s="8" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="B894" s="6" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="895" spans="1:2" x14ac:dyDescent="0.2">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="895" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A895" s="8" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="B895" s="6" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
     </row>
     <row r="896" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A896" s="8" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="B896" s="6" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
     </row>
     <row r="897" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A897" s="8" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="B897" s="6" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="898" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="898" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A898" s="8" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="B898" s="6" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
     </row>
     <row r="899" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A899" s="8" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="B899" s="6" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="900" spans="1:2" x14ac:dyDescent="0.2">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="900" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A900" s="8" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="B900" s="6" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
     </row>
     <row r="901" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A901" s="8" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="B901" s="6" t="s">
-        <v>333</v>
+        <v>295</v>
       </c>
     </row>
     <row r="902" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A902" s="8" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="B902" s="6" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="903" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A903" s="8" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B903" s="6" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
     </row>
     <row r="904" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A904" s="8" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="B904" s="6" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
     </row>
     <row r="905" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A905" s="8" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="B905" s="6" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
     </row>
     <row r="906" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A906" s="8" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="B906" s="6" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
     </row>
     <row r="907" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A907" s="8" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="B907" s="6" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
     </row>
     <row r="908" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A908" s="8" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="B908" s="6" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
     </row>
     <row r="909" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A909" s="8" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="B909" s="6" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
     </row>
     <row r="910" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A910" s="8" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="B910" s="6" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
     </row>
     <row r="911" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A911" s="8" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="B911" s="6" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
     </row>
     <row r="912" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A912" s="8" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="B912" s="6" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
     </row>
     <row r="913" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A913" s="8" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="B913" s="6" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
     </row>
     <row r="914" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A914" s="8" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="B914" s="6" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
     </row>
     <row r="915" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A915" s="8" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="B915" s="6" t="s">
-        <v>77</v>
+        <v>357</v>
       </c>
     </row>
     <row r="916" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A916" s="8" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="B916" s="6" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
     </row>
     <row r="917" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A917" s="8" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="B917" s="6" t="s">
-        <v>364</v>
+        <v>77</v>
       </c>
     </row>
     <row r="918" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A918" s="8" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="B918" s="6" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
     </row>
     <row r="919" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A919" s="8" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="B919" s="6" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
     </row>
     <row r="920" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A920" s="8" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
       <c r="B920" s="6" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
     </row>
     <row r="921" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A921" s="8" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="B921" s="6" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
     </row>
     <row r="922" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A922" s="8" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="B922" s="6" t="s">
-        <v>77</v>
+        <v>370</v>
       </c>
     </row>
     <row r="923" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A923" s="8" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="B923" s="6" t="s">
-        <v>281</v>
+        <v>372</v>
       </c>
     </row>
     <row r="924" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A924" s="8" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="B924" s="6" t="s">
-        <v>376</v>
+        <v>77</v>
       </c>
     </row>
     <row r="925" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A925" s="8" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="B925" s="6" t="s">
-        <v>378</v>
+        <v>281</v>
       </c>
     </row>
     <row r="926" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A926" s="8" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
       <c r="B926" s="6" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
     </row>
     <row r="927" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A927" s="8" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
       <c r="B927" s="6" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
     </row>
     <row r="928" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A928" s="8" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
       <c r="B928" s="6" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
     </row>
     <row r="929" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A929" s="8" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
       <c r="B929" s="6" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
     </row>
     <row r="930" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A930" s="8" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
       <c r="B930" s="6" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
     </row>
     <row r="931" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A931" s="8" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
       <c r="B931" s="6" t="s">
-        <v>175</v>
+        <v>386</v>
       </c>
     </row>
     <row r="932" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A932" s="8" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="B932" s="6" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
     </row>
     <row r="933" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A933" s="8" t="s">
+        <v>389</v>
+      </c>
+      <c r="B933" s="6" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="934" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A934" s="8" t="s">
+        <v>390</v>
+      </c>
+      <c r="B934" s="6" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="935" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A935" s="8" t="s">
         <v>392</v>
       </c>
-      <c r="B933" s="6" t="s">
+      <c r="B935" s="6" t="s">
         <v>393</v>
-      </c>
-    </row>
-    <row r="934" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A934" s="9" t="s">
-        <v>394</v>
-      </c>
-      <c r="B934" s="6" t="s">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="935" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A935" s="9" t="s">
-        <v>396</v>
-      </c>
-      <c r="B935" s="6" t="s">
-        <v>397</v>
       </c>
     </row>
     <row r="936" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A936" s="9" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
       <c r="B936" s="6" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
     </row>
     <row r="937" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A937" s="9" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
       <c r="B937" s="6" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
     </row>
     <row r="938" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A938" s="9" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="B938" s="6" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
     </row>
     <row r="939" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A939" s="9" t="s">
-        <v>404</v>
+        <v>400</v>
       </c>
       <c r="B939" s="6" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
     </row>
     <row r="940" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A940" s="9" t="s">
-        <v>406</v>
+        <v>402</v>
       </c>
       <c r="B940" s="6" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
     </row>
     <row r="941" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A941" s="9" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
       <c r="B941" s="6" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
     </row>
     <row r="942" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A942" s="9" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="B942" s="6" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
     </row>
     <row r="943" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A943" s="9" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="B943" s="6" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
     </row>
     <row r="944" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A944" s="9" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="B944" s="6" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
     </row>
     <row r="945" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A945" s="9" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="B945" s="6" t="s">
-        <v>215</v>
+        <v>412</v>
       </c>
     </row>
     <row r="946" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A946" s="9" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="B946" s="6" t="s">
-        <v>217</v>
+        <v>412</v>
       </c>
     </row>
     <row r="947" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A947" s="9" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="B947" s="6" t="s">
-        <v>401</v>
+        <v>215</v>
       </c>
     </row>
     <row r="948" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A948" s="9" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="B948" s="6" t="s">
-        <v>403</v>
+        <v>217</v>
       </c>
     </row>
     <row r="949" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A949" s="9" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="B949" s="6" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
     </row>
     <row r="950" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A950" s="9" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="B950" s="6" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
     </row>
     <row r="951" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A951" s="9" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="B951" s="6" t="s">
-        <v>395</v>
+        <v>405</v>
       </c>
     </row>
     <row r="952" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A952" s="9" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="B952" s="6" t="s">
-        <v>397</v>
+        <v>407</v>
       </c>
     </row>
     <row r="953" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A953" s="9" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="B953" s="6" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
     </row>
     <row r="954" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A954" s="9" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="B954" s="6" t="s">
-        <v>273</v>
+        <v>397</v>
       </c>
     </row>
     <row r="955" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A955" s="9" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="B955" s="6" t="s">
-        <v>275</v>
+        <v>399</v>
       </c>
     </row>
     <row r="956" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A956" s="9" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="B956" s="6" t="s">
-        <v>320</v>
+        <v>273</v>
       </c>
     </row>
     <row r="957" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A957" s="9" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="B957" s="6" t="s">
-        <v>281</v>
+        <v>275</v>
       </c>
     </row>
     <row r="958" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A958" s="9" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="B958" s="6" t="s">
-        <v>428</v>
+        <v>320</v>
       </c>
     </row>
     <row r="959" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A959" s="9" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
       <c r="B959" s="6" t="s">
-        <v>295</v>
+        <v>281</v>
       </c>
     </row>
     <row r="960" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A960" s="9" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
       <c r="B960" s="6" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
     </row>
     <row r="961" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A961" s="9" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="B961" s="6" t="s">
-        <v>433</v>
+        <v>295</v>
       </c>
     </row>
     <row r="962" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A962" s="9" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
       <c r="B962" s="6" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
     </row>
     <row r="963" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A963" s="9" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="B963" s="6" t="s">
-        <v>437</v>
+        <v>433</v>
       </c>
     </row>
     <row r="964" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A964" s="9" t="s">
-        <v>438</v>
+        <v>434</v>
       </c>
       <c r="B964" s="6" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
     </row>
     <row r="965" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A965" s="9" t="s">
-        <v>440</v>
+        <v>436</v>
       </c>
       <c r="B965" s="6" t="s">
-        <v>441</v>
+        <v>437</v>
       </c>
     </row>
     <row r="966" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A966" s="9" t="s">
-        <v>442</v>
+        <v>438</v>
       </c>
       <c r="B966" s="6" t="s">
-        <v>443</v>
+        <v>439</v>
       </c>
     </row>
     <row r="967" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A967" s="9" t="s">
-        <v>444</v>
+        <v>440</v>
       </c>
       <c r="B967" s="6" t="s">
-        <v>407</v>
+        <v>441</v>
       </c>
     </row>
     <row r="968" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A968" s="9" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
       <c r="B968" s="6" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
     </row>
     <row r="969" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A969" s="9" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
       <c r="B969" s="6" t="s">
-        <v>448</v>
+        <v>407</v>
       </c>
     </row>
     <row r="970" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A970" s="9" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
       <c r="B970" s="6" t="s">
-        <v>450</v>
+        <v>446</v>
       </c>
     </row>
     <row r="971" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A971" s="9" t="s">
-        <v>451</v>
+        <v>447</v>
       </c>
       <c r="B971" s="6" t="s">
-        <v>452</v>
+        <v>448</v>
       </c>
     </row>
     <row r="972" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A972" s="9" t="s">
-        <v>453</v>
+        <v>449</v>
       </c>
       <c r="B972" s="6" t="s">
-        <v>454</v>
+        <v>450</v>
       </c>
     </row>
     <row r="973" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A973" s="9" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
       <c r="B973" s="6" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
     </row>
     <row r="974" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A974" s="9" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
       <c r="B974" s="6" t="s">
-        <v>458</v>
+        <v>454</v>
       </c>
     </row>
     <row r="975" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A975" s="9" t="s">
-        <v>459</v>
+        <v>455</v>
       </c>
       <c r="B975" s="6" t="s">
-        <v>460</v>
+        <v>456</v>
       </c>
     </row>
     <row r="976" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A976" s="9" t="s">
-        <v>461</v>
+        <v>457</v>
       </c>
       <c r="B976" s="6" t="s">
-        <v>462</v>
+        <v>458</v>
       </c>
     </row>
     <row r="977" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A977" s="9" t="s">
-        <v>463</v>
+        <v>459</v>
       </c>
       <c r="B977" s="6" t="s">
-        <v>464</v>
+        <v>460</v>
       </c>
     </row>
     <row r="978" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A978" s="9" t="s">
-        <v>465</v>
+        <v>461</v>
       </c>
       <c r="B978" s="6" t="s">
-        <v>466</v>
+        <v>462</v>
       </c>
     </row>
     <row r="979" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A979" s="9" t="s">
-        <v>467</v>
+        <v>463</v>
       </c>
       <c r="B979" s="6" t="s">
-        <v>468</v>
+        <v>464</v>
       </c>
     </row>
     <row r="980" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A980" s="9" t="s">
-        <v>469</v>
+        <v>465</v>
       </c>
       <c r="B980" s="6" t="s">
-        <v>470</v>
+        <v>466</v>
       </c>
     </row>
     <row r="981" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A981" s="9" t="s">
-        <v>471</v>
+        <v>467</v>
       </c>
       <c r="B981" s="6" t="s">
-        <v>472</v>
+        <v>468</v>
       </c>
     </row>
     <row r="982" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A982" s="9" t="s">
-        <v>473</v>
+        <v>469</v>
       </c>
       <c r="B982" s="6" t="s">
-        <v>474</v>
+        <v>470</v>
       </c>
     </row>
     <row r="983" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A983" s="9" t="s">
-        <v>475</v>
+        <v>471</v>
       </c>
       <c r="B983" s="6" t="s">
-        <v>476</v>
+        <v>472</v>
       </c>
     </row>
     <row r="984" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A984" s="9" t="s">
-        <v>477</v>
+        <v>473</v>
       </c>
       <c r="B984" s="6" t="s">
-        <v>478</v>
+        <v>474</v>
       </c>
     </row>
     <row r="985" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A985" s="9" t="s">
-        <v>479</v>
+        <v>475</v>
       </c>
       <c r="B985" s="6" t="s">
-        <v>480</v>
+        <v>476</v>
       </c>
     </row>
     <row r="986" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A986" s="9" t="s">
-        <v>481</v>
+        <v>477</v>
       </c>
       <c r="B986" s="6" t="s">
-        <v>482</v>
+        <v>478</v>
       </c>
     </row>
     <row r="987" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A987" s="9" t="s">
-        <v>483</v>
+        <v>479</v>
       </c>
       <c r="B987" s="6" t="s">
-        <v>484</v>
+        <v>480</v>
       </c>
     </row>
     <row r="988" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A988" s="9" t="s">
-        <v>485</v>
+        <v>481</v>
       </c>
       <c r="B988" s="6" t="s">
-        <v>486</v>
+        <v>482</v>
       </c>
     </row>
     <row r="989" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A989" s="9" t="s">
-        <v>487</v>
+        <v>483</v>
       </c>
       <c r="B989" s="6" t="s">
-        <v>488</v>
+        <v>484</v>
       </c>
     </row>
     <row r="990" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A990" s="9" t="s">
-        <v>489</v>
+        <v>485</v>
       </c>
       <c r="B990" s="6" t="s">
-        <v>490</v>
+        <v>486</v>
       </c>
     </row>
     <row r="991" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A991" s="9" t="s">
-        <v>491</v>
+        <v>487</v>
       </c>
       <c r="B991" s="6" t="s">
-        <v>492</v>
+        <v>488</v>
       </c>
     </row>
     <row r="992" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A992" s="9" t="s">
-        <v>493</v>
+        <v>489</v>
       </c>
       <c r="B992" s="6" t="s">
-        <v>494</v>
+        <v>490</v>
       </c>
     </row>
     <row r="993" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A993" s="9" t="s">
-        <v>495</v>
+        <v>491</v>
       </c>
       <c r="B993" s="6" t="s">
-        <v>496</v>
+        <v>492</v>
       </c>
     </row>
     <row r="994" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A994" s="9" t="s">
-        <v>497</v>
+        <v>493</v>
       </c>
       <c r="B994" s="6" t="s">
-        <v>498</v>
+        <v>494</v>
       </c>
     </row>
     <row r="995" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A995" s="9" t="s">
-        <v>499</v>
+        <v>495</v>
       </c>
       <c r="B995" s="6" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
     </row>
     <row r="996" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A996" s="9" t="s">
-        <v>501</v>
+        <v>497</v>
       </c>
       <c r="B996" s="6" t="s">
-        <v>502</v>
+        <v>498</v>
       </c>
     </row>
     <row r="997" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A997" s="9" t="s">
-        <v>503</v>
+        <v>499</v>
       </c>
       <c r="B997" s="6" t="s">
-        <v>504</v>
+        <v>500</v>
       </c>
     </row>
     <row r="998" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A998" s="9" t="s">
-        <v>505</v>
+        <v>501</v>
       </c>
       <c r="B998" s="6" t="s">
-        <v>506</v>
+        <v>502</v>
       </c>
     </row>
     <row r="999" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A999" s="9" t="s">
-        <v>507</v>
+        <v>503</v>
       </c>
       <c r="B999" s="6" t="s">
-        <v>508</v>
+        <v>504</v>
       </c>
     </row>
     <row r="1000" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1000" s="9" t="s">
-        <v>509</v>
+        <v>505</v>
       </c>
       <c r="B1000" s="6" t="s">
-        <v>510</v>
+        <v>506</v>
       </c>
     </row>
     <row r="1001" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1001" s="9" t="s">
-        <v>511</v>
+        <v>507</v>
       </c>
       <c r="B1001" s="6" t="s">
-        <v>512</v>
+        <v>508</v>
       </c>
     </row>
     <row r="1002" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1002" s="9" t="s">
-        <v>513</v>
+        <v>509</v>
       </c>
       <c r="B1002" s="6" t="s">
-        <v>514</v>
+        <v>510</v>
       </c>
     </row>
     <row r="1003" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1003" s="9" t="s">
-        <v>515</v>
+        <v>511</v>
       </c>
       <c r="B1003" s="6" t="s">
-        <v>516</v>
+        <v>512</v>
       </c>
     </row>
     <row r="1004" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1004" s="9" t="s">
-        <v>517</v>
+        <v>513</v>
       </c>
       <c r="B1004" s="6" t="s">
-        <v>518</v>
+        <v>514</v>
       </c>
     </row>
     <row r="1005" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1005" s="9" t="s">
-        <v>519</v>
+        <v>515</v>
       </c>
       <c r="B1005" s="6" t="s">
-        <v>520</v>
+        <v>516</v>
       </c>
     </row>
     <row r="1006" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1006" s="9" t="s">
-        <v>521</v>
+        <v>517</v>
       </c>
       <c r="B1006" s="6" t="s">
-        <v>522</v>
+        <v>518</v>
       </c>
     </row>
     <row r="1007" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1007" s="9" t="s">
-        <v>523</v>
+        <v>519</v>
       </c>
       <c r="B1007" s="6" t="s">
-        <v>524</v>
+        <v>520</v>
       </c>
     </row>
     <row r="1008" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1008" s="9" t="s">
-        <v>525</v>
+        <v>521</v>
       </c>
       <c r="B1008" s="6" t="s">
-        <v>526</v>
+        <v>522</v>
       </c>
     </row>
     <row r="1009" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1009" s="9" t="s">
-        <v>527</v>
+        <v>523</v>
       </c>
       <c r="B1009" s="6" t="s">
-        <v>528</v>
+        <v>524</v>
       </c>
     </row>
     <row r="1010" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1010" s="9" t="s">
-        <v>529</v>
+        <v>525</v>
       </c>
       <c r="B1010" s="6" t="s">
-        <v>530</v>
+        <v>526</v>
       </c>
     </row>
     <row r="1011" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1011" s="9" t="s">
-        <v>531</v>
+        <v>527</v>
       </c>
       <c r="B1011" s="6" t="s">
-        <v>532</v>
+        <v>528</v>
       </c>
     </row>
     <row r="1012" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1012" s="9" t="s">
-        <v>533</v>
+        <v>529</v>
       </c>
       <c r="B1012" s="6" t="s">
-        <v>534</v>
+        <v>530</v>
       </c>
     </row>
     <row r="1013" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1013" s="9" t="s">
-        <v>535</v>
+        <v>531</v>
       </c>
       <c r="B1013" s="6" t="s">
-        <v>536</v>
+        <v>532</v>
       </c>
     </row>
     <row r="1014" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1014" s="9" t="s">
-        <v>537</v>
+        <v>533</v>
       </c>
       <c r="B1014" s="6" t="s">
-        <v>538</v>
+        <v>534</v>
       </c>
     </row>
     <row r="1015" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1015" s="9" t="s">
-        <v>539</v>
+        <v>535</v>
       </c>
       <c r="B1015" s="6" t="s">
-        <v>540</v>
+        <v>536</v>
       </c>
     </row>
     <row r="1016" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1016" s="9" t="s">
-        <v>541</v>
+        <v>537</v>
       </c>
       <c r="B1016" s="6" t="s">
-        <v>542</v>
+        <v>538</v>
       </c>
     </row>
     <row r="1017" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1017" s="9" t="s">
-        <v>543</v>
+        <v>539</v>
       </c>
       <c r="B1017" s="6" t="s">
-        <v>544</v>
+        <v>540</v>
       </c>
     </row>
     <row r="1018" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1018" s="9" t="s">
-        <v>545</v>
+        <v>541</v>
       </c>
       <c r="B1018" s="6" t="s">
-        <v>546</v>
+        <v>542</v>
       </c>
     </row>
     <row r="1019" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1019" s="9" t="s">
-        <v>547</v>
+        <v>543</v>
       </c>
       <c r="B1019" s="6" t="s">
-        <v>548</v>
+        <v>544</v>
       </c>
     </row>
     <row r="1020" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1020" s="9" t="s">
-        <v>549</v>
+        <v>545</v>
       </c>
       <c r="B1020" s="6" t="s">
-        <v>550</v>
+        <v>546</v>
       </c>
     </row>
     <row r="1021" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1021" s="9" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B1021" s="6" t="s">
-        <v>552</v>
+        <v>548</v>
       </c>
     </row>
     <row r="1022" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1022" s="9" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="B1022" s="6" t="s">
-        <v>554</v>
+        <v>550</v>
       </c>
     </row>
     <row r="1023" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1023" s="9" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
       <c r="B1023" s="6" t="s">
-        <v>556</v>
+        <v>552</v>
       </c>
     </row>
     <row r="1024" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1024" s="9" t="s">
-        <v>557</v>
+        <v>553</v>
       </c>
       <c r="B1024" s="6" t="s">
-        <v>558</v>
+        <v>554</v>
       </c>
     </row>
     <row r="1025" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1025" s="9" t="s">
-        <v>559</v>
+        <v>555</v>
       </c>
       <c r="B1025" s="6" t="s">
-        <v>560</v>
+        <v>556</v>
       </c>
     </row>
     <row r="1026" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1026" s="9" t="s">
-        <v>561</v>
+        <v>557</v>
       </c>
       <c r="B1026" s="6" t="s">
-        <v>562</v>
+        <v>558</v>
       </c>
     </row>
     <row r="1027" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1027" s="9" t="s">
-        <v>563</v>
+        <v>559</v>
       </c>
       <c r="B1027" s="6" t="s">
-        <v>564</v>
+        <v>560</v>
       </c>
     </row>
     <row r="1028" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1028" s="9" t="s">
-        <v>565</v>
+        <v>561</v>
       </c>
       <c r="B1028" s="6" t="s">
-        <v>566</v>
+        <v>562</v>
       </c>
     </row>
     <row r="1029" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1029" s="9" t="s">
-        <v>567</v>
+        <v>563</v>
       </c>
       <c r="B1029" s="6" t="s">
-        <v>568</v>
+        <v>564</v>
       </c>
     </row>
     <row r="1030" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1030" s="9" t="s">
-        <v>569</v>
+        <v>565</v>
       </c>
       <c r="B1030" s="6" t="s">
-        <v>570</v>
+        <v>566</v>
       </c>
     </row>
     <row r="1031" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1031" s="9" t="s">
-        <v>571</v>
+        <v>567</v>
       </c>
       <c r="B1031" s="6" t="s">
-        <v>572</v>
+        <v>568</v>
       </c>
     </row>
     <row r="1032" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1032" s="9" t="s">
-        <v>573</v>
+        <v>569</v>
       </c>
       <c r="B1032" s="6" t="s">
-        <v>574</v>
+        <v>570</v>
       </c>
     </row>
     <row r="1033" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1033" s="9" t="s">
-        <v>575</v>
+        <v>571</v>
       </c>
       <c r="B1033" s="6" t="s">
-        <v>576</v>
+        <v>572</v>
       </c>
     </row>
     <row r="1034" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1034" s="9" t="s">
-        <v>577</v>
+        <v>573</v>
       </c>
       <c r="B1034" s="6" t="s">
-        <v>578</v>
+        <v>574</v>
       </c>
     </row>
     <row r="1035" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1035" s="9" t="s">
-        <v>579</v>
+        <v>575</v>
       </c>
       <c r="B1035" s="6" t="s">
-        <v>580</v>
+        <v>576</v>
       </c>
     </row>
     <row r="1036" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1036" s="9" t="s">
-        <v>581</v>
+        <v>577</v>
       </c>
       <c r="B1036" s="6" t="s">
-        <v>582</v>
+        <v>578</v>
       </c>
     </row>
     <row r="1037" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1037" s="9" t="s">
-        <v>583</v>
+        <v>579</v>
       </c>
       <c r="B1037" s="6" t="s">
-        <v>584</v>
+        <v>580</v>
       </c>
     </row>
     <row r="1038" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1038" s="9" t="s">
-        <v>585</v>
+        <v>581</v>
       </c>
       <c r="B1038" s="6" t="s">
-        <v>586</v>
+        <v>582</v>
       </c>
     </row>
     <row r="1039" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1039" s="9" t="s">
-        <v>587</v>
+        <v>583</v>
       </c>
       <c r="B1039" s="6" t="s">
-        <v>588</v>
+        <v>584</v>
       </c>
     </row>
     <row r="1040" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1040" s="9" t="s">
-        <v>589</v>
+        <v>585</v>
       </c>
       <c r="B1040" s="6" t="s">
-        <v>590</v>
+        <v>586</v>
       </c>
     </row>
     <row r="1041" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1041" s="9" t="s">
-        <v>591</v>
+        <v>587</v>
       </c>
       <c r="B1041" s="6" t="s">
-        <v>592</v>
+        <v>588</v>
       </c>
     </row>
     <row r="1042" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1042" s="9" t="s">
-        <v>593</v>
+        <v>589</v>
       </c>
       <c r="B1042" s="6" t="s">
-        <v>594</v>
+        <v>590</v>
       </c>
     </row>
     <row r="1043" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1043" s="9" t="s">
-        <v>595</v>
+        <v>591</v>
       </c>
       <c r="B1043" s="6" t="s">
-        <v>596</v>
+        <v>592</v>
       </c>
     </row>
     <row r="1044" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1044" s="9" t="s">
-        <v>597</v>
+        <v>593</v>
       </c>
       <c r="B1044" s="6" t="s">
-        <v>598</v>
+        <v>594</v>
       </c>
     </row>
     <row r="1045" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1045" s="9" t="s">
-        <v>599</v>
+        <v>595</v>
       </c>
       <c r="B1045" s="6" t="s">
-        <v>600</v>
+        <v>596</v>
       </c>
     </row>
     <row r="1046" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1046" s="9" t="s">
-        <v>601</v>
+        <v>597</v>
       </c>
       <c r="B1046" s="6" t="s">
-        <v>602</v>
+        <v>598</v>
       </c>
     </row>
     <row r="1047" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1047" s="9" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
       <c r="B1047" s="6" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
     </row>
     <row r="1048" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1048" s="9" t="s">
-        <v>605</v>
+        <v>601</v>
       </c>
       <c r="B1048" s="6" t="s">
-        <v>606</v>
+        <v>602</v>
       </c>
     </row>
     <row r="1049" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1049" s="9" t="s">
-        <v>607</v>
+        <v>603</v>
       </c>
       <c r="B1049" s="6" t="s">
-        <v>608</v>
+        <v>604</v>
       </c>
     </row>
     <row r="1050" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1050" s="9" t="s">
-        <v>609</v>
+        <v>605</v>
       </c>
       <c r="B1050" s="6" t="s">
-        <v>610</v>
+        <v>606</v>
       </c>
     </row>
     <row r="1051" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1051" s="9" t="s">
-        <v>611</v>
+        <v>607</v>
       </c>
       <c r="B1051" s="6" t="s">
-        <v>612</v>
+        <v>608</v>
       </c>
     </row>
     <row r="1052" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1052" s="9" t="s">
-        <v>613</v>
+        <v>609</v>
       </c>
       <c r="B1052" s="6" t="s">
-        <v>614</v>
+        <v>610</v>
       </c>
     </row>
     <row r="1053" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1053" s="9" t="s">
-        <v>615</v>
+        <v>611</v>
       </c>
       <c r="B1053" s="6" t="s">
-        <v>616</v>
+        <v>612</v>
       </c>
     </row>
     <row r="1054" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1054" s="9" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="B1054" s="6" t="s">
-        <v>618</v>
+        <v>614</v>
       </c>
     </row>
     <row r="1055" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1055" s="9" t="s">
-        <v>619</v>
+        <v>615</v>
       </c>
       <c r="B1055" s="6" t="s">
-        <v>620</v>
+        <v>616</v>
       </c>
     </row>
     <row r="1056" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1056" s="9" t="s">
-        <v>621</v>
+        <v>617</v>
       </c>
       <c r="B1056" s="6" t="s">
-        <v>622</v>
+        <v>618</v>
       </c>
     </row>
     <row r="1057" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1057" s="9" t="s">
-        <v>623</v>
+        <v>619</v>
       </c>
       <c r="B1057" s="6" t="s">
-        <v>624</v>
+        <v>620</v>
       </c>
     </row>
     <row r="1058" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1058" s="9" t="s">
-        <v>625</v>
+        <v>621</v>
       </c>
       <c r="B1058" s="6" t="s">
-        <v>626</v>
+        <v>622</v>
       </c>
     </row>
     <row r="1059" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1059" s="9" t="s">
-        <v>627</v>
+        <v>623</v>
       </c>
       <c r="B1059" s="6" t="s">
-        <v>628</v>
+        <v>624</v>
       </c>
     </row>
     <row r="1060" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1060" s="9" t="s">
-        <v>629</v>
+        <v>625</v>
       </c>
       <c r="B1060" s="6" t="s">
-        <v>630</v>
+        <v>626</v>
       </c>
     </row>
     <row r="1061" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1061" s="9" t="s">
-        <v>631</v>
+        <v>627</v>
       </c>
       <c r="B1061" s="6" t="s">
-        <v>632</v>
+        <v>628</v>
       </c>
     </row>
     <row r="1062" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1062" s="9" t="s">
-        <v>633</v>
+        <v>629</v>
       </c>
       <c r="B1062" s="6" t="s">
-        <v>634</v>
+        <v>630</v>
       </c>
     </row>
     <row r="1063" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1063" s="9" t="s">
-        <v>635</v>
+        <v>631</v>
       </c>
       <c r="B1063" s="6" t="s">
-        <v>636</v>
+        <v>632</v>
       </c>
     </row>
     <row r="1064" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1064" s="9" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
       <c r="B1064" s="6" t="s">
-        <v>638</v>
+        <v>634</v>
       </c>
     </row>
     <row r="1065" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1065" s="9" t="s">
-        <v>639</v>
+        <v>635</v>
       </c>
       <c r="B1065" s="6" t="s">
-        <v>640</v>
+        <v>636</v>
       </c>
     </row>
     <row r="1066" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1066" s="9" t="s">
-        <v>641</v>
+        <v>637</v>
       </c>
       <c r="B1066" s="6" t="s">
-        <v>642</v>
+        <v>638</v>
       </c>
     </row>
     <row r="1067" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1067" s="9" t="s">
-        <v>643</v>
+        <v>639</v>
       </c>
       <c r="B1067" s="6" t="s">
-        <v>644</v>
+        <v>640</v>
       </c>
     </row>
     <row r="1068" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1068" s="9" t="s">
-        <v>645</v>
+        <v>641</v>
       </c>
       <c r="B1068" s="6" t="s">
-        <v>646</v>
+        <v>642</v>
       </c>
     </row>
     <row r="1069" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1069" s="9" t="s">
-        <v>647</v>
+        <v>643</v>
       </c>
       <c r="B1069" s="6" t="s">
-        <v>648</v>
+        <v>644</v>
       </c>
     </row>
     <row r="1070" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1070" s="9" t="s">
-        <v>649</v>
+        <v>645</v>
       </c>
       <c r="B1070" s="6" t="s">
-        <v>650</v>
+        <v>646</v>
       </c>
     </row>
     <row r="1071" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1071" s="9" t="s">
-        <v>651</v>
+        <v>647</v>
       </c>
       <c r="B1071" s="6" t="s">
-        <v>652</v>
+        <v>648</v>
       </c>
     </row>
     <row r="1072" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1072" s="9" t="s">
-        <v>653</v>
+        <v>649</v>
       </c>
       <c r="B1072" s="6" t="s">
-        <v>654</v>
+        <v>650</v>
       </c>
     </row>
     <row r="1073" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1073" s="9" t="s">
-        <v>655</v>
+        <v>651</v>
       </c>
       <c r="B1073" s="6" t="s">
-        <v>656</v>
+        <v>652</v>
       </c>
     </row>
     <row r="1074" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1074" s="9" t="s">
-        <v>657</v>
+        <v>653</v>
       </c>
       <c r="B1074" s="6" t="s">
-        <v>658</v>
+        <v>654</v>
       </c>
     </row>
     <row r="1075" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1075" s="9" t="s">
-        <v>659</v>
+        <v>655</v>
       </c>
       <c r="B1075" s="6" t="s">
-        <v>660</v>
+        <v>656</v>
       </c>
     </row>
     <row r="1076" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1076" s="9" t="s">
-        <v>661</v>
+        <v>657</v>
       </c>
       <c r="B1076" s="6" t="s">
-        <v>662</v>
+        <v>658</v>
       </c>
     </row>
     <row r="1077" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1077" s="9" t="s">
-        <v>663</v>
+        <v>659</v>
       </c>
       <c r="B1077" s="6" t="s">
-        <v>664</v>
+        <v>660</v>
       </c>
     </row>
     <row r="1078" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1078" s="9" t="s">
-        <v>665</v>
+        <v>661</v>
       </c>
       <c r="B1078" s="6" t="s">
-        <v>666</v>
+        <v>662</v>
       </c>
     </row>
     <row r="1079" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1079" s="9" t="s">
-        <v>667</v>
+        <v>663</v>
       </c>
       <c r="B1079" s="6" t="s">
-        <v>668</v>
+        <v>664</v>
       </c>
     </row>
     <row r="1080" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1080" s="9" t="s">
-        <v>669</v>
+        <v>665</v>
       </c>
       <c r="B1080" s="6" t="s">
-        <v>670</v>
+        <v>666</v>
       </c>
     </row>
     <row r="1081" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1081" s="9" t="s">
-        <v>671</v>
+        <v>667</v>
       </c>
       <c r="B1081" s="6" t="s">
-        <v>672</v>
+        <v>668</v>
       </c>
     </row>
     <row r="1082" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1082" s="9" t="s">
-        <v>673</v>
+        <v>669</v>
       </c>
       <c r="B1082" s="6" t="s">
-        <v>674</v>
+        <v>670</v>
       </c>
     </row>
     <row r="1083" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1083" s="9" t="s">
-        <v>675</v>
+        <v>671</v>
       </c>
       <c r="B1083" s="6" t="s">
-        <v>676</v>
+        <v>672</v>
       </c>
     </row>
     <row r="1084" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1084" s="9" t="s">
-        <v>677</v>
+        <v>673</v>
       </c>
       <c r="B1084" s="6" t="s">
-        <v>678</v>
+        <v>674</v>
       </c>
     </row>
     <row r="1085" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1085" s="9" t="s">
-        <v>679</v>
+        <v>675</v>
       </c>
       <c r="B1085" s="6" t="s">
-        <v>680</v>
+        <v>676</v>
       </c>
     </row>
     <row r="1086" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1086" s="9" t="s">
-        <v>681</v>
+        <v>677</v>
       </c>
       <c r="B1086" s="6" t="s">
-        <v>682</v>
+        <v>678</v>
       </c>
     </row>
     <row r="1087" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1087" s="9" t="s">
-        <v>683</v>
+        <v>679</v>
       </c>
       <c r="B1087" s="6" t="s">
-        <v>684</v>
+        <v>680</v>
       </c>
     </row>
     <row r="1088" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1088" s="9" t="s">
-        <v>685</v>
+        <v>681</v>
       </c>
       <c r="B1088" s="6" t="s">
-        <v>686</v>
+        <v>682</v>
       </c>
     </row>
     <row r="1089" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1089" s="9" t="s">
-        <v>687</v>
+        <v>683</v>
       </c>
       <c r="B1089" s="6" t="s">
-        <v>688</v>
+        <v>684</v>
       </c>
     </row>
     <row r="1090" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1090" s="9" t="s">
-        <v>689</v>
+        <v>685</v>
       </c>
       <c r="B1090" s="6" t="s">
-        <v>690</v>
+        <v>686</v>
       </c>
     </row>
     <row r="1091" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1091" s="9" t="s">
-        <v>691</v>
+        <v>687</v>
       </c>
       <c r="B1091" s="6" t="s">
-        <v>692</v>
+        <v>688</v>
       </c>
     </row>
     <row r="1092" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1092" s="9" t="s">
-        <v>693</v>
+        <v>689</v>
       </c>
       <c r="B1092" s="6" t="s">
-        <v>694</v>
+        <v>690</v>
       </c>
     </row>
     <row r="1093" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1093" s="9" t="s">
-        <v>695</v>
+        <v>691</v>
       </c>
       <c r="B1093" s="6" t="s">
-        <v>696</v>
+        <v>692</v>
       </c>
     </row>
     <row r="1094" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1094" s="9" t="s">
-        <v>697</v>
+        <v>693</v>
       </c>
       <c r="B1094" s="6" t="s">
-        <v>698</v>
+        <v>694</v>
       </c>
     </row>
     <row r="1095" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1095" s="9" t="s">
-        <v>699</v>
+        <v>695</v>
       </c>
       <c r="B1095" s="6" t="s">
-        <v>700</v>
+        <v>696</v>
       </c>
     </row>
     <row r="1096" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1096" s="9" t="s">
-        <v>701</v>
+        <v>697</v>
       </c>
       <c r="B1096" s="6" t="s">
-        <v>702</v>
+        <v>698</v>
       </c>
     </row>
     <row r="1097" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1097" s="9" t="s">
-        <v>703</v>
+        <v>699</v>
       </c>
       <c r="B1097" s="6" t="s">
-        <v>704</v>
+        <v>700</v>
       </c>
     </row>
     <row r="1098" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1098" s="9" t="s">
-        <v>705</v>
+        <v>701</v>
       </c>
       <c r="B1098" s="6" t="s">
-        <v>706</v>
+        <v>702</v>
       </c>
     </row>
     <row r="1099" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1099" s="9" t="s">
-        <v>707</v>
+        <v>703</v>
       </c>
       <c r="B1099" s="6" t="s">
-        <v>708</v>
+        <v>704</v>
       </c>
     </row>
     <row r="1100" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1100" s="9" t="s">
-        <v>709</v>
+        <v>705</v>
       </c>
       <c r="B1100" s="6" t="s">
-        <v>710</v>
+        <v>706</v>
       </c>
     </row>
     <row r="1101" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1101" s="9" t="s">
-        <v>711</v>
+        <v>707</v>
       </c>
       <c r="B1101" s="6" t="s">
-        <v>712</v>
+        <v>708</v>
       </c>
     </row>
     <row r="1102" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1102" s="9" t="s">
-        <v>713</v>
+        <v>709</v>
       </c>
       <c r="B1102" s="6" t="s">
-        <v>714</v>
+        <v>710</v>
       </c>
     </row>
     <row r="1103" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1103" s="9" t="s">
-        <v>715</v>
+        <v>711</v>
       </c>
       <c r="B1103" s="6" t="s">
-        <v>716</v>
+        <v>712</v>
       </c>
     </row>
     <row r="1104" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1104" s="9" t="s">
-        <v>717</v>
+        <v>713</v>
       </c>
       <c r="B1104" s="6" t="s">
-        <v>718</v>
+        <v>714</v>
       </c>
     </row>
     <row r="1105" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1105" s="9" t="s">
-        <v>719</v>
+        <v>715</v>
       </c>
       <c r="B1105" s="6" t="s">
-        <v>720</v>
+        <v>716</v>
       </c>
     </row>
     <row r="1106" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1106" s="9" t="s">
-        <v>721</v>
+        <v>717</v>
       </c>
       <c r="B1106" s="6" t="s">
-        <v>722</v>
+        <v>718</v>
       </c>
     </row>
     <row r="1107" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1107" s="9" t="s">
-        <v>723</v>
+        <v>719</v>
       </c>
       <c r="B1107" s="6" t="s">
-        <v>724</v>
+        <v>720</v>
       </c>
     </row>
     <row r="1108" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1108" s="9" t="s">
-        <v>725</v>
+        <v>721</v>
       </c>
       <c r="B1108" s="6" t="s">
-        <v>726</v>
+        <v>722</v>
       </c>
     </row>
     <row r="1109" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1109" s="9" t="s">
-        <v>727</v>
+        <v>723</v>
       </c>
       <c r="B1109" s="6" t="s">
-        <v>728</v>
+        <v>724</v>
       </c>
     </row>
     <row r="1110" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1110" s="9" t="s">
-        <v>729</v>
+        <v>725</v>
       </c>
       <c r="B1110" s="6" t="s">
-        <v>730</v>
+        <v>726</v>
       </c>
     </row>
     <row r="1111" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1111" s="9" t="s">
-        <v>731</v>
+        <v>727</v>
       </c>
       <c r="B1111" s="6" t="s">
-        <v>732</v>
+        <v>728</v>
       </c>
     </row>
     <row r="1112" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1112" s="9" t="s">
-        <v>733</v>
+        <v>729</v>
       </c>
       <c r="B1112" s="6" t="s">
-        <v>734</v>
+        <v>730</v>
       </c>
     </row>
     <row r="1113" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1113" s="9" t="s">
-        <v>735</v>
+        <v>731</v>
       </c>
       <c r="B1113" s="6" t="s">
-        <v>736</v>
+        <v>732</v>
       </c>
     </row>
     <row r="1114" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1114" s="9" t="s">
-        <v>737</v>
+        <v>733</v>
       </c>
       <c r="B1114" s="6" t="s">
-        <v>738</v>
+        <v>734</v>
       </c>
     </row>
     <row r="1115" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1115" s="9" t="s">
-        <v>739</v>
+        <v>735</v>
       </c>
       <c r="B1115" s="6" t="s">
-        <v>740</v>
+        <v>736</v>
       </c>
     </row>
     <row r="1116" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1116" s="9" t="s">
-        <v>741</v>
+        <v>737</v>
       </c>
       <c r="B1116" s="6" t="s">
-        <v>742</v>
+        <v>738</v>
       </c>
     </row>
     <row r="1117" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1117" s="9" t="s">
-        <v>743</v>
+        <v>739</v>
       </c>
       <c r="B1117" s="6" t="s">
-        <v>744</v>
+        <v>740</v>
       </c>
     </row>
     <row r="1118" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1118" s="9" t="s">
-        <v>745</v>
+        <v>741</v>
       </c>
       <c r="B1118" s="6" t="s">
-        <v>746</v>
+        <v>742</v>
       </c>
     </row>
     <row r="1119" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1119" s="9" t="s">
-        <v>747</v>
+        <v>743</v>
       </c>
       <c r="B1119" s="6" t="s">
-        <v>748</v>
+        <v>744</v>
       </c>
     </row>
     <row r="1120" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1120" s="9" t="s">
-        <v>749</v>
+        <v>745</v>
       </c>
       <c r="B1120" s="6" t="s">
-        <v>750</v>
+        <v>746</v>
       </c>
     </row>
     <row r="1121" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1121" s="9" t="s">
-        <v>751</v>
+        <v>747</v>
       </c>
       <c r="B1121" s="6" t="s">
-        <v>752</v>
+        <v>748</v>
       </c>
     </row>
     <row r="1122" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1122" s="9" t="s">
-        <v>753</v>
+        <v>749</v>
       </c>
       <c r="B1122" s="6" t="s">
-        <v>754</v>
+        <v>750</v>
       </c>
     </row>
     <row r="1123" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1123" s="9" t="s">
-        <v>755</v>
+        <v>751</v>
       </c>
       <c r="B1123" s="6" t="s">
-        <v>756</v>
+        <v>752</v>
       </c>
     </row>
     <row r="1124" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1124" s="9" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
       <c r="B1124" s="6" t="s">
-        <v>758</v>
+        <v>754</v>
       </c>
     </row>
     <row r="1125" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1125" s="9" t="s">
-        <v>759</v>
+        <v>755</v>
       </c>
       <c r="B1125" s="6" t="s">
-        <v>760</v>
+        <v>756</v>
       </c>
     </row>
     <row r="1126" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1126" s="9" t="s">
-        <v>761</v>
+        <v>757</v>
       </c>
       <c r="B1126" s="6" t="s">
-        <v>762</v>
+        <v>758</v>
       </c>
     </row>
     <row r="1127" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1127" s="9" t="s">
-        <v>763</v>
+        <v>759</v>
       </c>
       <c r="B1127" s="6" t="s">
-        <v>764</v>
+        <v>760</v>
       </c>
     </row>
     <row r="1128" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1128" s="9" t="s">
-        <v>765</v>
+        <v>761</v>
       </c>
       <c r="B1128" s="6" t="s">
-        <v>766</v>
+        <v>762</v>
       </c>
     </row>
     <row r="1129" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1129" s="9" t="s">
-        <v>767</v>
+        <v>763</v>
       </c>
       <c r="B1129" s="6" t="s">
-        <v>304</v>
+        <v>764</v>
       </c>
     </row>
     <row r="1130" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1130" s="9" t="s">
-        <v>768</v>
+        <v>765</v>
       </c>
       <c r="B1130" s="6" t="s">
-        <v>769</v>
+        <v>766</v>
       </c>
     </row>
     <row r="1131" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1131" s="9" t="s">
-        <v>770</v>
+        <v>767</v>
       </c>
       <c r="B1131" s="6" t="s">
-        <v>316</v>
+        <v>304</v>
       </c>
     </row>
     <row r="1132" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1132" s="9" t="s">
-        <v>771</v>
+        <v>768</v>
       </c>
       <c r="B1132" s="6" t="s">
-        <v>211</v>
+        <v>769</v>
       </c>
     </row>
     <row r="1133" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1133" s="9" t="s">
-        <v>772</v>
+        <v>770</v>
       </c>
       <c r="B1133" s="6" t="s">
-        <v>213</v>
+        <v>316</v>
       </c>
     </row>
     <row r="1134" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1134" s="9" t="s">
-        <v>773</v>
+        <v>771</v>
       </c>
       <c r="B1134" s="6" t="s">
-        <v>774</v>
-      </c>
-    </row>
-    <row r="1135" spans="1:2" ht="22.5" x14ac:dyDescent="0.2">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="1135" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1135" s="9" t="s">
-        <v>775</v>
-      </c>
-      <c r="B1135" s="7" t="s">
-        <v>312</v>
+        <v>772</v>
+      </c>
+      <c r="B1135" s="6" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="1136" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1136" s="9" t="s">
-        <v>776</v>
+        <v>773</v>
       </c>
       <c r="B1136" s="6" t="s">
-        <v>777</v>
-      </c>
-    </row>
-    <row r="1137" spans="1:2" x14ac:dyDescent="0.2">
+        <v>774</v>
+      </c>
+    </row>
+    <row r="1137" spans="1:2" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A1137" s="9" t="s">
-        <v>778</v>
-      </c>
-      <c r="B1137" s="6" t="s">
-        <v>308</v>
+        <v>775</v>
+      </c>
+      <c r="B1137" s="7" t="s">
+        <v>312</v>
       </c>
     </row>
     <row r="1138" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1138" s="9" t="s">
-        <v>779</v>
+        <v>776</v>
       </c>
       <c r="B1138" s="6" t="s">
-        <v>780</v>
+        <v>777</v>
       </c>
     </row>
     <row r="1139" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1139" s="9" t="s">
-        <v>781</v>
+        <v>778</v>
       </c>
       <c r="B1139" s="6" t="s">
-        <v>782</v>
+        <v>308</v>
       </c>
     </row>
     <row r="1140" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1140" s="9" t="s">
-        <v>783</v>
+        <v>779</v>
       </c>
       <c r="B1140" s="6" t="s">
-        <v>784</v>
+        <v>780</v>
       </c>
     </row>
     <row r="1141" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1141" s="9" t="s">
+        <v>781</v>
+      </c>
+      <c r="B1141" s="6" t="s">
+        <v>782</v>
+      </c>
+    </row>
+    <row r="1142" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1142" s="9" t="s">
+        <v>783</v>
+      </c>
+      <c r="B1142" s="6" t="s">
+        <v>784</v>
+      </c>
+    </row>
+    <row r="1143" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1143" s="9" t="s">
         <v>785</v>
       </c>
-      <c r="B1141" s="6" t="s">
+      <c r="B1143" s="6" t="s">
         <v>786</v>
       </c>
     </row>
-    <row r="1142" spans="1:2" ht="22.5" x14ac:dyDescent="0.2">
-      <c r="A1142" s="9" t="s">
+    <row r="1144" spans="1:2" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A1144" s="9" t="s">
         <v>787</v>
       </c>
-      <c r="B1142" s="6" t="s">
+      <c r="B1144" s="6" t="s">
         <v>788</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Give Arcane Warrior armour set on releasing spirit in brecilian ruins
In addition to unlocking the Arcane Warrior class, releasing the anciemt arcane warrior spirit now also provides the player with a set of armour and weapons. The rewards are based on The Ivory Tower and Nightfall Bloom mod with updated stats. The original mod had different armour for male and female but this has been fixed so a single set may be worn by either sex.

see #381
</commit_message>
<xml_diff>
--- a/source/tlk/strings.xlsx
+++ b/source/tlk/strings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\DAO\archid\source\tlk\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64F18D4E-305D-4294-830E-FAA4B4803AD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D0EE399-8079-4CCE-AD28-7A8EF2B8C905}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29190" yWindow="390" windowWidth="26610" windowHeight="16110" xr2:uid="{A42EE72D-E1C4-43B6-AEA5-0014ED5180B1}"/>
+    <workbookView xWindow="29535" yWindow="735" windowWidth="26610" windowHeight="16110" xr2:uid="{A42EE72D-E1C4-43B6-AEA5-0014ED5180B1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -289,13 +289,13 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Item restrictions</t>
         </r>
       </text>
     </comment>
-    <comment ref="A809" authorId="0" shapeId="0" xr:uid="{15B7CDC5-6F21-45A0-9997-3CC9AFCCF646}">
+    <comment ref="A823" authorId="0" shapeId="0" xr:uid="{15B7CDC5-6F21-45A0-9997-3CC9AFCCF646}">
       <text>
         <r>
           <rPr>
@@ -309,7 +309,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A936" authorId="0" shapeId="0" xr:uid="{08441945-669A-47E4-A77A-BA32248BBBE4}">
+    <comment ref="A950" authorId="0" shapeId="0" xr:uid="{08441945-669A-47E4-A77A-BA32248BBBE4}">
       <text>
         <r>
           <rPr>
@@ -342,7 +342,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1481" uniqueCount="1424">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1495" uniqueCount="1438">
   <si>
     <t>af_archid_en-us.tlk</t>
   </si>
@@ -4678,12 +4678,54 @@
   <si>
     <t>This plain looking ring was once the posession of a Telvinter mage who fell during the First Blight and subsequently found and worn by a Chasind chief during their occupation of Ostagar. How it came to be lost again is a mystery, but it's power has remain undimished over the ages.</t>
   </si>
+  <si>
+    <t>Ivory Tower Bulwark</t>
+  </si>
+  <si>
+    <t>This strange armour looks like a mage robe combined with plate armour. It was created for the Arcane Warrior guards who defended the elven magical towers. Its surface is unbearable cold to the human touch, but warm and pleasant to elven hands. Its appeling beauty is a reminder of what elves have lost and what they could again aspire to again.</t>
+  </si>
+  <si>
+    <t>Ivory Tower Spire</t>
+  </si>
+  <si>
+    <t>Elegant helmet of elven design that once belonged to a warmage guard. Its silvery white surface glitters under moonlight.</t>
+  </si>
+  <si>
+    <t>Ivory Tower Handguards</t>
+  </si>
+  <si>
+    <t>This pair of gloves may look heavy, but to an Arcane warrior they are incredibly light and flexible</t>
+  </si>
+  <si>
+    <t>Ivory Tower Foundation</t>
+  </si>
+  <si>
+    <t>Silvery white boots, covered in vine scrollwork and long forgotten runes</t>
+  </si>
+  <si>
+    <t>Blossom of Nightfall</t>
+  </si>
+  <si>
+    <t>Velvet blue and covered in stars and vines, as its sister longsword, this dagger radiates a strong arcane aura.</t>
+  </si>
+  <si>
+    <t>Dusk Fluorescence</t>
+  </si>
+  <si>
+    <t>The surface of this longsword is dark blue in colour with etching of a starry sky above vines and flowers.</t>
+  </si>
+  <si>
+    <t>Wall of Twilight</t>
+  </si>
+  <si>
+    <t>The strange metal of this shield not only deflects incoming attacks it also reflects its surroundings like a real mirror.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -4692,16 +4734,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="8"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="8"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <b/>
@@ -4717,18 +4754,19 @@
       <family val="2"/>
     </font>
     <font>
+      <b/>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="8"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="7">
@@ -4783,24 +4821,24 @@
   </cellStyleXfs>
   <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="2" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5119,10 +5157,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C8288F5-46B5-435A-B9FC-40522281A8A6}">
-  <dimension ref="A1:B1144"/>
+  <dimension ref="A1:B1158"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A758" workbookViewId="0">
-      <selection activeCell="B810" sqref="B810"/>
+    <sheetView tabSelected="1" topLeftCell="A800" workbookViewId="0">
+      <selection activeCell="B825" sqref="B825"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -6504,7 +6542,7 @@
       <c r="A172" s="3">
         <v>6610170</v>
       </c>
-      <c r="B172" s="10" t="s">
+      <c r="B172" s="7" t="s">
         <v>811</v>
       </c>
     </row>
@@ -11597,2690 +11635,2802 @@
       </c>
     </row>
     <row r="809" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A809" s="8" t="s">
+      <c r="A809" s="3">
+        <v>6610807</v>
+      </c>
+      <c r="B809" s="2" t="s">
+        <v>1424</v>
+      </c>
+    </row>
+    <row r="810" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A810" s="3">
+        <v>6610808</v>
+      </c>
+      <c r="B810" s="2" t="s">
+        <v>1425</v>
+      </c>
+    </row>
+    <row r="811" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A811" s="3">
+        <v>6610809</v>
+      </c>
+      <c r="B811" s="2" t="s">
+        <v>1426</v>
+      </c>
+    </row>
+    <row r="812" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A812" s="3">
+        <v>6610810</v>
+      </c>
+      <c r="B812" s="2" t="s">
+        <v>1427</v>
+      </c>
+    </row>
+    <row r="813" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A813" s="3">
+        <v>6610811</v>
+      </c>
+      <c r="B813" s="2" t="s">
+        <v>1428</v>
+      </c>
+    </row>
+    <row r="814" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A814" s="3">
+        <v>6610812</v>
+      </c>
+      <c r="B814" s="2" t="s">
+        <v>1429</v>
+      </c>
+    </row>
+    <row r="815" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A815" s="3">
+        <v>6610813</v>
+      </c>
+      <c r="B815" s="2" t="s">
+        <v>1430</v>
+      </c>
+    </row>
+    <row r="816" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A816" s="3">
+        <v>6610814</v>
+      </c>
+      <c r="B816" s="2" t="s">
+        <v>1431</v>
+      </c>
+    </row>
+    <row r="817" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A817" s="3">
+        <v>6610815</v>
+      </c>
+      <c r="B817" s="2" t="s">
+        <v>1432</v>
+      </c>
+    </row>
+    <row r="818" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A818" s="3">
+        <v>6610816</v>
+      </c>
+      <c r="B818" s="2" t="s">
+        <v>1433</v>
+      </c>
+    </row>
+    <row r="819" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A819" s="3">
+        <v>6610817</v>
+      </c>
+      <c r="B819" s="2" t="s">
+        <v>1434</v>
+      </c>
+    </row>
+    <row r="820" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A820" s="3">
+        <v>6610818</v>
+      </c>
+      <c r="B820" s="2" t="s">
+        <v>1435</v>
+      </c>
+    </row>
+    <row r="821" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A821" s="3">
+        <v>6610819</v>
+      </c>
+      <c r="B821" s="2" t="s">
+        <v>1436</v>
+      </c>
+    </row>
+    <row r="822" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A822" s="3">
+        <v>6610820</v>
+      </c>
+      <c r="B822" s="2" t="s">
+        <v>1437</v>
+      </c>
+    </row>
+    <row r="823" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A823" s="8" t="s">
         <v>150</v>
       </c>
-      <c r="B809" s="6" t="s">
+      <c r="B823" s="6" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="810" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A810" s="8" t="s">
+    <row r="824" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A824" s="8" t="s">
         <v>152</v>
       </c>
-      <c r="B810" s="6" t="s">
+      <c r="B824" s="6" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="811" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A811" s="8" t="s">
+    <row r="825" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A825" s="8" t="s">
         <v>154</v>
       </c>
-      <c r="B811" s="6" t="s">
+      <c r="B825" s="6" t="s">
         <v>155</v>
-      </c>
-    </row>
-    <row r="812" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A812" s="8" t="s">
-        <v>156</v>
-      </c>
-      <c r="B812" s="6" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="813" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A813" s="8" t="s">
-        <v>158</v>
-      </c>
-      <c r="B813" s="6" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="814" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
-      <c r="A814" s="8" t="s">
-        <v>160</v>
-      </c>
-      <c r="B814" s="6" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="815" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A815" s="8" t="s">
-        <v>162</v>
-      </c>
-      <c r="B815" s="6" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="816" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A816" s="8" t="s">
-        <v>164</v>
-      </c>
-      <c r="B816" s="6" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="817" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A817" s="8" t="s">
-        <v>166</v>
-      </c>
-      <c r="B817" s="6" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="818" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A818" s="8" t="s">
-        <v>168</v>
-      </c>
-      <c r="B818" s="6" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="819" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
-      <c r="A819" s="8" t="s">
-        <v>170</v>
-      </c>
-      <c r="B819" s="6" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="820" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A820" s="8" t="s">
-        <v>172</v>
-      </c>
-      <c r="B820" s="6" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="821" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A821" s="8" t="s">
-        <v>174</v>
-      </c>
-      <c r="B821" s="6" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="822" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A822" s="8" t="s">
-        <v>176</v>
-      </c>
-      <c r="B822" s="6" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="823" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
-      <c r="A823" s="8" t="s">
-        <v>177</v>
-      </c>
-      <c r="B823" s="6" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="824" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
-      <c r="A824" s="8" t="s">
-        <v>179</v>
-      </c>
-      <c r="B824" s="6" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="825" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
-      <c r="A825" s="8" t="s">
-        <v>181</v>
-      </c>
-      <c r="B825" s="6" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="826" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A826" s="8" t="s">
-        <v>183</v>
+        <v>156</v>
       </c>
       <c r="B826" s="6" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="827" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="827" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A827" s="8" t="s">
-        <v>185</v>
+        <v>158</v>
       </c>
       <c r="B827" s="6" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="828" spans="1:2" x14ac:dyDescent="0.2">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="828" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A828" s="8" t="s">
-        <v>187</v>
+        <v>160</v>
       </c>
       <c r="B828" s="6" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="829" spans="1:2" ht="90" x14ac:dyDescent="0.2">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="829" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A829" s="8" t="s">
-        <v>189</v>
+        <v>162</v>
       </c>
       <c r="B829" s="6" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="830" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="830" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A830" s="8" t="s">
-        <v>191</v>
+        <v>164</v>
       </c>
       <c r="B830" s="6" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="831" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="831" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A831" s="8" t="s">
-        <v>193</v>
+        <v>166</v>
       </c>
       <c r="B831" s="6" t="s">
-        <v>194</v>
+        <v>167</v>
       </c>
     </row>
     <row r="832" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A832" s="8" t="s">
-        <v>195</v>
+        <v>168</v>
       </c>
       <c r="B832" s="6" t="s">
-        <v>196</v>
+        <v>169</v>
       </c>
     </row>
     <row r="833" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A833" s="8" t="s">
-        <v>197</v>
+        <v>170</v>
       </c>
       <c r="B833" s="6" t="s">
-        <v>198</v>
+        <v>171</v>
       </c>
     </row>
     <row r="834" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A834" s="8" t="s">
-        <v>199</v>
+        <v>172</v>
       </c>
       <c r="B834" s="6" t="s">
-        <v>200</v>
+        <v>173</v>
       </c>
     </row>
     <row r="835" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A835" s="8" t="s">
-        <v>201</v>
+        <v>174</v>
       </c>
       <c r="B835" s="6" t="s">
-        <v>202</v>
+        <v>175</v>
       </c>
     </row>
     <row r="836" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A836" s="8" t="s">
-        <v>203</v>
+        <v>176</v>
       </c>
       <c r="B836" s="6" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="837" spans="1:2" x14ac:dyDescent="0.2">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="837" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A837" s="8" t="s">
-        <v>204</v>
+        <v>177</v>
       </c>
       <c r="B837" s="6" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="838" spans="1:2" x14ac:dyDescent="0.2">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="838" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A838" s="8" t="s">
-        <v>206</v>
+        <v>179</v>
       </c>
       <c r="B838" s="6" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="839" spans="1:2" x14ac:dyDescent="0.2">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="839" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A839" s="8" t="s">
-        <v>208</v>
+        <v>181</v>
       </c>
       <c r="B839" s="6" t="s">
-        <v>209</v>
+        <v>182</v>
       </c>
     </row>
     <row r="840" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A840" s="8" t="s">
-        <v>210</v>
+        <v>183</v>
       </c>
       <c r="B840" s="6" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="841" spans="1:2" x14ac:dyDescent="0.2">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="841" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A841" s="8" t="s">
-        <v>212</v>
+        <v>185</v>
       </c>
       <c r="B841" s="6" t="s">
-        <v>213</v>
+        <v>186</v>
       </c>
     </row>
     <row r="842" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A842" s="8" t="s">
-        <v>214</v>
+        <v>187</v>
       </c>
       <c r="B842" s="6" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="843" spans="1:2" x14ac:dyDescent="0.2">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="843" spans="1:2" ht="90" x14ac:dyDescent="0.2">
       <c r="A843" s="8" t="s">
-        <v>216</v>
+        <v>189</v>
       </c>
       <c r="B843" s="6" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="844" spans="1:2" x14ac:dyDescent="0.2">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="844" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A844" s="8" t="s">
-        <v>218</v>
+        <v>191</v>
       </c>
       <c r="B844" s="6" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="845" spans="1:2" x14ac:dyDescent="0.2">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="845" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A845" s="8" t="s">
-        <v>220</v>
+        <v>193</v>
       </c>
       <c r="B845" s="6" t="s">
-        <v>221</v>
+        <v>194</v>
       </c>
     </row>
     <row r="846" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A846" s="8" t="s">
-        <v>222</v>
+        <v>195</v>
       </c>
       <c r="B846" s="6" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="847" spans="1:2" x14ac:dyDescent="0.2">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="847" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A847" s="8" t="s">
-        <v>224</v>
+        <v>197</v>
       </c>
       <c r="B847" s="6" t="s">
-        <v>225</v>
+        <v>198</v>
       </c>
     </row>
     <row r="848" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A848" s="8" t="s">
-        <v>226</v>
+        <v>199</v>
       </c>
       <c r="B848" s="6" t="s">
-        <v>227</v>
+        <v>200</v>
       </c>
     </row>
     <row r="849" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A849" s="8" t="s">
-        <v>228</v>
+        <v>201</v>
       </c>
       <c r="B849" s="6" t="s">
-        <v>229</v>
+        <v>202</v>
       </c>
     </row>
     <row r="850" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A850" s="8" t="s">
-        <v>230</v>
+        <v>203</v>
       </c>
       <c r="B850" s="6" t="s">
-        <v>231</v>
+        <v>153</v>
       </c>
     </row>
     <row r="851" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A851" s="8" t="s">
-        <v>232</v>
+        <v>204</v>
       </c>
       <c r="B851" s="6" t="s">
-        <v>233</v>
+        <v>205</v>
       </c>
     </row>
     <row r="852" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A852" s="8" t="s">
-        <v>234</v>
+        <v>206</v>
       </c>
       <c r="B852" s="6" t="s">
-        <v>235</v>
+        <v>207</v>
       </c>
     </row>
     <row r="853" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A853" s="8" t="s">
-        <v>236</v>
+        <v>208</v>
       </c>
       <c r="B853" s="6" t="s">
-        <v>237</v>
+        <v>209</v>
       </c>
     </row>
     <row r="854" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A854" s="8" t="s">
-        <v>238</v>
+        <v>210</v>
       </c>
       <c r="B854" s="6" t="s">
-        <v>239</v>
+        <v>211</v>
       </c>
     </row>
     <row r="855" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A855" s="8" t="s">
-        <v>240</v>
+        <v>212</v>
       </c>
       <c r="B855" s="6" t="s">
-        <v>241</v>
+        <v>213</v>
       </c>
     </row>
     <row r="856" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A856" s="8" t="s">
-        <v>242</v>
+        <v>214</v>
       </c>
       <c r="B856" s="6" t="s">
-        <v>243</v>
+        <v>215</v>
       </c>
     </row>
     <row r="857" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A857" s="8" t="s">
-        <v>244</v>
+        <v>216</v>
       </c>
       <c r="B857" s="6" t="s">
-        <v>245</v>
+        <v>217</v>
       </c>
     </row>
     <row r="858" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A858" s="8" t="s">
-        <v>246</v>
+        <v>218</v>
       </c>
       <c r="B858" s="6" t="s">
-        <v>247</v>
+        <v>219</v>
       </c>
     </row>
     <row r="859" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A859" s="8" t="s">
-        <v>248</v>
+        <v>220</v>
       </c>
       <c r="B859" s="6" t="s">
-        <v>249</v>
+        <v>221</v>
       </c>
     </row>
     <row r="860" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A860" s="8" t="s">
-        <v>250</v>
+        <v>222</v>
       </c>
       <c r="B860" s="6" t="s">
-        <v>251</v>
+        <v>223</v>
       </c>
     </row>
     <row r="861" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A861" s="8" t="s">
-        <v>252</v>
+        <v>224</v>
       </c>
       <c r="B861" s="6" t="s">
-        <v>253</v>
+        <v>225</v>
       </c>
     </row>
     <row r="862" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A862" s="8" t="s">
-        <v>254</v>
+        <v>226</v>
       </c>
       <c r="B862" s="6" t="s">
-        <v>255</v>
+        <v>227</v>
       </c>
     </row>
     <row r="863" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A863" s="8" t="s">
-        <v>256</v>
+        <v>228</v>
       </c>
       <c r="B863" s="6" t="s">
-        <v>257</v>
+        <v>229</v>
       </c>
     </row>
     <row r="864" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A864" s="8" t="s">
-        <v>258</v>
+        <v>230</v>
       </c>
       <c r="B864" s="6" t="s">
-        <v>259</v>
+        <v>231</v>
       </c>
     </row>
     <row r="865" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A865" s="8" t="s">
-        <v>260</v>
+        <v>232</v>
       </c>
       <c r="B865" s="6" t="s">
-        <v>261</v>
+        <v>233</v>
       </c>
     </row>
     <row r="866" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A866" s="8" t="s">
-        <v>262</v>
+        <v>234</v>
       </c>
       <c r="B866" s="6" t="s">
-        <v>263</v>
+        <v>235</v>
       </c>
     </row>
     <row r="867" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A867" s="8" t="s">
-        <v>264</v>
+        <v>236</v>
       </c>
       <c r="B867" s="6" t="s">
-        <v>265</v>
+        <v>237</v>
       </c>
     </row>
     <row r="868" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A868" s="8" t="s">
-        <v>266</v>
+        <v>238</v>
       </c>
       <c r="B868" s="6" t="s">
-        <v>267</v>
+        <v>239</v>
       </c>
     </row>
     <row r="869" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A869" s="8" t="s">
-        <v>268</v>
+        <v>240</v>
       </c>
       <c r="B869" s="6" t="s">
-        <v>269</v>
+        <v>241</v>
       </c>
     </row>
     <row r="870" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A870" s="8" t="s">
-        <v>270</v>
+        <v>242</v>
       </c>
       <c r="B870" s="6" t="s">
-        <v>271</v>
+        <v>243</v>
       </c>
     </row>
     <row r="871" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A871" s="8" t="s">
-        <v>272</v>
+        <v>244</v>
       </c>
       <c r="B871" s="6" t="s">
-        <v>273</v>
+        <v>245</v>
       </c>
     </row>
     <row r="872" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A872" s="8" t="s">
-        <v>274</v>
+        <v>246</v>
       </c>
       <c r="B872" s="6" t="s">
-        <v>275</v>
+        <v>247</v>
       </c>
     </row>
     <row r="873" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A873" s="8" t="s">
-        <v>276</v>
+        <v>248</v>
       </c>
       <c r="B873" s="6" t="s">
-        <v>277</v>
+        <v>249</v>
       </c>
     </row>
     <row r="874" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A874" s="8" t="s">
-        <v>278</v>
+        <v>250</v>
       </c>
       <c r="B874" s="6" t="s">
-        <v>279</v>
+        <v>251</v>
       </c>
     </row>
     <row r="875" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A875" s="8" t="s">
-        <v>280</v>
+        <v>252</v>
       </c>
       <c r="B875" s="6" t="s">
-        <v>281</v>
+        <v>253</v>
       </c>
     </row>
     <row r="876" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A876" s="8" t="s">
-        <v>282</v>
+        <v>254</v>
       </c>
       <c r="B876" s="6" t="s">
-        <v>283</v>
+        <v>255</v>
       </c>
     </row>
     <row r="877" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A877" s="8" t="s">
-        <v>284</v>
+        <v>256</v>
       </c>
       <c r="B877" s="6" t="s">
-        <v>285</v>
+        <v>257</v>
       </c>
     </row>
     <row r="878" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A878" s="8" t="s">
-        <v>286</v>
+        <v>258</v>
       </c>
       <c r="B878" s="6" t="s">
-        <v>287</v>
+        <v>259</v>
       </c>
     </row>
     <row r="879" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A879" s="8" t="s">
-        <v>288</v>
+        <v>260</v>
       </c>
       <c r="B879" s="6" t="s">
-        <v>289</v>
+        <v>261</v>
       </c>
     </row>
     <row r="880" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A880" s="8" t="s">
-        <v>290</v>
+        <v>262</v>
       </c>
       <c r="B880" s="6" t="s">
-        <v>291</v>
+        <v>263</v>
       </c>
     </row>
     <row r="881" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A881" s="8" t="s">
-        <v>292</v>
+        <v>264</v>
       </c>
       <c r="B881" s="6" t="s">
-        <v>293</v>
+        <v>265</v>
       </c>
     </row>
     <row r="882" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A882" s="8" t="s">
-        <v>294</v>
+        <v>266</v>
       </c>
       <c r="B882" s="6" t="s">
-        <v>295</v>
+        <v>267</v>
       </c>
     </row>
     <row r="883" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A883" s="8" t="s">
-        <v>296</v>
+        <v>268</v>
       </c>
       <c r="B883" s="6" t="s">
-        <v>295</v>
+        <v>269</v>
       </c>
     </row>
     <row r="884" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A884" s="8" t="s">
-        <v>297</v>
+        <v>270</v>
       </c>
       <c r="B884" s="6" t="s">
-        <v>298</v>
+        <v>271</v>
       </c>
     </row>
     <row r="885" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A885" s="8" t="s">
-        <v>299</v>
+        <v>272</v>
       </c>
       <c r="B885" s="6" t="s">
-        <v>237</v>
+        <v>273</v>
       </c>
     </row>
     <row r="886" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A886" s="8" t="s">
-        <v>300</v>
+        <v>274</v>
       </c>
       <c r="B886" s="6" t="s">
-        <v>239</v>
+        <v>275</v>
       </c>
     </row>
     <row r="887" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A887" s="8" t="s">
-        <v>301</v>
+        <v>276</v>
       </c>
       <c r="B887" s="6" t="s">
-        <v>302</v>
+        <v>277</v>
       </c>
     </row>
     <row r="888" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A888" s="8" t="s">
-        <v>303</v>
+        <v>278</v>
       </c>
       <c r="B888" s="6" t="s">
-        <v>304</v>
+        <v>279</v>
       </c>
     </row>
     <row r="889" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A889" s="8" t="s">
-        <v>305</v>
+        <v>280</v>
       </c>
       <c r="B889" s="6" t="s">
-        <v>306</v>
+        <v>281</v>
       </c>
     </row>
     <row r="890" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A890" s="8" t="s">
-        <v>307</v>
+        <v>282</v>
       </c>
       <c r="B890" s="6" t="s">
-        <v>308</v>
+        <v>283</v>
       </c>
     </row>
     <row r="891" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A891" s="8" t="s">
-        <v>309</v>
+        <v>284</v>
       </c>
       <c r="B891" s="6" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="892" spans="1:2" ht="22.5" x14ac:dyDescent="0.2">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="892" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A892" s="8" t="s">
-        <v>311</v>
-      </c>
-      <c r="B892" s="7" t="s">
-        <v>312</v>
+        <v>286</v>
+      </c>
+      <c r="B892" s="6" t="s">
+        <v>287</v>
       </c>
     </row>
     <row r="893" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A893" s="8" t="s">
-        <v>313</v>
+        <v>288</v>
       </c>
       <c r="B893" s="6" t="s">
-        <v>314</v>
+        <v>289</v>
       </c>
     </row>
     <row r="894" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A894" s="8" t="s">
-        <v>315</v>
+        <v>290</v>
       </c>
       <c r="B894" s="6" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="895" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="895" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A895" s="8" t="s">
-        <v>317</v>
+        <v>292</v>
       </c>
       <c r="B895" s="6" t="s">
-        <v>318</v>
+        <v>293</v>
       </c>
     </row>
     <row r="896" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A896" s="8" t="s">
-        <v>319</v>
+        <v>294</v>
       </c>
       <c r="B896" s="6" t="s">
-        <v>320</v>
+        <v>295</v>
       </c>
     </row>
     <row r="897" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A897" s="8" t="s">
-        <v>321</v>
+        <v>296</v>
       </c>
       <c r="B897" s="6" t="s">
-        <v>322</v>
+        <v>295</v>
       </c>
     </row>
     <row r="898" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A898" s="8" t="s">
-        <v>323</v>
+        <v>297</v>
       </c>
       <c r="B898" s="6" t="s">
-        <v>324</v>
+        <v>298</v>
       </c>
     </row>
     <row r="899" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A899" s="8" t="s">
-        <v>325</v>
+        <v>299</v>
       </c>
       <c r="B899" s="6" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="900" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="900" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A900" s="8" t="s">
-        <v>327</v>
+        <v>300</v>
       </c>
       <c r="B900" s="6" t="s">
-        <v>328</v>
+        <v>239</v>
       </c>
     </row>
     <row r="901" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A901" s="8" t="s">
-        <v>329</v>
+        <v>301</v>
       </c>
       <c r="B901" s="6" t="s">
-        <v>295</v>
+        <v>302</v>
       </c>
     </row>
     <row r="902" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A902" s="8" t="s">
-        <v>330</v>
+        <v>303</v>
       </c>
       <c r="B902" s="6" t="s">
-        <v>331</v>
+        <v>304</v>
       </c>
     </row>
     <row r="903" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A903" s="8" t="s">
-        <v>332</v>
+        <v>305</v>
       </c>
       <c r="B903" s="6" t="s">
-        <v>333</v>
+        <v>306</v>
       </c>
     </row>
     <row r="904" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A904" s="8" t="s">
-        <v>334</v>
+        <v>307</v>
       </c>
       <c r="B904" s="6" t="s">
-        <v>335</v>
+        <v>308</v>
       </c>
     </row>
     <row r="905" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A905" s="8" t="s">
-        <v>336</v>
+        <v>309</v>
       </c>
       <c r="B905" s="6" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="906" spans="1:2" x14ac:dyDescent="0.2">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="906" spans="1:2" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A906" s="8" t="s">
-        <v>338</v>
-      </c>
-      <c r="B906" s="6" t="s">
-        <v>339</v>
+        <v>311</v>
+      </c>
+      <c r="B906" s="9" t="s">
+        <v>312</v>
       </c>
     </row>
     <row r="907" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A907" s="8" t="s">
-        <v>340</v>
+        <v>313</v>
       </c>
       <c r="B907" s="6" t="s">
-        <v>341</v>
+        <v>314</v>
       </c>
     </row>
     <row r="908" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A908" s="8" t="s">
-        <v>342</v>
+        <v>315</v>
       </c>
       <c r="B908" s="6" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="909" spans="1:2" x14ac:dyDescent="0.2">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="909" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A909" s="8" t="s">
-        <v>344</v>
+        <v>317</v>
       </c>
       <c r="B909" s="6" t="s">
-        <v>345</v>
+        <v>318</v>
       </c>
     </row>
     <row r="910" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A910" s="8" t="s">
-        <v>346</v>
+        <v>319</v>
       </c>
       <c r="B910" s="6" t="s">
-        <v>347</v>
+        <v>320</v>
       </c>
     </row>
     <row r="911" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A911" s="8" t="s">
-        <v>348</v>
+        <v>321</v>
       </c>
       <c r="B911" s="6" t="s">
-        <v>349</v>
+        <v>322</v>
       </c>
     </row>
     <row r="912" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A912" s="8" t="s">
-        <v>350</v>
+        <v>323</v>
       </c>
       <c r="B912" s="6" t="s">
-        <v>351</v>
+        <v>324</v>
       </c>
     </row>
     <row r="913" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A913" s="8" t="s">
-        <v>352</v>
+        <v>325</v>
       </c>
       <c r="B913" s="6" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="914" spans="1:2" x14ac:dyDescent="0.2">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="914" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A914" s="8" t="s">
-        <v>354</v>
+        <v>327</v>
       </c>
       <c r="B914" s="6" t="s">
-        <v>355</v>
+        <v>328</v>
       </c>
     </row>
     <row r="915" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A915" s="8" t="s">
-        <v>356</v>
+        <v>329</v>
       </c>
       <c r="B915" s="6" t="s">
-        <v>357</v>
+        <v>295</v>
       </c>
     </row>
     <row r="916" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A916" s="8" t="s">
-        <v>358</v>
+        <v>330</v>
       </c>
       <c r="B916" s="6" t="s">
-        <v>359</v>
+        <v>331</v>
       </c>
     </row>
     <row r="917" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A917" s="8" t="s">
-        <v>360</v>
+        <v>332</v>
       </c>
       <c r="B917" s="6" t="s">
-        <v>77</v>
+        <v>333</v>
       </c>
     </row>
     <row r="918" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A918" s="8" t="s">
-        <v>361</v>
+        <v>334</v>
       </c>
       <c r="B918" s="6" t="s">
-        <v>362</v>
+        <v>335</v>
       </c>
     </row>
     <row r="919" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A919" s="8" t="s">
-        <v>363</v>
+        <v>336</v>
       </c>
       <c r="B919" s="6" t="s">
-        <v>364</v>
+        <v>337</v>
       </c>
     </row>
     <row r="920" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A920" s="8" t="s">
-        <v>365</v>
+        <v>338</v>
       </c>
       <c r="B920" s="6" t="s">
-        <v>366</v>
+        <v>339</v>
       </c>
     </row>
     <row r="921" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A921" s="8" t="s">
-        <v>367</v>
+        <v>340</v>
       </c>
       <c r="B921" s="6" t="s">
-        <v>368</v>
+        <v>341</v>
       </c>
     </row>
     <row r="922" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A922" s="8" t="s">
-        <v>369</v>
+        <v>342</v>
       </c>
       <c r="B922" s="6" t="s">
-        <v>370</v>
+        <v>343</v>
       </c>
     </row>
     <row r="923" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A923" s="8" t="s">
-        <v>371</v>
+        <v>344</v>
       </c>
       <c r="B923" s="6" t="s">
-        <v>372</v>
+        <v>345</v>
       </c>
     </row>
     <row r="924" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A924" s="8" t="s">
-        <v>373</v>
+        <v>346</v>
       </c>
       <c r="B924" s="6" t="s">
-        <v>77</v>
+        <v>347</v>
       </c>
     </row>
     <row r="925" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A925" s="8" t="s">
-        <v>374</v>
+        <v>348</v>
       </c>
       <c r="B925" s="6" t="s">
-        <v>281</v>
+        <v>349</v>
       </c>
     </row>
     <row r="926" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A926" s="8" t="s">
-        <v>375</v>
+        <v>350</v>
       </c>
       <c r="B926" s="6" t="s">
-        <v>376</v>
+        <v>351</v>
       </c>
     </row>
     <row r="927" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A927" s="8" t="s">
-        <v>377</v>
+        <v>352</v>
       </c>
       <c r="B927" s="6" t="s">
-        <v>378</v>
+        <v>353</v>
       </c>
     </row>
     <row r="928" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A928" s="8" t="s">
-        <v>379</v>
+        <v>354</v>
       </c>
       <c r="B928" s="6" t="s">
-        <v>380</v>
+        <v>355</v>
       </c>
     </row>
     <row r="929" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A929" s="8" t="s">
-        <v>381</v>
+        <v>356</v>
       </c>
       <c r="B929" s="6" t="s">
-        <v>382</v>
+        <v>357</v>
       </c>
     </row>
     <row r="930" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A930" s="8" t="s">
-        <v>383</v>
+        <v>358</v>
       </c>
       <c r="B930" s="6" t="s">
-        <v>384</v>
+        <v>359</v>
       </c>
     </row>
     <row r="931" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A931" s="8" t="s">
-        <v>385</v>
+        <v>360</v>
       </c>
       <c r="B931" s="6" t="s">
-        <v>386</v>
+        <v>77</v>
       </c>
     </row>
     <row r="932" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A932" s="8" t="s">
-        <v>387</v>
+        <v>361</v>
       </c>
       <c r="B932" s="6" t="s">
-        <v>388</v>
+        <v>362</v>
       </c>
     </row>
     <row r="933" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A933" s="8" t="s">
-        <v>389</v>
+        <v>363</v>
       </c>
       <c r="B933" s="6" t="s">
-        <v>175</v>
+        <v>364</v>
       </c>
     </row>
     <row r="934" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A934" s="8" t="s">
-        <v>390</v>
+        <v>365</v>
       </c>
       <c r="B934" s="6" t="s">
-        <v>391</v>
+        <v>366</v>
       </c>
     </row>
     <row r="935" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A935" s="8" t="s">
+        <v>367</v>
+      </c>
+      <c r="B935" s="6" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="936" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A936" s="8" t="s">
+        <v>369</v>
+      </c>
+      <c r="B936" s="6" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="937" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A937" s="8" t="s">
+        <v>371</v>
+      </c>
+      <c r="B937" s="6" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="938" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A938" s="8" t="s">
+        <v>373</v>
+      </c>
+      <c r="B938" s="6" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="939" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A939" s="8" t="s">
+        <v>374</v>
+      </c>
+      <c r="B939" s="6" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="940" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A940" s="8" t="s">
+        <v>375</v>
+      </c>
+      <c r="B940" s="6" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="941" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A941" s="8" t="s">
+        <v>377</v>
+      </c>
+      <c r="B941" s="6" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="942" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A942" s="8" t="s">
+        <v>379</v>
+      </c>
+      <c r="B942" s="6" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="943" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A943" s="8" t="s">
+        <v>381</v>
+      </c>
+      <c r="B943" s="6" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="944" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A944" s="8" t="s">
+        <v>383</v>
+      </c>
+      <c r="B944" s="6" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="945" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A945" s="8" t="s">
+        <v>385</v>
+      </c>
+      <c r="B945" s="6" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="946" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A946" s="8" t="s">
+        <v>387</v>
+      </c>
+      <c r="B946" s="6" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="947" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A947" s="8" t="s">
+        <v>389</v>
+      </c>
+      <c r="B947" s="6" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="948" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A948" s="8" t="s">
+        <v>390</v>
+      </c>
+      <c r="B948" s="6" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="949" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A949" s="8" t="s">
         <v>392</v>
       </c>
-      <c r="B935" s="6" t="s">
+      <c r="B949" s="6" t="s">
         <v>393</v>
       </c>
     </row>
-    <row r="936" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A936" s="9" t="s">
+    <row r="950" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A950" s="10" t="s">
         <v>394</v>
       </c>
-      <c r="B936" s="6" t="s">
+      <c r="B950" s="6" t="s">
         <v>395</v>
       </c>
     </row>
-    <row r="937" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A937" s="9" t="s">
+    <row r="951" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A951" s="10" t="s">
         <v>396</v>
       </c>
-      <c r="B937" s="6" t="s">
+      <c r="B951" s="6" t="s">
         <v>397</v>
       </c>
     </row>
-    <row r="938" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A938" s="9" t="s">
+    <row r="952" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A952" s="10" t="s">
         <v>398</v>
       </c>
-      <c r="B938" s="6" t="s">
+      <c r="B952" s="6" t="s">
         <v>399</v>
       </c>
     </row>
-    <row r="939" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A939" s="9" t="s">
+    <row r="953" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A953" s="10" t="s">
         <v>400</v>
       </c>
-      <c r="B939" s="6" t="s">
+      <c r="B953" s="6" t="s">
         <v>401</v>
       </c>
     </row>
-    <row r="940" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A940" s="9" t="s">
+    <row r="954" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A954" s="10" t="s">
         <v>402</v>
       </c>
-      <c r="B940" s="6" t="s">
+      <c r="B954" s="6" t="s">
         <v>403</v>
       </c>
     </row>
-    <row r="941" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A941" s="9" t="s">
+    <row r="955" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A955" s="10" t="s">
         <v>404</v>
       </c>
-      <c r="B941" s="6" t="s">
+      <c r="B955" s="6" t="s">
         <v>405</v>
       </c>
     </row>
-    <row r="942" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A942" s="9" t="s">
+    <row r="956" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A956" s="10" t="s">
         <v>406</v>
       </c>
-      <c r="B942" s="6" t="s">
+      <c r="B956" s="6" t="s">
         <v>407</v>
       </c>
     </row>
-    <row r="943" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A943" s="9" t="s">
+    <row r="957" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A957" s="10" t="s">
         <v>408</v>
       </c>
-      <c r="B943" s="6" t="s">
+      <c r="B957" s="6" t="s">
         <v>409</v>
       </c>
     </row>
-    <row r="944" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A944" s="9" t="s">
+    <row r="958" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A958" s="10" t="s">
         <v>410</v>
       </c>
-      <c r="B944" s="6" t="s">
+      <c r="B958" s="6" t="s">
         <v>409</v>
       </c>
     </row>
-    <row r="945" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A945" s="9" t="s">
+    <row r="959" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A959" s="10" t="s">
         <v>411</v>
       </c>
-      <c r="B945" s="6" t="s">
+      <c r="B959" s="6" t="s">
         <v>412</v>
       </c>
     </row>
-    <row r="946" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A946" s="9" t="s">
+    <row r="960" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A960" s="10" t="s">
         <v>413</v>
       </c>
-      <c r="B946" s="6" t="s">
+      <c r="B960" s="6" t="s">
         <v>412</v>
       </c>
     </row>
-    <row r="947" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A947" s="9" t="s">
+    <row r="961" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A961" s="10" t="s">
         <v>414</v>
       </c>
-      <c r="B947" s="6" t="s">
+      <c r="B961" s="6" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="948" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A948" s="9" t="s">
+    <row r="962" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A962" s="10" t="s">
         <v>415</v>
       </c>
-      <c r="B948" s="6" t="s">
+      <c r="B962" s="6" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="949" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A949" s="9" t="s">
+    <row r="963" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A963" s="10" t="s">
         <v>416</v>
       </c>
-      <c r="B949" s="6" t="s">
+      <c r="B963" s="6" t="s">
         <v>401</v>
       </c>
     </row>
-    <row r="950" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A950" s="9" t="s">
+    <row r="964" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A964" s="10" t="s">
         <v>417</v>
       </c>
-      <c r="B950" s="6" t="s">
+      <c r="B964" s="6" t="s">
         <v>403</v>
       </c>
     </row>
-    <row r="951" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A951" s="9" t="s">
+    <row r="965" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A965" s="10" t="s">
         <v>418</v>
       </c>
-      <c r="B951" s="6" t="s">
+      <c r="B965" s="6" t="s">
         <v>405</v>
       </c>
     </row>
-    <row r="952" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A952" s="9" t="s">
+    <row r="966" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A966" s="10" t="s">
         <v>419</v>
       </c>
-      <c r="B952" s="6" t="s">
+      <c r="B966" s="6" t="s">
         <v>407</v>
       </c>
     </row>
-    <row r="953" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A953" s="9" t="s">
+    <row r="967" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A967" s="10" t="s">
         <v>420</v>
       </c>
-      <c r="B953" s="6" t="s">
+      <c r="B967" s="6" t="s">
         <v>395</v>
       </c>
     </row>
-    <row r="954" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A954" s="9" t="s">
+    <row r="968" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A968" s="10" t="s">
         <v>421</v>
       </c>
-      <c r="B954" s="6" t="s">
+      <c r="B968" s="6" t="s">
         <v>397</v>
       </c>
     </row>
-    <row r="955" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A955" s="9" t="s">
+    <row r="969" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A969" s="10" t="s">
         <v>422</v>
       </c>
-      <c r="B955" s="6" t="s">
+      <c r="B969" s="6" t="s">
         <v>399</v>
       </c>
     </row>
-    <row r="956" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A956" s="9" t="s">
+    <row r="970" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A970" s="10" t="s">
         <v>423</v>
       </c>
-      <c r="B956" s="6" t="s">
+      <c r="B970" s="6" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="957" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A957" s="9" t="s">
+    <row r="971" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A971" s="10" t="s">
         <v>424</v>
       </c>
-      <c r="B957" s="6" t="s">
+      <c r="B971" s="6" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="958" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A958" s="9" t="s">
+    <row r="972" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A972" s="10" t="s">
         <v>425</v>
       </c>
-      <c r="B958" s="6" t="s">
+      <c r="B972" s="6" t="s">
         <v>320</v>
       </c>
     </row>
-    <row r="959" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A959" s="9" t="s">
+    <row r="973" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A973" s="10" t="s">
         <v>426</v>
       </c>
-      <c r="B959" s="6" t="s">
+      <c r="B973" s="6" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="960" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A960" s="9" t="s">
+    <row r="974" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A974" s="10" t="s">
         <v>427</v>
       </c>
-      <c r="B960" s="6" t="s">
+      <c r="B974" s="6" t="s">
         <v>428</v>
       </c>
     </row>
-    <row r="961" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A961" s="9" t="s">
+    <row r="975" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A975" s="10" t="s">
         <v>429</v>
       </c>
-      <c r="B961" s="6" t="s">
+      <c r="B975" s="6" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="962" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A962" s="9" t="s">
+    <row r="976" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A976" s="10" t="s">
         <v>430</v>
       </c>
-      <c r="B962" s="6" t="s">
+      <c r="B976" s="6" t="s">
         <v>431</v>
       </c>
     </row>
-    <row r="963" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A963" s="9" t="s">
+    <row r="977" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A977" s="10" t="s">
         <v>432</v>
       </c>
-      <c r="B963" s="6" t="s">
+      <c r="B977" s="6" t="s">
         <v>433</v>
       </c>
     </row>
-    <row r="964" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A964" s="9" t="s">
+    <row r="978" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A978" s="10" t="s">
         <v>434</v>
       </c>
-      <c r="B964" s="6" t="s">
+      <c r="B978" s="6" t="s">
         <v>435</v>
       </c>
     </row>
-    <row r="965" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A965" s="9" t="s">
+    <row r="979" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A979" s="10" t="s">
         <v>436</v>
       </c>
-      <c r="B965" s="6" t="s">
+      <c r="B979" s="6" t="s">
         <v>437</v>
       </c>
     </row>
-    <row r="966" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A966" s="9" t="s">
+    <row r="980" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A980" s="10" t="s">
         <v>438</v>
       </c>
-      <c r="B966" s="6" t="s">
+      <c r="B980" s="6" t="s">
         <v>439</v>
       </c>
     </row>
-    <row r="967" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A967" s="9" t="s">
+    <row r="981" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A981" s="10" t="s">
         <v>440</v>
       </c>
-      <c r="B967" s="6" t="s">
+      <c r="B981" s="6" t="s">
         <v>441</v>
       </c>
     </row>
-    <row r="968" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A968" s="9" t="s">
+    <row r="982" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A982" s="10" t="s">
         <v>442</v>
       </c>
-      <c r="B968" s="6" t="s">
+      <c r="B982" s="6" t="s">
         <v>443</v>
       </c>
     </row>
-    <row r="969" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A969" s="9" t="s">
+    <row r="983" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A983" s="10" t="s">
         <v>444</v>
       </c>
-      <c r="B969" s="6" t="s">
+      <c r="B983" s="6" t="s">
         <v>407</v>
       </c>
     </row>
-    <row r="970" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A970" s="9" t="s">
+    <row r="984" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A984" s="10" t="s">
         <v>445</v>
       </c>
-      <c r="B970" s="6" t="s">
+      <c r="B984" s="6" t="s">
         <v>446</v>
       </c>
     </row>
-    <row r="971" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A971" s="9" t="s">
+    <row r="985" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A985" s="10" t="s">
         <v>447</v>
       </c>
-      <c r="B971" s="6" t="s">
+      <c r="B985" s="6" t="s">
         <v>448</v>
       </c>
     </row>
-    <row r="972" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A972" s="9" t="s">
+    <row r="986" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A986" s="10" t="s">
         <v>449</v>
       </c>
-      <c r="B972" s="6" t="s">
+      <c r="B986" s="6" t="s">
         <v>450</v>
       </c>
     </row>
-    <row r="973" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A973" s="9" t="s">
+    <row r="987" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A987" s="10" t="s">
         <v>451</v>
       </c>
-      <c r="B973" s="6" t="s">
+      <c r="B987" s="6" t="s">
         <v>452</v>
       </c>
     </row>
-    <row r="974" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A974" s="9" t="s">
+    <row r="988" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A988" s="10" t="s">
         <v>453</v>
       </c>
-      <c r="B974" s="6" t="s">
+      <c r="B988" s="6" t="s">
         <v>454</v>
       </c>
     </row>
-    <row r="975" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A975" s="9" t="s">
+    <row r="989" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A989" s="10" t="s">
         <v>455</v>
       </c>
-      <c r="B975" s="6" t="s">
+      <c r="B989" s="6" t="s">
         <v>456</v>
       </c>
     </row>
-    <row r="976" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A976" s="9" t="s">
+    <row r="990" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A990" s="10" t="s">
         <v>457</v>
       </c>
-      <c r="B976" s="6" t="s">
+      <c r="B990" s="6" t="s">
         <v>458</v>
       </c>
     </row>
-    <row r="977" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A977" s="9" t="s">
+    <row r="991" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A991" s="10" t="s">
         <v>459</v>
       </c>
-      <c r="B977" s="6" t="s">
+      <c r="B991" s="6" t="s">
         <v>460</v>
       </c>
     </row>
-    <row r="978" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A978" s="9" t="s">
+    <row r="992" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A992" s="10" t="s">
         <v>461</v>
       </c>
-      <c r="B978" s="6" t="s">
+      <c r="B992" s="6" t="s">
         <v>462</v>
       </c>
     </row>
-    <row r="979" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A979" s="9" t="s">
+    <row r="993" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A993" s="10" t="s">
         <v>463</v>
       </c>
-      <c r="B979" s="6" t="s">
+      <c r="B993" s="6" t="s">
         <v>464</v>
       </c>
     </row>
-    <row r="980" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A980" s="9" t="s">
+    <row r="994" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A994" s="10" t="s">
         <v>465</v>
       </c>
-      <c r="B980" s="6" t="s">
+      <c r="B994" s="6" t="s">
         <v>466</v>
       </c>
     </row>
-    <row r="981" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A981" s="9" t="s">
+    <row r="995" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A995" s="10" t="s">
         <v>467</v>
       </c>
-      <c r="B981" s="6" t="s">
+      <c r="B995" s="6" t="s">
         <v>468</v>
       </c>
     </row>
-    <row r="982" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A982" s="9" t="s">
+    <row r="996" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A996" s="10" t="s">
         <v>469</v>
       </c>
-      <c r="B982" s="6" t="s">
+      <c r="B996" s="6" t="s">
         <v>470</v>
       </c>
     </row>
-    <row r="983" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A983" s="9" t="s">
+    <row r="997" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A997" s="10" t="s">
         <v>471</v>
       </c>
-      <c r="B983" s="6" t="s">
+      <c r="B997" s="6" t="s">
         <v>472</v>
       </c>
     </row>
-    <row r="984" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A984" s="9" t="s">
+    <row r="998" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A998" s="10" t="s">
         <v>473</v>
       </c>
-      <c r="B984" s="6" t="s">
+      <c r="B998" s="6" t="s">
         <v>474</v>
       </c>
     </row>
-    <row r="985" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A985" s="9" t="s">
+    <row r="999" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A999" s="10" t="s">
         <v>475</v>
       </c>
-      <c r="B985" s="6" t="s">
+      <c r="B999" s="6" t="s">
         <v>476</v>
       </c>
     </row>
-    <row r="986" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A986" s="9" t="s">
+    <row r="1000" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1000" s="10" t="s">
         <v>477</v>
       </c>
-      <c r="B986" s="6" t="s">
+      <c r="B1000" s="6" t="s">
         <v>478</v>
       </c>
     </row>
-    <row r="987" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A987" s="9" t="s">
+    <row r="1001" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1001" s="10" t="s">
         <v>479</v>
       </c>
-      <c r="B987" s="6" t="s">
+      <c r="B1001" s="6" t="s">
         <v>480</v>
       </c>
     </row>
-    <row r="988" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A988" s="9" t="s">
+    <row r="1002" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1002" s="10" t="s">
         <v>481</v>
       </c>
-      <c r="B988" s="6" t="s">
+      <c r="B1002" s="6" t="s">
         <v>482</v>
       </c>
     </row>
-    <row r="989" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A989" s="9" t="s">
+    <row r="1003" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1003" s="10" t="s">
         <v>483</v>
       </c>
-      <c r="B989" s="6" t="s">
+      <c r="B1003" s="6" t="s">
         <v>484</v>
       </c>
     </row>
-    <row r="990" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A990" s="9" t="s">
+    <row r="1004" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1004" s="10" t="s">
         <v>485</v>
       </c>
-      <c r="B990" s="6" t="s">
+      <c r="B1004" s="6" t="s">
         <v>486</v>
       </c>
     </row>
-    <row r="991" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A991" s="9" t="s">
+    <row r="1005" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1005" s="10" t="s">
         <v>487</v>
       </c>
-      <c r="B991" s="6" t="s">
+      <c r="B1005" s="6" t="s">
         <v>488</v>
       </c>
     </row>
-    <row r="992" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A992" s="9" t="s">
+    <row r="1006" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1006" s="10" t="s">
         <v>489</v>
       </c>
-      <c r="B992" s="6" t="s">
+      <c r="B1006" s="6" t="s">
         <v>490</v>
       </c>
     </row>
-    <row r="993" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A993" s="9" t="s">
+    <row r="1007" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1007" s="10" t="s">
         <v>491</v>
       </c>
-      <c r="B993" s="6" t="s">
+      <c r="B1007" s="6" t="s">
         <v>492</v>
       </c>
     </row>
-    <row r="994" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A994" s="9" t="s">
+    <row r="1008" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1008" s="10" t="s">
         <v>493</v>
       </c>
-      <c r="B994" s="6" t="s">
+      <c r="B1008" s="6" t="s">
         <v>494</v>
       </c>
     </row>
-    <row r="995" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A995" s="9" t="s">
+    <row r="1009" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1009" s="10" t="s">
         <v>495</v>
       </c>
-      <c r="B995" s="6" t="s">
+      <c r="B1009" s="6" t="s">
         <v>496</v>
       </c>
     </row>
-    <row r="996" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A996" s="9" t="s">
+    <row r="1010" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1010" s="10" t="s">
         <v>497</v>
       </c>
-      <c r="B996" s="6" t="s">
+      <c r="B1010" s="6" t="s">
         <v>498</v>
       </c>
     </row>
-    <row r="997" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A997" s="9" t="s">
+    <row r="1011" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1011" s="10" t="s">
         <v>499</v>
       </c>
-      <c r="B997" s="6" t="s">
+      <c r="B1011" s="6" t="s">
         <v>500</v>
       </c>
     </row>
-    <row r="998" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A998" s="9" t="s">
+    <row r="1012" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1012" s="10" t="s">
         <v>501</v>
       </c>
-      <c r="B998" s="6" t="s">
+      <c r="B1012" s="6" t="s">
         <v>502</v>
       </c>
     </row>
-    <row r="999" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A999" s="9" t="s">
+    <row r="1013" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1013" s="10" t="s">
         <v>503</v>
       </c>
-      <c r="B999" s="6" t="s">
+      <c r="B1013" s="6" t="s">
         <v>504</v>
       </c>
     </row>
-    <row r="1000" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1000" s="9" t="s">
+    <row r="1014" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1014" s="10" t="s">
         <v>505</v>
       </c>
-      <c r="B1000" s="6" t="s">
+      <c r="B1014" s="6" t="s">
         <v>506</v>
       </c>
     </row>
-    <row r="1001" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1001" s="9" t="s">
+    <row r="1015" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1015" s="10" t="s">
         <v>507</v>
       </c>
-      <c r="B1001" s="6" t="s">
+      <c r="B1015" s="6" t="s">
         <v>508</v>
       </c>
     </row>
-    <row r="1002" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1002" s="9" t="s">
+    <row r="1016" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1016" s="10" t="s">
         <v>509</v>
       </c>
-      <c r="B1002" s="6" t="s">
+      <c r="B1016" s="6" t="s">
         <v>510</v>
       </c>
     </row>
-    <row r="1003" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1003" s="9" t="s">
+    <row r="1017" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1017" s="10" t="s">
         <v>511</v>
       </c>
-      <c r="B1003" s="6" t="s">
+      <c r="B1017" s="6" t="s">
         <v>512</v>
       </c>
     </row>
-    <row r="1004" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1004" s="9" t="s">
+    <row r="1018" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1018" s="10" t="s">
         <v>513</v>
       </c>
-      <c r="B1004" s="6" t="s">
+      <c r="B1018" s="6" t="s">
         <v>514</v>
       </c>
     </row>
-    <row r="1005" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1005" s="9" t="s">
+    <row r="1019" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1019" s="10" t="s">
         <v>515</v>
       </c>
-      <c r="B1005" s="6" t="s">
+      <c r="B1019" s="6" t="s">
         <v>516</v>
       </c>
     </row>
-    <row r="1006" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1006" s="9" t="s">
+    <row r="1020" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1020" s="10" t="s">
         <v>517</v>
       </c>
-      <c r="B1006" s="6" t="s">
+      <c r="B1020" s="6" t="s">
         <v>518</v>
       </c>
     </row>
-    <row r="1007" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1007" s="9" t="s">
+    <row r="1021" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1021" s="10" t="s">
         <v>519</v>
       </c>
-      <c r="B1007" s="6" t="s">
+      <c r="B1021" s="6" t="s">
         <v>520</v>
       </c>
     </row>
-    <row r="1008" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1008" s="9" t="s">
+    <row r="1022" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1022" s="10" t="s">
         <v>521</v>
       </c>
-      <c r="B1008" s="6" t="s">
+      <c r="B1022" s="6" t="s">
         <v>522</v>
       </c>
     </row>
-    <row r="1009" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1009" s="9" t="s">
+    <row r="1023" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1023" s="10" t="s">
         <v>523</v>
       </c>
-      <c r="B1009" s="6" t="s">
+      <c r="B1023" s="6" t="s">
         <v>524</v>
       </c>
     </row>
-    <row r="1010" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1010" s="9" t="s">
+    <row r="1024" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1024" s="10" t="s">
         <v>525</v>
       </c>
-      <c r="B1010" s="6" t="s">
+      <c r="B1024" s="6" t="s">
         <v>526</v>
       </c>
     </row>
-    <row r="1011" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1011" s="9" t="s">
+    <row r="1025" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1025" s="10" t="s">
         <v>527</v>
       </c>
-      <c r="B1011" s="6" t="s">
+      <c r="B1025" s="6" t="s">
         <v>528</v>
       </c>
     </row>
-    <row r="1012" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1012" s="9" t="s">
+    <row r="1026" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1026" s="10" t="s">
         <v>529</v>
       </c>
-      <c r="B1012" s="6" t="s">
+      <c r="B1026" s="6" t="s">
         <v>530</v>
       </c>
     </row>
-    <row r="1013" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1013" s="9" t="s">
+    <row r="1027" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1027" s="10" t="s">
         <v>531</v>
       </c>
-      <c r="B1013" s="6" t="s">
+      <c r="B1027" s="6" t="s">
         <v>532</v>
       </c>
     </row>
-    <row r="1014" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1014" s="9" t="s">
+    <row r="1028" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1028" s="10" t="s">
         <v>533</v>
       </c>
-      <c r="B1014" s="6" t="s">
+      <c r="B1028" s="6" t="s">
         <v>534</v>
       </c>
     </row>
-    <row r="1015" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1015" s="9" t="s">
+    <row r="1029" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1029" s="10" t="s">
         <v>535</v>
       </c>
-      <c r="B1015" s="6" t="s">
+      <c r="B1029" s="6" t="s">
         <v>536</v>
       </c>
     </row>
-    <row r="1016" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1016" s="9" t="s">
+    <row r="1030" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1030" s="10" t="s">
         <v>537</v>
       </c>
-      <c r="B1016" s="6" t="s">
+      <c r="B1030" s="6" t="s">
         <v>538</v>
       </c>
     </row>
-    <row r="1017" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1017" s="9" t="s">
+    <row r="1031" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1031" s="10" t="s">
         <v>539</v>
       </c>
-      <c r="B1017" s="6" t="s">
+      <c r="B1031" s="6" t="s">
         <v>540</v>
       </c>
     </row>
-    <row r="1018" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1018" s="9" t="s">
+    <row r="1032" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1032" s="10" t="s">
         <v>541</v>
       </c>
-      <c r="B1018" s="6" t="s">
+      <c r="B1032" s="6" t="s">
         <v>542</v>
       </c>
     </row>
-    <row r="1019" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1019" s="9" t="s">
+    <row r="1033" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1033" s="10" t="s">
         <v>543</v>
       </c>
-      <c r="B1019" s="6" t="s">
+      <c r="B1033" s="6" t="s">
         <v>544</v>
       </c>
     </row>
-    <row r="1020" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1020" s="9" t="s">
+    <row r="1034" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1034" s="10" t="s">
         <v>545</v>
       </c>
-      <c r="B1020" s="6" t="s">
+      <c r="B1034" s="6" t="s">
         <v>546</v>
       </c>
     </row>
-    <row r="1021" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1021" s="9" t="s">
+    <row r="1035" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1035" s="10" t="s">
         <v>547</v>
       </c>
-      <c r="B1021" s="6" t="s">
+      <c r="B1035" s="6" t="s">
         <v>548</v>
       </c>
     </row>
-    <row r="1022" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1022" s="9" t="s">
+    <row r="1036" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1036" s="10" t="s">
         <v>549</v>
       </c>
-      <c r="B1022" s="6" t="s">
+      <c r="B1036" s="6" t="s">
         <v>550</v>
       </c>
     </row>
-    <row r="1023" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1023" s="9" t="s">
+    <row r="1037" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1037" s="10" t="s">
         <v>551</v>
       </c>
-      <c r="B1023" s="6" t="s">
+      <c r="B1037" s="6" t="s">
         <v>552</v>
       </c>
     </row>
-    <row r="1024" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1024" s="9" t="s">
+    <row r="1038" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1038" s="10" t="s">
         <v>553</v>
       </c>
-      <c r="B1024" s="6" t="s">
+      <c r="B1038" s="6" t="s">
         <v>554</v>
       </c>
     </row>
-    <row r="1025" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1025" s="9" t="s">
+    <row r="1039" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1039" s="10" t="s">
         <v>555</v>
       </c>
-      <c r="B1025" s="6" t="s">
+      <c r="B1039" s="6" t="s">
         <v>556</v>
       </c>
     </row>
-    <row r="1026" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1026" s="9" t="s">
+    <row r="1040" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1040" s="10" t="s">
         <v>557</v>
       </c>
-      <c r="B1026" s="6" t="s">
+      <c r="B1040" s="6" t="s">
         <v>558</v>
       </c>
     </row>
-    <row r="1027" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1027" s="9" t="s">
+    <row r="1041" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1041" s="10" t="s">
         <v>559</v>
       </c>
-      <c r="B1027" s="6" t="s">
+      <c r="B1041" s="6" t="s">
         <v>560</v>
       </c>
     </row>
-    <row r="1028" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1028" s="9" t="s">
+    <row r="1042" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1042" s="10" t="s">
         <v>561</v>
       </c>
-      <c r="B1028" s="6" t="s">
+      <c r="B1042" s="6" t="s">
         <v>562</v>
       </c>
     </row>
-    <row r="1029" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1029" s="9" t="s">
+    <row r="1043" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1043" s="10" t="s">
         <v>563</v>
       </c>
-      <c r="B1029" s="6" t="s">
+      <c r="B1043" s="6" t="s">
         <v>564</v>
       </c>
     </row>
-    <row r="1030" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1030" s="9" t="s">
+    <row r="1044" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1044" s="10" t="s">
         <v>565</v>
       </c>
-      <c r="B1030" s="6" t="s">
+      <c r="B1044" s="6" t="s">
         <v>566</v>
       </c>
     </row>
-    <row r="1031" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1031" s="9" t="s">
+    <row r="1045" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1045" s="10" t="s">
         <v>567</v>
       </c>
-      <c r="B1031" s="6" t="s">
+      <c r="B1045" s="6" t="s">
         <v>568</v>
       </c>
     </row>
-    <row r="1032" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1032" s="9" t="s">
+    <row r="1046" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1046" s="10" t="s">
         <v>569</v>
       </c>
-      <c r="B1032" s="6" t="s">
+      <c r="B1046" s="6" t="s">
         <v>570</v>
       </c>
     </row>
-    <row r="1033" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1033" s="9" t="s">
+    <row r="1047" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1047" s="10" t="s">
         <v>571</v>
       </c>
-      <c r="B1033" s="6" t="s">
+      <c r="B1047" s="6" t="s">
         <v>572</v>
       </c>
     </row>
-    <row r="1034" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1034" s="9" t="s">
+    <row r="1048" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1048" s="10" t="s">
         <v>573</v>
       </c>
-      <c r="B1034" s="6" t="s">
+      <c r="B1048" s="6" t="s">
         <v>574</v>
       </c>
     </row>
-    <row r="1035" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1035" s="9" t="s">
+    <row r="1049" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1049" s="10" t="s">
         <v>575</v>
       </c>
-      <c r="B1035" s="6" t="s">
+      <c r="B1049" s="6" t="s">
         <v>576</v>
       </c>
     </row>
-    <row r="1036" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1036" s="9" t="s">
+    <row r="1050" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1050" s="10" t="s">
         <v>577</v>
       </c>
-      <c r="B1036" s="6" t="s">
+      <c r="B1050" s="6" t="s">
         <v>578</v>
       </c>
     </row>
-    <row r="1037" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1037" s="9" t="s">
+    <row r="1051" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1051" s="10" t="s">
         <v>579</v>
       </c>
-      <c r="B1037" s="6" t="s">
+      <c r="B1051" s="6" t="s">
         <v>580</v>
       </c>
     </row>
-    <row r="1038" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1038" s="9" t="s">
+    <row r="1052" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1052" s="10" t="s">
         <v>581</v>
       </c>
-      <c r="B1038" s="6" t="s">
+      <c r="B1052" s="6" t="s">
         <v>582</v>
       </c>
     </row>
-    <row r="1039" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1039" s="9" t="s">
+    <row r="1053" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1053" s="10" t="s">
         <v>583</v>
       </c>
-      <c r="B1039" s="6" t="s">
+      <c r="B1053" s="6" t="s">
         <v>584</v>
       </c>
     </row>
-    <row r="1040" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1040" s="9" t="s">
+    <row r="1054" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1054" s="10" t="s">
         <v>585</v>
       </c>
-      <c r="B1040" s="6" t="s">
+      <c r="B1054" s="6" t="s">
         <v>586</v>
       </c>
     </row>
-    <row r="1041" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1041" s="9" t="s">
+    <row r="1055" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1055" s="10" t="s">
         <v>587</v>
       </c>
-      <c r="B1041" s="6" t="s">
+      <c r="B1055" s="6" t="s">
         <v>588</v>
       </c>
     </row>
-    <row r="1042" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1042" s="9" t="s">
+    <row r="1056" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1056" s="10" t="s">
         <v>589</v>
       </c>
-      <c r="B1042" s="6" t="s">
+      <c r="B1056" s="6" t="s">
         <v>590</v>
       </c>
     </row>
-    <row r="1043" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1043" s="9" t="s">
+    <row r="1057" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1057" s="10" t="s">
         <v>591</v>
       </c>
-      <c r="B1043" s="6" t="s">
+      <c r="B1057" s="6" t="s">
         <v>592</v>
       </c>
     </row>
-    <row r="1044" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1044" s="9" t="s">
+    <row r="1058" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1058" s="10" t="s">
         <v>593</v>
       </c>
-      <c r="B1044" s="6" t="s">
+      <c r="B1058" s="6" t="s">
         <v>594</v>
       </c>
     </row>
-    <row r="1045" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1045" s="9" t="s">
+    <row r="1059" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1059" s="10" t="s">
         <v>595</v>
       </c>
-      <c r="B1045" s="6" t="s">
+      <c r="B1059" s="6" t="s">
         <v>596</v>
       </c>
     </row>
-    <row r="1046" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1046" s="9" t="s">
+    <row r="1060" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1060" s="10" t="s">
         <v>597</v>
       </c>
-      <c r="B1046" s="6" t="s">
+      <c r="B1060" s="6" t="s">
         <v>598</v>
       </c>
     </row>
-    <row r="1047" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1047" s="9" t="s">
+    <row r="1061" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1061" s="10" t="s">
         <v>599</v>
       </c>
-      <c r="B1047" s="6" t="s">
+      <c r="B1061" s="6" t="s">
         <v>600</v>
       </c>
     </row>
-    <row r="1048" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1048" s="9" t="s">
+    <row r="1062" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1062" s="10" t="s">
         <v>601</v>
       </c>
-      <c r="B1048" s="6" t="s">
+      <c r="B1062" s="6" t="s">
         <v>602</v>
       </c>
     </row>
-    <row r="1049" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1049" s="9" t="s">
+    <row r="1063" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1063" s="10" t="s">
         <v>603</v>
       </c>
-      <c r="B1049" s="6" t="s">
+      <c r="B1063" s="6" t="s">
         <v>604</v>
       </c>
     </row>
-    <row r="1050" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1050" s="9" t="s">
+    <row r="1064" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1064" s="10" t="s">
         <v>605</v>
       </c>
-      <c r="B1050" s="6" t="s">
+      <c r="B1064" s="6" t="s">
         <v>606</v>
       </c>
     </row>
-    <row r="1051" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1051" s="9" t="s">
+    <row r="1065" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1065" s="10" t="s">
         <v>607</v>
       </c>
-      <c r="B1051" s="6" t="s">
+      <c r="B1065" s="6" t="s">
         <v>608</v>
       </c>
     </row>
-    <row r="1052" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1052" s="9" t="s">
+    <row r="1066" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1066" s="10" t="s">
         <v>609</v>
       </c>
-      <c r="B1052" s="6" t="s">
+      <c r="B1066" s="6" t="s">
         <v>610</v>
       </c>
     </row>
-    <row r="1053" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1053" s="9" t="s">
+    <row r="1067" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1067" s="10" t="s">
         <v>611</v>
       </c>
-      <c r="B1053" s="6" t="s">
+      <c r="B1067" s="6" t="s">
         <v>612</v>
       </c>
     </row>
-    <row r="1054" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1054" s="9" t="s">
+    <row r="1068" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1068" s="10" t="s">
         <v>613</v>
       </c>
-      <c r="B1054" s="6" t="s">
+      <c r="B1068" s="6" t="s">
         <v>614</v>
       </c>
     </row>
-    <row r="1055" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1055" s="9" t="s">
+    <row r="1069" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1069" s="10" t="s">
         <v>615</v>
       </c>
-      <c r="B1055" s="6" t="s">
+      <c r="B1069" s="6" t="s">
         <v>616</v>
       </c>
     </row>
-    <row r="1056" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1056" s="9" t="s">
+    <row r="1070" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1070" s="10" t="s">
         <v>617</v>
       </c>
-      <c r="B1056" s="6" t="s">
+      <c r="B1070" s="6" t="s">
         <v>618</v>
       </c>
     </row>
-    <row r="1057" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1057" s="9" t="s">
+    <row r="1071" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1071" s="10" t="s">
         <v>619</v>
       </c>
-      <c r="B1057" s="6" t="s">
+      <c r="B1071" s="6" t="s">
         <v>620</v>
       </c>
     </row>
-    <row r="1058" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1058" s="9" t="s">
+    <row r="1072" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1072" s="10" t="s">
         <v>621</v>
       </c>
-      <c r="B1058" s="6" t="s">
+      <c r="B1072" s="6" t="s">
         <v>622</v>
       </c>
     </row>
-    <row r="1059" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1059" s="9" t="s">
+    <row r="1073" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1073" s="10" t="s">
         <v>623</v>
       </c>
-      <c r="B1059" s="6" t="s">
+      <c r="B1073" s="6" t="s">
         <v>624</v>
       </c>
     </row>
-    <row r="1060" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1060" s="9" t="s">
+    <row r="1074" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1074" s="10" t="s">
         <v>625</v>
       </c>
-      <c r="B1060" s="6" t="s">
+      <c r="B1074" s="6" t="s">
         <v>626</v>
       </c>
     </row>
-    <row r="1061" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1061" s="9" t="s">
+    <row r="1075" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1075" s="10" t="s">
         <v>627</v>
       </c>
-      <c r="B1061" s="6" t="s">
+      <c r="B1075" s="6" t="s">
         <v>628</v>
       </c>
     </row>
-    <row r="1062" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1062" s="9" t="s">
+    <row r="1076" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1076" s="10" t="s">
         <v>629</v>
       </c>
-      <c r="B1062" s="6" t="s">
+      <c r="B1076" s="6" t="s">
         <v>630</v>
       </c>
     </row>
-    <row r="1063" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1063" s="9" t="s">
+    <row r="1077" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1077" s="10" t="s">
         <v>631</v>
       </c>
-      <c r="B1063" s="6" t="s">
+      <c r="B1077" s="6" t="s">
         <v>632</v>
       </c>
     </row>
-    <row r="1064" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1064" s="9" t="s">
+    <row r="1078" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1078" s="10" t="s">
         <v>633</v>
       </c>
-      <c r="B1064" s="6" t="s">
+      <c r="B1078" s="6" t="s">
         <v>634</v>
       </c>
     </row>
-    <row r="1065" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1065" s="9" t="s">
+    <row r="1079" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1079" s="10" t="s">
         <v>635</v>
       </c>
-      <c r="B1065" s="6" t="s">
+      <c r="B1079" s="6" t="s">
         <v>636</v>
       </c>
     </row>
-    <row r="1066" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1066" s="9" t="s">
+    <row r="1080" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1080" s="10" t="s">
         <v>637</v>
       </c>
-      <c r="B1066" s="6" t="s">
+      <c r="B1080" s="6" t="s">
         <v>638</v>
       </c>
     </row>
-    <row r="1067" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1067" s="9" t="s">
+    <row r="1081" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1081" s="10" t="s">
         <v>639</v>
       </c>
-      <c r="B1067" s="6" t="s">
+      <c r="B1081" s="6" t="s">
         <v>640</v>
       </c>
     </row>
-    <row r="1068" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1068" s="9" t="s">
+    <row r="1082" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1082" s="10" t="s">
         <v>641</v>
       </c>
-      <c r="B1068" s="6" t="s">
+      <c r="B1082" s="6" t="s">
         <v>642</v>
       </c>
     </row>
-    <row r="1069" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1069" s="9" t="s">
+    <row r="1083" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1083" s="10" t="s">
         <v>643</v>
       </c>
-      <c r="B1069" s="6" t="s">
+      <c r="B1083" s="6" t="s">
         <v>644</v>
       </c>
     </row>
-    <row r="1070" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1070" s="9" t="s">
+    <row r="1084" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1084" s="10" t="s">
         <v>645</v>
       </c>
-      <c r="B1070" s="6" t="s">
+      <c r="B1084" s="6" t="s">
         <v>646</v>
       </c>
     </row>
-    <row r="1071" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1071" s="9" t="s">
+    <row r="1085" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1085" s="10" t="s">
         <v>647</v>
       </c>
-      <c r="B1071" s="6" t="s">
+      <c r="B1085" s="6" t="s">
         <v>648</v>
       </c>
     </row>
-    <row r="1072" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1072" s="9" t="s">
+    <row r="1086" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1086" s="10" t="s">
         <v>649</v>
       </c>
-      <c r="B1072" s="6" t="s">
+      <c r="B1086" s="6" t="s">
         <v>650</v>
       </c>
     </row>
-    <row r="1073" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1073" s="9" t="s">
+    <row r="1087" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1087" s="10" t="s">
         <v>651</v>
       </c>
-      <c r="B1073" s="6" t="s">
+      <c r="B1087" s="6" t="s">
         <v>652</v>
       </c>
     </row>
-    <row r="1074" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1074" s="9" t="s">
+    <row r="1088" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1088" s="10" t="s">
         <v>653</v>
       </c>
-      <c r="B1074" s="6" t="s">
+      <c r="B1088" s="6" t="s">
         <v>654</v>
       </c>
     </row>
-    <row r="1075" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1075" s="9" t="s">
+    <row r="1089" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1089" s="10" t="s">
         <v>655</v>
       </c>
-      <c r="B1075" s="6" t="s">
+      <c r="B1089" s="6" t="s">
         <v>656</v>
       </c>
     </row>
-    <row r="1076" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1076" s="9" t="s">
+    <row r="1090" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1090" s="10" t="s">
         <v>657</v>
       </c>
-      <c r="B1076" s="6" t="s">
+      <c r="B1090" s="6" t="s">
         <v>658</v>
       </c>
     </row>
-    <row r="1077" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1077" s="9" t="s">
+    <row r="1091" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1091" s="10" t="s">
         <v>659</v>
       </c>
-      <c r="B1077" s="6" t="s">
+      <c r="B1091" s="6" t="s">
         <v>660</v>
       </c>
     </row>
-    <row r="1078" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1078" s="9" t="s">
+    <row r="1092" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1092" s="10" t="s">
         <v>661</v>
       </c>
-      <c r="B1078" s="6" t="s">
+      <c r="B1092" s="6" t="s">
         <v>662</v>
       </c>
     </row>
-    <row r="1079" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1079" s="9" t="s">
+    <row r="1093" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1093" s="10" t="s">
         <v>663</v>
       </c>
-      <c r="B1079" s="6" t="s">
+      <c r="B1093" s="6" t="s">
         <v>664</v>
       </c>
     </row>
-    <row r="1080" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1080" s="9" t="s">
+    <row r="1094" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1094" s="10" t="s">
         <v>665</v>
       </c>
-      <c r="B1080" s="6" t="s">
+      <c r="B1094" s="6" t="s">
         <v>666</v>
       </c>
     </row>
-    <row r="1081" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1081" s="9" t="s">
+    <row r="1095" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1095" s="10" t="s">
         <v>667</v>
       </c>
-      <c r="B1081" s="6" t="s">
+      <c r="B1095" s="6" t="s">
         <v>668</v>
       </c>
     </row>
-    <row r="1082" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1082" s="9" t="s">
+    <row r="1096" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1096" s="10" t="s">
         <v>669</v>
       </c>
-      <c r="B1082" s="6" t="s">
+      <c r="B1096" s="6" t="s">
         <v>670</v>
       </c>
     </row>
-    <row r="1083" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1083" s="9" t="s">
+    <row r="1097" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1097" s="10" t="s">
         <v>671</v>
       </c>
-      <c r="B1083" s="6" t="s">
+      <c r="B1097" s="6" t="s">
         <v>672</v>
       </c>
     </row>
-    <row r="1084" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1084" s="9" t="s">
+    <row r="1098" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1098" s="10" t="s">
         <v>673</v>
       </c>
-      <c r="B1084" s="6" t="s">
+      <c r="B1098" s="6" t="s">
         <v>674</v>
       </c>
     </row>
-    <row r="1085" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1085" s="9" t="s">
+    <row r="1099" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1099" s="10" t="s">
         <v>675</v>
       </c>
-      <c r="B1085" s="6" t="s">
+      <c r="B1099" s="6" t="s">
         <v>676</v>
       </c>
     </row>
-    <row r="1086" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1086" s="9" t="s">
+    <row r="1100" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1100" s="10" t="s">
         <v>677</v>
       </c>
-      <c r="B1086" s="6" t="s">
+      <c r="B1100" s="6" t="s">
         <v>678</v>
       </c>
     </row>
-    <row r="1087" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1087" s="9" t="s">
+    <row r="1101" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1101" s="10" t="s">
         <v>679</v>
       </c>
-      <c r="B1087" s="6" t="s">
+      <c r="B1101" s="6" t="s">
         <v>680</v>
       </c>
     </row>
-    <row r="1088" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1088" s="9" t="s">
+    <row r="1102" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1102" s="10" t="s">
         <v>681</v>
       </c>
-      <c r="B1088" s="6" t="s">
+      <c r="B1102" s="6" t="s">
         <v>682</v>
       </c>
     </row>
-    <row r="1089" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1089" s="9" t="s">
+    <row r="1103" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1103" s="10" t="s">
         <v>683</v>
       </c>
-      <c r="B1089" s="6" t="s">
+      <c r="B1103" s="6" t="s">
         <v>684</v>
       </c>
     </row>
-    <row r="1090" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1090" s="9" t="s">
+    <row r="1104" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1104" s="10" t="s">
         <v>685</v>
       </c>
-      <c r="B1090" s="6" t="s">
+      <c r="B1104" s="6" t="s">
         <v>686</v>
       </c>
     </row>
-    <row r="1091" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1091" s="9" t="s">
+    <row r="1105" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1105" s="10" t="s">
         <v>687</v>
       </c>
-      <c r="B1091" s="6" t="s">
+      <c r="B1105" s="6" t="s">
         <v>688</v>
       </c>
     </row>
-    <row r="1092" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1092" s="9" t="s">
+    <row r="1106" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1106" s="10" t="s">
         <v>689</v>
       </c>
-      <c r="B1092" s="6" t="s">
+      <c r="B1106" s="6" t="s">
         <v>690</v>
       </c>
     </row>
-    <row r="1093" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1093" s="9" t="s">
+    <row r="1107" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1107" s="10" t="s">
         <v>691</v>
       </c>
-      <c r="B1093" s="6" t="s">
+      <c r="B1107" s="6" t="s">
         <v>692</v>
       </c>
     </row>
-    <row r="1094" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1094" s="9" t="s">
+    <row r="1108" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1108" s="10" t="s">
         <v>693</v>
       </c>
-      <c r="B1094" s="6" t="s">
+      <c r="B1108" s="6" t="s">
         <v>694</v>
       </c>
     </row>
-    <row r="1095" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1095" s="9" t="s">
+    <row r="1109" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1109" s="10" t="s">
         <v>695</v>
       </c>
-      <c r="B1095" s="6" t="s">
+      <c r="B1109" s="6" t="s">
         <v>696</v>
       </c>
     </row>
-    <row r="1096" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1096" s="9" t="s">
+    <row r="1110" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1110" s="10" t="s">
         <v>697</v>
       </c>
-      <c r="B1096" s="6" t="s">
+      <c r="B1110" s="6" t="s">
         <v>698</v>
       </c>
     </row>
-    <row r="1097" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1097" s="9" t="s">
+    <row r="1111" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1111" s="10" t="s">
         <v>699</v>
       </c>
-      <c r="B1097" s="6" t="s">
+      <c r="B1111" s="6" t="s">
         <v>700</v>
       </c>
     </row>
-    <row r="1098" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1098" s="9" t="s">
+    <row r="1112" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1112" s="10" t="s">
         <v>701</v>
       </c>
-      <c r="B1098" s="6" t="s">
+      <c r="B1112" s="6" t="s">
         <v>702</v>
       </c>
     </row>
-    <row r="1099" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1099" s="9" t="s">
+    <row r="1113" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1113" s="10" t="s">
         <v>703</v>
       </c>
-      <c r="B1099" s="6" t="s">
+      <c r="B1113" s="6" t="s">
         <v>704</v>
       </c>
     </row>
-    <row r="1100" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1100" s="9" t="s">
+    <row r="1114" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1114" s="10" t="s">
         <v>705</v>
       </c>
-      <c r="B1100" s="6" t="s">
+      <c r="B1114" s="6" t="s">
         <v>706</v>
       </c>
     </row>
-    <row r="1101" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1101" s="9" t="s">
+    <row r="1115" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1115" s="10" t="s">
         <v>707</v>
       </c>
-      <c r="B1101" s="6" t="s">
+      <c r="B1115" s="6" t="s">
         <v>708</v>
       </c>
     </row>
-    <row r="1102" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1102" s="9" t="s">
+    <row r="1116" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1116" s="10" t="s">
         <v>709</v>
       </c>
-      <c r="B1102" s="6" t="s">
+      <c r="B1116" s="6" t="s">
         <v>710</v>
       </c>
     </row>
-    <row r="1103" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1103" s="9" t="s">
+    <row r="1117" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1117" s="10" t="s">
         <v>711</v>
       </c>
-      <c r="B1103" s="6" t="s">
+      <c r="B1117" s="6" t="s">
         <v>712</v>
       </c>
     </row>
-    <row r="1104" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1104" s="9" t="s">
+    <row r="1118" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1118" s="10" t="s">
         <v>713</v>
       </c>
-      <c r="B1104" s="6" t="s">
+      <c r="B1118" s="6" t="s">
         <v>714</v>
       </c>
     </row>
-    <row r="1105" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1105" s="9" t="s">
+    <row r="1119" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1119" s="10" t="s">
         <v>715</v>
       </c>
-      <c r="B1105" s="6" t="s">
+      <c r="B1119" s="6" t="s">
         <v>716</v>
       </c>
     </row>
-    <row r="1106" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1106" s="9" t="s">
+    <row r="1120" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1120" s="10" t="s">
         <v>717</v>
       </c>
-      <c r="B1106" s="6" t="s">
+      <c r="B1120" s="6" t="s">
         <v>718</v>
       </c>
     </row>
-    <row r="1107" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1107" s="9" t="s">
+    <row r="1121" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1121" s="10" t="s">
         <v>719</v>
       </c>
-      <c r="B1107" s="6" t="s">
+      <c r="B1121" s="6" t="s">
         <v>720</v>
       </c>
     </row>
-    <row r="1108" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1108" s="9" t="s">
+    <row r="1122" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1122" s="10" t="s">
         <v>721</v>
       </c>
-      <c r="B1108" s="6" t="s">
+      <c r="B1122" s="6" t="s">
         <v>722</v>
       </c>
     </row>
-    <row r="1109" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1109" s="9" t="s">
+    <row r="1123" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1123" s="10" t="s">
         <v>723</v>
       </c>
-      <c r="B1109" s="6" t="s">
+      <c r="B1123" s="6" t="s">
         <v>724</v>
       </c>
     </row>
-    <row r="1110" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1110" s="9" t="s">
+    <row r="1124" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1124" s="10" t="s">
         <v>725</v>
       </c>
-      <c r="B1110" s="6" t="s">
+      <c r="B1124" s="6" t="s">
         <v>726</v>
       </c>
     </row>
-    <row r="1111" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1111" s="9" t="s">
+    <row r="1125" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1125" s="10" t="s">
         <v>727</v>
       </c>
-      <c r="B1111" s="6" t="s">
+      <c r="B1125" s="6" t="s">
         <v>728</v>
       </c>
     </row>
-    <row r="1112" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1112" s="9" t="s">
+    <row r="1126" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1126" s="10" t="s">
         <v>729</v>
       </c>
-      <c r="B1112" s="6" t="s">
+      <c r="B1126" s="6" t="s">
         <v>730</v>
       </c>
     </row>
-    <row r="1113" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1113" s="9" t="s">
+    <row r="1127" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1127" s="10" t="s">
         <v>731</v>
       </c>
-      <c r="B1113" s="6" t="s">
+      <c r="B1127" s="6" t="s">
         <v>732</v>
       </c>
     </row>
-    <row r="1114" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1114" s="9" t="s">
+    <row r="1128" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1128" s="10" t="s">
         <v>733</v>
       </c>
-      <c r="B1114" s="6" t="s">
+      <c r="B1128" s="6" t="s">
         <v>734</v>
       </c>
     </row>
-    <row r="1115" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1115" s="9" t="s">
+    <row r="1129" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1129" s="10" t="s">
         <v>735</v>
       </c>
-      <c r="B1115" s="6" t="s">
+      <c r="B1129" s="6" t="s">
         <v>736</v>
       </c>
     </row>
-    <row r="1116" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1116" s="9" t="s">
+    <row r="1130" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1130" s="10" t="s">
         <v>737</v>
       </c>
-      <c r="B1116" s="6" t="s">
+      <c r="B1130" s="6" t="s">
         <v>738</v>
       </c>
     </row>
-    <row r="1117" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1117" s="9" t="s">
+    <row r="1131" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1131" s="10" t="s">
         <v>739</v>
       </c>
-      <c r="B1117" s="6" t="s">
+      <c r="B1131" s="6" t="s">
         <v>740</v>
       </c>
     </row>
-    <row r="1118" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1118" s="9" t="s">
+    <row r="1132" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1132" s="10" t="s">
         <v>741</v>
       </c>
-      <c r="B1118" s="6" t="s">
+      <c r="B1132" s="6" t="s">
         <v>742</v>
       </c>
     </row>
-    <row r="1119" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1119" s="9" t="s">
+    <row r="1133" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1133" s="10" t="s">
         <v>743</v>
       </c>
-      <c r="B1119" s="6" t="s">
+      <c r="B1133" s="6" t="s">
         <v>744</v>
       </c>
     </row>
-    <row r="1120" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1120" s="9" t="s">
+    <row r="1134" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1134" s="10" t="s">
         <v>745</v>
       </c>
-      <c r="B1120" s="6" t="s">
+      <c r="B1134" s="6" t="s">
         <v>746</v>
       </c>
     </row>
-    <row r="1121" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1121" s="9" t="s">
+    <row r="1135" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1135" s="10" t="s">
         <v>747</v>
       </c>
-      <c r="B1121" s="6" t="s">
+      <c r="B1135" s="6" t="s">
         <v>748</v>
       </c>
     </row>
-    <row r="1122" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1122" s="9" t="s">
+    <row r="1136" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1136" s="10" t="s">
         <v>749</v>
       </c>
-      <c r="B1122" s="6" t="s">
+      <c r="B1136" s="6" t="s">
         <v>750</v>
       </c>
     </row>
-    <row r="1123" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1123" s="9" t="s">
+    <row r="1137" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1137" s="10" t="s">
         <v>751</v>
       </c>
-      <c r="B1123" s="6" t="s">
+      <c r="B1137" s="6" t="s">
         <v>752</v>
       </c>
     </row>
-    <row r="1124" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1124" s="9" t="s">
+    <row r="1138" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1138" s="10" t="s">
         <v>753</v>
       </c>
-      <c r="B1124" s="6" t="s">
+      <c r="B1138" s="6" t="s">
         <v>754</v>
       </c>
     </row>
-    <row r="1125" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1125" s="9" t="s">
+    <row r="1139" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1139" s="10" t="s">
         <v>755</v>
       </c>
-      <c r="B1125" s="6" t="s">
+      <c r="B1139" s="6" t="s">
         <v>756</v>
       </c>
     </row>
-    <row r="1126" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1126" s="9" t="s">
+    <row r="1140" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1140" s="10" t="s">
         <v>757</v>
       </c>
-      <c r="B1126" s="6" t="s">
+      <c r="B1140" s="6" t="s">
         <v>758</v>
       </c>
     </row>
-    <row r="1127" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1127" s="9" t="s">
+    <row r="1141" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1141" s="10" t="s">
         <v>759</v>
       </c>
-      <c r="B1127" s="6" t="s">
+      <c r="B1141" s="6" t="s">
         <v>760</v>
       </c>
     </row>
-    <row r="1128" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1128" s="9" t="s">
+    <row r="1142" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1142" s="10" t="s">
         <v>761</v>
       </c>
-      <c r="B1128" s="6" t="s">
+      <c r="B1142" s="6" t="s">
         <v>762</v>
       </c>
     </row>
-    <row r="1129" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1129" s="9" t="s">
+    <row r="1143" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1143" s="10" t="s">
         <v>763</v>
       </c>
-      <c r="B1129" s="6" t="s">
+      <c r="B1143" s="6" t="s">
         <v>764</v>
       </c>
     </row>
-    <row r="1130" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1130" s="9" t="s">
+    <row r="1144" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1144" s="10" t="s">
         <v>765</v>
       </c>
-      <c r="B1130" s="6" t="s">
+      <c r="B1144" s="6" t="s">
         <v>766</v>
       </c>
     </row>
-    <row r="1131" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1131" s="9" t="s">
+    <row r="1145" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1145" s="10" t="s">
         <v>767</v>
       </c>
-      <c r="B1131" s="6" t="s">
+      <c r="B1145" s="6" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="1132" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1132" s="9" t="s">
+    <row r="1146" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1146" s="10" t="s">
         <v>768</v>
       </c>
-      <c r="B1132" s="6" t="s">
+      <c r="B1146" s="6" t="s">
         <v>769</v>
       </c>
     </row>
-    <row r="1133" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1133" s="9" t="s">
+    <row r="1147" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1147" s="10" t="s">
         <v>770</v>
       </c>
-      <c r="B1133" s="6" t="s">
+      <c r="B1147" s="6" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="1134" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1134" s="9" t="s">
+    <row r="1148" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1148" s="10" t="s">
         <v>771</v>
       </c>
-      <c r="B1134" s="6" t="s">
+      <c r="B1148" s="6" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="1135" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1135" s="9" t="s">
+    <row r="1149" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1149" s="10" t="s">
         <v>772</v>
       </c>
-      <c r="B1135" s="6" t="s">
+      <c r="B1149" s="6" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="1136" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1136" s="9" t="s">
+    <row r="1150" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1150" s="10" t="s">
         <v>773</v>
       </c>
-      <c r="B1136" s="6" t="s">
+      <c r="B1150" s="6" t="s">
         <v>774</v>
       </c>
     </row>
-    <row r="1137" spans="1:2" ht="22.5" x14ac:dyDescent="0.2">
-      <c r="A1137" s="9" t="s">
+    <row r="1151" spans="1:2" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A1151" s="10" t="s">
         <v>775</v>
       </c>
-      <c r="B1137" s="7" t="s">
+      <c r="B1151" s="9" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="1138" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1138" s="9" t="s">
+    <row r="1152" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1152" s="10" t="s">
         <v>776</v>
       </c>
-      <c r="B1138" s="6" t="s">
+      <c r="B1152" s="6" t="s">
         <v>777</v>
       </c>
     </row>
-    <row r="1139" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1139" s="9" t="s">
+    <row r="1153" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1153" s="10" t="s">
         <v>778</v>
       </c>
-      <c r="B1139" s="6" t="s">
+      <c r="B1153" s="6" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="1140" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1140" s="9" t="s">
+    <row r="1154" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1154" s="10" t="s">
         <v>779</v>
       </c>
-      <c r="B1140" s="6" t="s">
+      <c r="B1154" s="6" t="s">
         <v>780</v>
       </c>
     </row>
-    <row r="1141" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1141" s="9" t="s">
+    <row r="1155" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1155" s="10" t="s">
         <v>781</v>
       </c>
-      <c r="B1141" s="6" t="s">
+      <c r="B1155" s="6" t="s">
         <v>782</v>
       </c>
     </row>
-    <row r="1142" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1142" s="9" t="s">
+    <row r="1156" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1156" s="10" t="s">
         <v>783</v>
       </c>
-      <c r="B1142" s="6" t="s">
+      <c r="B1156" s="6" t="s">
         <v>784</v>
       </c>
     </row>
-    <row r="1143" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1143" s="9" t="s">
+    <row r="1157" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1157" s="10" t="s">
         <v>785</v>
       </c>
-      <c r="B1143" s="6" t="s">
+      <c r="B1157" s="6" t="s">
         <v>786</v>
       </c>
     </row>
-    <row r="1144" spans="1:2" ht="22.5" x14ac:dyDescent="0.2">
-      <c r="A1144" s="9" t="s">
+    <row r="1158" spans="1:2" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A1158" s="10" t="s">
         <v>787</v>
       </c>
-      <c r="B1144" s="6" t="s">
+      <c r="B1158" s="6" t="s">
         <v>788</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add 'Wings of Velvet'
Added the mage set and placed into a chest in the Great Hall (lvl 3) of the Broken Circle quest line

see #383
</commit_message>
<xml_diff>
--- a/source/tlk/strings.xlsx
+++ b/source/tlk/strings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\DAO\archid\source\tlk\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D0EE399-8079-4CCE-AD28-7A8EF2B8C905}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7731DB2E-48CF-405E-B4A6-8CF047A13BB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29535" yWindow="735" windowWidth="26610" windowHeight="16110" xr2:uid="{A42EE72D-E1C4-43B6-AEA5-0014ED5180B1}"/>
+    <workbookView xWindow="29190" yWindow="390" windowWidth="26610" windowHeight="16110" xr2:uid="{A42EE72D-E1C4-43B6-AEA5-0014ED5180B1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -295,7 +295,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A823" authorId="0" shapeId="0" xr:uid="{15B7CDC5-6F21-45A0-9997-3CC9AFCCF646}">
+    <comment ref="A833" authorId="0" shapeId="0" xr:uid="{15B7CDC5-6F21-45A0-9997-3CC9AFCCF646}">
       <text>
         <r>
           <rPr>
@@ -309,7 +309,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A950" authorId="0" shapeId="0" xr:uid="{08441945-669A-47E4-A77A-BA32248BBBE4}">
+    <comment ref="A960" authorId="0" shapeId="0" xr:uid="{08441945-669A-47E4-A77A-BA32248BBBE4}">
       <text>
         <r>
           <rPr>
@@ -342,7 +342,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1495" uniqueCount="1438">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1505" uniqueCount="1448">
   <si>
     <t>af_archid_en-us.tlk</t>
   </si>
@@ -4720,14 +4720,51 @@
   <si>
     <t>The strange metal of this shield not only deflects incoming attacks it also reflects its surroundings like a real mirror.</t>
   </si>
+  <si>
+    <t>Crescent Talons</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Light boots covered in vines and with and ornate toecap in the form of a bird of preys talons. </t>
+  </si>
+  <si>
+    <t>Feathers of Dusk</t>
+  </si>
+  <si>
+    <t>Beautiful and ornate this robe was custom made for an elven archmage that lived in Halamshiral before the dark clouds of  human  intolerance thickened above the Dales. It is made from the fabric akin to leather by the look of it, but to the touch it is astonishingly close to the brocade.  Adorned by the blue jewels that are cased in unknown silvery metal. The surface is covered in floral elements with the embroidery in satin-stitch of the owl's head that is clearly seen on robes front hem.</t>
+  </si>
+  <si>
+    <t>Claws of Twilight</t>
+  </si>
+  <si>
+    <t>Adorned with embroidery of feathers, floral patterns and strange, long forgotten runes this pair of delicate gloves as clearly made for ancient elven mage whose name was lost long ago.</t>
+  </si>
+  <si>
+    <t>Nights Eyes</t>
+  </si>
+  <si>
+    <t>This hood is made from the strange material that is similar to the leather and brocade at the same time. Patterns on the surface are done in a manner of exotic plants and strange swirls, but the main element is an owl's head that is embroidered in silk on the temple of the hood. This piece of mage armor is clearly of elven work that was created many centuries ago. It's really a miracle that it still look and fill like it have been made just now and especially for you.</t>
+  </si>
+  <si>
+    <t>Lance of Moonlight</t>
+  </si>
+  <si>
+    <t>This ornate stave looks newly done but feel like a truly ancient item. Two black dragons are holding a ball of clear blue color. If you look at it long enough you will see the summer night sky that full of stars.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -4819,26 +4856,30 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="2" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5157,10 +5198,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C8288F5-46B5-435A-B9FC-40522281A8A6}">
-  <dimension ref="A1:B1158"/>
+  <dimension ref="A1:B1168"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A800" workbookViewId="0">
-      <selection activeCell="B825" sqref="B825"/>
+    <sheetView tabSelected="1" topLeftCell="A785" workbookViewId="0">
+      <selection activeCell="B826" sqref="B826"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -11747,1128 +11788,1128 @@
       </c>
     </row>
     <row r="823" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A823" s="8" t="s">
+      <c r="A823" s="4">
+        <v>6610821</v>
+      </c>
+      <c r="B823" s="2" t="s">
+        <v>1438</v>
+      </c>
+    </row>
+    <row r="824" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A824" s="4">
+        <v>6610822</v>
+      </c>
+      <c r="B824" s="11" t="s">
+        <v>1439</v>
+      </c>
+    </row>
+    <row r="825" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A825" s="4">
+        <v>6610823</v>
+      </c>
+      <c r="B825" s="2" t="s">
+        <v>1440</v>
+      </c>
+    </row>
+    <row r="826" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A826" s="4">
+        <v>6610824</v>
+      </c>
+      <c r="B826" s="12" t="s">
+        <v>1441</v>
+      </c>
+    </row>
+    <row r="827" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A827" s="4">
+        <v>6610825</v>
+      </c>
+      <c r="B827" s="2" t="s">
+        <v>1442</v>
+      </c>
+    </row>
+    <row r="828" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A828" s="4">
+        <v>6610826</v>
+      </c>
+      <c r="B828" s="12" t="s">
+        <v>1443</v>
+      </c>
+    </row>
+    <row r="829" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A829" s="4">
+        <v>6610827</v>
+      </c>
+      <c r="B829" s="2" t="s">
+        <v>1444</v>
+      </c>
+    </row>
+    <row r="830" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A830" s="4">
+        <v>6610828</v>
+      </c>
+      <c r="B830" s="12" t="s">
+        <v>1445</v>
+      </c>
+    </row>
+    <row r="831" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A831" s="4">
+        <v>6610829</v>
+      </c>
+      <c r="B831" s="2" t="s">
+        <v>1446</v>
+      </c>
+    </row>
+    <row r="832" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A832" s="4">
+        <v>6610830</v>
+      </c>
+      <c r="B832" s="2" t="s">
+        <v>1447</v>
+      </c>
+    </row>
+    <row r="833" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A833" s="8" t="s">
         <v>150</v>
       </c>
-      <c r="B823" s="6" t="s">
+      <c r="B833" s="6" t="s">
         <v>151</v>
-      </c>
-    </row>
-    <row r="824" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A824" s="8" t="s">
-        <v>152</v>
-      </c>
-      <c r="B824" s="6" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="825" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A825" s="8" t="s">
-        <v>154</v>
-      </c>
-      <c r="B825" s="6" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="826" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A826" s="8" t="s">
-        <v>156</v>
-      </c>
-      <c r="B826" s="6" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="827" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A827" s="8" t="s">
-        <v>158</v>
-      </c>
-      <c r="B827" s="6" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="828" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
-      <c r="A828" s="8" t="s">
-        <v>160</v>
-      </c>
-      <c r="B828" s="6" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="829" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A829" s="8" t="s">
-        <v>162</v>
-      </c>
-      <c r="B829" s="6" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="830" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A830" s="8" t="s">
-        <v>164</v>
-      </c>
-      <c r="B830" s="6" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="831" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A831" s="8" t="s">
-        <v>166</v>
-      </c>
-      <c r="B831" s="6" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="832" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A832" s="8" t="s">
-        <v>168</v>
-      </c>
-      <c r="B832" s="6" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="833" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
-      <c r="A833" s="8" t="s">
-        <v>170</v>
-      </c>
-      <c r="B833" s="6" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="834" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A834" s="8" t="s">
-        <v>172</v>
+        <v>152</v>
       </c>
       <c r="B834" s="6" t="s">
-        <v>173</v>
+        <v>153</v>
       </c>
     </row>
     <row r="835" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A835" s="8" t="s">
-        <v>174</v>
+        <v>154</v>
       </c>
       <c r="B835" s="6" t="s">
-        <v>175</v>
+        <v>155</v>
       </c>
     </row>
     <row r="836" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A836" s="8" t="s">
-        <v>176</v>
+        <v>156</v>
       </c>
       <c r="B836" s="6" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="837" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="837" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A837" s="8" t="s">
-        <v>177</v>
+        <v>158</v>
       </c>
       <c r="B837" s="6" t="s">
-        <v>178</v>
+        <v>159</v>
       </c>
     </row>
     <row r="838" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A838" s="8" t="s">
-        <v>179</v>
+        <v>160</v>
       </c>
       <c r="B838" s="6" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="839" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="839" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A839" s="8" t="s">
-        <v>181</v>
+        <v>162</v>
       </c>
       <c r="B839" s="6" t="s">
-        <v>182</v>
+        <v>163</v>
       </c>
     </row>
     <row r="840" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A840" s="8" t="s">
-        <v>183</v>
+        <v>164</v>
       </c>
       <c r="B840" s="6" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="841" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="841" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A841" s="8" t="s">
-        <v>185</v>
+        <v>166</v>
       </c>
       <c r="B841" s="6" t="s">
-        <v>186</v>
+        <v>167</v>
       </c>
     </row>
     <row r="842" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A842" s="8" t="s">
-        <v>187</v>
+        <v>168</v>
       </c>
       <c r="B842" s="6" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="843" spans="1:2" ht="90" x14ac:dyDescent="0.2">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="843" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A843" s="8" t="s">
-        <v>189</v>
+        <v>170</v>
       </c>
       <c r="B843" s="6" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="844" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="844" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A844" s="8" t="s">
-        <v>191</v>
+        <v>172</v>
       </c>
       <c r="B844" s="6" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="845" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="845" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A845" s="8" t="s">
-        <v>193</v>
+        <v>174</v>
       </c>
       <c r="B845" s="6" t="s">
-        <v>194</v>
+        <v>175</v>
       </c>
     </row>
     <row r="846" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A846" s="8" t="s">
-        <v>195</v>
+        <v>176</v>
       </c>
       <c r="B846" s="6" t="s">
-        <v>196</v>
+        <v>151</v>
       </c>
     </row>
     <row r="847" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A847" s="8" t="s">
-        <v>197</v>
+        <v>177</v>
       </c>
       <c r="B847" s="6" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="848" spans="1:2" x14ac:dyDescent="0.2">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="848" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A848" s="8" t="s">
-        <v>199</v>
+        <v>179</v>
       </c>
       <c r="B848" s="6" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="849" spans="1:2" x14ac:dyDescent="0.2">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="849" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A849" s="8" t="s">
-        <v>201</v>
+        <v>181</v>
       </c>
       <c r="B849" s="6" t="s">
-        <v>202</v>
+        <v>182</v>
       </c>
     </row>
     <row r="850" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A850" s="8" t="s">
-        <v>203</v>
+        <v>183</v>
       </c>
       <c r="B850" s="6" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="851" spans="1:2" x14ac:dyDescent="0.2">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="851" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A851" s="8" t="s">
-        <v>204</v>
+        <v>185</v>
       </c>
       <c r="B851" s="6" t="s">
-        <v>205</v>
+        <v>186</v>
       </c>
     </row>
     <row r="852" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A852" s="8" t="s">
-        <v>206</v>
+        <v>187</v>
       </c>
       <c r="B852" s="6" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="853" spans="1:2" x14ac:dyDescent="0.2">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="853" spans="1:2" ht="90" x14ac:dyDescent="0.2">
       <c r="A853" s="8" t="s">
-        <v>208</v>
+        <v>189</v>
       </c>
       <c r="B853" s="6" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="854" spans="1:2" x14ac:dyDescent="0.2">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="854" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A854" s="8" t="s">
-        <v>210</v>
+        <v>191</v>
       </c>
       <c r="B854" s="6" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="855" spans="1:2" x14ac:dyDescent="0.2">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="855" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A855" s="8" t="s">
-        <v>212</v>
+        <v>193</v>
       </c>
       <c r="B855" s="6" t="s">
-        <v>213</v>
+        <v>194</v>
       </c>
     </row>
     <row r="856" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A856" s="8" t="s">
-        <v>214</v>
+        <v>195</v>
       </c>
       <c r="B856" s="6" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="857" spans="1:2" x14ac:dyDescent="0.2">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="857" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A857" s="8" t="s">
-        <v>216</v>
+        <v>197</v>
       </c>
       <c r="B857" s="6" t="s">
-        <v>217</v>
+        <v>198</v>
       </c>
     </row>
     <row r="858" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A858" s="8" t="s">
-        <v>218</v>
+        <v>199</v>
       </c>
       <c r="B858" s="6" t="s">
-        <v>219</v>
+        <v>200</v>
       </c>
     </row>
     <row r="859" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A859" s="8" t="s">
-        <v>220</v>
+        <v>201</v>
       </c>
       <c r="B859" s="6" t="s">
-        <v>221</v>
+        <v>202</v>
       </c>
     </row>
     <row r="860" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A860" s="8" t="s">
-        <v>222</v>
+        <v>203</v>
       </c>
       <c r="B860" s="6" t="s">
-        <v>223</v>
+        <v>153</v>
       </c>
     </row>
     <row r="861" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A861" s="8" t="s">
-        <v>224</v>
+        <v>204</v>
       </c>
       <c r="B861" s="6" t="s">
-        <v>225</v>
+        <v>205</v>
       </c>
     </row>
     <row r="862" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A862" s="8" t="s">
-        <v>226</v>
+        <v>206</v>
       </c>
       <c r="B862" s="6" t="s">
-        <v>227</v>
+        <v>207</v>
       </c>
     </row>
     <row r="863" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A863" s="8" t="s">
-        <v>228</v>
+        <v>208</v>
       </c>
       <c r="B863" s="6" t="s">
-        <v>229</v>
+        <v>209</v>
       </c>
     </row>
     <row r="864" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A864" s="8" t="s">
-        <v>230</v>
+        <v>210</v>
       </c>
       <c r="B864" s="6" t="s">
-        <v>231</v>
+        <v>211</v>
       </c>
     </row>
     <row r="865" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A865" s="8" t="s">
-        <v>232</v>
+        <v>212</v>
       </c>
       <c r="B865" s="6" t="s">
-        <v>233</v>
+        <v>213</v>
       </c>
     </row>
     <row r="866" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A866" s="8" t="s">
-        <v>234</v>
+        <v>214</v>
       </c>
       <c r="B866" s="6" t="s">
-        <v>235</v>
+        <v>215</v>
       </c>
     </row>
     <row r="867" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A867" s="8" t="s">
-        <v>236</v>
+        <v>216</v>
       </c>
       <c r="B867" s="6" t="s">
-        <v>237</v>
+        <v>217</v>
       </c>
     </row>
     <row r="868" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A868" s="8" t="s">
-        <v>238</v>
+        <v>218</v>
       </c>
       <c r="B868" s="6" t="s">
-        <v>239</v>
+        <v>219</v>
       </c>
     </row>
     <row r="869" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A869" s="8" t="s">
-        <v>240</v>
+        <v>220</v>
       </c>
       <c r="B869" s="6" t="s">
-        <v>241</v>
+        <v>221</v>
       </c>
     </row>
     <row r="870" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A870" s="8" t="s">
-        <v>242</v>
+        <v>222</v>
       </c>
       <c r="B870" s="6" t="s">
-        <v>243</v>
+        <v>223</v>
       </c>
     </row>
     <row r="871" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A871" s="8" t="s">
-        <v>244</v>
+        <v>224</v>
       </c>
       <c r="B871" s="6" t="s">
-        <v>245</v>
+        <v>225</v>
       </c>
     </row>
     <row r="872" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A872" s="8" t="s">
-        <v>246</v>
+        <v>226</v>
       </c>
       <c r="B872" s="6" t="s">
-        <v>247</v>
+        <v>227</v>
       </c>
     </row>
     <row r="873" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A873" s="8" t="s">
-        <v>248</v>
+        <v>228</v>
       </c>
       <c r="B873" s="6" t="s">
-        <v>249</v>
+        <v>229</v>
       </c>
     </row>
     <row r="874" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A874" s="8" t="s">
-        <v>250</v>
+        <v>230</v>
       </c>
       <c r="B874" s="6" t="s">
-        <v>251</v>
+        <v>231</v>
       </c>
     </row>
     <row r="875" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A875" s="8" t="s">
-        <v>252</v>
+        <v>232</v>
       </c>
       <c r="B875" s="6" t="s">
-        <v>253</v>
+        <v>233</v>
       </c>
     </row>
     <row r="876" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A876" s="8" t="s">
-        <v>254</v>
+        <v>234</v>
       </c>
       <c r="B876" s="6" t="s">
-        <v>255</v>
+        <v>235</v>
       </c>
     </row>
     <row r="877" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A877" s="8" t="s">
-        <v>256</v>
+        <v>236</v>
       </c>
       <c r="B877" s="6" t="s">
-        <v>257</v>
+        <v>237</v>
       </c>
     </row>
     <row r="878" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A878" s="8" t="s">
-        <v>258</v>
+        <v>238</v>
       </c>
       <c r="B878" s="6" t="s">
-        <v>259</v>
+        <v>239</v>
       </c>
     </row>
     <row r="879" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A879" s="8" t="s">
-        <v>260</v>
+        <v>240</v>
       </c>
       <c r="B879" s="6" t="s">
-        <v>261</v>
+        <v>241</v>
       </c>
     </row>
     <row r="880" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A880" s="8" t="s">
-        <v>262</v>
+        <v>242</v>
       </c>
       <c r="B880" s="6" t="s">
-        <v>263</v>
+        <v>243</v>
       </c>
     </row>
     <row r="881" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A881" s="8" t="s">
-        <v>264</v>
+        <v>244</v>
       </c>
       <c r="B881" s="6" t="s">
-        <v>265</v>
+        <v>245</v>
       </c>
     </row>
     <row r="882" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A882" s="8" t="s">
-        <v>266</v>
+        <v>246</v>
       </c>
       <c r="B882" s="6" t="s">
-        <v>267</v>
+        <v>247</v>
       </c>
     </row>
     <row r="883" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A883" s="8" t="s">
-        <v>268</v>
+        <v>248</v>
       </c>
       <c r="B883" s="6" t="s">
-        <v>269</v>
+        <v>249</v>
       </c>
     </row>
     <row r="884" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A884" s="8" t="s">
-        <v>270</v>
+        <v>250</v>
       </c>
       <c r="B884" s="6" t="s">
-        <v>271</v>
+        <v>251</v>
       </c>
     </row>
     <row r="885" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A885" s="8" t="s">
-        <v>272</v>
+        <v>252</v>
       </c>
       <c r="B885" s="6" t="s">
-        <v>273</v>
+        <v>253</v>
       </c>
     </row>
     <row r="886" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A886" s="8" t="s">
-        <v>274</v>
+        <v>254</v>
       </c>
       <c r="B886" s="6" t="s">
-        <v>275</v>
+        <v>255</v>
       </c>
     </row>
     <row r="887" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A887" s="8" t="s">
-        <v>276</v>
+        <v>256</v>
       </c>
       <c r="B887" s="6" t="s">
-        <v>277</v>
+        <v>257</v>
       </c>
     </row>
     <row r="888" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A888" s="8" t="s">
-        <v>278</v>
+        <v>258</v>
       </c>
       <c r="B888" s="6" t="s">
-        <v>279</v>
+        <v>259</v>
       </c>
     </row>
     <row r="889" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A889" s="8" t="s">
-        <v>280</v>
+        <v>260</v>
       </c>
       <c r="B889" s="6" t="s">
-        <v>281</v>
+        <v>261</v>
       </c>
     </row>
     <row r="890" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A890" s="8" t="s">
-        <v>282</v>
+        <v>262</v>
       </c>
       <c r="B890" s="6" t="s">
-        <v>283</v>
+        <v>263</v>
       </c>
     </row>
     <row r="891" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A891" s="8" t="s">
-        <v>284</v>
+        <v>264</v>
       </c>
       <c r="B891" s="6" t="s">
-        <v>285</v>
+        <v>265</v>
       </c>
     </row>
     <row r="892" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A892" s="8" t="s">
-        <v>286</v>
+        <v>266</v>
       </c>
       <c r="B892" s="6" t="s">
-        <v>287</v>
+        <v>267</v>
       </c>
     </row>
     <row r="893" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A893" s="8" t="s">
-        <v>288</v>
+        <v>268</v>
       </c>
       <c r="B893" s="6" t="s">
-        <v>289</v>
+        <v>269</v>
       </c>
     </row>
     <row r="894" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A894" s="8" t="s">
-        <v>290</v>
+        <v>270</v>
       </c>
       <c r="B894" s="6" t="s">
-        <v>291</v>
+        <v>271</v>
       </c>
     </row>
     <row r="895" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A895" s="8" t="s">
-        <v>292</v>
+        <v>272</v>
       </c>
       <c r="B895" s="6" t="s">
-        <v>293</v>
+        <v>273</v>
       </c>
     </row>
     <row r="896" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A896" s="8" t="s">
-        <v>294</v>
+        <v>274</v>
       </c>
       <c r="B896" s="6" t="s">
-        <v>295</v>
+        <v>275</v>
       </c>
     </row>
     <row r="897" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A897" s="8" t="s">
-        <v>296</v>
+        <v>276</v>
       </c>
       <c r="B897" s="6" t="s">
-        <v>295</v>
+        <v>277</v>
       </c>
     </row>
     <row r="898" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A898" s="8" t="s">
-        <v>297</v>
+        <v>278</v>
       </c>
       <c r="B898" s="6" t="s">
-        <v>298</v>
+        <v>279</v>
       </c>
     </row>
     <row r="899" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A899" s="8" t="s">
-        <v>299</v>
+        <v>280</v>
       </c>
       <c r="B899" s="6" t="s">
-        <v>237</v>
+        <v>281</v>
       </c>
     </row>
     <row r="900" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A900" s="8" t="s">
-        <v>300</v>
+        <v>282</v>
       </c>
       <c r="B900" s="6" t="s">
-        <v>239</v>
+        <v>283</v>
       </c>
     </row>
     <row r="901" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A901" s="8" t="s">
-        <v>301</v>
+        <v>284</v>
       </c>
       <c r="B901" s="6" t="s">
-        <v>302</v>
+        <v>285</v>
       </c>
     </row>
     <row r="902" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A902" s="8" t="s">
-        <v>303</v>
+        <v>286</v>
       </c>
       <c r="B902" s="6" t="s">
-        <v>304</v>
+        <v>287</v>
       </c>
     </row>
     <row r="903" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A903" s="8" t="s">
-        <v>305</v>
+        <v>288</v>
       </c>
       <c r="B903" s="6" t="s">
-        <v>306</v>
+        <v>289</v>
       </c>
     </row>
     <row r="904" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A904" s="8" t="s">
-        <v>307</v>
+        <v>290</v>
       </c>
       <c r="B904" s="6" t="s">
-        <v>308</v>
+        <v>291</v>
       </c>
     </row>
     <row r="905" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A905" s="8" t="s">
-        <v>309</v>
+        <v>292</v>
       </c>
       <c r="B905" s="6" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="906" spans="1:2" ht="22.5" x14ac:dyDescent="0.2">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="906" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A906" s="8" t="s">
-        <v>311</v>
-      </c>
-      <c r="B906" s="9" t="s">
-        <v>312</v>
+        <v>294</v>
+      </c>
+      <c r="B906" s="6" t="s">
+        <v>295</v>
       </c>
     </row>
     <row r="907" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A907" s="8" t="s">
-        <v>313</v>
+        <v>296</v>
       </c>
       <c r="B907" s="6" t="s">
-        <v>314</v>
+        <v>295</v>
       </c>
     </row>
     <row r="908" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A908" s="8" t="s">
-        <v>315</v>
+        <v>297</v>
       </c>
       <c r="B908" s="6" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="909" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="909" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A909" s="8" t="s">
-        <v>317</v>
+        <v>299</v>
       </c>
       <c r="B909" s="6" t="s">
-        <v>318</v>
+        <v>237</v>
       </c>
     </row>
     <row r="910" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A910" s="8" t="s">
-        <v>319</v>
+        <v>300</v>
       </c>
       <c r="B910" s="6" t="s">
-        <v>320</v>
+        <v>239</v>
       </c>
     </row>
     <row r="911" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A911" s="8" t="s">
-        <v>321</v>
+        <v>301</v>
       </c>
       <c r="B911" s="6" t="s">
-        <v>322</v>
+        <v>302</v>
       </c>
     </row>
     <row r="912" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A912" s="8" t="s">
-        <v>323</v>
+        <v>303</v>
       </c>
       <c r="B912" s="6" t="s">
-        <v>324</v>
+        <v>304</v>
       </c>
     </row>
     <row r="913" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A913" s="8" t="s">
-        <v>325</v>
+        <v>305</v>
       </c>
       <c r="B913" s="6" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="914" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="914" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A914" s="8" t="s">
-        <v>327</v>
+        <v>307</v>
       </c>
       <c r="B914" s="6" t="s">
-        <v>328</v>
+        <v>308</v>
       </c>
     </row>
     <row r="915" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A915" s="8" t="s">
-        <v>329</v>
+        <v>309</v>
       </c>
       <c r="B915" s="6" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="916" spans="1:2" x14ac:dyDescent="0.2">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="916" spans="1:2" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A916" s="8" t="s">
-        <v>330</v>
-      </c>
-      <c r="B916" s="6" t="s">
-        <v>331</v>
+        <v>311</v>
+      </c>
+      <c r="B916" s="9" t="s">
+        <v>312</v>
       </c>
     </row>
     <row r="917" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A917" s="8" t="s">
-        <v>332</v>
+        <v>313</v>
       </c>
       <c r="B917" s="6" t="s">
-        <v>333</v>
+        <v>314</v>
       </c>
     </row>
     <row r="918" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A918" s="8" t="s">
-        <v>334</v>
+        <v>315</v>
       </c>
       <c r="B918" s="6" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="919" spans="1:2" x14ac:dyDescent="0.2">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="919" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A919" s="8" t="s">
-        <v>336</v>
+        <v>317</v>
       </c>
       <c r="B919" s="6" t="s">
-        <v>337</v>
+        <v>318</v>
       </c>
     </row>
     <row r="920" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A920" s="8" t="s">
-        <v>338</v>
+        <v>319</v>
       </c>
       <c r="B920" s="6" t="s">
-        <v>339</v>
+        <v>320</v>
       </c>
     </row>
     <row r="921" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A921" s="8" t="s">
-        <v>340</v>
+        <v>321</v>
       </c>
       <c r="B921" s="6" t="s">
-        <v>341</v>
+        <v>322</v>
       </c>
     </row>
     <row r="922" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A922" s="8" t="s">
-        <v>342</v>
+        <v>323</v>
       </c>
       <c r="B922" s="6" t="s">
-        <v>343</v>
+        <v>324</v>
       </c>
     </row>
     <row r="923" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A923" s="8" t="s">
-        <v>344</v>
+        <v>325</v>
       </c>
       <c r="B923" s="6" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="924" spans="1:2" x14ac:dyDescent="0.2">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="924" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A924" s="8" t="s">
-        <v>346</v>
+        <v>327</v>
       </c>
       <c r="B924" s="6" t="s">
-        <v>347</v>
+        <v>328</v>
       </c>
     </row>
     <row r="925" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A925" s="8" t="s">
-        <v>348</v>
+        <v>329</v>
       </c>
       <c r="B925" s="6" t="s">
-        <v>349</v>
+        <v>295</v>
       </c>
     </row>
     <row r="926" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A926" s="8" t="s">
-        <v>350</v>
+        <v>330</v>
       </c>
       <c r="B926" s="6" t="s">
-        <v>351</v>
+        <v>331</v>
       </c>
     </row>
     <row r="927" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A927" s="8" t="s">
-        <v>352</v>
+        <v>332</v>
       </c>
       <c r="B927" s="6" t="s">
-        <v>353</v>
+        <v>333</v>
       </c>
     </row>
     <row r="928" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A928" s="8" t="s">
-        <v>354</v>
+        <v>334</v>
       </c>
       <c r="B928" s="6" t="s">
-        <v>355</v>
+        <v>335</v>
       </c>
     </row>
     <row r="929" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A929" s="8" t="s">
-        <v>356</v>
+        <v>336</v>
       </c>
       <c r="B929" s="6" t="s">
-        <v>357</v>
+        <v>337</v>
       </c>
     </row>
     <row r="930" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A930" s="8" t="s">
-        <v>358</v>
+        <v>338</v>
       </c>
       <c r="B930" s="6" t="s">
-        <v>359</v>
+        <v>339</v>
       </c>
     </row>
     <row r="931" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A931" s="8" t="s">
-        <v>360</v>
+        <v>340</v>
       </c>
       <c r="B931" s="6" t="s">
-        <v>77</v>
+        <v>341</v>
       </c>
     </row>
     <row r="932" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A932" s="8" t="s">
-        <v>361</v>
+        <v>342</v>
       </c>
       <c r="B932" s="6" t="s">
-        <v>362</v>
+        <v>343</v>
       </c>
     </row>
     <row r="933" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A933" s="8" t="s">
-        <v>363</v>
+        <v>344</v>
       </c>
       <c r="B933" s="6" t="s">
-        <v>364</v>
+        <v>345</v>
       </c>
     </row>
     <row r="934" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A934" s="8" t="s">
-        <v>365</v>
+        <v>346</v>
       </c>
       <c r="B934" s="6" t="s">
-        <v>366</v>
+        <v>347</v>
       </c>
     </row>
     <row r="935" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A935" s="8" t="s">
-        <v>367</v>
+        <v>348</v>
       </c>
       <c r="B935" s="6" t="s">
-        <v>368</v>
+        <v>349</v>
       </c>
     </row>
     <row r="936" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A936" s="8" t="s">
-        <v>369</v>
+        <v>350</v>
       </c>
       <c r="B936" s="6" t="s">
-        <v>370</v>
+        <v>351</v>
       </c>
     </row>
     <row r="937" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A937" s="8" t="s">
-        <v>371</v>
+        <v>352</v>
       </c>
       <c r="B937" s="6" t="s">
-        <v>372</v>
+        <v>353</v>
       </c>
     </row>
     <row r="938" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A938" s="8" t="s">
-        <v>373</v>
+        <v>354</v>
       </c>
       <c r="B938" s="6" t="s">
-        <v>77</v>
+        <v>355</v>
       </c>
     </row>
     <row r="939" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A939" s="8" t="s">
-        <v>374</v>
+        <v>356</v>
       </c>
       <c r="B939" s="6" t="s">
-        <v>281</v>
+        <v>357</v>
       </c>
     </row>
     <row r="940" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A940" s="8" t="s">
-        <v>375</v>
+        <v>358</v>
       </c>
       <c r="B940" s="6" t="s">
-        <v>376</v>
+        <v>359</v>
       </c>
     </row>
     <row r="941" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A941" s="8" t="s">
-        <v>377</v>
+        <v>360</v>
       </c>
       <c r="B941" s="6" t="s">
-        <v>378</v>
+        <v>77</v>
       </c>
     </row>
     <row r="942" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A942" s="8" t="s">
-        <v>379</v>
+        <v>361</v>
       </c>
       <c r="B942" s="6" t="s">
-        <v>380</v>
+        <v>362</v>
       </c>
     </row>
     <row r="943" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A943" s="8" t="s">
-        <v>381</v>
+        <v>363</v>
       </c>
       <c r="B943" s="6" t="s">
-        <v>382</v>
+        <v>364</v>
       </c>
     </row>
     <row r="944" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A944" s="8" t="s">
-        <v>383</v>
+        <v>365</v>
       </c>
       <c r="B944" s="6" t="s">
-        <v>384</v>
+        <v>366</v>
       </c>
     </row>
     <row r="945" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A945" s="8" t="s">
-        <v>385</v>
+        <v>367</v>
       </c>
       <c r="B945" s="6" t="s">
-        <v>386</v>
+        <v>368</v>
       </c>
     </row>
     <row r="946" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A946" s="8" t="s">
-        <v>387</v>
+        <v>369</v>
       </c>
       <c r="B946" s="6" t="s">
-        <v>388</v>
+        <v>370</v>
       </c>
     </row>
     <row r="947" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A947" s="8" t="s">
-        <v>389</v>
+        <v>371</v>
       </c>
       <c r="B947" s="6" t="s">
-        <v>175</v>
+        <v>372</v>
       </c>
     </row>
     <row r="948" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A948" s="8" t="s">
-        <v>390</v>
+        <v>373</v>
       </c>
       <c r="B948" s="6" t="s">
-        <v>391</v>
+        <v>77</v>
       </c>
     </row>
     <row r="949" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A949" s="8" t="s">
+        <v>374</v>
+      </c>
+      <c r="B949" s="6" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="950" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A950" s="8" t="s">
+        <v>375</v>
+      </c>
+      <c r="B950" s="6" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="951" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A951" s="8" t="s">
+        <v>377</v>
+      </c>
+      <c r="B951" s="6" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="952" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A952" s="8" t="s">
+        <v>379</v>
+      </c>
+      <c r="B952" s="6" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="953" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A953" s="8" t="s">
+        <v>381</v>
+      </c>
+      <c r="B953" s="6" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="954" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A954" s="8" t="s">
+        <v>383</v>
+      </c>
+      <c r="B954" s="6" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="955" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A955" s="8" t="s">
+        <v>385</v>
+      </c>
+      <c r="B955" s="6" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="956" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A956" s="8" t="s">
+        <v>387</v>
+      </c>
+      <c r="B956" s="6" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="957" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A957" s="8" t="s">
+        <v>389</v>
+      </c>
+      <c r="B957" s="6" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="958" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A958" s="8" t="s">
+        <v>390</v>
+      </c>
+      <c r="B958" s="6" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="959" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A959" s="8" t="s">
         <v>392</v>
       </c>
-      <c r="B949" s="6" t="s">
+      <c r="B959" s="6" t="s">
         <v>393</v>
-      </c>
-    </row>
-    <row r="950" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A950" s="10" t="s">
-        <v>394</v>
-      </c>
-      <c r="B950" s="6" t="s">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="951" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A951" s="10" t="s">
-        <v>396</v>
-      </c>
-      <c r="B951" s="6" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="952" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A952" s="10" t="s">
-        <v>398</v>
-      </c>
-      <c r="B952" s="6" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="953" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A953" s="10" t="s">
-        <v>400</v>
-      </c>
-      <c r="B953" s="6" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="954" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A954" s="10" t="s">
-        <v>402</v>
-      </c>
-      <c r="B954" s="6" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="955" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A955" s="10" t="s">
-        <v>404</v>
-      </c>
-      <c r="B955" s="6" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="956" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A956" s="10" t="s">
-        <v>406</v>
-      </c>
-      <c r="B956" s="6" t="s">
-        <v>407</v>
-      </c>
-    </row>
-    <row r="957" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A957" s="10" t="s">
-        <v>408</v>
-      </c>
-      <c r="B957" s="6" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="958" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A958" s="10" t="s">
-        <v>410</v>
-      </c>
-      <c r="B958" s="6" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="959" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A959" s="10" t="s">
-        <v>411</v>
-      </c>
-      <c r="B959" s="6" t="s">
-        <v>412</v>
       </c>
     </row>
     <row r="960" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A960" s="10" t="s">
-        <v>413</v>
+        <v>394</v>
       </c>
       <c r="B960" s="6" t="s">
-        <v>412</v>
+        <v>395</v>
       </c>
     </row>
     <row r="961" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A961" s="10" t="s">
-        <v>414</v>
+        <v>396</v>
       </c>
       <c r="B961" s="6" t="s">
-        <v>215</v>
+        <v>397</v>
       </c>
     </row>
     <row r="962" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A962" s="10" t="s">
-        <v>415</v>
+        <v>398</v>
       </c>
       <c r="B962" s="6" t="s">
-        <v>217</v>
+        <v>399</v>
       </c>
     </row>
     <row r="963" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A963" s="10" t="s">
-        <v>416</v>
+        <v>400</v>
       </c>
       <c r="B963" s="6" t="s">
         <v>401</v>
@@ -12876,7 +12917,7 @@
     </row>
     <row r="964" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A964" s="10" t="s">
-        <v>417</v>
+        <v>402</v>
       </c>
       <c r="B964" s="6" t="s">
         <v>403</v>
@@ -12884,7 +12925,7 @@
     </row>
     <row r="965" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A965" s="10" t="s">
-        <v>418</v>
+        <v>404</v>
       </c>
       <c r="B965" s="6" t="s">
         <v>405</v>
@@ -12892,7 +12933,7 @@
     </row>
     <row r="966" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A966" s="10" t="s">
-        <v>419</v>
+        <v>406</v>
       </c>
       <c r="B966" s="6" t="s">
         <v>407</v>
@@ -12900,1537 +12941,1617 @@
     </row>
     <row r="967" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A967" s="10" t="s">
-        <v>420</v>
+        <v>408</v>
       </c>
       <c r="B967" s="6" t="s">
-        <v>395</v>
+        <v>409</v>
       </c>
     </row>
     <row r="968" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A968" s="10" t="s">
-        <v>421</v>
+        <v>410</v>
       </c>
       <c r="B968" s="6" t="s">
-        <v>397</v>
+        <v>409</v>
       </c>
     </row>
     <row r="969" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A969" s="10" t="s">
-        <v>422</v>
+        <v>411</v>
       </c>
       <c r="B969" s="6" t="s">
-        <v>399</v>
+        <v>412</v>
       </c>
     </row>
     <row r="970" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A970" s="10" t="s">
-        <v>423</v>
+        <v>413</v>
       </c>
       <c r="B970" s="6" t="s">
-        <v>273</v>
+        <v>412</v>
       </c>
     </row>
     <row r="971" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A971" s="10" t="s">
-        <v>424</v>
+        <v>414</v>
       </c>
       <c r="B971" s="6" t="s">
-        <v>275</v>
+        <v>215</v>
       </c>
     </row>
     <row r="972" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A972" s="10" t="s">
-        <v>425</v>
+        <v>415</v>
       </c>
       <c r="B972" s="6" t="s">
-        <v>320</v>
+        <v>217</v>
       </c>
     </row>
     <row r="973" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A973" s="10" t="s">
-        <v>426</v>
+        <v>416</v>
       </c>
       <c r="B973" s="6" t="s">
-        <v>281</v>
+        <v>401</v>
       </c>
     </row>
     <row r="974" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A974" s="10" t="s">
-        <v>427</v>
+        <v>417</v>
       </c>
       <c r="B974" s="6" t="s">
-        <v>428</v>
+        <v>403</v>
       </c>
     </row>
     <row r="975" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A975" s="10" t="s">
-        <v>429</v>
+        <v>418</v>
       </c>
       <c r="B975" s="6" t="s">
-        <v>295</v>
+        <v>405</v>
       </c>
     </row>
     <row r="976" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A976" s="10" t="s">
-        <v>430</v>
+        <v>419</v>
       </c>
       <c r="B976" s="6" t="s">
-        <v>431</v>
+        <v>407</v>
       </c>
     </row>
     <row r="977" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A977" s="10" t="s">
-        <v>432</v>
+        <v>420</v>
       </c>
       <c r="B977" s="6" t="s">
-        <v>433</v>
+        <v>395</v>
       </c>
     </row>
     <row r="978" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A978" s="10" t="s">
-        <v>434</v>
+        <v>421</v>
       </c>
       <c r="B978" s="6" t="s">
-        <v>435</v>
+        <v>397</v>
       </c>
     </row>
     <row r="979" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A979" s="10" t="s">
-        <v>436</v>
+        <v>422</v>
       </c>
       <c r="B979" s="6" t="s">
-        <v>437</v>
+        <v>399</v>
       </c>
     </row>
     <row r="980" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A980" s="10" t="s">
-        <v>438</v>
+        <v>423</v>
       </c>
       <c r="B980" s="6" t="s">
-        <v>439</v>
+        <v>273</v>
       </c>
     </row>
     <row r="981" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A981" s="10" t="s">
-        <v>440</v>
+        <v>424</v>
       </c>
       <c r="B981" s="6" t="s">
-        <v>441</v>
+        <v>275</v>
       </c>
     </row>
     <row r="982" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A982" s="10" t="s">
-        <v>442</v>
+        <v>425</v>
       </c>
       <c r="B982" s="6" t="s">
-        <v>443</v>
+        <v>320</v>
       </c>
     </row>
     <row r="983" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A983" s="10" t="s">
-        <v>444</v>
+        <v>426</v>
       </c>
       <c r="B983" s="6" t="s">
-        <v>407</v>
+        <v>281</v>
       </c>
     </row>
     <row r="984" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A984" s="10" t="s">
-        <v>445</v>
+        <v>427</v>
       </c>
       <c r="B984" s="6" t="s">
-        <v>446</v>
+        <v>428</v>
       </c>
     </row>
     <row r="985" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A985" s="10" t="s">
-        <v>447</v>
+        <v>429</v>
       </c>
       <c r="B985" s="6" t="s">
-        <v>448</v>
+        <v>295</v>
       </c>
     </row>
     <row r="986" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A986" s="10" t="s">
-        <v>449</v>
+        <v>430</v>
       </c>
       <c r="B986" s="6" t="s">
-        <v>450</v>
+        <v>431</v>
       </c>
     </row>
     <row r="987" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A987" s="10" t="s">
-        <v>451</v>
+        <v>432</v>
       </c>
       <c r="B987" s="6" t="s">
-        <v>452</v>
+        <v>433</v>
       </c>
     </row>
     <row r="988" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A988" s="10" t="s">
-        <v>453</v>
+        <v>434</v>
       </c>
       <c r="B988" s="6" t="s">
-        <v>454</v>
+        <v>435</v>
       </c>
     </row>
     <row r="989" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A989" s="10" t="s">
-        <v>455</v>
+        <v>436</v>
       </c>
       <c r="B989" s="6" t="s">
-        <v>456</v>
+        <v>437</v>
       </c>
     </row>
     <row r="990" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A990" s="10" t="s">
-        <v>457</v>
+        <v>438</v>
       </c>
       <c r="B990" s="6" t="s">
-        <v>458</v>
+        <v>439</v>
       </c>
     </row>
     <row r="991" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A991" s="10" t="s">
-        <v>459</v>
+        <v>440</v>
       </c>
       <c r="B991" s="6" t="s">
-        <v>460</v>
+        <v>441</v>
       </c>
     </row>
     <row r="992" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A992" s="10" t="s">
-        <v>461</v>
+        <v>442</v>
       </c>
       <c r="B992" s="6" t="s">
-        <v>462</v>
+        <v>443</v>
       </c>
     </row>
     <row r="993" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A993" s="10" t="s">
-        <v>463</v>
+        <v>444</v>
       </c>
       <c r="B993" s="6" t="s">
-        <v>464</v>
+        <v>407</v>
       </c>
     </row>
     <row r="994" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A994" s="10" t="s">
-        <v>465</v>
+        <v>445</v>
       </c>
       <c r="B994" s="6" t="s">
-        <v>466</v>
+        <v>446</v>
       </c>
     </row>
     <row r="995" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A995" s="10" t="s">
-        <v>467</v>
+        <v>447</v>
       </c>
       <c r="B995" s="6" t="s">
-        <v>468</v>
+        <v>448</v>
       </c>
     </row>
     <row r="996" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A996" s="10" t="s">
-        <v>469</v>
+        <v>449</v>
       </c>
       <c r="B996" s="6" t="s">
-        <v>470</v>
+        <v>450</v>
       </c>
     </row>
     <row r="997" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A997" s="10" t="s">
-        <v>471</v>
+        <v>451</v>
       </c>
       <c r="B997" s="6" t="s">
-        <v>472</v>
+        <v>452</v>
       </c>
     </row>
     <row r="998" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A998" s="10" t="s">
-        <v>473</v>
+        <v>453</v>
       </c>
       <c r="B998" s="6" t="s">
-        <v>474</v>
+        <v>454</v>
       </c>
     </row>
     <row r="999" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A999" s="10" t="s">
-        <v>475</v>
+        <v>455</v>
       </c>
       <c r="B999" s="6" t="s">
-        <v>476</v>
+        <v>456</v>
       </c>
     </row>
     <row r="1000" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1000" s="10" t="s">
-        <v>477</v>
+        <v>457</v>
       </c>
       <c r="B1000" s="6" t="s">
-        <v>478</v>
+        <v>458</v>
       </c>
     </row>
     <row r="1001" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1001" s="10" t="s">
-        <v>479</v>
+        <v>459</v>
       </c>
       <c r="B1001" s="6" t="s">
-        <v>480</v>
+        <v>460</v>
       </c>
     </row>
     <row r="1002" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1002" s="10" t="s">
-        <v>481</v>
+        <v>461</v>
       </c>
       <c r="B1002" s="6" t="s">
-        <v>482</v>
+        <v>462</v>
       </c>
     </row>
     <row r="1003" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1003" s="10" t="s">
-        <v>483</v>
+        <v>463</v>
       </c>
       <c r="B1003" s="6" t="s">
-        <v>484</v>
+        <v>464</v>
       </c>
     </row>
     <row r="1004" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1004" s="10" t="s">
-        <v>485</v>
+        <v>465</v>
       </c>
       <c r="B1004" s="6" t="s">
-        <v>486</v>
+        <v>466</v>
       </c>
     </row>
     <row r="1005" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1005" s="10" t="s">
-        <v>487</v>
+        <v>467</v>
       </c>
       <c r="B1005" s="6" t="s">
-        <v>488</v>
+        <v>468</v>
       </c>
     </row>
     <row r="1006" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1006" s="10" t="s">
-        <v>489</v>
+        <v>469</v>
       </c>
       <c r="B1006" s="6" t="s">
-        <v>490</v>
+        <v>470</v>
       </c>
     </row>
     <row r="1007" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1007" s="10" t="s">
-        <v>491</v>
+        <v>471</v>
       </c>
       <c r="B1007" s="6" t="s">
-        <v>492</v>
+        <v>472</v>
       </c>
     </row>
     <row r="1008" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1008" s="10" t="s">
-        <v>493</v>
+        <v>473</v>
       </c>
       <c r="B1008" s="6" t="s">
-        <v>494</v>
+        <v>474</v>
       </c>
     </row>
     <row r="1009" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1009" s="10" t="s">
-        <v>495</v>
+        <v>475</v>
       </c>
       <c r="B1009" s="6" t="s">
-        <v>496</v>
+        <v>476</v>
       </c>
     </row>
     <row r="1010" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1010" s="10" t="s">
-        <v>497</v>
+        <v>477</v>
       </c>
       <c r="B1010" s="6" t="s">
-        <v>498</v>
+        <v>478</v>
       </c>
     </row>
     <row r="1011" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1011" s="10" t="s">
-        <v>499</v>
+        <v>479</v>
       </c>
       <c r="B1011" s="6" t="s">
-        <v>500</v>
+        <v>480</v>
       </c>
     </row>
     <row r="1012" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1012" s="10" t="s">
-        <v>501</v>
+        <v>481</v>
       </c>
       <c r="B1012" s="6" t="s">
-        <v>502</v>
+        <v>482</v>
       </c>
     </row>
     <row r="1013" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1013" s="10" t="s">
-        <v>503</v>
+        <v>483</v>
       </c>
       <c r="B1013" s="6" t="s">
-        <v>504</v>
+        <v>484</v>
       </c>
     </row>
     <row r="1014" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1014" s="10" t="s">
-        <v>505</v>
+        <v>485</v>
       </c>
       <c r="B1014" s="6" t="s">
-        <v>506</v>
+        <v>486</v>
       </c>
     </row>
     <row r="1015" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1015" s="10" t="s">
-        <v>507</v>
+        <v>487</v>
       </c>
       <c r="B1015" s="6" t="s">
-        <v>508</v>
+        <v>488</v>
       </c>
     </row>
     <row r="1016" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1016" s="10" t="s">
-        <v>509</v>
+        <v>489</v>
       </c>
       <c r="B1016" s="6" t="s">
-        <v>510</v>
+        <v>490</v>
       </c>
     </row>
     <row r="1017" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1017" s="10" t="s">
-        <v>511</v>
+        <v>491</v>
       </c>
       <c r="B1017" s="6" t="s">
-        <v>512</v>
+        <v>492</v>
       </c>
     </row>
     <row r="1018" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1018" s="10" t="s">
-        <v>513</v>
+        <v>493</v>
       </c>
       <c r="B1018" s="6" t="s">
-        <v>514</v>
+        <v>494</v>
       </c>
     </row>
     <row r="1019" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1019" s="10" t="s">
-        <v>515</v>
+        <v>495</v>
       </c>
       <c r="B1019" s="6" t="s">
-        <v>516</v>
+        <v>496</v>
       </c>
     </row>
     <row r="1020" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1020" s="10" t="s">
-        <v>517</v>
+        <v>497</v>
       </c>
       <c r="B1020" s="6" t="s">
-        <v>518</v>
+        <v>498</v>
       </c>
     </row>
     <row r="1021" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1021" s="10" t="s">
-        <v>519</v>
+        <v>499</v>
       </c>
       <c r="B1021" s="6" t="s">
-        <v>520</v>
+        <v>500</v>
       </c>
     </row>
     <row r="1022" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1022" s="10" t="s">
-        <v>521</v>
+        <v>501</v>
       </c>
       <c r="B1022" s="6" t="s">
-        <v>522</v>
+        <v>502</v>
       </c>
     </row>
     <row r="1023" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1023" s="10" t="s">
-        <v>523</v>
+        <v>503</v>
       </c>
       <c r="B1023" s="6" t="s">
-        <v>524</v>
+        <v>504</v>
       </c>
     </row>
     <row r="1024" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1024" s="10" t="s">
-        <v>525</v>
+        <v>505</v>
       </c>
       <c r="B1024" s="6" t="s">
-        <v>526</v>
+        <v>506</v>
       </c>
     </row>
     <row r="1025" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1025" s="10" t="s">
-        <v>527</v>
+        <v>507</v>
       </c>
       <c r="B1025" s="6" t="s">
-        <v>528</v>
+        <v>508</v>
       </c>
     </row>
     <row r="1026" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1026" s="10" t="s">
-        <v>529</v>
+        <v>509</v>
       </c>
       <c r="B1026" s="6" t="s">
-        <v>530</v>
+        <v>510</v>
       </c>
     </row>
     <row r="1027" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1027" s="10" t="s">
-        <v>531</v>
+        <v>511</v>
       </c>
       <c r="B1027" s="6" t="s">
-        <v>532</v>
+        <v>512</v>
       </c>
     </row>
     <row r="1028" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1028" s="10" t="s">
-        <v>533</v>
+        <v>513</v>
       </c>
       <c r="B1028" s="6" t="s">
-        <v>534</v>
+        <v>514</v>
       </c>
     </row>
     <row r="1029" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1029" s="10" t="s">
-        <v>535</v>
+        <v>515</v>
       </c>
       <c r="B1029" s="6" t="s">
-        <v>536</v>
+        <v>516</v>
       </c>
     </row>
     <row r="1030" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1030" s="10" t="s">
-        <v>537</v>
+        <v>517</v>
       </c>
       <c r="B1030" s="6" t="s">
-        <v>538</v>
+        <v>518</v>
       </c>
     </row>
     <row r="1031" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1031" s="10" t="s">
-        <v>539</v>
+        <v>519</v>
       </c>
       <c r="B1031" s="6" t="s">
-        <v>540</v>
+        <v>520</v>
       </c>
     </row>
     <row r="1032" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1032" s="10" t="s">
-        <v>541</v>
+        <v>521</v>
       </c>
       <c r="B1032" s="6" t="s">
-        <v>542</v>
+        <v>522</v>
       </c>
     </row>
     <row r="1033" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1033" s="10" t="s">
-        <v>543</v>
+        <v>523</v>
       </c>
       <c r="B1033" s="6" t="s">
-        <v>544</v>
+        <v>524</v>
       </c>
     </row>
     <row r="1034" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1034" s="10" t="s">
-        <v>545</v>
+        <v>525</v>
       </c>
       <c r="B1034" s="6" t="s">
-        <v>546</v>
+        <v>526</v>
       </c>
     </row>
     <row r="1035" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1035" s="10" t="s">
-        <v>547</v>
+        <v>527</v>
       </c>
       <c r="B1035" s="6" t="s">
-        <v>548</v>
+        <v>528</v>
       </c>
     </row>
     <row r="1036" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1036" s="10" t="s">
-        <v>549</v>
+        <v>529</v>
       </c>
       <c r="B1036" s="6" t="s">
-        <v>550</v>
+        <v>530</v>
       </c>
     </row>
     <row r="1037" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1037" s="10" t="s">
-        <v>551</v>
+        <v>531</v>
       </c>
       <c r="B1037" s="6" t="s">
-        <v>552</v>
+        <v>532</v>
       </c>
     </row>
     <row r="1038" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1038" s="10" t="s">
-        <v>553</v>
+        <v>533</v>
       </c>
       <c r="B1038" s="6" t="s">
-        <v>554</v>
+        <v>534</v>
       </c>
     </row>
     <row r="1039" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1039" s="10" t="s">
-        <v>555</v>
+        <v>535</v>
       </c>
       <c r="B1039" s="6" t="s">
-        <v>556</v>
+        <v>536</v>
       </c>
     </row>
     <row r="1040" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1040" s="10" t="s">
-        <v>557</v>
+        <v>537</v>
       </c>
       <c r="B1040" s="6" t="s">
-        <v>558</v>
+        <v>538</v>
       </c>
     </row>
     <row r="1041" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1041" s="10" t="s">
-        <v>559</v>
+        <v>539</v>
       </c>
       <c r="B1041" s="6" t="s">
-        <v>560</v>
+        <v>540</v>
       </c>
     </row>
     <row r="1042" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1042" s="10" t="s">
-        <v>561</v>
+        <v>541</v>
       </c>
       <c r="B1042" s="6" t="s">
-        <v>562</v>
+        <v>542</v>
       </c>
     </row>
     <row r="1043" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1043" s="10" t="s">
-        <v>563</v>
+        <v>543</v>
       </c>
       <c r="B1043" s="6" t="s">
-        <v>564</v>
+        <v>544</v>
       </c>
     </row>
     <row r="1044" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1044" s="10" t="s">
-        <v>565</v>
+        <v>545</v>
       </c>
       <c r="B1044" s="6" t="s">
-        <v>566</v>
+        <v>546</v>
       </c>
     </row>
     <row r="1045" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1045" s="10" t="s">
-        <v>567</v>
+        <v>547</v>
       </c>
       <c r="B1045" s="6" t="s">
-        <v>568</v>
+        <v>548</v>
       </c>
     </row>
     <row r="1046" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1046" s="10" t="s">
-        <v>569</v>
+        <v>549</v>
       </c>
       <c r="B1046" s="6" t="s">
-        <v>570</v>
+        <v>550</v>
       </c>
     </row>
     <row r="1047" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1047" s="10" t="s">
-        <v>571</v>
+        <v>551</v>
       </c>
       <c r="B1047" s="6" t="s">
-        <v>572</v>
+        <v>552</v>
       </c>
     </row>
     <row r="1048" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1048" s="10" t="s">
-        <v>573</v>
+        <v>553</v>
       </c>
       <c r="B1048" s="6" t="s">
-        <v>574</v>
+        <v>554</v>
       </c>
     </row>
     <row r="1049" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1049" s="10" t="s">
-        <v>575</v>
+        <v>555</v>
       </c>
       <c r="B1049" s="6" t="s">
-        <v>576</v>
+        <v>556</v>
       </c>
     </row>
     <row r="1050" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1050" s="10" t="s">
-        <v>577</v>
+        <v>557</v>
       </c>
       <c r="B1050" s="6" t="s">
-        <v>578</v>
+        <v>558</v>
       </c>
     </row>
     <row r="1051" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1051" s="10" t="s">
-        <v>579</v>
+        <v>559</v>
       </c>
       <c r="B1051" s="6" t="s">
-        <v>580</v>
+        <v>560</v>
       </c>
     </row>
     <row r="1052" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1052" s="10" t="s">
-        <v>581</v>
+        <v>561</v>
       </c>
       <c r="B1052" s="6" t="s">
-        <v>582</v>
+        <v>562</v>
       </c>
     </row>
     <row r="1053" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1053" s="10" t="s">
-        <v>583</v>
+        <v>563</v>
       </c>
       <c r="B1053" s="6" t="s">
-        <v>584</v>
+        <v>564</v>
       </c>
     </row>
     <row r="1054" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1054" s="10" t="s">
-        <v>585</v>
+        <v>565</v>
       </c>
       <c r="B1054" s="6" t="s">
-        <v>586</v>
+        <v>566</v>
       </c>
     </row>
     <row r="1055" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1055" s="10" t="s">
-        <v>587</v>
+        <v>567</v>
       </c>
       <c r="B1055" s="6" t="s">
-        <v>588</v>
+        <v>568</v>
       </c>
     </row>
     <row r="1056" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1056" s="10" t="s">
-        <v>589</v>
+        <v>569</v>
       </c>
       <c r="B1056" s="6" t="s">
-        <v>590</v>
+        <v>570</v>
       </c>
     </row>
     <row r="1057" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1057" s="10" t="s">
-        <v>591</v>
+        <v>571</v>
       </c>
       <c r="B1057" s="6" t="s">
-        <v>592</v>
+        <v>572</v>
       </c>
     </row>
     <row r="1058" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1058" s="10" t="s">
-        <v>593</v>
+        <v>573</v>
       </c>
       <c r="B1058" s="6" t="s">
-        <v>594</v>
+        <v>574</v>
       </c>
     </row>
     <row r="1059" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1059" s="10" t="s">
-        <v>595</v>
+        <v>575</v>
       </c>
       <c r="B1059" s="6" t="s">
-        <v>596</v>
+        <v>576</v>
       </c>
     </row>
     <row r="1060" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1060" s="10" t="s">
-        <v>597</v>
+        <v>577</v>
       </c>
       <c r="B1060" s="6" t="s">
-        <v>598</v>
+        <v>578</v>
       </c>
     </row>
     <row r="1061" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1061" s="10" t="s">
-        <v>599</v>
+        <v>579</v>
       </c>
       <c r="B1061" s="6" t="s">
-        <v>600</v>
+        <v>580</v>
       </c>
     </row>
     <row r="1062" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1062" s="10" t="s">
-        <v>601</v>
+        <v>581</v>
       </c>
       <c r="B1062" s="6" t="s">
-        <v>602</v>
+        <v>582</v>
       </c>
     </row>
     <row r="1063" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1063" s="10" t="s">
-        <v>603</v>
+        <v>583</v>
       </c>
       <c r="B1063" s="6" t="s">
-        <v>604</v>
+        <v>584</v>
       </c>
     </row>
     <row r="1064" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1064" s="10" t="s">
-        <v>605</v>
+        <v>585</v>
       </c>
       <c r="B1064" s="6" t="s">
-        <v>606</v>
+        <v>586</v>
       </c>
     </row>
     <row r="1065" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1065" s="10" t="s">
-        <v>607</v>
+        <v>587</v>
       </c>
       <c r="B1065" s="6" t="s">
-        <v>608</v>
+        <v>588</v>
       </c>
     </row>
     <row r="1066" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1066" s="10" t="s">
-        <v>609</v>
+        <v>589</v>
       </c>
       <c r="B1066" s="6" t="s">
-        <v>610</v>
+        <v>590</v>
       </c>
     </row>
     <row r="1067" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1067" s="10" t="s">
-        <v>611</v>
+        <v>591</v>
       </c>
       <c r="B1067" s="6" t="s">
-        <v>612</v>
+        <v>592</v>
       </c>
     </row>
     <row r="1068" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1068" s="10" t="s">
-        <v>613</v>
+        <v>593</v>
       </c>
       <c r="B1068" s="6" t="s">
-        <v>614</v>
+        <v>594</v>
       </c>
     </row>
     <row r="1069" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1069" s="10" t="s">
-        <v>615</v>
+        <v>595</v>
       </c>
       <c r="B1069" s="6" t="s">
-        <v>616</v>
+        <v>596</v>
       </c>
     </row>
     <row r="1070" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1070" s="10" t="s">
-        <v>617</v>
+        <v>597</v>
       </c>
       <c r="B1070" s="6" t="s">
-        <v>618</v>
+        <v>598</v>
       </c>
     </row>
     <row r="1071" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1071" s="10" t="s">
-        <v>619</v>
+        <v>599</v>
       </c>
       <c r="B1071" s="6" t="s">
-        <v>620</v>
+        <v>600</v>
       </c>
     </row>
     <row r="1072" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1072" s="10" t="s">
-        <v>621</v>
+        <v>601</v>
       </c>
       <c r="B1072" s="6" t="s">
-        <v>622</v>
+        <v>602</v>
       </c>
     </row>
     <row r="1073" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1073" s="10" t="s">
-        <v>623</v>
+        <v>603</v>
       </c>
       <c r="B1073" s="6" t="s">
-        <v>624</v>
+        <v>604</v>
       </c>
     </row>
     <row r="1074" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1074" s="10" t="s">
-        <v>625</v>
+        <v>605</v>
       </c>
       <c r="B1074" s="6" t="s">
-        <v>626</v>
+        <v>606</v>
       </c>
     </row>
     <row r="1075" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1075" s="10" t="s">
-        <v>627</v>
+        <v>607</v>
       </c>
       <c r="B1075" s="6" t="s">
-        <v>628</v>
+        <v>608</v>
       </c>
     </row>
     <row r="1076" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1076" s="10" t="s">
-        <v>629</v>
+        <v>609</v>
       </c>
       <c r="B1076" s="6" t="s">
-        <v>630</v>
+        <v>610</v>
       </c>
     </row>
     <row r="1077" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1077" s="10" t="s">
-        <v>631</v>
+        <v>611</v>
       </c>
       <c r="B1077" s="6" t="s">
-        <v>632</v>
+        <v>612</v>
       </c>
     </row>
     <row r="1078" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1078" s="10" t="s">
-        <v>633</v>
+        <v>613</v>
       </c>
       <c r="B1078" s="6" t="s">
-        <v>634</v>
+        <v>614</v>
       </c>
     </row>
     <row r="1079" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1079" s="10" t="s">
-        <v>635</v>
+        <v>615</v>
       </c>
       <c r="B1079" s="6" t="s">
-        <v>636</v>
+        <v>616</v>
       </c>
     </row>
     <row r="1080" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1080" s="10" t="s">
-        <v>637</v>
+        <v>617</v>
       </c>
       <c r="B1080" s="6" t="s">
-        <v>638</v>
+        <v>618</v>
       </c>
     </row>
     <row r="1081" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1081" s="10" t="s">
-        <v>639</v>
+        <v>619</v>
       </c>
       <c r="B1081" s="6" t="s">
-        <v>640</v>
+        <v>620</v>
       </c>
     </row>
     <row r="1082" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1082" s="10" t="s">
-        <v>641</v>
+        <v>621</v>
       </c>
       <c r="B1082" s="6" t="s">
-        <v>642</v>
+        <v>622</v>
       </c>
     </row>
     <row r="1083" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1083" s="10" t="s">
-        <v>643</v>
+        <v>623</v>
       </c>
       <c r="B1083" s="6" t="s">
-        <v>644</v>
+        <v>624</v>
       </c>
     </row>
     <row r="1084" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1084" s="10" t="s">
-        <v>645</v>
+        <v>625</v>
       </c>
       <c r="B1084" s="6" t="s">
-        <v>646</v>
+        <v>626</v>
       </c>
     </row>
     <row r="1085" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1085" s="10" t="s">
-        <v>647</v>
+        <v>627</v>
       </c>
       <c r="B1085" s="6" t="s">
-        <v>648</v>
+        <v>628</v>
       </c>
     </row>
     <row r="1086" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1086" s="10" t="s">
-        <v>649</v>
+        <v>629</v>
       </c>
       <c r="B1086" s="6" t="s">
-        <v>650</v>
+        <v>630</v>
       </c>
     </row>
     <row r="1087" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1087" s="10" t="s">
-        <v>651</v>
+        <v>631</v>
       </c>
       <c r="B1087" s="6" t="s">
-        <v>652</v>
+        <v>632</v>
       </c>
     </row>
     <row r="1088" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1088" s="10" t="s">
-        <v>653</v>
+        <v>633</v>
       </c>
       <c r="B1088" s="6" t="s">
-        <v>654</v>
+        <v>634</v>
       </c>
     </row>
     <row r="1089" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1089" s="10" t="s">
-        <v>655</v>
+        <v>635</v>
       </c>
       <c r="B1089" s="6" t="s">
-        <v>656</v>
+        <v>636</v>
       </c>
     </row>
     <row r="1090" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1090" s="10" t="s">
-        <v>657</v>
+        <v>637</v>
       </c>
       <c r="B1090" s="6" t="s">
-        <v>658</v>
+        <v>638</v>
       </c>
     </row>
     <row r="1091" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1091" s="10" t="s">
-        <v>659</v>
+        <v>639</v>
       </c>
       <c r="B1091" s="6" t="s">
-        <v>660</v>
+        <v>640</v>
       </c>
     </row>
     <row r="1092" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1092" s="10" t="s">
-        <v>661</v>
+        <v>641</v>
       </c>
       <c r="B1092" s="6" t="s">
-        <v>662</v>
+        <v>642</v>
       </c>
     </row>
     <row r="1093" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1093" s="10" t="s">
-        <v>663</v>
+        <v>643</v>
       </c>
       <c r="B1093" s="6" t="s">
-        <v>664</v>
+        <v>644</v>
       </c>
     </row>
     <row r="1094" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1094" s="10" t="s">
-        <v>665</v>
+        <v>645</v>
       </c>
       <c r="B1094" s="6" t="s">
-        <v>666</v>
+        <v>646</v>
       </c>
     </row>
     <row r="1095" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1095" s="10" t="s">
-        <v>667</v>
+        <v>647</v>
       </c>
       <c r="B1095" s="6" t="s">
-        <v>668</v>
+        <v>648</v>
       </c>
     </row>
     <row r="1096" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1096" s="10" t="s">
-        <v>669</v>
+        <v>649</v>
       </c>
       <c r="B1096" s="6" t="s">
-        <v>670</v>
+        <v>650</v>
       </c>
     </row>
     <row r="1097" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1097" s="10" t="s">
-        <v>671</v>
+        <v>651</v>
       </c>
       <c r="B1097" s="6" t="s">
-        <v>672</v>
+        <v>652</v>
       </c>
     </row>
     <row r="1098" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1098" s="10" t="s">
-        <v>673</v>
+        <v>653</v>
       </c>
       <c r="B1098" s="6" t="s">
-        <v>674</v>
+        <v>654</v>
       </c>
     </row>
     <row r="1099" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1099" s="10" t="s">
-        <v>675</v>
+        <v>655</v>
       </c>
       <c r="B1099" s="6" t="s">
-        <v>676</v>
+        <v>656</v>
       </c>
     </row>
     <row r="1100" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1100" s="10" t="s">
-        <v>677</v>
+        <v>657</v>
       </c>
       <c r="B1100" s="6" t="s">
-        <v>678</v>
+        <v>658</v>
       </c>
     </row>
     <row r="1101" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1101" s="10" t="s">
-        <v>679</v>
+        <v>659</v>
       </c>
       <c r="B1101" s="6" t="s">
-        <v>680</v>
+        <v>660</v>
       </c>
     </row>
     <row r="1102" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1102" s="10" t="s">
-        <v>681</v>
+        <v>661</v>
       </c>
       <c r="B1102" s="6" t="s">
-        <v>682</v>
+        <v>662</v>
       </c>
     </row>
     <row r="1103" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1103" s="10" t="s">
-        <v>683</v>
+        <v>663</v>
       </c>
       <c r="B1103" s="6" t="s">
-        <v>684</v>
+        <v>664</v>
       </c>
     </row>
     <row r="1104" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1104" s="10" t="s">
-        <v>685</v>
+        <v>665</v>
       </c>
       <c r="B1104" s="6" t="s">
-        <v>686</v>
+        <v>666</v>
       </c>
     </row>
     <row r="1105" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1105" s="10" t="s">
-        <v>687</v>
+        <v>667</v>
       </c>
       <c r="B1105" s="6" t="s">
-        <v>688</v>
+        <v>668</v>
       </c>
     </row>
     <row r="1106" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1106" s="10" t="s">
-        <v>689</v>
+        <v>669</v>
       </c>
       <c r="B1106" s="6" t="s">
-        <v>690</v>
+        <v>670</v>
       </c>
     </row>
     <row r="1107" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1107" s="10" t="s">
-        <v>691</v>
+        <v>671</v>
       </c>
       <c r="B1107" s="6" t="s">
-        <v>692</v>
+        <v>672</v>
       </c>
     </row>
     <row r="1108" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1108" s="10" t="s">
-        <v>693</v>
+        <v>673</v>
       </c>
       <c r="B1108" s="6" t="s">
-        <v>694</v>
+        <v>674</v>
       </c>
     </row>
     <row r="1109" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1109" s="10" t="s">
-        <v>695</v>
+        <v>675</v>
       </c>
       <c r="B1109" s="6" t="s">
-        <v>696</v>
+        <v>676</v>
       </c>
     </row>
     <row r="1110" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1110" s="10" t="s">
-        <v>697</v>
+        <v>677</v>
       </c>
       <c r="B1110" s="6" t="s">
-        <v>698</v>
+        <v>678</v>
       </c>
     </row>
     <row r="1111" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1111" s="10" t="s">
-        <v>699</v>
+        <v>679</v>
       </c>
       <c r="B1111" s="6" t="s">
-        <v>700</v>
+        <v>680</v>
       </c>
     </row>
     <row r="1112" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1112" s="10" t="s">
-        <v>701</v>
+        <v>681</v>
       </c>
       <c r="B1112" s="6" t="s">
-        <v>702</v>
+        <v>682</v>
       </c>
     </row>
     <row r="1113" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1113" s="10" t="s">
-        <v>703</v>
+        <v>683</v>
       </c>
       <c r="B1113" s="6" t="s">
-        <v>704</v>
+        <v>684</v>
       </c>
     </row>
     <row r="1114" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1114" s="10" t="s">
-        <v>705</v>
+        <v>685</v>
       </c>
       <c r="B1114" s="6" t="s">
-        <v>706</v>
+        <v>686</v>
       </c>
     </row>
     <row r="1115" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1115" s="10" t="s">
-        <v>707</v>
+        <v>687</v>
       </c>
       <c r="B1115" s="6" t="s">
-        <v>708</v>
+        <v>688</v>
       </c>
     </row>
     <row r="1116" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1116" s="10" t="s">
-        <v>709</v>
+        <v>689</v>
       </c>
       <c r="B1116" s="6" t="s">
-        <v>710</v>
+        <v>690</v>
       </c>
     </row>
     <row r="1117" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1117" s="10" t="s">
-        <v>711</v>
+        <v>691</v>
       </c>
       <c r="B1117" s="6" t="s">
-        <v>712</v>
+        <v>692</v>
       </c>
     </row>
     <row r="1118" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1118" s="10" t="s">
-        <v>713</v>
+        <v>693</v>
       </c>
       <c r="B1118" s="6" t="s">
-        <v>714</v>
+        <v>694</v>
       </c>
     </row>
     <row r="1119" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1119" s="10" t="s">
-        <v>715</v>
+        <v>695</v>
       </c>
       <c r="B1119" s="6" t="s">
-        <v>716</v>
+        <v>696</v>
       </c>
     </row>
     <row r="1120" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1120" s="10" t="s">
-        <v>717</v>
+        <v>697</v>
       </c>
       <c r="B1120" s="6" t="s">
-        <v>718</v>
+        <v>698</v>
       </c>
     </row>
     <row r="1121" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1121" s="10" t="s">
-        <v>719</v>
+        <v>699</v>
       </c>
       <c r="B1121" s="6" t="s">
-        <v>720</v>
+        <v>700</v>
       </c>
     </row>
     <row r="1122" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1122" s="10" t="s">
-        <v>721</v>
+        <v>701</v>
       </c>
       <c r="B1122" s="6" t="s">
-        <v>722</v>
+        <v>702</v>
       </c>
     </row>
     <row r="1123" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1123" s="10" t="s">
-        <v>723</v>
+        <v>703</v>
       </c>
       <c r="B1123" s="6" t="s">
-        <v>724</v>
+        <v>704</v>
       </c>
     </row>
     <row r="1124" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1124" s="10" t="s">
-        <v>725</v>
+        <v>705</v>
       </c>
       <c r="B1124" s="6" t="s">
-        <v>726</v>
+        <v>706</v>
       </c>
     </row>
     <row r="1125" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1125" s="10" t="s">
-        <v>727</v>
+        <v>707</v>
       </c>
       <c r="B1125" s="6" t="s">
-        <v>728</v>
+        <v>708</v>
       </c>
     </row>
     <row r="1126" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1126" s="10" t="s">
-        <v>729</v>
+        <v>709</v>
       </c>
       <c r="B1126" s="6" t="s">
-        <v>730</v>
+        <v>710</v>
       </c>
     </row>
     <row r="1127" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1127" s="10" t="s">
-        <v>731</v>
+        <v>711</v>
       </c>
       <c r="B1127" s="6" t="s">
-        <v>732</v>
+        <v>712</v>
       </c>
     </row>
     <row r="1128" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1128" s="10" t="s">
-        <v>733</v>
+        <v>713</v>
       </c>
       <c r="B1128" s="6" t="s">
-        <v>734</v>
+        <v>714</v>
       </c>
     </row>
     <row r="1129" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1129" s="10" t="s">
-        <v>735</v>
+        <v>715</v>
       </c>
       <c r="B1129" s="6" t="s">
-        <v>736</v>
+        <v>716</v>
       </c>
     </row>
     <row r="1130" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1130" s="10" t="s">
-        <v>737</v>
+        <v>717</v>
       </c>
       <c r="B1130" s="6" t="s">
-        <v>738</v>
+        <v>718</v>
       </c>
     </row>
     <row r="1131" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1131" s="10" t="s">
-        <v>739</v>
+        <v>719</v>
       </c>
       <c r="B1131" s="6" t="s">
-        <v>740</v>
+        <v>720</v>
       </c>
     </row>
     <row r="1132" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1132" s="10" t="s">
-        <v>741</v>
+        <v>721</v>
       </c>
       <c r="B1132" s="6" t="s">
-        <v>742</v>
+        <v>722</v>
       </c>
     </row>
     <row r="1133" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1133" s="10" t="s">
-        <v>743</v>
+        <v>723</v>
       </c>
       <c r="B1133" s="6" t="s">
-        <v>744</v>
+        <v>724</v>
       </c>
     </row>
     <row r="1134" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1134" s="10" t="s">
-        <v>745</v>
+        <v>725</v>
       </c>
       <c r="B1134" s="6" t="s">
-        <v>746</v>
+        <v>726</v>
       </c>
     </row>
     <row r="1135" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1135" s="10" t="s">
-        <v>747</v>
+        <v>727</v>
       </c>
       <c r="B1135" s="6" t="s">
-        <v>748</v>
+        <v>728</v>
       </c>
     </row>
     <row r="1136" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1136" s="10" t="s">
-        <v>749</v>
+        <v>729</v>
       </c>
       <c r="B1136" s="6" t="s">
-        <v>750</v>
+        <v>730</v>
       </c>
     </row>
     <row r="1137" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1137" s="10" t="s">
-        <v>751</v>
+        <v>731</v>
       </c>
       <c r="B1137" s="6" t="s">
-        <v>752</v>
+        <v>732</v>
       </c>
     </row>
     <row r="1138" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1138" s="10" t="s">
-        <v>753</v>
+        <v>733</v>
       </c>
       <c r="B1138" s="6" t="s">
-        <v>754</v>
+        <v>734</v>
       </c>
     </row>
     <row r="1139" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1139" s="10" t="s">
-        <v>755</v>
+        <v>735</v>
       </c>
       <c r="B1139" s="6" t="s">
-        <v>756</v>
+        <v>736</v>
       </c>
     </row>
     <row r="1140" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1140" s="10" t="s">
-        <v>757</v>
+        <v>737</v>
       </c>
       <c r="B1140" s="6" t="s">
-        <v>758</v>
+        <v>738</v>
       </c>
     </row>
     <row r="1141" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1141" s="10" t="s">
-        <v>759</v>
+        <v>739</v>
       </c>
       <c r="B1141" s="6" t="s">
-        <v>760</v>
+        <v>740</v>
       </c>
     </row>
     <row r="1142" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1142" s="10" t="s">
-        <v>761</v>
+        <v>741</v>
       </c>
       <c r="B1142" s="6" t="s">
-        <v>762</v>
+        <v>742</v>
       </c>
     </row>
     <row r="1143" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1143" s="10" t="s">
-        <v>763</v>
+        <v>743</v>
       </c>
       <c r="B1143" s="6" t="s">
-        <v>764</v>
+        <v>744</v>
       </c>
     </row>
     <row r="1144" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1144" s="10" t="s">
-        <v>765</v>
+        <v>745</v>
       </c>
       <c r="B1144" s="6" t="s">
-        <v>766</v>
+        <v>746</v>
       </c>
     </row>
     <row r="1145" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1145" s="10" t="s">
-        <v>767</v>
+        <v>747</v>
       </c>
       <c r="B1145" s="6" t="s">
-        <v>304</v>
+        <v>748</v>
       </c>
     </row>
     <row r="1146" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1146" s="10" t="s">
-        <v>768</v>
+        <v>749</v>
       </c>
       <c r="B1146" s="6" t="s">
-        <v>769</v>
+        <v>750</v>
       </c>
     </row>
     <row r="1147" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1147" s="10" t="s">
-        <v>770</v>
+        <v>751</v>
       </c>
       <c r="B1147" s="6" t="s">
-        <v>316</v>
+        <v>752</v>
       </c>
     </row>
     <row r="1148" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1148" s="10" t="s">
-        <v>771</v>
+        <v>753</v>
       </c>
       <c r="B1148" s="6" t="s">
-        <v>211</v>
+        <v>754</v>
       </c>
     </row>
     <row r="1149" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1149" s="10" t="s">
-        <v>772</v>
+        <v>755</v>
       </c>
       <c r="B1149" s="6" t="s">
-        <v>213</v>
+        <v>756</v>
       </c>
     </row>
     <row r="1150" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1150" s="10" t="s">
-        <v>773</v>
+        <v>757</v>
       </c>
       <c r="B1150" s="6" t="s">
-        <v>774</v>
-      </c>
-    </row>
-    <row r="1151" spans="1:2" ht="22.5" x14ac:dyDescent="0.2">
+        <v>758</v>
+      </c>
+    </row>
+    <row r="1151" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1151" s="10" t="s">
-        <v>775</v>
-      </c>
-      <c r="B1151" s="9" t="s">
-        <v>312</v>
+        <v>759</v>
+      </c>
+      <c r="B1151" s="6" t="s">
+        <v>760</v>
       </c>
     </row>
     <row r="1152" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1152" s="10" t="s">
-        <v>776</v>
+        <v>761</v>
       </c>
       <c r="B1152" s="6" t="s">
-        <v>777</v>
+        <v>762</v>
       </c>
     </row>
     <row r="1153" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1153" s="10" t="s">
-        <v>778</v>
+        <v>763</v>
       </c>
       <c r="B1153" s="6" t="s">
-        <v>308</v>
+        <v>764</v>
       </c>
     </row>
     <row r="1154" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1154" s="10" t="s">
-        <v>779</v>
+        <v>765</v>
       </c>
       <c r="B1154" s="6" t="s">
-        <v>780</v>
+        <v>766</v>
       </c>
     </row>
     <row r="1155" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1155" s="10" t="s">
-        <v>781</v>
+        <v>767</v>
       </c>
       <c r="B1155" s="6" t="s">
-        <v>782</v>
+        <v>304</v>
       </c>
     </row>
     <row r="1156" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1156" s="10" t="s">
-        <v>783</v>
+        <v>768</v>
       </c>
       <c r="B1156" s="6" t="s">
-        <v>784</v>
+        <v>769</v>
       </c>
     </row>
     <row r="1157" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1157" s="10" t="s">
+        <v>770</v>
+      </c>
+      <c r="B1157" s="6" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="1158" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1158" s="10" t="s">
+        <v>771</v>
+      </c>
+      <c r="B1158" s="6" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="1159" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1159" s="10" t="s">
+        <v>772</v>
+      </c>
+      <c r="B1159" s="6" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="1160" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1160" s="10" t="s">
+        <v>773</v>
+      </c>
+      <c r="B1160" s="6" t="s">
+        <v>774</v>
+      </c>
+    </row>
+    <row r="1161" spans="1:2" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A1161" s="10" t="s">
+        <v>775</v>
+      </c>
+      <c r="B1161" s="9" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="1162" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1162" s="10" t="s">
+        <v>776</v>
+      </c>
+      <c r="B1162" s="6" t="s">
+        <v>777</v>
+      </c>
+    </row>
+    <row r="1163" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1163" s="10" t="s">
+        <v>778</v>
+      </c>
+      <c r="B1163" s="6" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="1164" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1164" s="10" t="s">
+        <v>779</v>
+      </c>
+      <c r="B1164" s="6" t="s">
+        <v>780</v>
+      </c>
+    </row>
+    <row r="1165" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1165" s="10" t="s">
+        <v>781</v>
+      </c>
+      <c r="B1165" s="6" t="s">
+        <v>782</v>
+      </c>
+    </row>
+    <row r="1166" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1166" s="10" t="s">
+        <v>783</v>
+      </c>
+      <c r="B1166" s="6" t="s">
+        <v>784</v>
+      </c>
+    </row>
+    <row r="1167" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1167" s="10" t="s">
         <v>785</v>
       </c>
-      <c r="B1157" s="6" t="s">
+      <c r="B1167" s="6" t="s">
         <v>786</v>
       </c>
     </row>
-    <row r="1158" spans="1:2" ht="22.5" x14ac:dyDescent="0.2">
-      <c r="A1158" s="10" t="s">
+    <row r="1168" spans="1:2" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A1168" s="10" t="s">
         <v>787</v>
       </c>
-      <c r="B1158" s="6" t="s">
+      <c r="B1168" s="6" t="s">
         <v>788</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add 'Legacy of Sundown'
Full set of a light armor of elven craft for rogues made in a gold-orange-olive coloring with a marching set of two daggers two swords and a bow.
I have modified the stats to fit better into the power curve of my game.

These have been placed into the chest in the West Brecilian forest that appears if you defeat the Greater Shade at the ensorcelled camp.

see #384
</commit_message>
<xml_diff>
--- a/source/tlk/strings.xlsx
+++ b/source/tlk/strings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\DAO\archid\source\tlk\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7731DB2E-48CF-405E-B4A6-8CF047A13BB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DC1BC48-7B48-47B5-8EFB-9DD8F2557F77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29190" yWindow="390" windowWidth="26610" windowHeight="16110" xr2:uid="{A42EE72D-E1C4-43B6-AEA5-0014ED5180B1}"/>
+    <workbookView xWindow="2355" yWindow="360" windowWidth="26610" windowHeight="16110" xr2:uid="{A42EE72D-E1C4-43B6-AEA5-0014ED5180B1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -295,7 +295,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A833" authorId="0" shapeId="0" xr:uid="{15B7CDC5-6F21-45A0-9997-3CC9AFCCF646}">
+    <comment ref="A847" authorId="0" shapeId="0" xr:uid="{15B7CDC5-6F21-45A0-9997-3CC9AFCCF646}">
       <text>
         <r>
           <rPr>
@@ -309,7 +309,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A960" authorId="0" shapeId="0" xr:uid="{08441945-669A-47E4-A77A-BA32248BBBE4}">
+    <comment ref="A974" authorId="0" shapeId="0" xr:uid="{08441945-669A-47E4-A77A-BA32248BBBE4}">
       <text>
         <r>
           <rPr>
@@ -342,7 +342,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1505" uniqueCount="1448">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1519" uniqueCount="1462">
   <si>
     <t>af_archid_en-us.tlk</t>
   </si>
@@ -4750,14 +4750,63 @@
   <si>
     <t>This ornate stave looks newly done but feel like a truly ancient item. Two black dragons are holding a ball of clear blue color. If you look at it long enough you will see the summer night sky that full of stars.</t>
   </si>
+  <si>
+    <t>Sundown Boots</t>
+  </si>
+  <si>
+    <t>These boots, from the sundown hunter ranger equipment, are crafted from some form of extremely tough, but flexible, leatherand enscribed with feather designs and patterns. On inspection they appear to be bright in colour but when worn they seem to deflect the eye.</t>
+  </si>
+  <si>
+    <t>Sundown Chestpiece</t>
+  </si>
+  <si>
+    <t>This chest armour, from the sundown hunter ranger equipment, is crafted from some form of extremely tough, but flexible, leather and enscribed with feather designs and patterns.</t>
+  </si>
+  <si>
+    <t>Sundown Gloves</t>
+  </si>
+  <si>
+    <t>These gloves, like the rest of the sundown hunter ranger equipment, is crafted from some form of extremely tough, but flexible, leather and enscribed with feather designs and patterns.</t>
+  </si>
+  <si>
+    <t>Sundown Helmet</t>
+  </si>
+  <si>
+    <t>This helmet, like the rest of the sundown hunter ranger equipment, is crafted from some form of extremely tough, but flexible, leather and enscribed with feather designs and patterns.</t>
+  </si>
+  <si>
+    <t>Sundown Longbow</t>
+  </si>
+  <si>
+    <t>This elegant bow of elven craft seems not to have been shaped out of wood, instead it looks to have been grown into the shape somehow. It is decorated with gems, gold and strips of wonderfully manufactured leather.</t>
+  </si>
+  <si>
+    <t>Sunrise</t>
+  </si>
+  <si>
+    <t>Sunset</t>
+  </si>
+  <si>
+    <t>Daybreak</t>
+  </si>
+  <si>
+    <t>Nightfall</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -4856,29 +4905,31 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="3" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="2" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -5198,10 +5249,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C8288F5-46B5-435A-B9FC-40522281A8A6}">
-  <dimension ref="A1:B1168"/>
+  <dimension ref="A1:B1182"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A785" workbookViewId="0">
-      <selection activeCell="B826" sqref="B826"/>
+    <sheetView tabSelected="1" topLeftCell="A815" workbookViewId="0">
+      <selection activeCell="B851" sqref="B851"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -11867,2691 +11918,2803 @@
         <v>1447</v>
       </c>
     </row>
-    <row r="833" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A833" s="8" t="s">
+    <row r="833" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A833" s="13">
+        <v>6610831</v>
+      </c>
+      <c r="B833" s="14" t="s">
+        <v>1448</v>
+      </c>
+    </row>
+    <row r="834" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A834" s="13">
+        <v>6610832</v>
+      </c>
+      <c r="B834" s="14" t="s">
+        <v>1449</v>
+      </c>
+    </row>
+    <row r="835" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A835" s="13">
+        <v>6610833</v>
+      </c>
+      <c r="B835" s="14" t="s">
+        <v>1450</v>
+      </c>
+    </row>
+    <row r="836" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A836" s="13">
+        <v>6610834</v>
+      </c>
+      <c r="B836" s="14" t="s">
+        <v>1451</v>
+      </c>
+    </row>
+    <row r="837" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A837" s="13">
+        <v>6610835</v>
+      </c>
+      <c r="B837" s="14" t="s">
+        <v>1452</v>
+      </c>
+    </row>
+    <row r="838" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A838" s="13">
+        <v>6610836</v>
+      </c>
+      <c r="B838" s="14" t="s">
+        <v>1453</v>
+      </c>
+    </row>
+    <row r="839" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A839" s="13">
+        <v>6610837</v>
+      </c>
+      <c r="B839" s="14" t="s">
+        <v>1454</v>
+      </c>
+    </row>
+    <row r="840" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A840" s="13">
+        <v>6610838</v>
+      </c>
+      <c r="B840" s="14" t="s">
+        <v>1455</v>
+      </c>
+    </row>
+    <row r="841" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A841" s="13">
+        <v>6610839</v>
+      </c>
+      <c r="B841" s="14" t="s">
+        <v>1456</v>
+      </c>
+    </row>
+    <row r="842" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A842" s="13">
+        <v>6610840</v>
+      </c>
+      <c r="B842" s="14" t="s">
+        <v>1457</v>
+      </c>
+    </row>
+    <row r="843" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A843" s="13">
+        <v>6610841</v>
+      </c>
+      <c r="B843" s="14" t="s">
+        <v>1458</v>
+      </c>
+    </row>
+    <row r="844" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A844" s="13">
+        <v>6610842</v>
+      </c>
+      <c r="B844" s="14" t="s">
+        <v>1459</v>
+      </c>
+    </row>
+    <row r="845" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A845" s="13">
+        <v>6610843</v>
+      </c>
+      <c r="B845" s="14" t="s">
+        <v>1460</v>
+      </c>
+    </row>
+    <row r="846" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A846" s="13">
+        <v>6610844</v>
+      </c>
+      <c r="B846" s="14" t="s">
+        <v>1461</v>
+      </c>
+    </row>
+    <row r="847" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A847" s="8" t="s">
         <v>150</v>
       </c>
-      <c r="B833" s="6" t="s">
+      <c r="B847" s="6" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="834" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A834" s="8" t="s">
+    <row r="848" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A848" s="8" t="s">
         <v>152</v>
       </c>
-      <c r="B834" s="6" t="s">
+      <c r="B848" s="6" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="835" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A835" s="8" t="s">
+    <row r="849" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A849" s="8" t="s">
         <v>154</v>
       </c>
-      <c r="B835" s="6" t="s">
+      <c r="B849" s="6" t="s">
         <v>155</v>
-      </c>
-    </row>
-    <row r="836" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A836" s="8" t="s">
-        <v>156</v>
-      </c>
-      <c r="B836" s="6" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="837" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A837" s="8" t="s">
-        <v>158</v>
-      </c>
-      <c r="B837" s="6" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="838" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
-      <c r="A838" s="8" t="s">
-        <v>160</v>
-      </c>
-      <c r="B838" s="6" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="839" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A839" s="8" t="s">
-        <v>162</v>
-      </c>
-      <c r="B839" s="6" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="840" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A840" s="8" t="s">
-        <v>164</v>
-      </c>
-      <c r="B840" s="6" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="841" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A841" s="8" t="s">
-        <v>166</v>
-      </c>
-      <c r="B841" s="6" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="842" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A842" s="8" t="s">
-        <v>168</v>
-      </c>
-      <c r="B842" s="6" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="843" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
-      <c r="A843" s="8" t="s">
-        <v>170</v>
-      </c>
-      <c r="B843" s="6" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="844" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A844" s="8" t="s">
-        <v>172</v>
-      </c>
-      <c r="B844" s="6" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="845" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A845" s="8" t="s">
-        <v>174</v>
-      </c>
-      <c r="B845" s="6" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="846" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A846" s="8" t="s">
-        <v>176</v>
-      </c>
-      <c r="B846" s="6" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="847" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
-      <c r="A847" s="8" t="s">
-        <v>177</v>
-      </c>
-      <c r="B847" s="6" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="848" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
-      <c r="A848" s="8" t="s">
-        <v>179</v>
-      </c>
-      <c r="B848" s="6" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="849" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
-      <c r="A849" s="8" t="s">
-        <v>181</v>
-      </c>
-      <c r="B849" s="6" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="850" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A850" s="8" t="s">
-        <v>183</v>
+        <v>156</v>
       </c>
       <c r="B850" s="6" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="851" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="851" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A851" s="8" t="s">
-        <v>185</v>
+        <v>158</v>
       </c>
       <c r="B851" s="6" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="852" spans="1:2" x14ac:dyDescent="0.2">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="852" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A852" s="8" t="s">
-        <v>187</v>
+        <v>160</v>
       </c>
       <c r="B852" s="6" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="853" spans="1:2" ht="90" x14ac:dyDescent="0.2">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="853" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A853" s="8" t="s">
-        <v>189</v>
+        <v>162</v>
       </c>
       <c r="B853" s="6" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="854" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="854" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A854" s="8" t="s">
-        <v>191</v>
+        <v>164</v>
       </c>
       <c r="B854" s="6" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="855" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="855" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A855" s="8" t="s">
-        <v>193</v>
+        <v>166</v>
       </c>
       <c r="B855" s="6" t="s">
-        <v>194</v>
+        <v>167</v>
       </c>
     </row>
     <row r="856" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A856" s="8" t="s">
-        <v>195</v>
+        <v>168</v>
       </c>
       <c r="B856" s="6" t="s">
-        <v>196</v>
+        <v>169</v>
       </c>
     </row>
     <row r="857" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A857" s="8" t="s">
-        <v>197</v>
+        <v>170</v>
       </c>
       <c r="B857" s="6" t="s">
-        <v>198</v>
+        <v>171</v>
       </c>
     </row>
     <row r="858" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A858" s="8" t="s">
-        <v>199</v>
+        <v>172</v>
       </c>
       <c r="B858" s="6" t="s">
-        <v>200</v>
+        <v>173</v>
       </c>
     </row>
     <row r="859" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A859" s="8" t="s">
-        <v>201</v>
+        <v>174</v>
       </c>
       <c r="B859" s="6" t="s">
-        <v>202</v>
+        <v>175</v>
       </c>
     </row>
     <row r="860" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A860" s="8" t="s">
-        <v>203</v>
+        <v>176</v>
       </c>
       <c r="B860" s="6" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="861" spans="1:2" x14ac:dyDescent="0.2">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="861" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A861" s="8" t="s">
-        <v>204</v>
+        <v>177</v>
       </c>
       <c r="B861" s="6" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="862" spans="1:2" x14ac:dyDescent="0.2">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="862" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A862" s="8" t="s">
-        <v>206</v>
+        <v>179</v>
       </c>
       <c r="B862" s="6" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="863" spans="1:2" x14ac:dyDescent="0.2">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="863" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A863" s="8" t="s">
-        <v>208</v>
+        <v>181</v>
       </c>
       <c r="B863" s="6" t="s">
-        <v>209</v>
+        <v>182</v>
       </c>
     </row>
     <row r="864" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A864" s="8" t="s">
-        <v>210</v>
+        <v>183</v>
       </c>
       <c r="B864" s="6" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="865" spans="1:2" x14ac:dyDescent="0.2">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="865" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A865" s="8" t="s">
-        <v>212</v>
+        <v>185</v>
       </c>
       <c r="B865" s="6" t="s">
-        <v>213</v>
+        <v>186</v>
       </c>
     </row>
     <row r="866" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A866" s="8" t="s">
-        <v>214</v>
+        <v>187</v>
       </c>
       <c r="B866" s="6" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="867" spans="1:2" x14ac:dyDescent="0.2">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="867" spans="1:2" ht="90" x14ac:dyDescent="0.2">
       <c r="A867" s="8" t="s">
-        <v>216</v>
+        <v>189</v>
       </c>
       <c r="B867" s="6" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="868" spans="1:2" x14ac:dyDescent="0.2">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="868" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A868" s="8" t="s">
-        <v>218</v>
+        <v>191</v>
       </c>
       <c r="B868" s="6" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="869" spans="1:2" x14ac:dyDescent="0.2">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="869" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A869" s="8" t="s">
-        <v>220</v>
+        <v>193</v>
       </c>
       <c r="B869" s="6" t="s">
-        <v>221</v>
+        <v>194</v>
       </c>
     </row>
     <row r="870" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A870" s="8" t="s">
-        <v>222</v>
+        <v>195</v>
       </c>
       <c r="B870" s="6" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="871" spans="1:2" x14ac:dyDescent="0.2">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="871" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A871" s="8" t="s">
-        <v>224</v>
+        <v>197</v>
       </c>
       <c r="B871" s="6" t="s">
-        <v>225</v>
+        <v>198</v>
       </c>
     </row>
     <row r="872" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A872" s="8" t="s">
-        <v>226</v>
+        <v>199</v>
       </c>
       <c r="B872" s="6" t="s">
-        <v>227</v>
+        <v>200</v>
       </c>
     </row>
     <row r="873" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A873" s="8" t="s">
-        <v>228</v>
+        <v>201</v>
       </c>
       <c r="B873" s="6" t="s">
-        <v>229</v>
+        <v>202</v>
       </c>
     </row>
     <row r="874" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A874" s="8" t="s">
-        <v>230</v>
+        <v>203</v>
       </c>
       <c r="B874" s="6" t="s">
-        <v>231</v>
+        <v>153</v>
       </c>
     </row>
     <row r="875" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A875" s="8" t="s">
-        <v>232</v>
+        <v>204</v>
       </c>
       <c r="B875" s="6" t="s">
-        <v>233</v>
+        <v>205</v>
       </c>
     </row>
     <row r="876" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A876" s="8" t="s">
-        <v>234</v>
+        <v>206</v>
       </c>
       <c r="B876" s="6" t="s">
-        <v>235</v>
+        <v>207</v>
       </c>
     </row>
     <row r="877" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A877" s="8" t="s">
-        <v>236</v>
+        <v>208</v>
       </c>
       <c r="B877" s="6" t="s">
-        <v>237</v>
+        <v>209</v>
       </c>
     </row>
     <row r="878" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A878" s="8" t="s">
-        <v>238</v>
+        <v>210</v>
       </c>
       <c r="B878" s="6" t="s">
-        <v>239</v>
+        <v>211</v>
       </c>
     </row>
     <row r="879" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A879" s="8" t="s">
-        <v>240</v>
+        <v>212</v>
       </c>
       <c r="B879" s="6" t="s">
-        <v>241</v>
+        <v>213</v>
       </c>
     </row>
     <row r="880" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A880" s="8" t="s">
-        <v>242</v>
+        <v>214</v>
       </c>
       <c r="B880" s="6" t="s">
-        <v>243</v>
+        <v>215</v>
       </c>
     </row>
     <row r="881" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A881" s="8" t="s">
-        <v>244</v>
+        <v>216</v>
       </c>
       <c r="B881" s="6" t="s">
-        <v>245</v>
+        <v>217</v>
       </c>
     </row>
     <row r="882" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A882" s="8" t="s">
-        <v>246</v>
+        <v>218</v>
       </c>
       <c r="B882" s="6" t="s">
-        <v>247</v>
+        <v>219</v>
       </c>
     </row>
     <row r="883" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A883" s="8" t="s">
-        <v>248</v>
+        <v>220</v>
       </c>
       <c r="B883" s="6" t="s">
-        <v>249</v>
+        <v>221</v>
       </c>
     </row>
     <row r="884" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A884" s="8" t="s">
-        <v>250</v>
+        <v>222</v>
       </c>
       <c r="B884" s="6" t="s">
-        <v>251</v>
+        <v>223</v>
       </c>
     </row>
     <row r="885" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A885" s="8" t="s">
-        <v>252</v>
+        <v>224</v>
       </c>
       <c r="B885" s="6" t="s">
-        <v>253</v>
+        <v>225</v>
       </c>
     </row>
     <row r="886" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A886" s="8" t="s">
-        <v>254</v>
+        <v>226</v>
       </c>
       <c r="B886" s="6" t="s">
-        <v>255</v>
+        <v>227</v>
       </c>
     </row>
     <row r="887" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A887" s="8" t="s">
-        <v>256</v>
+        <v>228</v>
       </c>
       <c r="B887" s="6" t="s">
-        <v>257</v>
+        <v>229</v>
       </c>
     </row>
     <row r="888" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A888" s="8" t="s">
-        <v>258</v>
+        <v>230</v>
       </c>
       <c r="B888" s="6" t="s">
-        <v>259</v>
+        <v>231</v>
       </c>
     </row>
     <row r="889" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A889" s="8" t="s">
-        <v>260</v>
+        <v>232</v>
       </c>
       <c r="B889" s="6" t="s">
-        <v>261</v>
+        <v>233</v>
       </c>
     </row>
     <row r="890" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A890" s="8" t="s">
-        <v>262</v>
+        <v>234</v>
       </c>
       <c r="B890" s="6" t="s">
-        <v>263</v>
+        <v>235</v>
       </c>
     </row>
     <row r="891" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A891" s="8" t="s">
-        <v>264</v>
+        <v>236</v>
       </c>
       <c r="B891" s="6" t="s">
-        <v>265</v>
+        <v>237</v>
       </c>
     </row>
     <row r="892" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A892" s="8" t="s">
-        <v>266</v>
+        <v>238</v>
       </c>
       <c r="B892" s="6" t="s">
-        <v>267</v>
+        <v>239</v>
       </c>
     </row>
     <row r="893" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A893" s="8" t="s">
-        <v>268</v>
+        <v>240</v>
       </c>
       <c r="B893" s="6" t="s">
-        <v>269</v>
+        <v>241</v>
       </c>
     </row>
     <row r="894" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A894" s="8" t="s">
-        <v>270</v>
+        <v>242</v>
       </c>
       <c r="B894" s="6" t="s">
-        <v>271</v>
+        <v>243</v>
       </c>
     </row>
     <row r="895" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A895" s="8" t="s">
-        <v>272</v>
+        <v>244</v>
       </c>
       <c r="B895" s="6" t="s">
-        <v>273</v>
+        <v>245</v>
       </c>
     </row>
     <row r="896" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A896" s="8" t="s">
-        <v>274</v>
+        <v>246</v>
       </c>
       <c r="B896" s="6" t="s">
-        <v>275</v>
+        <v>247</v>
       </c>
     </row>
     <row r="897" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A897" s="8" t="s">
-        <v>276</v>
+        <v>248</v>
       </c>
       <c r="B897" s="6" t="s">
-        <v>277</v>
+        <v>249</v>
       </c>
     </row>
     <row r="898" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A898" s="8" t="s">
-        <v>278</v>
+        <v>250</v>
       </c>
       <c r="B898" s="6" t="s">
-        <v>279</v>
+        <v>251</v>
       </c>
     </row>
     <row r="899" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A899" s="8" t="s">
-        <v>280</v>
+        <v>252</v>
       </c>
       <c r="B899" s="6" t="s">
-        <v>281</v>
+        <v>253</v>
       </c>
     </row>
     <row r="900" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A900" s="8" t="s">
-        <v>282</v>
+        <v>254</v>
       </c>
       <c r="B900" s="6" t="s">
-        <v>283</v>
+        <v>255</v>
       </c>
     </row>
     <row r="901" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A901" s="8" t="s">
-        <v>284</v>
+        <v>256</v>
       </c>
       <c r="B901" s="6" t="s">
-        <v>285</v>
+        <v>257</v>
       </c>
     </row>
     <row r="902" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A902" s="8" t="s">
-        <v>286</v>
+        <v>258</v>
       </c>
       <c r="B902" s="6" t="s">
-        <v>287</v>
+        <v>259</v>
       </c>
     </row>
     <row r="903" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A903" s="8" t="s">
-        <v>288</v>
+        <v>260</v>
       </c>
       <c r="B903" s="6" t="s">
-        <v>289</v>
+        <v>261</v>
       </c>
     </row>
     <row r="904" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A904" s="8" t="s">
-        <v>290</v>
+        <v>262</v>
       </c>
       <c r="B904" s="6" t="s">
-        <v>291</v>
+        <v>263</v>
       </c>
     </row>
     <row r="905" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A905" s="8" t="s">
-        <v>292</v>
+        <v>264</v>
       </c>
       <c r="B905" s="6" t="s">
-        <v>293</v>
+        <v>265</v>
       </c>
     </row>
     <row r="906" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A906" s="8" t="s">
-        <v>294</v>
+        <v>266</v>
       </c>
       <c r="B906" s="6" t="s">
-        <v>295</v>
+        <v>267</v>
       </c>
     </row>
     <row r="907" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A907" s="8" t="s">
-        <v>296</v>
+        <v>268</v>
       </c>
       <c r="B907" s="6" t="s">
-        <v>295</v>
+        <v>269</v>
       </c>
     </row>
     <row r="908" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A908" s="8" t="s">
-        <v>297</v>
+        <v>270</v>
       </c>
       <c r="B908" s="6" t="s">
-        <v>298</v>
+        <v>271</v>
       </c>
     </row>
     <row r="909" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A909" s="8" t="s">
-        <v>299</v>
+        <v>272</v>
       </c>
       <c r="B909" s="6" t="s">
-        <v>237</v>
+        <v>273</v>
       </c>
     </row>
     <row r="910" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A910" s="8" t="s">
-        <v>300</v>
+        <v>274</v>
       </c>
       <c r="B910" s="6" t="s">
-        <v>239</v>
+        <v>275</v>
       </c>
     </row>
     <row r="911" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A911" s="8" t="s">
-        <v>301</v>
+        <v>276</v>
       </c>
       <c r="B911" s="6" t="s">
-        <v>302</v>
+        <v>277</v>
       </c>
     </row>
     <row r="912" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A912" s="8" t="s">
-        <v>303</v>
+        <v>278</v>
       </c>
       <c r="B912" s="6" t="s">
-        <v>304</v>
+        <v>279</v>
       </c>
     </row>
     <row r="913" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A913" s="8" t="s">
-        <v>305</v>
+        <v>280</v>
       </c>
       <c r="B913" s="6" t="s">
-        <v>306</v>
+        <v>281</v>
       </c>
     </row>
     <row r="914" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A914" s="8" t="s">
-        <v>307</v>
+        <v>282</v>
       </c>
       <c r="B914" s="6" t="s">
-        <v>308</v>
+        <v>283</v>
       </c>
     </row>
     <row r="915" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A915" s="8" t="s">
-        <v>309</v>
+        <v>284</v>
       </c>
       <c r="B915" s="6" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="916" spans="1:2" ht="22.5" x14ac:dyDescent="0.2">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="916" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A916" s="8" t="s">
-        <v>311</v>
-      </c>
-      <c r="B916" s="9" t="s">
-        <v>312</v>
+        <v>286</v>
+      </c>
+      <c r="B916" s="6" t="s">
+        <v>287</v>
       </c>
     </row>
     <row r="917" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A917" s="8" t="s">
-        <v>313</v>
+        <v>288</v>
       </c>
       <c r="B917" s="6" t="s">
-        <v>314</v>
+        <v>289</v>
       </c>
     </row>
     <row r="918" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A918" s="8" t="s">
-        <v>315</v>
+        <v>290</v>
       </c>
       <c r="B918" s="6" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="919" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="919" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A919" s="8" t="s">
-        <v>317</v>
+        <v>292</v>
       </c>
       <c r="B919" s="6" t="s">
-        <v>318</v>
+        <v>293</v>
       </c>
     </row>
     <row r="920" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A920" s="8" t="s">
-        <v>319</v>
+        <v>294</v>
       </c>
       <c r="B920" s="6" t="s">
-        <v>320</v>
+        <v>295</v>
       </c>
     </row>
     <row r="921" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A921" s="8" t="s">
-        <v>321</v>
+        <v>296</v>
       </c>
       <c r="B921" s="6" t="s">
-        <v>322</v>
+        <v>295</v>
       </c>
     </row>
     <row r="922" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A922" s="8" t="s">
-        <v>323</v>
+        <v>297</v>
       </c>
       <c r="B922" s="6" t="s">
-        <v>324</v>
+        <v>298</v>
       </c>
     </row>
     <row r="923" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A923" s="8" t="s">
-        <v>325</v>
+        <v>299</v>
       </c>
       <c r="B923" s="6" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="924" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="924" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A924" s="8" t="s">
-        <v>327</v>
+        <v>300</v>
       </c>
       <c r="B924" s="6" t="s">
-        <v>328</v>
+        <v>239</v>
       </c>
     </row>
     <row r="925" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A925" s="8" t="s">
-        <v>329</v>
+        <v>301</v>
       </c>
       <c r="B925" s="6" t="s">
-        <v>295</v>
+        <v>302</v>
       </c>
     </row>
     <row r="926" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A926" s="8" t="s">
-        <v>330</v>
+        <v>303</v>
       </c>
       <c r="B926" s="6" t="s">
-        <v>331</v>
+        <v>304</v>
       </c>
     </row>
     <row r="927" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A927" s="8" t="s">
-        <v>332</v>
+        <v>305</v>
       </c>
       <c r="B927" s="6" t="s">
-        <v>333</v>
+        <v>306</v>
       </c>
     </row>
     <row r="928" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A928" s="8" t="s">
-        <v>334</v>
+        <v>307</v>
       </c>
       <c r="B928" s="6" t="s">
-        <v>335</v>
+        <v>308</v>
       </c>
     </row>
     <row r="929" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A929" s="8" t="s">
-        <v>336</v>
+        <v>309</v>
       </c>
       <c r="B929" s="6" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="930" spans="1:2" x14ac:dyDescent="0.2">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="930" spans="1:2" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A930" s="8" t="s">
-        <v>338</v>
-      </c>
-      <c r="B930" s="6" t="s">
-        <v>339</v>
+        <v>311</v>
+      </c>
+      <c r="B930" s="9" t="s">
+        <v>312</v>
       </c>
     </row>
     <row r="931" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A931" s="8" t="s">
-        <v>340</v>
+        <v>313</v>
       </c>
       <c r="B931" s="6" t="s">
-        <v>341</v>
+        <v>314</v>
       </c>
     </row>
     <row r="932" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A932" s="8" t="s">
-        <v>342</v>
+        <v>315</v>
       </c>
       <c r="B932" s="6" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="933" spans="1:2" x14ac:dyDescent="0.2">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="933" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A933" s="8" t="s">
-        <v>344</v>
+        <v>317</v>
       </c>
       <c r="B933" s="6" t="s">
-        <v>345</v>
+        <v>318</v>
       </c>
     </row>
     <row r="934" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A934" s="8" t="s">
-        <v>346</v>
+        <v>319</v>
       </c>
       <c r="B934" s="6" t="s">
-        <v>347</v>
+        <v>320</v>
       </c>
     </row>
     <row r="935" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A935" s="8" t="s">
-        <v>348</v>
+        <v>321</v>
       </c>
       <c r="B935" s="6" t="s">
-        <v>349</v>
+        <v>322</v>
       </c>
     </row>
     <row r="936" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A936" s="8" t="s">
-        <v>350</v>
+        <v>323</v>
       </c>
       <c r="B936" s="6" t="s">
-        <v>351</v>
+        <v>324</v>
       </c>
     </row>
     <row r="937" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A937" s="8" t="s">
-        <v>352</v>
+        <v>325</v>
       </c>
       <c r="B937" s="6" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="938" spans="1:2" x14ac:dyDescent="0.2">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="938" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A938" s="8" t="s">
-        <v>354</v>
+        <v>327</v>
       </c>
       <c r="B938" s="6" t="s">
-        <v>355</v>
+        <v>328</v>
       </c>
     </row>
     <row r="939" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A939" s="8" t="s">
-        <v>356</v>
+        <v>329</v>
       </c>
       <c r="B939" s="6" t="s">
-        <v>357</v>
+        <v>295</v>
       </c>
     </row>
     <row r="940" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A940" s="8" t="s">
-        <v>358</v>
+        <v>330</v>
       </c>
       <c r="B940" s="6" t="s">
-        <v>359</v>
+        <v>331</v>
       </c>
     </row>
     <row r="941" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A941" s="8" t="s">
-        <v>360</v>
+        <v>332</v>
       </c>
       <c r="B941" s="6" t="s">
-        <v>77</v>
+        <v>333</v>
       </c>
     </row>
     <row r="942" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A942" s="8" t="s">
-        <v>361</v>
+        <v>334</v>
       </c>
       <c r="B942" s="6" t="s">
-        <v>362</v>
+        <v>335</v>
       </c>
     </row>
     <row r="943" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A943" s="8" t="s">
-        <v>363</v>
+        <v>336</v>
       </c>
       <c r="B943" s="6" t="s">
-        <v>364</v>
+        <v>337</v>
       </c>
     </row>
     <row r="944" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A944" s="8" t="s">
-        <v>365</v>
+        <v>338</v>
       </c>
       <c r="B944" s="6" t="s">
-        <v>366</v>
+        <v>339</v>
       </c>
     </row>
     <row r="945" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A945" s="8" t="s">
-        <v>367</v>
+        <v>340</v>
       </c>
       <c r="B945" s="6" t="s">
-        <v>368</v>
+        <v>341</v>
       </c>
     </row>
     <row r="946" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A946" s="8" t="s">
-        <v>369</v>
+        <v>342</v>
       </c>
       <c r="B946" s="6" t="s">
-        <v>370</v>
+        <v>343</v>
       </c>
     </row>
     <row r="947" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A947" s="8" t="s">
-        <v>371</v>
+        <v>344</v>
       </c>
       <c r="B947" s="6" t="s">
-        <v>372</v>
+        <v>345</v>
       </c>
     </row>
     <row r="948" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A948" s="8" t="s">
-        <v>373</v>
+        <v>346</v>
       </c>
       <c r="B948" s="6" t="s">
-        <v>77</v>
+        <v>347</v>
       </c>
     </row>
     <row r="949" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A949" s="8" t="s">
-        <v>374</v>
+        <v>348</v>
       </c>
       <c r="B949" s="6" t="s">
-        <v>281</v>
+        <v>349</v>
       </c>
     </row>
     <row r="950" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A950" s="8" t="s">
-        <v>375</v>
+        <v>350</v>
       </c>
       <c r="B950" s="6" t="s">
-        <v>376</v>
+        <v>351</v>
       </c>
     </row>
     <row r="951" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A951" s="8" t="s">
-        <v>377</v>
+        <v>352</v>
       </c>
       <c r="B951" s="6" t="s">
-        <v>378</v>
+        <v>353</v>
       </c>
     </row>
     <row r="952" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A952" s="8" t="s">
-        <v>379</v>
+        <v>354</v>
       </c>
       <c r="B952" s="6" t="s">
-        <v>380</v>
+        <v>355</v>
       </c>
     </row>
     <row r="953" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A953" s="8" t="s">
-        <v>381</v>
+        <v>356</v>
       </c>
       <c r="B953" s="6" t="s">
-        <v>382</v>
+        <v>357</v>
       </c>
     </row>
     <row r="954" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A954" s="8" t="s">
-        <v>383</v>
+        <v>358</v>
       </c>
       <c r="B954" s="6" t="s">
-        <v>384</v>
+        <v>359</v>
       </c>
     </row>
     <row r="955" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A955" s="8" t="s">
-        <v>385</v>
+        <v>360</v>
       </c>
       <c r="B955" s="6" t="s">
-        <v>386</v>
+        <v>77</v>
       </c>
     </row>
     <row r="956" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A956" s="8" t="s">
-        <v>387</v>
+        <v>361</v>
       </c>
       <c r="B956" s="6" t="s">
-        <v>388</v>
+        <v>362</v>
       </c>
     </row>
     <row r="957" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A957" s="8" t="s">
-        <v>389</v>
+        <v>363</v>
       </c>
       <c r="B957" s="6" t="s">
-        <v>175</v>
+        <v>364</v>
       </c>
     </row>
     <row r="958" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A958" s="8" t="s">
-        <v>390</v>
+        <v>365</v>
       </c>
       <c r="B958" s="6" t="s">
-        <v>391</v>
+        <v>366</v>
       </c>
     </row>
     <row r="959" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A959" s="8" t="s">
+        <v>367</v>
+      </c>
+      <c r="B959" s="6" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="960" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A960" s="8" t="s">
+        <v>369</v>
+      </c>
+      <c r="B960" s="6" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="961" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A961" s="8" t="s">
+        <v>371</v>
+      </c>
+      <c r="B961" s="6" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="962" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A962" s="8" t="s">
+        <v>373</v>
+      </c>
+      <c r="B962" s="6" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="963" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A963" s="8" t="s">
+        <v>374</v>
+      </c>
+      <c r="B963" s="6" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="964" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A964" s="8" t="s">
+        <v>375</v>
+      </c>
+      <c r="B964" s="6" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="965" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A965" s="8" t="s">
+        <v>377</v>
+      </c>
+      <c r="B965" s="6" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="966" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A966" s="8" t="s">
+        <v>379</v>
+      </c>
+      <c r="B966" s="6" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="967" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A967" s="8" t="s">
+        <v>381</v>
+      </c>
+      <c r="B967" s="6" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="968" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A968" s="8" t="s">
+        <v>383</v>
+      </c>
+      <c r="B968" s="6" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="969" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A969" s="8" t="s">
+        <v>385</v>
+      </c>
+      <c r="B969" s="6" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="970" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A970" s="8" t="s">
+        <v>387</v>
+      </c>
+      <c r="B970" s="6" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="971" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A971" s="8" t="s">
+        <v>389</v>
+      </c>
+      <c r="B971" s="6" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="972" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A972" s="8" t="s">
+        <v>390</v>
+      </c>
+      <c r="B972" s="6" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="973" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A973" s="8" t="s">
         <v>392</v>
       </c>
-      <c r="B959" s="6" t="s">
+      <c r="B973" s="6" t="s">
         <v>393</v>
-      </c>
-    </row>
-    <row r="960" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A960" s="10" t="s">
-        <v>394</v>
-      </c>
-      <c r="B960" s="6" t="s">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="961" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A961" s="10" t="s">
-        <v>396</v>
-      </c>
-      <c r="B961" s="6" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="962" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A962" s="10" t="s">
-        <v>398</v>
-      </c>
-      <c r="B962" s="6" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="963" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A963" s="10" t="s">
-        <v>400</v>
-      </c>
-      <c r="B963" s="6" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="964" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A964" s="10" t="s">
-        <v>402</v>
-      </c>
-      <c r="B964" s="6" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="965" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A965" s="10" t="s">
-        <v>404</v>
-      </c>
-      <c r="B965" s="6" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="966" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A966" s="10" t="s">
-        <v>406</v>
-      </c>
-      <c r="B966" s="6" t="s">
-        <v>407</v>
-      </c>
-    </row>
-    <row r="967" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A967" s="10" t="s">
-        <v>408</v>
-      </c>
-      <c r="B967" s="6" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="968" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A968" s="10" t="s">
-        <v>410</v>
-      </c>
-      <c r="B968" s="6" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="969" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A969" s="10" t="s">
-        <v>411</v>
-      </c>
-      <c r="B969" s="6" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="970" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A970" s="10" t="s">
-        <v>413</v>
-      </c>
-      <c r="B970" s="6" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="971" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A971" s="10" t="s">
-        <v>414</v>
-      </c>
-      <c r="B971" s="6" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="972" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A972" s="10" t="s">
-        <v>415</v>
-      </c>
-      <c r="B972" s="6" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="973" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A973" s="10" t="s">
-        <v>416</v>
-      </c>
-      <c r="B973" s="6" t="s">
-        <v>401</v>
       </c>
     </row>
     <row r="974" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A974" s="10" t="s">
-        <v>417</v>
+        <v>394</v>
       </c>
       <c r="B974" s="6" t="s">
-        <v>403</v>
+        <v>395</v>
       </c>
     </row>
     <row r="975" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A975" s="10" t="s">
-        <v>418</v>
+        <v>396</v>
       </c>
       <c r="B975" s="6" t="s">
-        <v>405</v>
+        <v>397</v>
       </c>
     </row>
     <row r="976" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A976" s="10" t="s">
-        <v>419</v>
+        <v>398</v>
       </c>
       <c r="B976" s="6" t="s">
-        <v>407</v>
+        <v>399</v>
       </c>
     </row>
     <row r="977" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A977" s="10" t="s">
-        <v>420</v>
+        <v>400</v>
       </c>
       <c r="B977" s="6" t="s">
-        <v>395</v>
+        <v>401</v>
       </c>
     </row>
     <row r="978" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A978" s="10" t="s">
-        <v>421</v>
+        <v>402</v>
       </c>
       <c r="B978" s="6" t="s">
-        <v>397</v>
+        <v>403</v>
       </c>
     </row>
     <row r="979" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A979" s="10" t="s">
-        <v>422</v>
+        <v>404</v>
       </c>
       <c r="B979" s="6" t="s">
-        <v>399</v>
+        <v>405</v>
       </c>
     </row>
     <row r="980" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A980" s="10" t="s">
-        <v>423</v>
+        <v>406</v>
       </c>
       <c r="B980" s="6" t="s">
-        <v>273</v>
+        <v>407</v>
       </c>
     </row>
     <row r="981" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A981" s="10" t="s">
-        <v>424</v>
+        <v>408</v>
       </c>
       <c r="B981" s="6" t="s">
-        <v>275</v>
+        <v>409</v>
       </c>
     </row>
     <row r="982" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A982" s="10" t="s">
-        <v>425</v>
+        <v>410</v>
       </c>
       <c r="B982" s="6" t="s">
-        <v>320</v>
+        <v>409</v>
       </c>
     </row>
     <row r="983" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A983" s="10" t="s">
-        <v>426</v>
+        <v>411</v>
       </c>
       <c r="B983" s="6" t="s">
-        <v>281</v>
+        <v>412</v>
       </c>
     </row>
     <row r="984" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A984" s="10" t="s">
-        <v>427</v>
+        <v>413</v>
       </c>
       <c r="B984" s="6" t="s">
-        <v>428</v>
+        <v>412</v>
       </c>
     </row>
     <row r="985" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A985" s="10" t="s">
-        <v>429</v>
+        <v>414</v>
       </c>
       <c r="B985" s="6" t="s">
-        <v>295</v>
+        <v>215</v>
       </c>
     </row>
     <row r="986" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A986" s="10" t="s">
-        <v>430</v>
+        <v>415</v>
       </c>
       <c r="B986" s="6" t="s">
-        <v>431</v>
+        <v>217</v>
       </c>
     </row>
     <row r="987" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A987" s="10" t="s">
-        <v>432</v>
+        <v>416</v>
       </c>
       <c r="B987" s="6" t="s">
-        <v>433</v>
+        <v>401</v>
       </c>
     </row>
     <row r="988" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A988" s="10" t="s">
-        <v>434</v>
+        <v>417</v>
       </c>
       <c r="B988" s="6" t="s">
-        <v>435</v>
+        <v>403</v>
       </c>
     </row>
     <row r="989" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A989" s="10" t="s">
-        <v>436</v>
+        <v>418</v>
       </c>
       <c r="B989" s="6" t="s">
-        <v>437</v>
+        <v>405</v>
       </c>
     </row>
     <row r="990" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A990" s="10" t="s">
-        <v>438</v>
+        <v>419</v>
       </c>
       <c r="B990" s="6" t="s">
-        <v>439</v>
+        <v>407</v>
       </c>
     </row>
     <row r="991" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A991" s="10" t="s">
-        <v>440</v>
+        <v>420</v>
       </c>
       <c r="B991" s="6" t="s">
-        <v>441</v>
+        <v>395</v>
       </c>
     </row>
     <row r="992" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A992" s="10" t="s">
-        <v>442</v>
+        <v>421</v>
       </c>
       <c r="B992" s="6" t="s">
-        <v>443</v>
+        <v>397</v>
       </c>
     </row>
     <row r="993" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A993" s="10" t="s">
-        <v>444</v>
+        <v>422</v>
       </c>
       <c r="B993" s="6" t="s">
-        <v>407</v>
+        <v>399</v>
       </c>
     </row>
     <row r="994" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A994" s="10" t="s">
-        <v>445</v>
+        <v>423</v>
       </c>
       <c r="B994" s="6" t="s">
-        <v>446</v>
+        <v>273</v>
       </c>
     </row>
     <row r="995" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A995" s="10" t="s">
-        <v>447</v>
+        <v>424</v>
       </c>
       <c r="B995" s="6" t="s">
-        <v>448</v>
+        <v>275</v>
       </c>
     </row>
     <row r="996" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A996" s="10" t="s">
-        <v>449</v>
+        <v>425</v>
       </c>
       <c r="B996" s="6" t="s">
-        <v>450</v>
+        <v>320</v>
       </c>
     </row>
     <row r="997" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A997" s="10" t="s">
-        <v>451</v>
+        <v>426</v>
       </c>
       <c r="B997" s="6" t="s">
-        <v>452</v>
+        <v>281</v>
       </c>
     </row>
     <row r="998" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A998" s="10" t="s">
-        <v>453</v>
+        <v>427</v>
       </c>
       <c r="B998" s="6" t="s">
-        <v>454</v>
+        <v>428</v>
       </c>
     </row>
     <row r="999" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A999" s="10" t="s">
-        <v>455</v>
+        <v>429</v>
       </c>
       <c r="B999" s="6" t="s">
-        <v>456</v>
+        <v>295</v>
       </c>
     </row>
     <row r="1000" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1000" s="10" t="s">
-        <v>457</v>
+        <v>430</v>
       </c>
       <c r="B1000" s="6" t="s">
-        <v>458</v>
+        <v>431</v>
       </c>
     </row>
     <row r="1001" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1001" s="10" t="s">
-        <v>459</v>
+        <v>432</v>
       </c>
       <c r="B1001" s="6" t="s">
-        <v>460</v>
+        <v>433</v>
       </c>
     </row>
     <row r="1002" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1002" s="10" t="s">
-        <v>461</v>
+        <v>434</v>
       </c>
       <c r="B1002" s="6" t="s">
-        <v>462</v>
+        <v>435</v>
       </c>
     </row>
     <row r="1003" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1003" s="10" t="s">
-        <v>463</v>
+        <v>436</v>
       </c>
       <c r="B1003" s="6" t="s">
-        <v>464</v>
+        <v>437</v>
       </c>
     </row>
     <row r="1004" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1004" s="10" t="s">
-        <v>465</v>
+        <v>438</v>
       </c>
       <c r="B1004" s="6" t="s">
-        <v>466</v>
+        <v>439</v>
       </c>
     </row>
     <row r="1005" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1005" s="10" t="s">
-        <v>467</v>
+        <v>440</v>
       </c>
       <c r="B1005" s="6" t="s">
-        <v>468</v>
+        <v>441</v>
       </c>
     </row>
     <row r="1006" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1006" s="10" t="s">
-        <v>469</v>
+        <v>442</v>
       </c>
       <c r="B1006" s="6" t="s">
-        <v>470</v>
+        <v>443</v>
       </c>
     </row>
     <row r="1007" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1007" s="10" t="s">
-        <v>471</v>
+        <v>444</v>
       </c>
       <c r="B1007" s="6" t="s">
-        <v>472</v>
+        <v>407</v>
       </c>
     </row>
     <row r="1008" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1008" s="10" t="s">
-        <v>473</v>
+        <v>445</v>
       </c>
       <c r="B1008" s="6" t="s">
-        <v>474</v>
+        <v>446</v>
       </c>
     </row>
     <row r="1009" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1009" s="10" t="s">
-        <v>475</v>
+        <v>447</v>
       </c>
       <c r="B1009" s="6" t="s">
-        <v>476</v>
+        <v>448</v>
       </c>
     </row>
     <row r="1010" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1010" s="10" t="s">
-        <v>477</v>
+        <v>449</v>
       </c>
       <c r="B1010" s="6" t="s">
-        <v>478</v>
+        <v>450</v>
       </c>
     </row>
     <row r="1011" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1011" s="10" t="s">
-        <v>479</v>
+        <v>451</v>
       </c>
       <c r="B1011" s="6" t="s">
-        <v>480</v>
+        <v>452</v>
       </c>
     </row>
     <row r="1012" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1012" s="10" t="s">
-        <v>481</v>
+        <v>453</v>
       </c>
       <c r="B1012" s="6" t="s">
-        <v>482</v>
+        <v>454</v>
       </c>
     </row>
     <row r="1013" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1013" s="10" t="s">
-        <v>483</v>
+        <v>455</v>
       </c>
       <c r="B1013" s="6" t="s">
-        <v>484</v>
+        <v>456</v>
       </c>
     </row>
     <row r="1014" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1014" s="10" t="s">
-        <v>485</v>
+        <v>457</v>
       </c>
       <c r="B1014" s="6" t="s">
-        <v>486</v>
+        <v>458</v>
       </c>
     </row>
     <row r="1015" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1015" s="10" t="s">
-        <v>487</v>
+        <v>459</v>
       </c>
       <c r="B1015" s="6" t="s">
-        <v>488</v>
+        <v>460</v>
       </c>
     </row>
     <row r="1016" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1016" s="10" t="s">
-        <v>489</v>
+        <v>461</v>
       </c>
       <c r="B1016" s="6" t="s">
-        <v>490</v>
+        <v>462</v>
       </c>
     </row>
     <row r="1017" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1017" s="10" t="s">
-        <v>491</v>
+        <v>463</v>
       </c>
       <c r="B1017" s="6" t="s">
-        <v>492</v>
+        <v>464</v>
       </c>
     </row>
     <row r="1018" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1018" s="10" t="s">
-        <v>493</v>
+        <v>465</v>
       </c>
       <c r="B1018" s="6" t="s">
-        <v>494</v>
+        <v>466</v>
       </c>
     </row>
     <row r="1019" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1019" s="10" t="s">
-        <v>495</v>
+        <v>467</v>
       </c>
       <c r="B1019" s="6" t="s">
-        <v>496</v>
+        <v>468</v>
       </c>
     </row>
     <row r="1020" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1020" s="10" t="s">
-        <v>497</v>
+        <v>469</v>
       </c>
       <c r="B1020" s="6" t="s">
-        <v>498</v>
+        <v>470</v>
       </c>
     </row>
     <row r="1021" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1021" s="10" t="s">
-        <v>499</v>
+        <v>471</v>
       </c>
       <c r="B1021" s="6" t="s">
-        <v>500</v>
+        <v>472</v>
       </c>
     </row>
     <row r="1022" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1022" s="10" t="s">
-        <v>501</v>
+        <v>473</v>
       </c>
       <c r="B1022" s="6" t="s">
-        <v>502</v>
+        <v>474</v>
       </c>
     </row>
     <row r="1023" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1023" s="10" t="s">
-        <v>503</v>
+        <v>475</v>
       </c>
       <c r="B1023" s="6" t="s">
-        <v>504</v>
+        <v>476</v>
       </c>
     </row>
     <row r="1024" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1024" s="10" t="s">
-        <v>505</v>
+        <v>477</v>
       </c>
       <c r="B1024" s="6" t="s">
-        <v>506</v>
+        <v>478</v>
       </c>
     </row>
     <row r="1025" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1025" s="10" t="s">
-        <v>507</v>
+        <v>479</v>
       </c>
       <c r="B1025" s="6" t="s">
-        <v>508</v>
+        <v>480</v>
       </c>
     </row>
     <row r="1026" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1026" s="10" t="s">
-        <v>509</v>
+        <v>481</v>
       </c>
       <c r="B1026" s="6" t="s">
-        <v>510</v>
+        <v>482</v>
       </c>
     </row>
     <row r="1027" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1027" s="10" t="s">
-        <v>511</v>
+        <v>483</v>
       </c>
       <c r="B1027" s="6" t="s">
-        <v>512</v>
+        <v>484</v>
       </c>
     </row>
     <row r="1028" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1028" s="10" t="s">
-        <v>513</v>
+        <v>485</v>
       </c>
       <c r="B1028" s="6" t="s">
-        <v>514</v>
+        <v>486</v>
       </c>
     </row>
     <row r="1029" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1029" s="10" t="s">
-        <v>515</v>
+        <v>487</v>
       </c>
       <c r="B1029" s="6" t="s">
-        <v>516</v>
+        <v>488</v>
       </c>
     </row>
     <row r="1030" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1030" s="10" t="s">
-        <v>517</v>
+        <v>489</v>
       </c>
       <c r="B1030" s="6" t="s">
-        <v>518</v>
+        <v>490</v>
       </c>
     </row>
     <row r="1031" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1031" s="10" t="s">
-        <v>519</v>
+        <v>491</v>
       </c>
       <c r="B1031" s="6" t="s">
-        <v>520</v>
+        <v>492</v>
       </c>
     </row>
     <row r="1032" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1032" s="10" t="s">
-        <v>521</v>
+        <v>493</v>
       </c>
       <c r="B1032" s="6" t="s">
-        <v>522</v>
+        <v>494</v>
       </c>
     </row>
     <row r="1033" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1033" s="10" t="s">
-        <v>523</v>
+        <v>495</v>
       </c>
       <c r="B1033" s="6" t="s">
-        <v>524</v>
+        <v>496</v>
       </c>
     </row>
     <row r="1034" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1034" s="10" t="s">
-        <v>525</v>
+        <v>497</v>
       </c>
       <c r="B1034" s="6" t="s">
-        <v>526</v>
+        <v>498</v>
       </c>
     </row>
     <row r="1035" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1035" s="10" t="s">
-        <v>527</v>
+        <v>499</v>
       </c>
       <c r="B1035" s="6" t="s">
-        <v>528</v>
+        <v>500</v>
       </c>
     </row>
     <row r="1036" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1036" s="10" t="s">
-        <v>529</v>
+        <v>501</v>
       </c>
       <c r="B1036" s="6" t="s">
-        <v>530</v>
+        <v>502</v>
       </c>
     </row>
     <row r="1037" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1037" s="10" t="s">
-        <v>531</v>
+        <v>503</v>
       </c>
       <c r="B1037" s="6" t="s">
-        <v>532</v>
+        <v>504</v>
       </c>
     </row>
     <row r="1038" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1038" s="10" t="s">
-        <v>533</v>
+        <v>505</v>
       </c>
       <c r="B1038" s="6" t="s">
-        <v>534</v>
+        <v>506</v>
       </c>
     </row>
     <row r="1039" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1039" s="10" t="s">
-        <v>535</v>
+        <v>507</v>
       </c>
       <c r="B1039" s="6" t="s">
-        <v>536</v>
+        <v>508</v>
       </c>
     </row>
     <row r="1040" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1040" s="10" t="s">
-        <v>537</v>
+        <v>509</v>
       </c>
       <c r="B1040" s="6" t="s">
-        <v>538</v>
+        <v>510</v>
       </c>
     </row>
     <row r="1041" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1041" s="10" t="s">
-        <v>539</v>
+        <v>511</v>
       </c>
       <c r="B1041" s="6" t="s">
-        <v>540</v>
+        <v>512</v>
       </c>
     </row>
     <row r="1042" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1042" s="10" t="s">
-        <v>541</v>
+        <v>513</v>
       </c>
       <c r="B1042" s="6" t="s">
-        <v>542</v>
+        <v>514</v>
       </c>
     </row>
     <row r="1043" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1043" s="10" t="s">
-        <v>543</v>
+        <v>515</v>
       </c>
       <c r="B1043" s="6" t="s">
-        <v>544</v>
+        <v>516</v>
       </c>
     </row>
     <row r="1044" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1044" s="10" t="s">
-        <v>545</v>
+        <v>517</v>
       </c>
       <c r="B1044" s="6" t="s">
-        <v>546</v>
+        <v>518</v>
       </c>
     </row>
     <row r="1045" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1045" s="10" t="s">
-        <v>547</v>
+        <v>519</v>
       </c>
       <c r="B1045" s="6" t="s">
-        <v>548</v>
+        <v>520</v>
       </c>
     </row>
     <row r="1046" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1046" s="10" t="s">
-        <v>549</v>
+        <v>521</v>
       </c>
       <c r="B1046" s="6" t="s">
-        <v>550</v>
+        <v>522</v>
       </c>
     </row>
     <row r="1047" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1047" s="10" t="s">
-        <v>551</v>
+        <v>523</v>
       </c>
       <c r="B1047" s="6" t="s">
-        <v>552</v>
+        <v>524</v>
       </c>
     </row>
     <row r="1048" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1048" s="10" t="s">
-        <v>553</v>
+        <v>525</v>
       </c>
       <c r="B1048" s="6" t="s">
-        <v>554</v>
+        <v>526</v>
       </c>
     </row>
     <row r="1049" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1049" s="10" t="s">
-        <v>555</v>
+        <v>527</v>
       </c>
       <c r="B1049" s="6" t="s">
-        <v>556</v>
+        <v>528</v>
       </c>
     </row>
     <row r="1050" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1050" s="10" t="s">
-        <v>557</v>
+        <v>529</v>
       </c>
       <c r="B1050" s="6" t="s">
-        <v>558</v>
+        <v>530</v>
       </c>
     </row>
     <row r="1051" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1051" s="10" t="s">
-        <v>559</v>
+        <v>531</v>
       </c>
       <c r="B1051" s="6" t="s">
-        <v>560</v>
+        <v>532</v>
       </c>
     </row>
     <row r="1052" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1052" s="10" t="s">
-        <v>561</v>
+        <v>533</v>
       </c>
       <c r="B1052" s="6" t="s">
-        <v>562</v>
+        <v>534</v>
       </c>
     </row>
     <row r="1053" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1053" s="10" t="s">
-        <v>563</v>
+        <v>535</v>
       </c>
       <c r="B1053" s="6" t="s">
-        <v>564</v>
+        <v>536</v>
       </c>
     </row>
     <row r="1054" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1054" s="10" t="s">
-        <v>565</v>
+        <v>537</v>
       </c>
       <c r="B1054" s="6" t="s">
-        <v>566</v>
+        <v>538</v>
       </c>
     </row>
     <row r="1055" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1055" s="10" t="s">
-        <v>567</v>
+        <v>539</v>
       </c>
       <c r="B1055" s="6" t="s">
-        <v>568</v>
+        <v>540</v>
       </c>
     </row>
     <row r="1056" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1056" s="10" t="s">
-        <v>569</v>
+        <v>541</v>
       </c>
       <c r="B1056" s="6" t="s">
-        <v>570</v>
+        <v>542</v>
       </c>
     </row>
     <row r="1057" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1057" s="10" t="s">
-        <v>571</v>
+        <v>543</v>
       </c>
       <c r="B1057" s="6" t="s">
-        <v>572</v>
+        <v>544</v>
       </c>
     </row>
     <row r="1058" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1058" s="10" t="s">
-        <v>573</v>
+        <v>545</v>
       </c>
       <c r="B1058" s="6" t="s">
-        <v>574</v>
+        <v>546</v>
       </c>
     </row>
     <row r="1059" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1059" s="10" t="s">
-        <v>575</v>
+        <v>547</v>
       </c>
       <c r="B1059" s="6" t="s">
-        <v>576</v>
+        <v>548</v>
       </c>
     </row>
     <row r="1060" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1060" s="10" t="s">
-        <v>577</v>
+        <v>549</v>
       </c>
       <c r="B1060" s="6" t="s">
-        <v>578</v>
+        <v>550</v>
       </c>
     </row>
     <row r="1061" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1061" s="10" t="s">
-        <v>579</v>
+        <v>551</v>
       </c>
       <c r="B1061" s="6" t="s">
-        <v>580</v>
+        <v>552</v>
       </c>
     </row>
     <row r="1062" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1062" s="10" t="s">
-        <v>581</v>
+        <v>553</v>
       </c>
       <c r="B1062" s="6" t="s">
-        <v>582</v>
+        <v>554</v>
       </c>
     </row>
     <row r="1063" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1063" s="10" t="s">
-        <v>583</v>
+        <v>555</v>
       </c>
       <c r="B1063" s="6" t="s">
-        <v>584</v>
+        <v>556</v>
       </c>
     </row>
     <row r="1064" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1064" s="10" t="s">
-        <v>585</v>
+        <v>557</v>
       </c>
       <c r="B1064" s="6" t="s">
-        <v>586</v>
+        <v>558</v>
       </c>
     </row>
     <row r="1065" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1065" s="10" t="s">
-        <v>587</v>
+        <v>559</v>
       </c>
       <c r="B1065" s="6" t="s">
-        <v>588</v>
+        <v>560</v>
       </c>
     </row>
     <row r="1066" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1066" s="10" t="s">
-        <v>589</v>
+        <v>561</v>
       </c>
       <c r="B1066" s="6" t="s">
-        <v>590</v>
+        <v>562</v>
       </c>
     </row>
     <row r="1067" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1067" s="10" t="s">
-        <v>591</v>
+        <v>563</v>
       </c>
       <c r="B1067" s="6" t="s">
-        <v>592</v>
+        <v>564</v>
       </c>
     </row>
     <row r="1068" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1068" s="10" t="s">
-        <v>593</v>
+        <v>565</v>
       </c>
       <c r="B1068" s="6" t="s">
-        <v>594</v>
+        <v>566</v>
       </c>
     </row>
     <row r="1069" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1069" s="10" t="s">
-        <v>595</v>
+        <v>567</v>
       </c>
       <c r="B1069" s="6" t="s">
-        <v>596</v>
+        <v>568</v>
       </c>
     </row>
     <row r="1070" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1070" s="10" t="s">
-        <v>597</v>
+        <v>569</v>
       </c>
       <c r="B1070" s="6" t="s">
-        <v>598</v>
+        <v>570</v>
       </c>
     </row>
     <row r="1071" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1071" s="10" t="s">
-        <v>599</v>
+        <v>571</v>
       </c>
       <c r="B1071" s="6" t="s">
-        <v>600</v>
+        <v>572</v>
       </c>
     </row>
     <row r="1072" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1072" s="10" t="s">
-        <v>601</v>
+        <v>573</v>
       </c>
       <c r="B1072" s="6" t="s">
-        <v>602</v>
+        <v>574</v>
       </c>
     </row>
     <row r="1073" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1073" s="10" t="s">
-        <v>603</v>
+        <v>575</v>
       </c>
       <c r="B1073" s="6" t="s">
-        <v>604</v>
+        <v>576</v>
       </c>
     </row>
     <row r="1074" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1074" s="10" t="s">
-        <v>605</v>
+        <v>577</v>
       </c>
       <c r="B1074" s="6" t="s">
-        <v>606</v>
+        <v>578</v>
       </c>
     </row>
     <row r="1075" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1075" s="10" t="s">
-        <v>607</v>
+        <v>579</v>
       </c>
       <c r="B1075" s="6" t="s">
-        <v>608</v>
+        <v>580</v>
       </c>
     </row>
     <row r="1076" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1076" s="10" t="s">
-        <v>609</v>
+        <v>581</v>
       </c>
       <c r="B1076" s="6" t="s">
-        <v>610</v>
+        <v>582</v>
       </c>
     </row>
     <row r="1077" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1077" s="10" t="s">
-        <v>611</v>
+        <v>583</v>
       </c>
       <c r="B1077" s="6" t="s">
-        <v>612</v>
+        <v>584</v>
       </c>
     </row>
     <row r="1078" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1078" s="10" t="s">
-        <v>613</v>
+        <v>585</v>
       </c>
       <c r="B1078" s="6" t="s">
-        <v>614</v>
+        <v>586</v>
       </c>
     </row>
     <row r="1079" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1079" s="10" t="s">
-        <v>615</v>
+        <v>587</v>
       </c>
       <c r="B1079" s="6" t="s">
-        <v>616</v>
+        <v>588</v>
       </c>
     </row>
     <row r="1080" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1080" s="10" t="s">
-        <v>617</v>
+        <v>589</v>
       </c>
       <c r="B1080" s="6" t="s">
-        <v>618</v>
+        <v>590</v>
       </c>
     </row>
     <row r="1081" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1081" s="10" t="s">
-        <v>619</v>
+        <v>591</v>
       </c>
       <c r="B1081" s="6" t="s">
-        <v>620</v>
+        <v>592</v>
       </c>
     </row>
     <row r="1082" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1082" s="10" t="s">
-        <v>621</v>
+        <v>593</v>
       </c>
       <c r="B1082" s="6" t="s">
-        <v>622</v>
+        <v>594</v>
       </c>
     </row>
     <row r="1083" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1083" s="10" t="s">
-        <v>623</v>
+        <v>595</v>
       </c>
       <c r="B1083" s="6" t="s">
-        <v>624</v>
+        <v>596</v>
       </c>
     </row>
     <row r="1084" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1084" s="10" t="s">
-        <v>625</v>
+        <v>597</v>
       </c>
       <c r="B1084" s="6" t="s">
-        <v>626</v>
+        <v>598</v>
       </c>
     </row>
     <row r="1085" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1085" s="10" t="s">
-        <v>627</v>
+        <v>599</v>
       </c>
       <c r="B1085" s="6" t="s">
-        <v>628</v>
+        <v>600</v>
       </c>
     </row>
     <row r="1086" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1086" s="10" t="s">
-        <v>629</v>
+        <v>601</v>
       </c>
       <c r="B1086" s="6" t="s">
-        <v>630</v>
+        <v>602</v>
       </c>
     </row>
     <row r="1087" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1087" s="10" t="s">
-        <v>631</v>
+        <v>603</v>
       </c>
       <c r="B1087" s="6" t="s">
-        <v>632</v>
+        <v>604</v>
       </c>
     </row>
     <row r="1088" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1088" s="10" t="s">
-        <v>633</v>
+        <v>605</v>
       </c>
       <c r="B1088" s="6" t="s">
-        <v>634</v>
+        <v>606</v>
       </c>
     </row>
     <row r="1089" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1089" s="10" t="s">
-        <v>635</v>
+        <v>607</v>
       </c>
       <c r="B1089" s="6" t="s">
-        <v>636</v>
+        <v>608</v>
       </c>
     </row>
     <row r="1090" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1090" s="10" t="s">
-        <v>637</v>
+        <v>609</v>
       </c>
       <c r="B1090" s="6" t="s">
-        <v>638</v>
+        <v>610</v>
       </c>
     </row>
     <row r="1091" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1091" s="10" t="s">
-        <v>639</v>
+        <v>611</v>
       </c>
       <c r="B1091" s="6" t="s">
-        <v>640</v>
+        <v>612</v>
       </c>
     </row>
     <row r="1092" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1092" s="10" t="s">
-        <v>641</v>
+        <v>613</v>
       </c>
       <c r="B1092" s="6" t="s">
-        <v>642</v>
+        <v>614</v>
       </c>
     </row>
     <row r="1093" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1093" s="10" t="s">
-        <v>643</v>
+        <v>615</v>
       </c>
       <c r="B1093" s="6" t="s">
-        <v>644</v>
+        <v>616</v>
       </c>
     </row>
     <row r="1094" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1094" s="10" t="s">
-        <v>645</v>
+        <v>617</v>
       </c>
       <c r="B1094" s="6" t="s">
-        <v>646</v>
+        <v>618</v>
       </c>
     </row>
     <row r="1095" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1095" s="10" t="s">
-        <v>647</v>
+        <v>619</v>
       </c>
       <c r="B1095" s="6" t="s">
-        <v>648</v>
+        <v>620</v>
       </c>
     </row>
     <row r="1096" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1096" s="10" t="s">
-        <v>649</v>
+        <v>621</v>
       </c>
       <c r="B1096" s="6" t="s">
-        <v>650</v>
+        <v>622</v>
       </c>
     </row>
     <row r="1097" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1097" s="10" t="s">
-        <v>651</v>
+        <v>623</v>
       </c>
       <c r="B1097" s="6" t="s">
-        <v>652</v>
+        <v>624</v>
       </c>
     </row>
     <row r="1098" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1098" s="10" t="s">
-        <v>653</v>
+        <v>625</v>
       </c>
       <c r="B1098" s="6" t="s">
-        <v>654</v>
+        <v>626</v>
       </c>
     </row>
     <row r="1099" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1099" s="10" t="s">
-        <v>655</v>
+        <v>627</v>
       </c>
       <c r="B1099" s="6" t="s">
-        <v>656</v>
+        <v>628</v>
       </c>
     </row>
     <row r="1100" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1100" s="10" t="s">
-        <v>657</v>
+        <v>629</v>
       </c>
       <c r="B1100" s="6" t="s">
-        <v>658</v>
+        <v>630</v>
       </c>
     </row>
     <row r="1101" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1101" s="10" t="s">
-        <v>659</v>
+        <v>631</v>
       </c>
       <c r="B1101" s="6" t="s">
-        <v>660</v>
+        <v>632</v>
       </c>
     </row>
     <row r="1102" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1102" s="10" t="s">
-        <v>661</v>
+        <v>633</v>
       </c>
       <c r="B1102" s="6" t="s">
-        <v>662</v>
+        <v>634</v>
       </c>
     </row>
     <row r="1103" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1103" s="10" t="s">
-        <v>663</v>
+        <v>635</v>
       </c>
       <c r="B1103" s="6" t="s">
-        <v>664</v>
+        <v>636</v>
       </c>
     </row>
     <row r="1104" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1104" s="10" t="s">
-        <v>665</v>
+        <v>637</v>
       </c>
       <c r="B1104" s="6" t="s">
-        <v>666</v>
+        <v>638</v>
       </c>
     </row>
     <row r="1105" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1105" s="10" t="s">
-        <v>667</v>
+        <v>639</v>
       </c>
       <c r="B1105" s="6" t="s">
-        <v>668</v>
+        <v>640</v>
       </c>
     </row>
     <row r="1106" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1106" s="10" t="s">
-        <v>669</v>
+        <v>641</v>
       </c>
       <c r="B1106" s="6" t="s">
-        <v>670</v>
+        <v>642</v>
       </c>
     </row>
     <row r="1107" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1107" s="10" t="s">
-        <v>671</v>
+        <v>643</v>
       </c>
       <c r="B1107" s="6" t="s">
-        <v>672</v>
+        <v>644</v>
       </c>
     </row>
     <row r="1108" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1108" s="10" t="s">
-        <v>673</v>
+        <v>645</v>
       </c>
       <c r="B1108" s="6" t="s">
-        <v>674</v>
+        <v>646</v>
       </c>
     </row>
     <row r="1109" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1109" s="10" t="s">
-        <v>675</v>
+        <v>647</v>
       </c>
       <c r="B1109" s="6" t="s">
-        <v>676</v>
+        <v>648</v>
       </c>
     </row>
     <row r="1110" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1110" s="10" t="s">
-        <v>677</v>
+        <v>649</v>
       </c>
       <c r="B1110" s="6" t="s">
-        <v>678</v>
+        <v>650</v>
       </c>
     </row>
     <row r="1111" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1111" s="10" t="s">
-        <v>679</v>
+        <v>651</v>
       </c>
       <c r="B1111" s="6" t="s">
-        <v>680</v>
+        <v>652</v>
       </c>
     </row>
     <row r="1112" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1112" s="10" t="s">
-        <v>681</v>
+        <v>653</v>
       </c>
       <c r="B1112" s="6" t="s">
-        <v>682</v>
+        <v>654</v>
       </c>
     </row>
     <row r="1113" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1113" s="10" t="s">
-        <v>683</v>
+        <v>655</v>
       </c>
       <c r="B1113" s="6" t="s">
-        <v>684</v>
+        <v>656</v>
       </c>
     </row>
     <row r="1114" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1114" s="10" t="s">
-        <v>685</v>
+        <v>657</v>
       </c>
       <c r="B1114" s="6" t="s">
-        <v>686</v>
+        <v>658</v>
       </c>
     </row>
     <row r="1115" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1115" s="10" t="s">
-        <v>687</v>
+        <v>659</v>
       </c>
       <c r="B1115" s="6" t="s">
-        <v>688</v>
+        <v>660</v>
       </c>
     </row>
     <row r="1116" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1116" s="10" t="s">
-        <v>689</v>
+        <v>661</v>
       </c>
       <c r="B1116" s="6" t="s">
-        <v>690</v>
+        <v>662</v>
       </c>
     </row>
     <row r="1117" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1117" s="10" t="s">
-        <v>691</v>
+        <v>663</v>
       </c>
       <c r="B1117" s="6" t="s">
-        <v>692</v>
+        <v>664</v>
       </c>
     </row>
     <row r="1118" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1118" s="10" t="s">
-        <v>693</v>
+        <v>665</v>
       </c>
       <c r="B1118" s="6" t="s">
-        <v>694</v>
+        <v>666</v>
       </c>
     </row>
     <row r="1119" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1119" s="10" t="s">
-        <v>695</v>
+        <v>667</v>
       </c>
       <c r="B1119" s="6" t="s">
-        <v>696</v>
+        <v>668</v>
       </c>
     </row>
     <row r="1120" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1120" s="10" t="s">
-        <v>697</v>
+        <v>669</v>
       </c>
       <c r="B1120" s="6" t="s">
-        <v>698</v>
+        <v>670</v>
       </c>
     </row>
     <row r="1121" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1121" s="10" t="s">
-        <v>699</v>
+        <v>671</v>
       </c>
       <c r="B1121" s="6" t="s">
-        <v>700</v>
+        <v>672</v>
       </c>
     </row>
     <row r="1122" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1122" s="10" t="s">
-        <v>701</v>
+        <v>673</v>
       </c>
       <c r="B1122" s="6" t="s">
-        <v>702</v>
+        <v>674</v>
       </c>
     </row>
     <row r="1123" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1123" s="10" t="s">
-        <v>703</v>
+        <v>675</v>
       </c>
       <c r="B1123" s="6" t="s">
-        <v>704</v>
+        <v>676</v>
       </c>
     </row>
     <row r="1124" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1124" s="10" t="s">
-        <v>705</v>
+        <v>677</v>
       </c>
       <c r="B1124" s="6" t="s">
-        <v>706</v>
+        <v>678</v>
       </c>
     </row>
     <row r="1125" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1125" s="10" t="s">
-        <v>707</v>
+        <v>679</v>
       </c>
       <c r="B1125" s="6" t="s">
-        <v>708</v>
+        <v>680</v>
       </c>
     </row>
     <row r="1126" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1126" s="10" t="s">
-        <v>709</v>
+        <v>681</v>
       </c>
       <c r="B1126" s="6" t="s">
-        <v>710</v>
+        <v>682</v>
       </c>
     </row>
     <row r="1127" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1127" s="10" t="s">
-        <v>711</v>
+        <v>683</v>
       </c>
       <c r="B1127" s="6" t="s">
-        <v>712</v>
+        <v>684</v>
       </c>
     </row>
     <row r="1128" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1128" s="10" t="s">
-        <v>713</v>
+        <v>685</v>
       </c>
       <c r="B1128" s="6" t="s">
-        <v>714</v>
+        <v>686</v>
       </c>
     </row>
     <row r="1129" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1129" s="10" t="s">
-        <v>715</v>
+        <v>687</v>
       </c>
       <c r="B1129" s="6" t="s">
-        <v>716</v>
+        <v>688</v>
       </c>
     </row>
     <row r="1130" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1130" s="10" t="s">
-        <v>717</v>
+        <v>689</v>
       </c>
       <c r="B1130" s="6" t="s">
-        <v>718</v>
+        <v>690</v>
       </c>
     </row>
     <row r="1131" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1131" s="10" t="s">
-        <v>719</v>
+        <v>691</v>
       </c>
       <c r="B1131" s="6" t="s">
-        <v>720</v>
+        <v>692</v>
       </c>
     </row>
     <row r="1132" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1132" s="10" t="s">
-        <v>721</v>
+        <v>693</v>
       </c>
       <c r="B1132" s="6" t="s">
-        <v>722</v>
+        <v>694</v>
       </c>
     </row>
     <row r="1133" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1133" s="10" t="s">
-        <v>723</v>
+        <v>695</v>
       </c>
       <c r="B1133" s="6" t="s">
-        <v>724</v>
+        <v>696</v>
       </c>
     </row>
     <row r="1134" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1134" s="10" t="s">
-        <v>725</v>
+        <v>697</v>
       </c>
       <c r="B1134" s="6" t="s">
-        <v>726</v>
+        <v>698</v>
       </c>
     </row>
     <row r="1135" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1135" s="10" t="s">
-        <v>727</v>
+        <v>699</v>
       </c>
       <c r="B1135" s="6" t="s">
-        <v>728</v>
+        <v>700</v>
       </c>
     </row>
     <row r="1136" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1136" s="10" t="s">
-        <v>729</v>
+        <v>701</v>
       </c>
       <c r="B1136" s="6" t="s">
-        <v>730</v>
+        <v>702</v>
       </c>
     </row>
     <row r="1137" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1137" s="10" t="s">
-        <v>731</v>
+        <v>703</v>
       </c>
       <c r="B1137" s="6" t="s">
-        <v>732</v>
+        <v>704</v>
       </c>
     </row>
     <row r="1138" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1138" s="10" t="s">
-        <v>733</v>
+        <v>705</v>
       </c>
       <c r="B1138" s="6" t="s">
-        <v>734</v>
+        <v>706</v>
       </c>
     </row>
     <row r="1139" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1139" s="10" t="s">
-        <v>735</v>
+        <v>707</v>
       </c>
       <c r="B1139" s="6" t="s">
-        <v>736</v>
+        <v>708</v>
       </c>
     </row>
     <row r="1140" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1140" s="10" t="s">
-        <v>737</v>
+        <v>709</v>
       </c>
       <c r="B1140" s="6" t="s">
-        <v>738</v>
+        <v>710</v>
       </c>
     </row>
     <row r="1141" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1141" s="10" t="s">
-        <v>739</v>
+        <v>711</v>
       </c>
       <c r="B1141" s="6" t="s">
-        <v>740</v>
+        <v>712</v>
       </c>
     </row>
     <row r="1142" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1142" s="10" t="s">
-        <v>741</v>
+        <v>713</v>
       </c>
       <c r="B1142" s="6" t="s">
-        <v>742</v>
+        <v>714</v>
       </c>
     </row>
     <row r="1143" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1143" s="10" t="s">
-        <v>743</v>
+        <v>715</v>
       </c>
       <c r="B1143" s="6" t="s">
-        <v>744</v>
+        <v>716</v>
       </c>
     </row>
     <row r="1144" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1144" s="10" t="s">
-        <v>745</v>
+        <v>717</v>
       </c>
       <c r="B1144" s="6" t="s">
-        <v>746</v>
+        <v>718</v>
       </c>
     </row>
     <row r="1145" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1145" s="10" t="s">
-        <v>747</v>
+        <v>719</v>
       </c>
       <c r="B1145" s="6" t="s">
-        <v>748</v>
+        <v>720</v>
       </c>
     </row>
     <row r="1146" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1146" s="10" t="s">
-        <v>749</v>
+        <v>721</v>
       </c>
       <c r="B1146" s="6" t="s">
-        <v>750</v>
+        <v>722</v>
       </c>
     </row>
     <row r="1147" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1147" s="10" t="s">
-        <v>751</v>
+        <v>723</v>
       </c>
       <c r="B1147" s="6" t="s">
-        <v>752</v>
+        <v>724</v>
       </c>
     </row>
     <row r="1148" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1148" s="10" t="s">
-        <v>753</v>
+        <v>725</v>
       </c>
       <c r="B1148" s="6" t="s">
-        <v>754</v>
+        <v>726</v>
       </c>
     </row>
     <row r="1149" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1149" s="10" t="s">
-        <v>755</v>
+        <v>727</v>
       </c>
       <c r="B1149" s="6" t="s">
-        <v>756</v>
+        <v>728</v>
       </c>
     </row>
     <row r="1150" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1150" s="10" t="s">
-        <v>757</v>
+        <v>729</v>
       </c>
       <c r="B1150" s="6" t="s">
-        <v>758</v>
+        <v>730</v>
       </c>
     </row>
     <row r="1151" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1151" s="10" t="s">
-        <v>759</v>
+        <v>731</v>
       </c>
       <c r="B1151" s="6" t="s">
-        <v>760</v>
+        <v>732</v>
       </c>
     </row>
     <row r="1152" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1152" s="10" t="s">
-        <v>761</v>
+        <v>733</v>
       </c>
       <c r="B1152" s="6" t="s">
-        <v>762</v>
+        <v>734</v>
       </c>
     </row>
     <row r="1153" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1153" s="10" t="s">
-        <v>763</v>
+        <v>735</v>
       </c>
       <c r="B1153" s="6" t="s">
-        <v>764</v>
+        <v>736</v>
       </c>
     </row>
     <row r="1154" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1154" s="10" t="s">
-        <v>765</v>
+        <v>737</v>
       </c>
       <c r="B1154" s="6" t="s">
-        <v>766</v>
+        <v>738</v>
       </c>
     </row>
     <row r="1155" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1155" s="10" t="s">
-        <v>767</v>
+        <v>739</v>
       </c>
       <c r="B1155" s="6" t="s">
-        <v>304</v>
+        <v>740</v>
       </c>
     </row>
     <row r="1156" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1156" s="10" t="s">
-        <v>768</v>
+        <v>741</v>
       </c>
       <c r="B1156" s="6" t="s">
-        <v>769</v>
+        <v>742</v>
       </c>
     </row>
     <row r="1157" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1157" s="10" t="s">
-        <v>770</v>
+        <v>743</v>
       </c>
       <c r="B1157" s="6" t="s">
-        <v>316</v>
+        <v>744</v>
       </c>
     </row>
     <row r="1158" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1158" s="10" t="s">
-        <v>771</v>
+        <v>745</v>
       </c>
       <c r="B1158" s="6" t="s">
-        <v>211</v>
+        <v>746</v>
       </c>
     </row>
     <row r="1159" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1159" s="10" t="s">
-        <v>772</v>
+        <v>747</v>
       </c>
       <c r="B1159" s="6" t="s">
-        <v>213</v>
+        <v>748</v>
       </c>
     </row>
     <row r="1160" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1160" s="10" t="s">
-        <v>773</v>
+        <v>749</v>
       </c>
       <c r="B1160" s="6" t="s">
-        <v>774</v>
-      </c>
-    </row>
-    <row r="1161" spans="1:2" ht="22.5" x14ac:dyDescent="0.2">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="1161" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1161" s="10" t="s">
-        <v>775</v>
-      </c>
-      <c r="B1161" s="9" t="s">
-        <v>312</v>
+        <v>751</v>
+      </c>
+      <c r="B1161" s="6" t="s">
+        <v>752</v>
       </c>
     </row>
     <row r="1162" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1162" s="10" t="s">
-        <v>776</v>
+        <v>753</v>
       </c>
       <c r="B1162" s="6" t="s">
-        <v>777</v>
+        <v>754</v>
       </c>
     </row>
     <row r="1163" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1163" s="10" t="s">
-        <v>778</v>
+        <v>755</v>
       </c>
       <c r="B1163" s="6" t="s">
-        <v>308</v>
+        <v>756</v>
       </c>
     </row>
     <row r="1164" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1164" s="10" t="s">
-        <v>779</v>
+        <v>757</v>
       </c>
       <c r="B1164" s="6" t="s">
-        <v>780</v>
+        <v>758</v>
       </c>
     </row>
     <row r="1165" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1165" s="10" t="s">
-        <v>781</v>
+        <v>759</v>
       </c>
       <c r="B1165" s="6" t="s">
-        <v>782</v>
+        <v>760</v>
       </c>
     </row>
     <row r="1166" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1166" s="10" t="s">
-        <v>783</v>
+        <v>761</v>
       </c>
       <c r="B1166" s="6" t="s">
-        <v>784</v>
+        <v>762</v>
       </c>
     </row>
     <row r="1167" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1167" s="10" t="s">
+        <v>763</v>
+      </c>
+      <c r="B1167" s="6" t="s">
+        <v>764</v>
+      </c>
+    </row>
+    <row r="1168" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1168" s="10" t="s">
+        <v>765</v>
+      </c>
+      <c r="B1168" s="6" t="s">
+        <v>766</v>
+      </c>
+    </row>
+    <row r="1169" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1169" s="10" t="s">
+        <v>767</v>
+      </c>
+      <c r="B1169" s="6" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="1170" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1170" s="10" t="s">
+        <v>768</v>
+      </c>
+      <c r="B1170" s="6" t="s">
+        <v>769</v>
+      </c>
+    </row>
+    <row r="1171" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1171" s="10" t="s">
+        <v>770</v>
+      </c>
+      <c r="B1171" s="6" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="1172" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1172" s="10" t="s">
+        <v>771</v>
+      </c>
+      <c r="B1172" s="6" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="1173" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1173" s="10" t="s">
+        <v>772</v>
+      </c>
+      <c r="B1173" s="6" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="1174" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1174" s="10" t="s">
+        <v>773</v>
+      </c>
+      <c r="B1174" s="6" t="s">
+        <v>774</v>
+      </c>
+    </row>
+    <row r="1175" spans="1:2" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A1175" s="10" t="s">
+        <v>775</v>
+      </c>
+      <c r="B1175" s="9" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="1176" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1176" s="10" t="s">
+        <v>776</v>
+      </c>
+      <c r="B1176" s="6" t="s">
+        <v>777</v>
+      </c>
+    </row>
+    <row r="1177" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1177" s="10" t="s">
+        <v>778</v>
+      </c>
+      <c r="B1177" s="6" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="1178" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1178" s="10" t="s">
+        <v>779</v>
+      </c>
+      <c r="B1178" s="6" t="s">
+        <v>780</v>
+      </c>
+    </row>
+    <row r="1179" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1179" s="10" t="s">
+        <v>781</v>
+      </c>
+      <c r="B1179" s="6" t="s">
+        <v>782</v>
+      </c>
+    </row>
+    <row r="1180" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1180" s="10" t="s">
+        <v>783</v>
+      </c>
+      <c r="B1180" s="6" t="s">
+        <v>784</v>
+      </c>
+    </row>
+    <row r="1181" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1181" s="10" t="s">
         <v>785</v>
       </c>
-      <c r="B1167" s="6" t="s">
+      <c r="B1181" s="6" t="s">
         <v>786</v>
       </c>
     </row>
-    <row r="1168" spans="1:2" ht="22.5" x14ac:dyDescent="0.2">
-      <c r="A1168" s="10" t="s">
+    <row r="1182" spans="1:2" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A1182" s="10" t="s">
         <v>787</v>
       </c>
-      <c r="B1168" s="6" t="s">
+      <c r="B1182" s="6" t="s">
         <v>788</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add 'Armor of Garahel'
This mod contains the armor and weapons of the legendary Grey Warden Garahel who ended the Fourth Blight.

A massive armour and sword set suitable for tanks if an appropriate shiled is found. The mod contains twin longswords whose stats have been modified to have one suitable for general enemies and one that is geared towards fighting archdemons.

see #390
</commit_message>
<xml_diff>
--- a/source/tlk/strings.xlsx
+++ b/source/tlk/strings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\DAO\archid\source\tlk\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{839294A5-BF0C-4C2E-9404-EB554C400CB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A208C17-F6EE-4F93-846F-53AEDFC424DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2430" yWindow="750" windowWidth="23640" windowHeight="16110" xr2:uid="{A42EE72D-E1C4-43B6-AEA5-0014ED5180B1}"/>
+    <workbookView xWindow="2865" yWindow="615" windowWidth="23640" windowHeight="16110" xr2:uid="{A42EE72D-E1C4-43B6-AEA5-0014ED5180B1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -295,7 +295,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A889" authorId="0" shapeId="0" xr:uid="{15B7CDC5-6F21-45A0-9997-3CC9AFCCF646}">
+    <comment ref="A899" authorId="0" shapeId="0" xr:uid="{15B7CDC5-6F21-45A0-9997-3CC9AFCCF646}">
       <text>
         <r>
           <rPr>
@@ -309,7 +309,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A1016" authorId="0" shapeId="0" xr:uid="{08441945-669A-47E4-A77A-BA32248BBBE4}">
+    <comment ref="A1026" authorId="0" shapeId="0" xr:uid="{08441945-669A-47E4-A77A-BA32248BBBE4}">
       <text>
         <r>
           <rPr>
@@ -342,7 +342,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1561" uniqueCount="1504">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1571" uniqueCount="1511">
   <si>
     <t>af_archid_en-us.tlk</t>
   </si>
@@ -4921,14 +4921,42 @@
   <si>
     <t>This medium helmet seems to enhance your mental faculties somehow alongside providing additionl protection.</t>
   </si>
+  <si>
+    <t>Garahel's Boots</t>
+  </si>
+  <si>
+    <t>Worn by the legendary grey warden Garahel during the battle of Ayesleigh, where he slew the archdemon Andoral and ended the fourth blight. This armour is a masterpiece crafted by the best grey warden blacksmiths and enchanted to enhance it's wearer. Althoughh it's owner has perished, the armour still survives to continue the fight.</t>
+  </si>
+  <si>
+    <t>Garahel's Armour</t>
+  </si>
+  <si>
+    <t>Garahel's Gauntlets</t>
+  </si>
+  <si>
+    <t>Garahel's Fury</t>
+  </si>
+  <si>
+    <t>Wielded by the legendary grey warden Garahel during the battle of Ayesleigh, where he slew the archdemon Andoral and ended the fourth blight. This weapon is a masterpiece crafted by the best grey warden blacksmiths and enchanted to enhance it's wearer. Althoughh it's owner has perished, the sword still survives to continue the fight.</t>
+  </si>
+  <si>
+    <t>Garahel's Vigilance</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -5020,26 +5048,27 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="2" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5358,10 +5387,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C8288F5-46B5-435A-B9FC-40522281A8A6}">
-  <dimension ref="A1:B1224"/>
+  <dimension ref="A1:B1234"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A842" workbookViewId="0">
-      <selection activeCell="B859" sqref="B859"/>
+    <sheetView tabSelected="1" topLeftCell="A860" workbookViewId="0">
+      <selection activeCell="B869" sqref="B869"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -12475,1129 +12504,1129 @@
         <v>1499</v>
       </c>
     </row>
-    <row r="889" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A889" s="8" t="s">
+    <row r="889" spans="1:2" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A889" s="4">
+        <v>6610855</v>
+      </c>
+      <c r="B889" s="11" t="s">
+        <v>1504</v>
+      </c>
+    </row>
+    <row r="890" spans="1:2" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A890" s="4">
+        <v>6610856</v>
+      </c>
+      <c r="B890" s="11" t="s">
+        <v>1505</v>
+      </c>
+    </row>
+    <row r="891" spans="1:2" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A891" s="4">
+        <v>6610857</v>
+      </c>
+      <c r="B891" s="11" t="s">
+        <v>1506</v>
+      </c>
+    </row>
+    <row r="892" spans="1:2" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A892" s="4">
+        <v>6610858</v>
+      </c>
+      <c r="B892" s="11" t="s">
+        <v>1505</v>
+      </c>
+    </row>
+    <row r="893" spans="1:2" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A893" s="4">
+        <v>6610859</v>
+      </c>
+      <c r="B893" s="11" t="s">
+        <v>1507</v>
+      </c>
+    </row>
+    <row r="894" spans="1:2" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A894" s="4">
+        <v>6610860</v>
+      </c>
+      <c r="B894" s="11" t="s">
+        <v>1505</v>
+      </c>
+    </row>
+    <row r="895" spans="1:2" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A895" s="4">
+        <v>6610861</v>
+      </c>
+      <c r="B895" s="11" t="s">
+        <v>1508</v>
+      </c>
+    </row>
+    <row r="896" spans="1:2" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A896" s="4">
+        <v>6610862</v>
+      </c>
+      <c r="B896" s="11" t="s">
+        <v>1509</v>
+      </c>
+    </row>
+    <row r="897" spans="1:2" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A897" s="4">
+        <v>6610863</v>
+      </c>
+      <c r="B897" s="11" t="s">
+        <v>1510</v>
+      </c>
+    </row>
+    <row r="898" spans="1:2" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A898" s="4">
+        <v>6610864</v>
+      </c>
+      <c r="B898" s="11" t="s">
+        <v>1509</v>
+      </c>
+    </row>
+    <row r="899" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A899" s="8" t="s">
         <v>150</v>
       </c>
-      <c r="B889" s="7" t="s">
+      <c r="B899" s="7" t="s">
         <v>151</v>
-      </c>
-    </row>
-    <row r="890" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A890" s="8" t="s">
-        <v>152</v>
-      </c>
-      <c r="B890" s="7" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="891" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A891" s="8" t="s">
-        <v>154</v>
-      </c>
-      <c r="B891" s="7" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="892" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A892" s="8" t="s">
-        <v>156</v>
-      </c>
-      <c r="B892" s="7" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="893" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A893" s="8" t="s">
-        <v>158</v>
-      </c>
-      <c r="B893" s="7" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="894" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
-      <c r="A894" s="8" t="s">
-        <v>160</v>
-      </c>
-      <c r="B894" s="7" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="895" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A895" s="8" t="s">
-        <v>162</v>
-      </c>
-      <c r="B895" s="7" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="896" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A896" s="8" t="s">
-        <v>164</v>
-      </c>
-      <c r="B896" s="7" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="897" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A897" s="8" t="s">
-        <v>166</v>
-      </c>
-      <c r="B897" s="7" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="898" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A898" s="8" t="s">
-        <v>168</v>
-      </c>
-      <c r="B898" s="7" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="899" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
-      <c r="A899" s="8" t="s">
-        <v>170</v>
-      </c>
-      <c r="B899" s="7" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="900" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A900" s="8" t="s">
-        <v>172</v>
+        <v>152</v>
       </c>
       <c r="B900" s="7" t="s">
-        <v>173</v>
+        <v>153</v>
       </c>
     </row>
     <row r="901" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A901" s="8" t="s">
-        <v>174</v>
+        <v>154</v>
       </c>
       <c r="B901" s="7" t="s">
-        <v>175</v>
+        <v>155</v>
       </c>
     </row>
     <row r="902" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A902" s="8" t="s">
-        <v>176</v>
+        <v>156</v>
       </c>
       <c r="B902" s="7" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="903" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="903" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A903" s="8" t="s">
-        <v>177</v>
+        <v>158</v>
       </c>
       <c r="B903" s="7" t="s">
-        <v>178</v>
+        <v>159</v>
       </c>
     </row>
     <row r="904" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A904" s="8" t="s">
-        <v>179</v>
+        <v>160</v>
       </c>
       <c r="B904" s="7" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="905" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="905" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A905" s="8" t="s">
-        <v>181</v>
+        <v>162</v>
       </c>
       <c r="B905" s="7" t="s">
-        <v>182</v>
+        <v>163</v>
       </c>
     </row>
     <row r="906" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A906" s="8" t="s">
-        <v>183</v>
+        <v>164</v>
       </c>
       <c r="B906" s="7" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="907" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="907" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A907" s="8" t="s">
-        <v>185</v>
+        <v>166</v>
       </c>
       <c r="B907" s="7" t="s">
-        <v>186</v>
+        <v>167</v>
       </c>
     </row>
     <row r="908" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A908" s="8" t="s">
-        <v>187</v>
+        <v>168</v>
       </c>
       <c r="B908" s="7" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="909" spans="1:2" ht="90" x14ac:dyDescent="0.2">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="909" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A909" s="8" t="s">
-        <v>189</v>
+        <v>170</v>
       </c>
       <c r="B909" s="7" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="910" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="910" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A910" s="8" t="s">
-        <v>191</v>
+        <v>172</v>
       </c>
       <c r="B910" s="7" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="911" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="911" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A911" s="8" t="s">
-        <v>193</v>
+        <v>174</v>
       </c>
       <c r="B911" s="7" t="s">
-        <v>194</v>
+        <v>175</v>
       </c>
     </row>
     <row r="912" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A912" s="8" t="s">
-        <v>195</v>
+        <v>176</v>
       </c>
       <c r="B912" s="7" t="s">
-        <v>196</v>
+        <v>151</v>
       </c>
     </row>
     <row r="913" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A913" s="8" t="s">
-        <v>197</v>
+        <v>177</v>
       </c>
       <c r="B913" s="7" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="914" spans="1:2" x14ac:dyDescent="0.2">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="914" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A914" s="8" t="s">
-        <v>199</v>
+        <v>179</v>
       </c>
       <c r="B914" s="7" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="915" spans="1:2" x14ac:dyDescent="0.2">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="915" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A915" s="8" t="s">
-        <v>201</v>
+        <v>181</v>
       </c>
       <c r="B915" s="7" t="s">
-        <v>202</v>
+        <v>182</v>
       </c>
     </row>
     <row r="916" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A916" s="8" t="s">
-        <v>203</v>
+        <v>183</v>
       </c>
       <c r="B916" s="7" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="917" spans="1:2" x14ac:dyDescent="0.2">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="917" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A917" s="8" t="s">
-        <v>204</v>
+        <v>185</v>
       </c>
       <c r="B917" s="7" t="s">
-        <v>205</v>
+        <v>186</v>
       </c>
     </row>
     <row r="918" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A918" s="8" t="s">
-        <v>206</v>
+        <v>187</v>
       </c>
       <c r="B918" s="7" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="919" spans="1:2" x14ac:dyDescent="0.2">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="919" spans="1:2" ht="90" x14ac:dyDescent="0.2">
       <c r="A919" s="8" t="s">
-        <v>208</v>
+        <v>189</v>
       </c>
       <c r="B919" s="7" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="920" spans="1:2" x14ac:dyDescent="0.2">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="920" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A920" s="8" t="s">
-        <v>210</v>
+        <v>191</v>
       </c>
       <c r="B920" s="7" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="921" spans="1:2" x14ac:dyDescent="0.2">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="921" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A921" s="8" t="s">
-        <v>212</v>
+        <v>193</v>
       </c>
       <c r="B921" s="7" t="s">
-        <v>213</v>
+        <v>194</v>
       </c>
     </row>
     <row r="922" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A922" s="8" t="s">
-        <v>214</v>
+        <v>195</v>
       </c>
       <c r="B922" s="7" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="923" spans="1:2" x14ac:dyDescent="0.2">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="923" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A923" s="8" t="s">
-        <v>216</v>
+        <v>197</v>
       </c>
       <c r="B923" s="7" t="s">
-        <v>217</v>
+        <v>198</v>
       </c>
     </row>
     <row r="924" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A924" s="8" t="s">
-        <v>218</v>
+        <v>199</v>
       </c>
       <c r="B924" s="7" t="s">
-        <v>219</v>
+        <v>200</v>
       </c>
     </row>
     <row r="925" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A925" s="8" t="s">
-        <v>220</v>
+        <v>201</v>
       </c>
       <c r="B925" s="7" t="s">
-        <v>221</v>
+        <v>202</v>
       </c>
     </row>
     <row r="926" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A926" s="8" t="s">
-        <v>222</v>
+        <v>203</v>
       </c>
       <c r="B926" s="7" t="s">
-        <v>223</v>
+        <v>153</v>
       </c>
     </row>
     <row r="927" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A927" s="8" t="s">
-        <v>224</v>
+        <v>204</v>
       </c>
       <c r="B927" s="7" t="s">
-        <v>225</v>
+        <v>205</v>
       </c>
     </row>
     <row r="928" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A928" s="8" t="s">
-        <v>226</v>
+        <v>206</v>
       </c>
       <c r="B928" s="7" t="s">
-        <v>227</v>
+        <v>207</v>
       </c>
     </row>
     <row r="929" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A929" s="8" t="s">
-        <v>228</v>
+        <v>208</v>
       </c>
       <c r="B929" s="7" t="s">
-        <v>229</v>
+        <v>209</v>
       </c>
     </row>
     <row r="930" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A930" s="8" t="s">
-        <v>230</v>
+        <v>210</v>
       </c>
       <c r="B930" s="7" t="s">
-        <v>231</v>
+        <v>211</v>
       </c>
     </row>
     <row r="931" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A931" s="8" t="s">
-        <v>232</v>
+        <v>212</v>
       </c>
       <c r="B931" s="7" t="s">
-        <v>233</v>
+        <v>213</v>
       </c>
     </row>
     <row r="932" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A932" s="8" t="s">
-        <v>234</v>
+        <v>214</v>
       </c>
       <c r="B932" s="7" t="s">
-        <v>235</v>
+        <v>215</v>
       </c>
     </row>
     <row r="933" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A933" s="8" t="s">
-        <v>236</v>
+        <v>216</v>
       </c>
       <c r="B933" s="7" t="s">
-        <v>237</v>
+        <v>217</v>
       </c>
     </row>
     <row r="934" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A934" s="8" t="s">
-        <v>238</v>
+        <v>218</v>
       </c>
       <c r="B934" s="7" t="s">
-        <v>239</v>
+        <v>219</v>
       </c>
     </row>
     <row r="935" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A935" s="8" t="s">
-        <v>240</v>
+        <v>220</v>
       </c>
       <c r="B935" s="7" t="s">
-        <v>241</v>
+        <v>221</v>
       </c>
     </row>
     <row r="936" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A936" s="8" t="s">
-        <v>242</v>
+        <v>222</v>
       </c>
       <c r="B936" s="7" t="s">
-        <v>243</v>
+        <v>223</v>
       </c>
     </row>
     <row r="937" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A937" s="8" t="s">
-        <v>244</v>
+        <v>224</v>
       </c>
       <c r="B937" s="7" t="s">
-        <v>245</v>
+        <v>225</v>
       </c>
     </row>
     <row r="938" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A938" s="8" t="s">
-        <v>246</v>
+        <v>226</v>
       </c>
       <c r="B938" s="7" t="s">
-        <v>247</v>
+        <v>227</v>
       </c>
     </row>
     <row r="939" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A939" s="8" t="s">
-        <v>248</v>
+        <v>228</v>
       </c>
       <c r="B939" s="7" t="s">
-        <v>249</v>
+        <v>229</v>
       </c>
     </row>
     <row r="940" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A940" s="8" t="s">
-        <v>250</v>
+        <v>230</v>
       </c>
       <c r="B940" s="7" t="s">
-        <v>251</v>
+        <v>231</v>
       </c>
     </row>
     <row r="941" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A941" s="8" t="s">
-        <v>252</v>
+        <v>232</v>
       </c>
       <c r="B941" s="7" t="s">
-        <v>253</v>
+        <v>233</v>
       </c>
     </row>
     <row r="942" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A942" s="8" t="s">
-        <v>254</v>
+        <v>234</v>
       </c>
       <c r="B942" s="7" t="s">
-        <v>255</v>
+        <v>235</v>
       </c>
     </row>
     <row r="943" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A943" s="8" t="s">
-        <v>256</v>
+        <v>236</v>
       </c>
       <c r="B943" s="7" t="s">
-        <v>257</v>
+        <v>237</v>
       </c>
     </row>
     <row r="944" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A944" s="8" t="s">
-        <v>258</v>
+        <v>238</v>
       </c>
       <c r="B944" s="7" t="s">
-        <v>259</v>
+        <v>239</v>
       </c>
     </row>
     <row r="945" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A945" s="8" t="s">
-        <v>260</v>
+        <v>240</v>
       </c>
       <c r="B945" s="7" t="s">
-        <v>261</v>
+        <v>241</v>
       </c>
     </row>
     <row r="946" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A946" s="8" t="s">
-        <v>262</v>
+        <v>242</v>
       </c>
       <c r="B946" s="7" t="s">
-        <v>263</v>
+        <v>243</v>
       </c>
     </row>
     <row r="947" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A947" s="8" t="s">
-        <v>264</v>
+        <v>244</v>
       </c>
       <c r="B947" s="7" t="s">
-        <v>265</v>
+        <v>245</v>
       </c>
     </row>
     <row r="948" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A948" s="8" t="s">
-        <v>266</v>
+        <v>246</v>
       </c>
       <c r="B948" s="7" t="s">
-        <v>267</v>
+        <v>247</v>
       </c>
     </row>
     <row r="949" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A949" s="8" t="s">
-        <v>268</v>
+        <v>248</v>
       </c>
       <c r="B949" s="7" t="s">
-        <v>269</v>
+        <v>249</v>
       </c>
     </row>
     <row r="950" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A950" s="8" t="s">
-        <v>270</v>
+        <v>250</v>
       </c>
       <c r="B950" s="7" t="s">
-        <v>271</v>
+        <v>251</v>
       </c>
     </row>
     <row r="951" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A951" s="8" t="s">
-        <v>272</v>
+        <v>252</v>
       </c>
       <c r="B951" s="7" t="s">
-        <v>273</v>
+        <v>253</v>
       </c>
     </row>
     <row r="952" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A952" s="8" t="s">
-        <v>274</v>
+        <v>254</v>
       </c>
       <c r="B952" s="7" t="s">
-        <v>275</v>
+        <v>255</v>
       </c>
     </row>
     <row r="953" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A953" s="8" t="s">
-        <v>276</v>
+        <v>256</v>
       </c>
       <c r="B953" s="7" t="s">
-        <v>277</v>
+        <v>257</v>
       </c>
     </row>
     <row r="954" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A954" s="8" t="s">
-        <v>278</v>
+        <v>258</v>
       </c>
       <c r="B954" s="7" t="s">
-        <v>279</v>
+        <v>259</v>
       </c>
     </row>
     <row r="955" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A955" s="8" t="s">
-        <v>280</v>
+        <v>260</v>
       </c>
       <c r="B955" s="7" t="s">
-        <v>281</v>
+        <v>261</v>
       </c>
     </row>
     <row r="956" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A956" s="8" t="s">
-        <v>282</v>
+        <v>262</v>
       </c>
       <c r="B956" s="7" t="s">
-        <v>283</v>
+        <v>263</v>
       </c>
     </row>
     <row r="957" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A957" s="8" t="s">
-        <v>284</v>
+        <v>264</v>
       </c>
       <c r="B957" s="7" t="s">
-        <v>285</v>
+        <v>265</v>
       </c>
     </row>
     <row r="958" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A958" s="8" t="s">
-        <v>286</v>
+        <v>266</v>
       </c>
       <c r="B958" s="7" t="s">
-        <v>287</v>
+        <v>267</v>
       </c>
     </row>
     <row r="959" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A959" s="8" t="s">
-        <v>288</v>
+        <v>268</v>
       </c>
       <c r="B959" s="7" t="s">
-        <v>289</v>
+        <v>269</v>
       </c>
     </row>
     <row r="960" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A960" s="8" t="s">
-        <v>290</v>
+        <v>270</v>
       </c>
       <c r="B960" s="7" t="s">
-        <v>291</v>
+        <v>271</v>
       </c>
     </row>
     <row r="961" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A961" s="8" t="s">
-        <v>292</v>
+        <v>272</v>
       </c>
       <c r="B961" s="7" t="s">
-        <v>293</v>
+        <v>273</v>
       </c>
     </row>
     <row r="962" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A962" s="8" t="s">
-        <v>294</v>
+        <v>274</v>
       </c>
       <c r="B962" s="7" t="s">
-        <v>295</v>
+        <v>275</v>
       </c>
     </row>
     <row r="963" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A963" s="8" t="s">
-        <v>296</v>
+        <v>276</v>
       </c>
       <c r="B963" s="7" t="s">
-        <v>295</v>
+        <v>277</v>
       </c>
     </row>
     <row r="964" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A964" s="8" t="s">
-        <v>297</v>
+        <v>278</v>
       </c>
       <c r="B964" s="7" t="s">
-        <v>298</v>
+        <v>279</v>
       </c>
     </row>
     <row r="965" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A965" s="8" t="s">
-        <v>299</v>
+        <v>280</v>
       </c>
       <c r="B965" s="7" t="s">
-        <v>237</v>
+        <v>281</v>
       </c>
     </row>
     <row r="966" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A966" s="8" t="s">
-        <v>300</v>
+        <v>282</v>
       </c>
       <c r="B966" s="7" t="s">
-        <v>239</v>
+        <v>283</v>
       </c>
     </row>
     <row r="967" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A967" s="8" t="s">
-        <v>301</v>
+        <v>284</v>
       </c>
       <c r="B967" s="7" t="s">
-        <v>302</v>
+        <v>285</v>
       </c>
     </row>
     <row r="968" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A968" s="8" t="s">
-        <v>303</v>
+        <v>286</v>
       </c>
       <c r="B968" s="7" t="s">
-        <v>304</v>
+        <v>287</v>
       </c>
     </row>
     <row r="969" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A969" s="8" t="s">
-        <v>305</v>
+        <v>288</v>
       </c>
       <c r="B969" s="7" t="s">
-        <v>306</v>
+        <v>289</v>
       </c>
     </row>
     <row r="970" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A970" s="8" t="s">
-        <v>307</v>
+        <v>290</v>
       </c>
       <c r="B970" s="7" t="s">
-        <v>308</v>
+        <v>291</v>
       </c>
     </row>
     <row r="971" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A971" s="8" t="s">
-        <v>309</v>
+        <v>292</v>
       </c>
       <c r="B971" s="7" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="972" spans="1:2" ht="22.5" x14ac:dyDescent="0.2">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="972" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A972" s="8" t="s">
-        <v>311</v>
-      </c>
-      <c r="B972" s="9" t="s">
-        <v>312</v>
+        <v>294</v>
+      </c>
+      <c r="B972" s="7" t="s">
+        <v>295</v>
       </c>
     </row>
     <row r="973" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A973" s="8" t="s">
-        <v>313</v>
+        <v>296</v>
       </c>
       <c r="B973" s="7" t="s">
-        <v>314</v>
+        <v>295</v>
       </c>
     </row>
     <row r="974" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A974" s="8" t="s">
-        <v>315</v>
+        <v>297</v>
       </c>
       <c r="B974" s="7" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="975" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="975" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A975" s="8" t="s">
-        <v>317</v>
+        <v>299</v>
       </c>
       <c r="B975" s="7" t="s">
-        <v>318</v>
+        <v>237</v>
       </c>
     </row>
     <row r="976" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A976" s="8" t="s">
-        <v>319</v>
+        <v>300</v>
       </c>
       <c r="B976" s="7" t="s">
-        <v>320</v>
+        <v>239</v>
       </c>
     </row>
     <row r="977" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A977" s="8" t="s">
-        <v>321</v>
+        <v>301</v>
       </c>
       <c r="B977" s="7" t="s">
-        <v>322</v>
+        <v>302</v>
       </c>
     </row>
     <row r="978" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A978" s="8" t="s">
-        <v>323</v>
+        <v>303</v>
       </c>
       <c r="B978" s="7" t="s">
-        <v>324</v>
+        <v>304</v>
       </c>
     </row>
     <row r="979" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A979" s="8" t="s">
-        <v>325</v>
+        <v>305</v>
       </c>
       <c r="B979" s="7" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="980" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="980" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A980" s="8" t="s">
-        <v>327</v>
+        <v>307</v>
       </c>
       <c r="B980" s="7" t="s">
-        <v>328</v>
+        <v>308</v>
       </c>
     </row>
     <row r="981" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A981" s="8" t="s">
-        <v>329</v>
+        <v>309</v>
       </c>
       <c r="B981" s="7" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="982" spans="1:2" x14ac:dyDescent="0.2">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="982" spans="1:2" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A982" s="8" t="s">
-        <v>330</v>
-      </c>
-      <c r="B982" s="7" t="s">
-        <v>331</v>
+        <v>311</v>
+      </c>
+      <c r="B982" s="9" t="s">
+        <v>312</v>
       </c>
     </row>
     <row r="983" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A983" s="8" t="s">
-        <v>332</v>
+        <v>313</v>
       </c>
       <c r="B983" s="7" t="s">
-        <v>333</v>
+        <v>314</v>
       </c>
     </row>
     <row r="984" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A984" s="8" t="s">
-        <v>334</v>
+        <v>315</v>
       </c>
       <c r="B984" s="7" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="985" spans="1:2" x14ac:dyDescent="0.2">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="985" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A985" s="8" t="s">
-        <v>336</v>
+        <v>317</v>
       </c>
       <c r="B985" s="7" t="s">
-        <v>337</v>
+        <v>318</v>
       </c>
     </row>
     <row r="986" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A986" s="8" t="s">
-        <v>338</v>
+        <v>319</v>
       </c>
       <c r="B986" s="7" t="s">
-        <v>339</v>
+        <v>320</v>
       </c>
     </row>
     <row r="987" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A987" s="8" t="s">
-        <v>340</v>
+        <v>321</v>
       </c>
       <c r="B987" s="7" t="s">
-        <v>341</v>
+        <v>322</v>
       </c>
     </row>
     <row r="988" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A988" s="8" t="s">
-        <v>342</v>
+        <v>323</v>
       </c>
       <c r="B988" s="7" t="s">
-        <v>343</v>
+        <v>324</v>
       </c>
     </row>
     <row r="989" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A989" s="8" t="s">
-        <v>344</v>
+        <v>325</v>
       </c>
       <c r="B989" s="7" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="990" spans="1:2" x14ac:dyDescent="0.2">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="990" spans="1:2" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A990" s="8" t="s">
-        <v>346</v>
+        <v>327</v>
       </c>
       <c r="B990" s="7" t="s">
-        <v>347</v>
+        <v>328</v>
       </c>
     </row>
     <row r="991" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A991" s="8" t="s">
-        <v>348</v>
+        <v>329</v>
       </c>
       <c r="B991" s="7" t="s">
-        <v>349</v>
+        <v>295</v>
       </c>
     </row>
     <row r="992" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A992" s="8" t="s">
-        <v>350</v>
+        <v>330</v>
       </c>
       <c r="B992" s="7" t="s">
-        <v>351</v>
+        <v>331</v>
       </c>
     </row>
     <row r="993" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A993" s="8" t="s">
-        <v>352</v>
+        <v>332</v>
       </c>
       <c r="B993" s="7" t="s">
-        <v>353</v>
+        <v>333</v>
       </c>
     </row>
     <row r="994" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A994" s="8" t="s">
-        <v>354</v>
+        <v>334</v>
       </c>
       <c r="B994" s="7" t="s">
-        <v>355</v>
+        <v>335</v>
       </c>
     </row>
     <row r="995" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A995" s="8" t="s">
-        <v>356</v>
+        <v>336</v>
       </c>
       <c r="B995" s="7" t="s">
-        <v>357</v>
+        <v>337</v>
       </c>
     </row>
     <row r="996" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A996" s="8" t="s">
-        <v>358</v>
+        <v>338</v>
       </c>
       <c r="B996" s="7" t="s">
-        <v>359</v>
+        <v>339</v>
       </c>
     </row>
     <row r="997" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A997" s="8" t="s">
-        <v>360</v>
+        <v>340</v>
       </c>
       <c r="B997" s="7" t="s">
-        <v>77</v>
+        <v>341</v>
       </c>
     </row>
     <row r="998" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A998" s="8" t="s">
-        <v>361</v>
+        <v>342</v>
       </c>
       <c r="B998" s="7" t="s">
-        <v>362</v>
+        <v>343</v>
       </c>
     </row>
     <row r="999" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A999" s="8" t="s">
-        <v>363</v>
+        <v>344</v>
       </c>
       <c r="B999" s="7" t="s">
-        <v>364</v>
+        <v>345</v>
       </c>
     </row>
     <row r="1000" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1000" s="8" t="s">
-        <v>365</v>
+        <v>346</v>
       </c>
       <c r="B1000" s="7" t="s">
-        <v>366</v>
+        <v>347</v>
       </c>
     </row>
     <row r="1001" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1001" s="8" t="s">
-        <v>367</v>
+        <v>348</v>
       </c>
       <c r="B1001" s="7" t="s">
-        <v>368</v>
+        <v>349</v>
       </c>
     </row>
     <row r="1002" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1002" s="8" t="s">
-        <v>369</v>
+        <v>350</v>
       </c>
       <c r="B1002" s="7" t="s">
-        <v>370</v>
+        <v>351</v>
       </c>
     </row>
     <row r="1003" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1003" s="8" t="s">
-        <v>371</v>
+        <v>352</v>
       </c>
       <c r="B1003" s="7" t="s">
-        <v>372</v>
+        <v>353</v>
       </c>
     </row>
     <row r="1004" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1004" s="8" t="s">
-        <v>373</v>
+        <v>354</v>
       </c>
       <c r="B1004" s="7" t="s">
-        <v>77</v>
+        <v>355</v>
       </c>
     </row>
     <row r="1005" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1005" s="8" t="s">
-        <v>374</v>
+        <v>356</v>
       </c>
       <c r="B1005" s="7" t="s">
-        <v>281</v>
+        <v>357</v>
       </c>
     </row>
     <row r="1006" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1006" s="8" t="s">
-        <v>375</v>
+        <v>358</v>
       </c>
       <c r="B1006" s="7" t="s">
-        <v>376</v>
+        <v>359</v>
       </c>
     </row>
     <row r="1007" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1007" s="8" t="s">
-        <v>377</v>
+        <v>360</v>
       </c>
       <c r="B1007" s="7" t="s">
-        <v>378</v>
+        <v>77</v>
       </c>
     </row>
     <row r="1008" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1008" s="8" t="s">
-        <v>379</v>
+        <v>361</v>
       </c>
       <c r="B1008" s="7" t="s">
-        <v>380</v>
+        <v>362</v>
       </c>
     </row>
     <row r="1009" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1009" s="8" t="s">
-        <v>381</v>
+        <v>363</v>
       </c>
       <c r="B1009" s="7" t="s">
-        <v>382</v>
+        <v>364</v>
       </c>
     </row>
     <row r="1010" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1010" s="8" t="s">
-        <v>383</v>
+        <v>365</v>
       </c>
       <c r="B1010" s="7" t="s">
-        <v>384</v>
+        <v>366</v>
       </c>
     </row>
     <row r="1011" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1011" s="8" t="s">
-        <v>385</v>
+        <v>367</v>
       </c>
       <c r="B1011" s="7" t="s">
-        <v>386</v>
+        <v>368</v>
       </c>
     </row>
     <row r="1012" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1012" s="8" t="s">
-        <v>387</v>
+        <v>369</v>
       </c>
       <c r="B1012" s="7" t="s">
-        <v>388</v>
+        <v>370</v>
       </c>
     </row>
     <row r="1013" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1013" s="8" t="s">
-        <v>389</v>
+        <v>371</v>
       </c>
       <c r="B1013" s="7" t="s">
-        <v>175</v>
+        <v>372</v>
       </c>
     </row>
     <row r="1014" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1014" s="8" t="s">
-        <v>390</v>
+        <v>373</v>
       </c>
       <c r="B1014" s="7" t="s">
-        <v>391</v>
+        <v>77</v>
       </c>
     </row>
     <row r="1015" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1015" s="8" t="s">
+        <v>374</v>
+      </c>
+      <c r="B1015" s="7" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="1016" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1016" s="8" t="s">
+        <v>375</v>
+      </c>
+      <c r="B1016" s="7" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="1017" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1017" s="8" t="s">
+        <v>377</v>
+      </c>
+      <c r="B1017" s="7" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="1018" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1018" s="8" t="s">
+        <v>379</v>
+      </c>
+      <c r="B1018" s="7" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="1019" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1019" s="8" t="s">
+        <v>381</v>
+      </c>
+      <c r="B1019" s="7" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="1020" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1020" s="8" t="s">
+        <v>383</v>
+      </c>
+      <c r="B1020" s="7" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="1021" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1021" s="8" t="s">
+        <v>385</v>
+      </c>
+      <c r="B1021" s="7" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="1022" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1022" s="8" t="s">
+        <v>387</v>
+      </c>
+      <c r="B1022" s="7" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="1023" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1023" s="8" t="s">
+        <v>389</v>
+      </c>
+      <c r="B1023" s="7" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="1024" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1024" s="8" t="s">
+        <v>390</v>
+      </c>
+      <c r="B1024" s="7" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="1025" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1025" s="8" t="s">
         <v>392</v>
       </c>
-      <c r="B1015" s="7" t="s">
+      <c r="B1025" s="7" t="s">
         <v>393</v>
-      </c>
-    </row>
-    <row r="1016" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1016" s="10" t="s">
-        <v>394</v>
-      </c>
-      <c r="B1016" s="7" t="s">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="1017" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1017" s="10" t="s">
-        <v>396</v>
-      </c>
-      <c r="B1017" s="7" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="1018" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1018" s="10" t="s">
-        <v>398</v>
-      </c>
-      <c r="B1018" s="7" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="1019" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1019" s="10" t="s">
-        <v>400</v>
-      </c>
-      <c r="B1019" s="7" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="1020" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1020" s="10" t="s">
-        <v>402</v>
-      </c>
-      <c r="B1020" s="7" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="1021" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1021" s="10" t="s">
-        <v>404</v>
-      </c>
-      <c r="B1021" s="7" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="1022" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1022" s="10" t="s">
-        <v>406</v>
-      </c>
-      <c r="B1022" s="7" t="s">
-        <v>407</v>
-      </c>
-    </row>
-    <row r="1023" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1023" s="10" t="s">
-        <v>408</v>
-      </c>
-      <c r="B1023" s="7" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="1024" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1024" s="10" t="s">
-        <v>410</v>
-      </c>
-      <c r="B1024" s="7" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="1025" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1025" s="10" t="s">
-        <v>411</v>
-      </c>
-      <c r="B1025" s="7" t="s">
-        <v>412</v>
       </c>
     </row>
     <row r="1026" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1026" s="10" t="s">
-        <v>413</v>
+        <v>394</v>
       </c>
       <c r="B1026" s="7" t="s">
-        <v>412</v>
+        <v>395</v>
       </c>
     </row>
     <row r="1027" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1027" s="10" t="s">
-        <v>414</v>
+        <v>396</v>
       </c>
       <c r="B1027" s="7" t="s">
-        <v>215</v>
+        <v>397</v>
       </c>
     </row>
     <row r="1028" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1028" s="10" t="s">
-        <v>415</v>
+        <v>398</v>
       </c>
       <c r="B1028" s="7" t="s">
-        <v>217</v>
+        <v>399</v>
       </c>
     </row>
     <row r="1029" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1029" s="10" t="s">
-        <v>416</v>
+        <v>400</v>
       </c>
       <c r="B1029" s="7" t="s">
         <v>401</v>
@@ -13605,7 +13634,7 @@
     </row>
     <row r="1030" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1030" s="10" t="s">
-        <v>417</v>
+        <v>402</v>
       </c>
       <c r="B1030" s="7" t="s">
         <v>403</v>
@@ -13613,7 +13642,7 @@
     </row>
     <row r="1031" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1031" s="10" t="s">
-        <v>418</v>
+        <v>404</v>
       </c>
       <c r="B1031" s="7" t="s">
         <v>405</v>
@@ -13621,7 +13650,7 @@
     </row>
     <row r="1032" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1032" s="10" t="s">
-        <v>419</v>
+        <v>406</v>
       </c>
       <c r="B1032" s="7" t="s">
         <v>407</v>
@@ -13629,1537 +13658,1617 @@
     </row>
     <row r="1033" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1033" s="10" t="s">
-        <v>420</v>
+        <v>408</v>
       </c>
       <c r="B1033" s="7" t="s">
-        <v>395</v>
+        <v>409</v>
       </c>
     </row>
     <row r="1034" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1034" s="10" t="s">
-        <v>421</v>
+        <v>410</v>
       </c>
       <c r="B1034" s="7" t="s">
-        <v>397</v>
+        <v>409</v>
       </c>
     </row>
     <row r="1035" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1035" s="10" t="s">
-        <v>422</v>
+        <v>411</v>
       </c>
       <c r="B1035" s="7" t="s">
-        <v>399</v>
+        <v>412</v>
       </c>
     </row>
     <row r="1036" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1036" s="10" t="s">
-        <v>423</v>
+        <v>413</v>
       </c>
       <c r="B1036" s="7" t="s">
-        <v>273</v>
+        <v>412</v>
       </c>
     </row>
     <row r="1037" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1037" s="10" t="s">
-        <v>424</v>
+        <v>414</v>
       </c>
       <c r="B1037" s="7" t="s">
-        <v>275</v>
+        <v>215</v>
       </c>
     </row>
     <row r="1038" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1038" s="10" t="s">
-        <v>425</v>
+        <v>415</v>
       </c>
       <c r="B1038" s="7" t="s">
-        <v>320</v>
+        <v>217</v>
       </c>
     </row>
     <row r="1039" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1039" s="10" t="s">
-        <v>426</v>
+        <v>416</v>
       </c>
       <c r="B1039" s="7" t="s">
-        <v>281</v>
+        <v>401</v>
       </c>
     </row>
     <row r="1040" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1040" s="10" t="s">
-        <v>427</v>
+        <v>417</v>
       </c>
       <c r="B1040" s="7" t="s">
-        <v>428</v>
+        <v>403</v>
       </c>
     </row>
     <row r="1041" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1041" s="10" t="s">
-        <v>429</v>
+        <v>418</v>
       </c>
       <c r="B1041" s="7" t="s">
-        <v>295</v>
+        <v>405</v>
       </c>
     </row>
     <row r="1042" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1042" s="10" t="s">
-        <v>430</v>
+        <v>419</v>
       </c>
       <c r="B1042" s="7" t="s">
-        <v>431</v>
+        <v>407</v>
       </c>
     </row>
     <row r="1043" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1043" s="10" t="s">
-        <v>432</v>
+        <v>420</v>
       </c>
       <c r="B1043" s="7" t="s">
-        <v>433</v>
+        <v>395</v>
       </c>
     </row>
     <row r="1044" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1044" s="10" t="s">
-        <v>434</v>
+        <v>421</v>
       </c>
       <c r="B1044" s="7" t="s">
-        <v>435</v>
+        <v>397</v>
       </c>
     </row>
     <row r="1045" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1045" s="10" t="s">
-        <v>436</v>
+        <v>422</v>
       </c>
       <c r="B1045" s="7" t="s">
-        <v>437</v>
+        <v>399</v>
       </c>
     </row>
     <row r="1046" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1046" s="10" t="s">
-        <v>438</v>
+        <v>423</v>
       </c>
       <c r="B1046" s="7" t="s">
-        <v>439</v>
+        <v>273</v>
       </c>
     </row>
     <row r="1047" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1047" s="10" t="s">
-        <v>440</v>
+        <v>424</v>
       </c>
       <c r="B1047" s="7" t="s">
-        <v>441</v>
+        <v>275</v>
       </c>
     </row>
     <row r="1048" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1048" s="10" t="s">
-        <v>442</v>
+        <v>425</v>
       </c>
       <c r="B1048" s="7" t="s">
-        <v>443</v>
+        <v>320</v>
       </c>
     </row>
     <row r="1049" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1049" s="10" t="s">
-        <v>444</v>
+        <v>426</v>
       </c>
       <c r="B1049" s="7" t="s">
-        <v>407</v>
+        <v>281</v>
       </c>
     </row>
     <row r="1050" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1050" s="10" t="s">
-        <v>445</v>
+        <v>427</v>
       </c>
       <c r="B1050" s="7" t="s">
-        <v>446</v>
+        <v>428</v>
       </c>
     </row>
     <row r="1051" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1051" s="10" t="s">
-        <v>447</v>
+        <v>429</v>
       </c>
       <c r="B1051" s="7" t="s">
-        <v>448</v>
+        <v>295</v>
       </c>
     </row>
     <row r="1052" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1052" s="10" t="s">
-        <v>449</v>
+        <v>430</v>
       </c>
       <c r="B1052" s="7" t="s">
-        <v>450</v>
+        <v>431</v>
       </c>
     </row>
     <row r="1053" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1053" s="10" t="s">
-        <v>451</v>
+        <v>432</v>
       </c>
       <c r="B1053" s="7" t="s">
-        <v>452</v>
+        <v>433</v>
       </c>
     </row>
     <row r="1054" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1054" s="10" t="s">
-        <v>453</v>
+        <v>434</v>
       </c>
       <c r="B1054" s="7" t="s">
-        <v>454</v>
+        <v>435</v>
       </c>
     </row>
     <row r="1055" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1055" s="10" t="s">
-        <v>455</v>
+        <v>436</v>
       </c>
       <c r="B1055" s="7" t="s">
-        <v>456</v>
+        <v>437</v>
       </c>
     </row>
     <row r="1056" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1056" s="10" t="s">
-        <v>457</v>
+        <v>438</v>
       </c>
       <c r="B1056" s="7" t="s">
-        <v>458</v>
+        <v>439</v>
       </c>
     </row>
     <row r="1057" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1057" s="10" t="s">
-        <v>459</v>
+        <v>440</v>
       </c>
       <c r="B1057" s="7" t="s">
-        <v>460</v>
+        <v>441</v>
       </c>
     </row>
     <row r="1058" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1058" s="10" t="s">
-        <v>461</v>
+        <v>442</v>
       </c>
       <c r="B1058" s="7" t="s">
-        <v>462</v>
+        <v>443</v>
       </c>
     </row>
     <row r="1059" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1059" s="10" t="s">
-        <v>463</v>
+        <v>444</v>
       </c>
       <c r="B1059" s="7" t="s">
-        <v>464</v>
+        <v>407</v>
       </c>
     </row>
     <row r="1060" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1060" s="10" t="s">
-        <v>465</v>
+        <v>445</v>
       </c>
       <c r="B1060" s="7" t="s">
-        <v>466</v>
+        <v>446</v>
       </c>
     </row>
     <row r="1061" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1061" s="10" t="s">
-        <v>467</v>
+        <v>447</v>
       </c>
       <c r="B1061" s="7" t="s">
-        <v>468</v>
+        <v>448</v>
       </c>
     </row>
     <row r="1062" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1062" s="10" t="s">
-        <v>469</v>
+        <v>449</v>
       </c>
       <c r="B1062" s="7" t="s">
-        <v>470</v>
+        <v>450</v>
       </c>
     </row>
     <row r="1063" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1063" s="10" t="s">
-        <v>471</v>
+        <v>451</v>
       </c>
       <c r="B1063" s="7" t="s">
-        <v>472</v>
+        <v>452</v>
       </c>
     </row>
     <row r="1064" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1064" s="10" t="s">
-        <v>473</v>
+        <v>453</v>
       </c>
       <c r="B1064" s="7" t="s">
-        <v>474</v>
+        <v>454</v>
       </c>
     </row>
     <row r="1065" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1065" s="10" t="s">
-        <v>475</v>
+        <v>455</v>
       </c>
       <c r="B1065" s="7" t="s">
-        <v>476</v>
+        <v>456</v>
       </c>
     </row>
     <row r="1066" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1066" s="10" t="s">
-        <v>477</v>
+        <v>457</v>
       </c>
       <c r="B1066" s="7" t="s">
-        <v>478</v>
+        <v>458</v>
       </c>
     </row>
     <row r="1067" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1067" s="10" t="s">
-        <v>479</v>
+        <v>459</v>
       </c>
       <c r="B1067" s="7" t="s">
-        <v>480</v>
+        <v>460</v>
       </c>
     </row>
     <row r="1068" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1068" s="10" t="s">
-        <v>481</v>
+        <v>461</v>
       </c>
       <c r="B1068" s="7" t="s">
-        <v>482</v>
+        <v>462</v>
       </c>
     </row>
     <row r="1069" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1069" s="10" t="s">
-        <v>483</v>
+        <v>463</v>
       </c>
       <c r="B1069" s="7" t="s">
-        <v>484</v>
+        <v>464</v>
       </c>
     </row>
     <row r="1070" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1070" s="10" t="s">
-        <v>485</v>
+        <v>465</v>
       </c>
       <c r="B1070" s="7" t="s">
-        <v>486</v>
+        <v>466</v>
       </c>
     </row>
     <row r="1071" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1071" s="10" t="s">
-        <v>487</v>
+        <v>467</v>
       </c>
       <c r="B1071" s="7" t="s">
-        <v>488</v>
+        <v>468</v>
       </c>
     </row>
     <row r="1072" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1072" s="10" t="s">
-        <v>489</v>
+        <v>469</v>
       </c>
       <c r="B1072" s="7" t="s">
-        <v>490</v>
+        <v>470</v>
       </c>
     </row>
     <row r="1073" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1073" s="10" t="s">
-        <v>491</v>
+        <v>471</v>
       </c>
       <c r="B1073" s="7" t="s">
-        <v>492</v>
+        <v>472</v>
       </c>
     </row>
     <row r="1074" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1074" s="10" t="s">
-        <v>493</v>
+        <v>473</v>
       </c>
       <c r="B1074" s="7" t="s">
-        <v>494</v>
+        <v>474</v>
       </c>
     </row>
     <row r="1075" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1075" s="10" t="s">
-        <v>495</v>
+        <v>475</v>
       </c>
       <c r="B1075" s="7" t="s">
-        <v>496</v>
+        <v>476</v>
       </c>
     </row>
     <row r="1076" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1076" s="10" t="s">
-        <v>497</v>
+        <v>477</v>
       </c>
       <c r="B1076" s="7" t="s">
-        <v>498</v>
+        <v>478</v>
       </c>
     </row>
     <row r="1077" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1077" s="10" t="s">
-        <v>499</v>
+        <v>479</v>
       </c>
       <c r="B1077" s="7" t="s">
-        <v>500</v>
+        <v>480</v>
       </c>
     </row>
     <row r="1078" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1078" s="10" t="s">
-        <v>501</v>
+        <v>481</v>
       </c>
       <c r="B1078" s="7" t="s">
-        <v>502</v>
+        <v>482</v>
       </c>
     </row>
     <row r="1079" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1079" s="10" t="s">
-        <v>503</v>
+        <v>483</v>
       </c>
       <c r="B1079" s="7" t="s">
-        <v>504</v>
+        <v>484</v>
       </c>
     </row>
     <row r="1080" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1080" s="10" t="s">
-        <v>505</v>
+        <v>485</v>
       </c>
       <c r="B1080" s="7" t="s">
-        <v>506</v>
+        <v>486</v>
       </c>
     </row>
     <row r="1081" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1081" s="10" t="s">
-        <v>507</v>
+        <v>487</v>
       </c>
       <c r="B1081" s="7" t="s">
-        <v>508</v>
+        <v>488</v>
       </c>
     </row>
     <row r="1082" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1082" s="10" t="s">
-        <v>509</v>
+        <v>489</v>
       </c>
       <c r="B1082" s="7" t="s">
-        <v>510</v>
+        <v>490</v>
       </c>
     </row>
     <row r="1083" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1083" s="10" t="s">
-        <v>511</v>
+        <v>491</v>
       </c>
       <c r="B1083" s="7" t="s">
-        <v>512</v>
+        <v>492</v>
       </c>
     </row>
     <row r="1084" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1084" s="10" t="s">
-        <v>513</v>
+        <v>493</v>
       </c>
       <c r="B1084" s="7" t="s">
-        <v>514</v>
+        <v>494</v>
       </c>
     </row>
     <row r="1085" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1085" s="10" t="s">
-        <v>515</v>
+        <v>495</v>
       </c>
       <c r="B1085" s="7" t="s">
-        <v>516</v>
+        <v>496</v>
       </c>
     </row>
     <row r="1086" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1086" s="10" t="s">
-        <v>517</v>
+        <v>497</v>
       </c>
       <c r="B1086" s="7" t="s">
-        <v>518</v>
+        <v>498</v>
       </c>
     </row>
     <row r="1087" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1087" s="10" t="s">
-        <v>519</v>
+        <v>499</v>
       </c>
       <c r="B1087" s="7" t="s">
-        <v>520</v>
+        <v>500</v>
       </c>
     </row>
     <row r="1088" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1088" s="10" t="s">
-        <v>521</v>
+        <v>501</v>
       </c>
       <c r="B1088" s="7" t="s">
-        <v>522</v>
+        <v>502</v>
       </c>
     </row>
     <row r="1089" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1089" s="10" t="s">
-        <v>523</v>
+        <v>503</v>
       </c>
       <c r="B1089" s="7" t="s">
-        <v>524</v>
+        <v>504</v>
       </c>
     </row>
     <row r="1090" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1090" s="10" t="s">
-        <v>525</v>
+        <v>505</v>
       </c>
       <c r="B1090" s="7" t="s">
-        <v>526</v>
+        <v>506</v>
       </c>
     </row>
     <row r="1091" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1091" s="10" t="s">
-        <v>527</v>
+        <v>507</v>
       </c>
       <c r="B1091" s="7" t="s">
-        <v>528</v>
+        <v>508</v>
       </c>
     </row>
     <row r="1092" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1092" s="10" t="s">
-        <v>529</v>
+        <v>509</v>
       </c>
       <c r="B1092" s="7" t="s">
-        <v>530</v>
+        <v>510</v>
       </c>
     </row>
     <row r="1093" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1093" s="10" t="s">
-        <v>531</v>
+        <v>511</v>
       </c>
       <c r="B1093" s="7" t="s">
-        <v>532</v>
+        <v>512</v>
       </c>
     </row>
     <row r="1094" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1094" s="10" t="s">
-        <v>533</v>
+        <v>513</v>
       </c>
       <c r="B1094" s="7" t="s">
-        <v>534</v>
+        <v>514</v>
       </c>
     </row>
     <row r="1095" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1095" s="10" t="s">
-        <v>535</v>
+        <v>515</v>
       </c>
       <c r="B1095" s="7" t="s">
-        <v>536</v>
+        <v>516</v>
       </c>
     </row>
     <row r="1096" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1096" s="10" t="s">
-        <v>537</v>
+        <v>517</v>
       </c>
       <c r="B1096" s="7" t="s">
-        <v>538</v>
+        <v>518</v>
       </c>
     </row>
     <row r="1097" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1097" s="10" t="s">
-        <v>539</v>
+        <v>519</v>
       </c>
       <c r="B1097" s="7" t="s">
-        <v>540</v>
+        <v>520</v>
       </c>
     </row>
     <row r="1098" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1098" s="10" t="s">
-        <v>541</v>
+        <v>521</v>
       </c>
       <c r="B1098" s="7" t="s">
-        <v>542</v>
+        <v>522</v>
       </c>
     </row>
     <row r="1099" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1099" s="10" t="s">
-        <v>543</v>
+        <v>523</v>
       </c>
       <c r="B1099" s="7" t="s">
-        <v>544</v>
+        <v>524</v>
       </c>
     </row>
     <row r="1100" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1100" s="10" t="s">
-        <v>545</v>
+        <v>525</v>
       </c>
       <c r="B1100" s="7" t="s">
-        <v>546</v>
+        <v>526</v>
       </c>
     </row>
     <row r="1101" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1101" s="10" t="s">
-        <v>547</v>
+        <v>527</v>
       </c>
       <c r="B1101" s="7" t="s">
-        <v>548</v>
+        <v>528</v>
       </c>
     </row>
     <row r="1102" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1102" s="10" t="s">
-        <v>549</v>
+        <v>529</v>
       </c>
       <c r="B1102" s="7" t="s">
-        <v>550</v>
+        <v>530</v>
       </c>
     </row>
     <row r="1103" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1103" s="10" t="s">
-        <v>551</v>
+        <v>531</v>
       </c>
       <c r="B1103" s="7" t="s">
-        <v>552</v>
+        <v>532</v>
       </c>
     </row>
     <row r="1104" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1104" s="10" t="s">
-        <v>553</v>
+        <v>533</v>
       </c>
       <c r="B1104" s="7" t="s">
-        <v>554</v>
+        <v>534</v>
       </c>
     </row>
     <row r="1105" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1105" s="10" t="s">
-        <v>555</v>
+        <v>535</v>
       </c>
       <c r="B1105" s="7" t="s">
-        <v>556</v>
+        <v>536</v>
       </c>
     </row>
     <row r="1106" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1106" s="10" t="s">
-        <v>557</v>
+        <v>537</v>
       </c>
       <c r="B1106" s="7" t="s">
-        <v>558</v>
+        <v>538</v>
       </c>
     </row>
     <row r="1107" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1107" s="10" t="s">
-        <v>559</v>
+        <v>539</v>
       </c>
       <c r="B1107" s="7" t="s">
-        <v>560</v>
+        <v>540</v>
       </c>
     </row>
     <row r="1108" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1108" s="10" t="s">
-        <v>561</v>
+        <v>541</v>
       </c>
       <c r="B1108" s="7" t="s">
-        <v>562</v>
+        <v>542</v>
       </c>
     </row>
     <row r="1109" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1109" s="10" t="s">
-        <v>563</v>
+        <v>543</v>
       </c>
       <c r="B1109" s="7" t="s">
-        <v>564</v>
+        <v>544</v>
       </c>
     </row>
     <row r="1110" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1110" s="10" t="s">
-        <v>565</v>
+        <v>545</v>
       </c>
       <c r="B1110" s="7" t="s">
-        <v>566</v>
+        <v>546</v>
       </c>
     </row>
     <row r="1111" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1111" s="10" t="s">
-        <v>567</v>
+        <v>547</v>
       </c>
       <c r="B1111" s="7" t="s">
-        <v>568</v>
+        <v>548</v>
       </c>
     </row>
     <row r="1112" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1112" s="10" t="s">
-        <v>569</v>
+        <v>549</v>
       </c>
       <c r="B1112" s="7" t="s">
-        <v>570</v>
+        <v>550</v>
       </c>
     </row>
     <row r="1113" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1113" s="10" t="s">
-        <v>571</v>
+        <v>551</v>
       </c>
       <c r="B1113" s="7" t="s">
-        <v>572</v>
+        <v>552</v>
       </c>
     </row>
     <row r="1114" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1114" s="10" t="s">
-        <v>573</v>
+        <v>553</v>
       </c>
       <c r="B1114" s="7" t="s">
-        <v>574</v>
+        <v>554</v>
       </c>
     </row>
     <row r="1115" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1115" s="10" t="s">
-        <v>575</v>
+        <v>555</v>
       </c>
       <c r="B1115" s="7" t="s">
-        <v>576</v>
+        <v>556</v>
       </c>
     </row>
     <row r="1116" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1116" s="10" t="s">
-        <v>577</v>
+        <v>557</v>
       </c>
       <c r="B1116" s="7" t="s">
-        <v>578</v>
+        <v>558</v>
       </c>
     </row>
     <row r="1117" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1117" s="10" t="s">
-        <v>579</v>
+        <v>559</v>
       </c>
       <c r="B1117" s="7" t="s">
-        <v>580</v>
+        <v>560</v>
       </c>
     </row>
     <row r="1118" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1118" s="10" t="s">
-        <v>581</v>
+        <v>561</v>
       </c>
       <c r="B1118" s="7" t="s">
-        <v>582</v>
+        <v>562</v>
       </c>
     </row>
     <row r="1119" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1119" s="10" t="s">
-        <v>583</v>
+        <v>563</v>
       </c>
       <c r="B1119" s="7" t="s">
-        <v>584</v>
+        <v>564</v>
       </c>
     </row>
     <row r="1120" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1120" s="10" t="s">
-        <v>585</v>
+        <v>565</v>
       </c>
       <c r="B1120" s="7" t="s">
-        <v>586</v>
+        <v>566</v>
       </c>
     </row>
     <row r="1121" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1121" s="10" t="s">
-        <v>587</v>
+        <v>567</v>
       </c>
       <c r="B1121" s="7" t="s">
-        <v>588</v>
+        <v>568</v>
       </c>
     </row>
     <row r="1122" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1122" s="10" t="s">
-        <v>589</v>
+        <v>569</v>
       </c>
       <c r="B1122" s="7" t="s">
-        <v>590</v>
+        <v>570</v>
       </c>
     </row>
     <row r="1123" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1123" s="10" t="s">
-        <v>591</v>
+        <v>571</v>
       </c>
       <c r="B1123" s="7" t="s">
-        <v>592</v>
+        <v>572</v>
       </c>
     </row>
     <row r="1124" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1124" s="10" t="s">
-        <v>593</v>
+        <v>573</v>
       </c>
       <c r="B1124" s="7" t="s">
-        <v>594</v>
+        <v>574</v>
       </c>
     </row>
     <row r="1125" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1125" s="10" t="s">
-        <v>595</v>
+        <v>575</v>
       </c>
       <c r="B1125" s="7" t="s">
-        <v>596</v>
+        <v>576</v>
       </c>
     </row>
     <row r="1126" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1126" s="10" t="s">
-        <v>597</v>
+        <v>577</v>
       </c>
       <c r="B1126" s="7" t="s">
-        <v>598</v>
+        <v>578</v>
       </c>
     </row>
     <row r="1127" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1127" s="10" t="s">
-        <v>599</v>
+        <v>579</v>
       </c>
       <c r="B1127" s="7" t="s">
-        <v>600</v>
+        <v>580</v>
       </c>
     </row>
     <row r="1128" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1128" s="10" t="s">
-        <v>601</v>
+        <v>581</v>
       </c>
       <c r="B1128" s="7" t="s">
-        <v>602</v>
+        <v>582</v>
       </c>
     </row>
     <row r="1129" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1129" s="10" t="s">
-        <v>603</v>
+        <v>583</v>
       </c>
       <c r="B1129" s="7" t="s">
-        <v>604</v>
+        <v>584</v>
       </c>
     </row>
     <row r="1130" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1130" s="10" t="s">
-        <v>605</v>
+        <v>585</v>
       </c>
       <c r="B1130" s="7" t="s">
-        <v>606</v>
+        <v>586</v>
       </c>
     </row>
     <row r="1131" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1131" s="10" t="s">
-        <v>607</v>
+        <v>587</v>
       </c>
       <c r="B1131" s="7" t="s">
-        <v>608</v>
+        <v>588</v>
       </c>
     </row>
     <row r="1132" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1132" s="10" t="s">
-        <v>609</v>
+        <v>589</v>
       </c>
       <c r="B1132" s="7" t="s">
-        <v>610</v>
+        <v>590</v>
       </c>
     </row>
     <row r="1133" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1133" s="10" t="s">
-        <v>611</v>
+        <v>591</v>
       </c>
       <c r="B1133" s="7" t="s">
-        <v>612</v>
+        <v>592</v>
       </c>
     </row>
     <row r="1134" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1134" s="10" t="s">
-        <v>613</v>
+        <v>593</v>
       </c>
       <c r="B1134" s="7" t="s">
-        <v>614</v>
+        <v>594</v>
       </c>
     </row>
     <row r="1135" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1135" s="10" t="s">
-        <v>615</v>
+        <v>595</v>
       </c>
       <c r="B1135" s="7" t="s">
-        <v>616</v>
+        <v>596</v>
       </c>
     </row>
     <row r="1136" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1136" s="10" t="s">
-        <v>617</v>
+        <v>597</v>
       </c>
       <c r="B1136" s="7" t="s">
-        <v>618</v>
+        <v>598</v>
       </c>
     </row>
     <row r="1137" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1137" s="10" t="s">
-        <v>619</v>
+        <v>599</v>
       </c>
       <c r="B1137" s="7" t="s">
-        <v>620</v>
+        <v>600</v>
       </c>
     </row>
     <row r="1138" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1138" s="10" t="s">
-        <v>621</v>
+        <v>601</v>
       </c>
       <c r="B1138" s="7" t="s">
-        <v>622</v>
+        <v>602</v>
       </c>
     </row>
     <row r="1139" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1139" s="10" t="s">
-        <v>623</v>
+        <v>603</v>
       </c>
       <c r="B1139" s="7" t="s">
-        <v>624</v>
+        <v>604</v>
       </c>
     </row>
     <row r="1140" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1140" s="10" t="s">
-        <v>625</v>
+        <v>605</v>
       </c>
       <c r="B1140" s="7" t="s">
-        <v>626</v>
+        <v>606</v>
       </c>
     </row>
     <row r="1141" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1141" s="10" t="s">
-        <v>627</v>
+        <v>607</v>
       </c>
       <c r="B1141" s="7" t="s">
-        <v>628</v>
+        <v>608</v>
       </c>
     </row>
     <row r="1142" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1142" s="10" t="s">
-        <v>629</v>
+        <v>609</v>
       </c>
       <c r="B1142" s="7" t="s">
-        <v>630</v>
+        <v>610</v>
       </c>
     </row>
     <row r="1143" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1143" s="10" t="s">
-        <v>631</v>
+        <v>611</v>
       </c>
       <c r="B1143" s="7" t="s">
-        <v>632</v>
+        <v>612</v>
       </c>
     </row>
     <row r="1144" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1144" s="10" t="s">
-        <v>633</v>
+        <v>613</v>
       </c>
       <c r="B1144" s="7" t="s">
-        <v>634</v>
+        <v>614</v>
       </c>
     </row>
     <row r="1145" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1145" s="10" t="s">
-        <v>635</v>
+        <v>615</v>
       </c>
       <c r="B1145" s="7" t="s">
-        <v>636</v>
+        <v>616</v>
       </c>
     </row>
     <row r="1146" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1146" s="10" t="s">
-        <v>637</v>
+        <v>617</v>
       </c>
       <c r="B1146" s="7" t="s">
-        <v>638</v>
+        <v>618</v>
       </c>
     </row>
     <row r="1147" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1147" s="10" t="s">
-        <v>639</v>
+        <v>619</v>
       </c>
       <c r="B1147" s="7" t="s">
-        <v>640</v>
+        <v>620</v>
       </c>
     </row>
     <row r="1148" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1148" s="10" t="s">
-        <v>641</v>
+        <v>621</v>
       </c>
       <c r="B1148" s="7" t="s">
-        <v>642</v>
+        <v>622</v>
       </c>
     </row>
     <row r="1149" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1149" s="10" t="s">
-        <v>643</v>
+        <v>623</v>
       </c>
       <c r="B1149" s="7" t="s">
-        <v>644</v>
+        <v>624</v>
       </c>
     </row>
     <row r="1150" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1150" s="10" t="s">
-        <v>645</v>
+        <v>625</v>
       </c>
       <c r="B1150" s="7" t="s">
-        <v>646</v>
+        <v>626</v>
       </c>
     </row>
     <row r="1151" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1151" s="10" t="s">
-        <v>647</v>
+        <v>627</v>
       </c>
       <c r="B1151" s="7" t="s">
-        <v>648</v>
+        <v>628</v>
       </c>
     </row>
     <row r="1152" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1152" s="10" t="s">
-        <v>649</v>
+        <v>629</v>
       </c>
       <c r="B1152" s="7" t="s">
-        <v>650</v>
+        <v>630</v>
       </c>
     </row>
     <row r="1153" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1153" s="10" t="s">
-        <v>651</v>
+        <v>631</v>
       </c>
       <c r="B1153" s="7" t="s">
-        <v>652</v>
+        <v>632</v>
       </c>
     </row>
     <row r="1154" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1154" s="10" t="s">
-        <v>653</v>
+        <v>633</v>
       </c>
       <c r="B1154" s="7" t="s">
-        <v>654</v>
+        <v>634</v>
       </c>
     </row>
     <row r="1155" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1155" s="10" t="s">
-        <v>655</v>
+        <v>635</v>
       </c>
       <c r="B1155" s="7" t="s">
-        <v>656</v>
+        <v>636</v>
       </c>
     </row>
     <row r="1156" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1156" s="10" t="s">
-        <v>657</v>
+        <v>637</v>
       </c>
       <c r="B1156" s="7" t="s">
-        <v>658</v>
+        <v>638</v>
       </c>
     </row>
     <row r="1157" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1157" s="10" t="s">
-        <v>659</v>
+        <v>639</v>
       </c>
       <c r="B1157" s="7" t="s">
-        <v>660</v>
+        <v>640</v>
       </c>
     </row>
     <row r="1158" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1158" s="10" t="s">
-        <v>661</v>
+        <v>641</v>
       </c>
       <c r="B1158" s="7" t="s">
-        <v>662</v>
+        <v>642</v>
       </c>
     </row>
     <row r="1159" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1159" s="10" t="s">
-        <v>663</v>
+        <v>643</v>
       </c>
       <c r="B1159" s="7" t="s">
-        <v>664</v>
+        <v>644</v>
       </c>
     </row>
     <row r="1160" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1160" s="10" t="s">
-        <v>665</v>
+        <v>645</v>
       </c>
       <c r="B1160" s="7" t="s">
-        <v>666</v>
+        <v>646</v>
       </c>
     </row>
     <row r="1161" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1161" s="10" t="s">
-        <v>667</v>
+        <v>647</v>
       </c>
       <c r="B1161" s="7" t="s">
-        <v>668</v>
+        <v>648</v>
       </c>
     </row>
     <row r="1162" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1162" s="10" t="s">
-        <v>669</v>
+        <v>649</v>
       </c>
       <c r="B1162" s="7" t="s">
-        <v>670</v>
+        <v>650</v>
       </c>
     </row>
     <row r="1163" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1163" s="10" t="s">
-        <v>671</v>
+        <v>651</v>
       </c>
       <c r="B1163" s="7" t="s">
-        <v>672</v>
+        <v>652</v>
       </c>
     </row>
     <row r="1164" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1164" s="10" t="s">
-        <v>673</v>
+        <v>653</v>
       </c>
       <c r="B1164" s="7" t="s">
-        <v>674</v>
+        <v>654</v>
       </c>
     </row>
     <row r="1165" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1165" s="10" t="s">
-        <v>675</v>
+        <v>655</v>
       </c>
       <c r="B1165" s="7" t="s">
-        <v>676</v>
+        <v>656</v>
       </c>
     </row>
     <row r="1166" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1166" s="10" t="s">
-        <v>677</v>
+        <v>657</v>
       </c>
       <c r="B1166" s="7" t="s">
-        <v>678</v>
+        <v>658</v>
       </c>
     </row>
     <row r="1167" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1167" s="10" t="s">
-        <v>679</v>
+        <v>659</v>
       </c>
       <c r="B1167" s="7" t="s">
-        <v>680</v>
+        <v>660</v>
       </c>
     </row>
     <row r="1168" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1168" s="10" t="s">
-        <v>681</v>
+        <v>661</v>
       </c>
       <c r="B1168" s="7" t="s">
-        <v>682</v>
+        <v>662</v>
       </c>
     </row>
     <row r="1169" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1169" s="10" t="s">
-        <v>683</v>
+        <v>663</v>
       </c>
       <c r="B1169" s="7" t="s">
-        <v>684</v>
+        <v>664</v>
       </c>
     </row>
     <row r="1170" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1170" s="10" t="s">
-        <v>685</v>
+        <v>665</v>
       </c>
       <c r="B1170" s="7" t="s">
-        <v>686</v>
+        <v>666</v>
       </c>
     </row>
     <row r="1171" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1171" s="10" t="s">
-        <v>687</v>
+        <v>667</v>
       </c>
       <c r="B1171" s="7" t="s">
-        <v>688</v>
+        <v>668</v>
       </c>
     </row>
     <row r="1172" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1172" s="10" t="s">
-        <v>689</v>
+        <v>669</v>
       </c>
       <c r="B1172" s="7" t="s">
-        <v>690</v>
+        <v>670</v>
       </c>
     </row>
     <row r="1173" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1173" s="10" t="s">
-        <v>691</v>
+        <v>671</v>
       </c>
       <c r="B1173" s="7" t="s">
-        <v>692</v>
+        <v>672</v>
       </c>
     </row>
     <row r="1174" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1174" s="10" t="s">
-        <v>693</v>
+        <v>673</v>
       </c>
       <c r="B1174" s="7" t="s">
-        <v>694</v>
+        <v>674</v>
       </c>
     </row>
     <row r="1175" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1175" s="10" t="s">
-        <v>695</v>
+        <v>675</v>
       </c>
       <c r="B1175" s="7" t="s">
-        <v>696</v>
+        <v>676</v>
       </c>
     </row>
     <row r="1176" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1176" s="10" t="s">
-        <v>697</v>
+        <v>677</v>
       </c>
       <c r="B1176" s="7" t="s">
-        <v>698</v>
+        <v>678</v>
       </c>
     </row>
     <row r="1177" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1177" s="10" t="s">
-        <v>699</v>
+        <v>679</v>
       </c>
       <c r="B1177" s="7" t="s">
-        <v>700</v>
+        <v>680</v>
       </c>
     </row>
     <row r="1178" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1178" s="10" t="s">
-        <v>701</v>
+        <v>681</v>
       </c>
       <c r="B1178" s="7" t="s">
-        <v>702</v>
+        <v>682</v>
       </c>
     </row>
     <row r="1179" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1179" s="10" t="s">
-        <v>703</v>
+        <v>683</v>
       </c>
       <c r="B1179" s="7" t="s">
-        <v>704</v>
+        <v>684</v>
       </c>
     </row>
     <row r="1180" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1180" s="10" t="s">
-        <v>705</v>
+        <v>685</v>
       </c>
       <c r="B1180" s="7" t="s">
-        <v>706</v>
+        <v>686</v>
       </c>
     </row>
     <row r="1181" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1181" s="10" t="s">
-        <v>707</v>
+        <v>687</v>
       </c>
       <c r="B1181" s="7" t="s">
-        <v>708</v>
+        <v>688</v>
       </c>
     </row>
     <row r="1182" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1182" s="10" t="s">
-        <v>709</v>
+        <v>689</v>
       </c>
       <c r="B1182" s="7" t="s">
-        <v>710</v>
+        <v>690</v>
       </c>
     </row>
     <row r="1183" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1183" s="10" t="s">
-        <v>711</v>
+        <v>691</v>
       </c>
       <c r="B1183" s="7" t="s">
-        <v>712</v>
+        <v>692</v>
       </c>
     </row>
     <row r="1184" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1184" s="10" t="s">
-        <v>713</v>
+        <v>693</v>
       </c>
       <c r="B1184" s="7" t="s">
-        <v>714</v>
+        <v>694</v>
       </c>
     </row>
     <row r="1185" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1185" s="10" t="s">
-        <v>715</v>
+        <v>695</v>
       </c>
       <c r="B1185" s="7" t="s">
-        <v>716</v>
+        <v>696</v>
       </c>
     </row>
     <row r="1186" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1186" s="10" t="s">
-        <v>717</v>
+        <v>697</v>
       </c>
       <c r="B1186" s="7" t="s">
-        <v>718</v>
+        <v>698</v>
       </c>
     </row>
     <row r="1187" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1187" s="10" t="s">
-        <v>719</v>
+        <v>699</v>
       </c>
       <c r="B1187" s="7" t="s">
-        <v>720</v>
+        <v>700</v>
       </c>
     </row>
     <row r="1188" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1188" s="10" t="s">
-        <v>721</v>
+        <v>701</v>
       </c>
       <c r="B1188" s="7" t="s">
-        <v>722</v>
+        <v>702</v>
       </c>
     </row>
     <row r="1189" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1189" s="10" t="s">
-        <v>723</v>
+        <v>703</v>
       </c>
       <c r="B1189" s="7" t="s">
-        <v>724</v>
+        <v>704</v>
       </c>
     </row>
     <row r="1190" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1190" s="10" t="s">
-        <v>725</v>
+        <v>705</v>
       </c>
       <c r="B1190" s="7" t="s">
-        <v>726</v>
+        <v>706</v>
       </c>
     </row>
     <row r="1191" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1191" s="10" t="s">
-        <v>727</v>
+        <v>707</v>
       </c>
       <c r="B1191" s="7" t="s">
-        <v>728</v>
+        <v>708</v>
       </c>
     </row>
     <row r="1192" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1192" s="10" t="s">
-        <v>729</v>
+        <v>709</v>
       </c>
       <c r="B1192" s="7" t="s">
-        <v>730</v>
+        <v>710</v>
       </c>
     </row>
     <row r="1193" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1193" s="10" t="s">
-        <v>731</v>
+        <v>711</v>
       </c>
       <c r="B1193" s="7" t="s">
-        <v>732</v>
+        <v>712</v>
       </c>
     </row>
     <row r="1194" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1194" s="10" t="s">
-        <v>733</v>
+        <v>713</v>
       </c>
       <c r="B1194" s="7" t="s">
-        <v>734</v>
+        <v>714</v>
       </c>
     </row>
     <row r="1195" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1195" s="10" t="s">
-        <v>735</v>
+        <v>715</v>
       </c>
       <c r="B1195" s="7" t="s">
-        <v>736</v>
+        <v>716</v>
       </c>
     </row>
     <row r="1196" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1196" s="10" t="s">
-        <v>737</v>
+        <v>717</v>
       </c>
       <c r="B1196" s="7" t="s">
-        <v>738</v>
+        <v>718</v>
       </c>
     </row>
     <row r="1197" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1197" s="10" t="s">
-        <v>739</v>
+        <v>719</v>
       </c>
       <c r="B1197" s="7" t="s">
-        <v>740</v>
+        <v>720</v>
       </c>
     </row>
     <row r="1198" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1198" s="10" t="s">
-        <v>741</v>
+        <v>721</v>
       </c>
       <c r="B1198" s="7" t="s">
-        <v>742</v>
+        <v>722</v>
       </c>
     </row>
     <row r="1199" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1199" s="10" t="s">
-        <v>743</v>
+        <v>723</v>
       </c>
       <c r="B1199" s="7" t="s">
-        <v>744</v>
+        <v>724</v>
       </c>
     </row>
     <row r="1200" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1200" s="10" t="s">
-        <v>745</v>
+        <v>725</v>
       </c>
       <c r="B1200" s="7" t="s">
-        <v>746</v>
+        <v>726</v>
       </c>
     </row>
     <row r="1201" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1201" s="10" t="s">
-        <v>747</v>
+        <v>727</v>
       </c>
       <c r="B1201" s="7" t="s">
-        <v>748</v>
+        <v>728</v>
       </c>
     </row>
     <row r="1202" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1202" s="10" t="s">
-        <v>749</v>
+        <v>729</v>
       </c>
       <c r="B1202" s="7" t="s">
-        <v>750</v>
+        <v>730</v>
       </c>
     </row>
     <row r="1203" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1203" s="10" t="s">
-        <v>751</v>
+        <v>731</v>
       </c>
       <c r="B1203" s="7" t="s">
-        <v>752</v>
+        <v>732</v>
       </c>
     </row>
     <row r="1204" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1204" s="10" t="s">
-        <v>753</v>
+        <v>733</v>
       </c>
       <c r="B1204" s="7" t="s">
-        <v>754</v>
+        <v>734</v>
       </c>
     </row>
     <row r="1205" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1205" s="10" t="s">
-        <v>755</v>
+        <v>735</v>
       </c>
       <c r="B1205" s="7" t="s">
-        <v>756</v>
+        <v>736</v>
       </c>
     </row>
     <row r="1206" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1206" s="10" t="s">
-        <v>757</v>
+        <v>737</v>
       </c>
       <c r="B1206" s="7" t="s">
-        <v>758</v>
+        <v>738</v>
       </c>
     </row>
     <row r="1207" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1207" s="10" t="s">
-        <v>759</v>
+        <v>739</v>
       </c>
       <c r="B1207" s="7" t="s">
-        <v>760</v>
+        <v>740</v>
       </c>
     </row>
     <row r="1208" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1208" s="10" t="s">
-        <v>761</v>
+        <v>741</v>
       </c>
       <c r="B1208" s="7" t="s">
-        <v>762</v>
+        <v>742</v>
       </c>
     </row>
     <row r="1209" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1209" s="10" t="s">
-        <v>763</v>
+        <v>743</v>
       </c>
       <c r="B1209" s="7" t="s">
-        <v>764</v>
+        <v>744</v>
       </c>
     </row>
     <row r="1210" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1210" s="10" t="s">
-        <v>765</v>
+        <v>745</v>
       </c>
       <c r="B1210" s="7" t="s">
-        <v>766</v>
+        <v>746</v>
       </c>
     </row>
     <row r="1211" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1211" s="10" t="s">
-        <v>767</v>
+        <v>747</v>
       </c>
       <c r="B1211" s="7" t="s">
-        <v>304</v>
+        <v>748</v>
       </c>
     </row>
     <row r="1212" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1212" s="10" t="s">
-        <v>768</v>
+        <v>749</v>
       </c>
       <c r="B1212" s="7" t="s">
-        <v>769</v>
+        <v>750</v>
       </c>
     </row>
     <row r="1213" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1213" s="10" t="s">
-        <v>770</v>
+        <v>751</v>
       </c>
       <c r="B1213" s="7" t="s">
-        <v>316</v>
+        <v>752</v>
       </c>
     </row>
     <row r="1214" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1214" s="10" t="s">
-        <v>771</v>
+        <v>753</v>
       </c>
       <c r="B1214" s="7" t="s">
-        <v>211</v>
+        <v>754</v>
       </c>
     </row>
     <row r="1215" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1215" s="10" t="s">
-        <v>772</v>
+        <v>755</v>
       </c>
       <c r="B1215" s="7" t="s">
-        <v>213</v>
+        <v>756</v>
       </c>
     </row>
     <row r="1216" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1216" s="10" t="s">
-        <v>773</v>
+        <v>757</v>
       </c>
       <c r="B1216" s="7" t="s">
-        <v>774</v>
-      </c>
-    </row>
-    <row r="1217" spans="1:2" ht="22.5" x14ac:dyDescent="0.2">
+        <v>758</v>
+      </c>
+    </row>
+    <row r="1217" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1217" s="10" t="s">
-        <v>775</v>
-      </c>
-      <c r="B1217" s="9" t="s">
-        <v>312</v>
+        <v>759</v>
+      </c>
+      <c r="B1217" s="7" t="s">
+        <v>760</v>
       </c>
     </row>
     <row r="1218" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1218" s="10" t="s">
-        <v>776</v>
+        <v>761</v>
       </c>
       <c r="B1218" s="7" t="s">
-        <v>777</v>
+        <v>762</v>
       </c>
     </row>
     <row r="1219" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1219" s="10" t="s">
-        <v>778</v>
+        <v>763</v>
       </c>
       <c r="B1219" s="7" t="s">
-        <v>308</v>
+        <v>764</v>
       </c>
     </row>
     <row r="1220" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1220" s="10" t="s">
-        <v>779</v>
+        <v>765</v>
       </c>
       <c r="B1220" s="7" t="s">
-        <v>780</v>
+        <v>766</v>
       </c>
     </row>
     <row r="1221" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1221" s="10" t="s">
-        <v>781</v>
+        <v>767</v>
       </c>
       <c r="B1221" s="7" t="s">
-        <v>782</v>
+        <v>304</v>
       </c>
     </row>
     <row r="1222" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1222" s="10" t="s">
-        <v>783</v>
+        <v>768</v>
       </c>
       <c r="B1222" s="7" t="s">
-        <v>784</v>
+        <v>769</v>
       </c>
     </row>
     <row r="1223" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1223" s="10" t="s">
+        <v>770</v>
+      </c>
+      <c r="B1223" s="7" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="1224" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1224" s="10" t="s">
+        <v>771</v>
+      </c>
+      <c r="B1224" s="7" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="1225" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1225" s="10" t="s">
+        <v>772</v>
+      </c>
+      <c r="B1225" s="7" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="1226" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1226" s="10" t="s">
+        <v>773</v>
+      </c>
+      <c r="B1226" s="7" t="s">
+        <v>774</v>
+      </c>
+    </row>
+    <row r="1227" spans="1:2" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A1227" s="10" t="s">
+        <v>775</v>
+      </c>
+      <c r="B1227" s="9" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="1228" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1228" s="10" t="s">
+        <v>776</v>
+      </c>
+      <c r="B1228" s="7" t="s">
+        <v>777</v>
+      </c>
+    </row>
+    <row r="1229" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1229" s="10" t="s">
+        <v>778</v>
+      </c>
+      <c r="B1229" s="7" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="1230" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1230" s="10" t="s">
+        <v>779</v>
+      </c>
+      <c r="B1230" s="7" t="s">
+        <v>780</v>
+      </c>
+    </row>
+    <row r="1231" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1231" s="10" t="s">
+        <v>781</v>
+      </c>
+      <c r="B1231" s="7" t="s">
+        <v>782</v>
+      </c>
+    </row>
+    <row r="1232" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1232" s="10" t="s">
+        <v>783</v>
+      </c>
+      <c r="B1232" s="7" t="s">
+        <v>784</v>
+      </c>
+    </row>
+    <row r="1233" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1233" s="10" t="s">
         <v>785</v>
       </c>
-      <c r="B1223" s="7" t="s">
+      <c r="B1233" s="7" t="s">
         <v>786</v>
       </c>
     </row>
-    <row r="1224" spans="1:2" ht="22.5" x14ac:dyDescent="0.2">
-      <c r="A1224" s="10" t="s">
+    <row r="1234" spans="1:2" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A1234" s="10" t="s">
         <v>787</v>
       </c>
-      <c r="B1224" s="7" t="s">
+      <c r="B1234" s="7" t="s">
         <v>788</v>
       </c>
     </row>

</xml_diff>